<commit_message>
Atualizaçao do arquivo planexamento.xlsx
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -385,15 +385,15 @@
   </sheetPr>
   <dimension ref="A1:K204"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D10" activeCellId="1" sqref="I10 D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -604,7 +604,9 @@
         <v>43865</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="9" t="n">
+        <v>0.0673611111111111</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -3930,10 +3932,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="I10 D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4178,18 +4180,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:MB9"/>
+  <dimension ref="A1:MB10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="16" style="0" width="6.71"/>
@@ -5337,6 +5339,11 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Atualizaçao do do planejamento e segundo arquivo de if_else
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve">não precisou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
   <si>
     <t xml:space="preserve">assunto</t>
@@ -217,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,6 +279,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -383,17 +390,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K204"/>
+  <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" activeCellId="1" sqref="I10 D10"/>
+      <selection pane="bottomRight" activeCell="D205" activeCellId="0" sqref="D205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -623,7 +630,9 @@
         <v>43866</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="9" t="n">
+        <v>0.141666666666667</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -3912,6 +3921,47 @@
       <c r="I204" s="7"/>
       <c r="J204" s="14"/>
       <c r="K204" s="14"/>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C205" s="15" t="n">
+        <f aca="false">SUM(C2:C204)</f>
+        <v>0.424305555555556</v>
+      </c>
+      <c r="D205" s="15" t="n">
+        <f aca="false">SUM(D2:D204)</f>
+        <v>0.55625</v>
+      </c>
+      <c r="E205" s="15" t="n">
+        <f aca="false">SUM(E2:E204)</f>
+        <v>0</v>
+      </c>
+      <c r="F205" s="15" t="n">
+        <f aca="false">SUM(F2:F204)</f>
+        <v>0</v>
+      </c>
+      <c r="G205" s="15" t="n">
+        <f aca="false">SUM(G2:G204)</f>
+        <v>0</v>
+      </c>
+      <c r="H205" s="15" t="n">
+        <f aca="false">SUM(H2:H204)</f>
+        <v>0</v>
+      </c>
+      <c r="I205" s="15" t="n">
+        <f aca="false">SUM(I2:I204)</f>
+        <v>0</v>
+      </c>
+      <c r="J205" s="15" t="n">
+        <f aca="false">SUM(J2:J204)</f>
+        <v>0</v>
+      </c>
+      <c r="K205" s="15" t="n">
+        <f aca="false">SUM(K2:K204)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3932,31 +3982,31 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="I10 D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="15" t="n">
+    <row r="1" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="16" t="n">
         <v>200</v>
       </c>
-      <c r="E1" s="15" t="n">
+      <c r="E1" s="16" t="n">
         <v>300</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>14</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,7 +4016,7 @@
       <c r="B2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="19" t="n">
         <f aca="false">B2/$B$11</f>
         <v>0.0207715133531157</v>
       </c>
@@ -3981,7 +4031,7 @@
       <c r="F2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="19" t="n">
+      <c r="G2" s="20" t="n">
         <f aca="false">D2-F2</f>
         <v>1</v>
       </c>
@@ -3993,7 +4043,7 @@
       <c r="B3" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="C3" s="18" t="n">
+      <c r="C3" s="19" t="n">
         <f aca="false">B3/$B$11</f>
         <v>0.154302670623145</v>
       </c>
@@ -4013,7 +4063,7 @@
       <c r="B4" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="C4" s="18" t="n">
+      <c r="C4" s="19" t="n">
         <f aca="false">B4/$B$11</f>
         <v>0.112759643916914</v>
       </c>
@@ -4033,7 +4083,7 @@
       <c r="B5" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="C5" s="19" t="n">
         <f aca="false">B5/$B$11</f>
         <v>0.106824925816024</v>
       </c>
@@ -4053,7 +4103,7 @@
       <c r="B6" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C6" s="18" t="n">
+      <c r="C6" s="19" t="n">
         <f aca="false">B6/$B$11</f>
         <v>0.124629080118694</v>
       </c>
@@ -4073,7 +4123,7 @@
       <c r="B7" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="19" t="n">
         <f aca="false">B7/$B$11</f>
         <v>0.0534124629080119</v>
       </c>
@@ -4093,7 +4143,7 @@
       <c r="B8" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="C8" s="18" t="n">
+      <c r="C8" s="19" t="n">
         <f aca="false">B8/$B$11</f>
         <v>0.189910979228487</v>
       </c>
@@ -4113,7 +4163,7 @@
       <c r="B9" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C9" s="18" t="n">
+      <c r="C9" s="19" t="n">
         <f aca="false">B9/$B$11</f>
         <v>0.0949554896142433</v>
       </c>
@@ -4133,7 +4183,7 @@
       <c r="B10" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="C10" s="18" t="n">
+      <c r="C10" s="19" t="n">
         <f aca="false">B10/$B$11</f>
         <v>0.142433234421365</v>
       </c>
@@ -4147,19 +4197,19 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="15" t="n">
+      <c r="B11" s="16" t="n">
         <f aca="false">SUM(B2:B10)</f>
         <v>337</v>
       </c>
-      <c r="C11" s="16" t="n">
+      <c r="C11" s="17" t="n">
         <f aca="false">B11/$B$11</f>
         <v>1</v>
       </c>
-      <c r="D11" s="15" t="n">
+      <c r="D11" s="16" t="n">
         <f aca="false">SUM(D2:D10)</f>
         <v>203</v>
       </c>
-      <c r="E11" s="15" t="n">
+      <c r="E11" s="16" t="n">
         <f aca="false">SUM(E2:E10)</f>
         <v>305</v>
       </c>
@@ -4180,13 +4230,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:MB10"/>
+  <dimension ref="A1:MB11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -4242,1106 +4292,1111 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="n">
+      <c r="A1" s="21" t="n">
         <v>43857</v>
       </c>
-      <c r="B1" s="20" t="n">
+      <c r="B1" s="21" t="n">
         <v>43858</v>
       </c>
-      <c r="C1" s="20" t="n">
+      <c r="C1" s="21" t="n">
         <v>43859</v>
       </c>
-      <c r="D1" s="20" t="n">
+      <c r="D1" s="21" t="n">
         <v>43860</v>
       </c>
-      <c r="E1" s="20" t="n">
+      <c r="E1" s="21" t="n">
         <v>43861</v>
       </c>
-      <c r="F1" s="20" t="n">
+      <c r="F1" s="21" t="n">
         <v>43862</v>
       </c>
-      <c r="G1" s="20" t="n">
+      <c r="G1" s="21" t="n">
         <v>43863</v>
       </c>
-      <c r="H1" s="20" t="n">
+      <c r="H1" s="21" t="n">
         <v>43864</v>
       </c>
-      <c r="I1" s="20" t="n">
+      <c r="I1" s="21" t="n">
         <v>43865</v>
       </c>
-      <c r="J1" s="20" t="n">
+      <c r="J1" s="21" t="n">
         <v>43866</v>
       </c>
-      <c r="K1" s="20" t="n">
+      <c r="K1" s="21" t="n">
         <v>43867</v>
       </c>
-      <c r="L1" s="20" t="n">
+      <c r="L1" s="21" t="n">
         <v>43868</v>
       </c>
-      <c r="M1" s="20" t="n">
+      <c r="M1" s="21" t="n">
         <v>43869</v>
       </c>
-      <c r="N1" s="20" t="n">
+      <c r="N1" s="21" t="n">
         <v>43870</v>
       </c>
-      <c r="O1" s="20" t="n">
+      <c r="O1" s="21" t="n">
         <v>43871</v>
       </c>
-      <c r="P1" s="20" t="n">
+      <c r="P1" s="21" t="n">
         <v>43872</v>
       </c>
-      <c r="Q1" s="20" t="n">
+      <c r="Q1" s="21" t="n">
         <v>43873</v>
       </c>
-      <c r="R1" s="20" t="n">
+      <c r="R1" s="21" t="n">
         <v>43874</v>
       </c>
-      <c r="S1" s="20" t="n">
+      <c r="S1" s="21" t="n">
         <v>43875</v>
       </c>
-      <c r="T1" s="20" t="n">
+      <c r="T1" s="21" t="n">
         <v>43876</v>
       </c>
-      <c r="U1" s="20" t="n">
+      <c r="U1" s="21" t="n">
         <v>43877</v>
       </c>
-      <c r="V1" s="20" t="n">
+      <c r="V1" s="21" t="n">
         <v>43878</v>
       </c>
-      <c r="W1" s="20" t="n">
+      <c r="W1" s="21" t="n">
         <v>43879</v>
       </c>
-      <c r="X1" s="20" t="n">
+      <c r="X1" s="21" t="n">
         <v>43880</v>
       </c>
-      <c r="Y1" s="20" t="n">
+      <c r="Y1" s="21" t="n">
         <v>43881</v>
       </c>
-      <c r="Z1" s="20" t="n">
+      <c r="Z1" s="21" t="n">
         <v>43882</v>
       </c>
-      <c r="AA1" s="20" t="n">
+      <c r="AA1" s="21" t="n">
         <v>43883</v>
       </c>
-      <c r="AB1" s="20" t="n">
+      <c r="AB1" s="21" t="n">
         <v>43884</v>
       </c>
-      <c r="AC1" s="20" t="n">
+      <c r="AC1" s="21" t="n">
         <v>43885</v>
       </c>
-      <c r="AD1" s="20" t="n">
+      <c r="AD1" s="21" t="n">
         <v>43886</v>
       </c>
-      <c r="AE1" s="20" t="n">
+      <c r="AE1" s="21" t="n">
         <v>43887</v>
       </c>
-      <c r="AF1" s="20" t="n">
+      <c r="AF1" s="21" t="n">
         <v>43888</v>
       </c>
-      <c r="AG1" s="20" t="n">
+      <c r="AG1" s="21" t="n">
         <v>43889</v>
       </c>
-      <c r="AH1" s="20" t="n">
+      <c r="AH1" s="21" t="n">
         <v>43890</v>
       </c>
-      <c r="AI1" s="20" t="n">
+      <c r="AI1" s="21" t="n">
         <v>43891</v>
       </c>
-      <c r="AJ1" s="20" t="n">
+      <c r="AJ1" s="21" t="n">
         <v>43892</v>
       </c>
-      <c r="AK1" s="20" t="n">
+      <c r="AK1" s="21" t="n">
         <v>43893</v>
       </c>
-      <c r="AL1" s="20" t="n">
+      <c r="AL1" s="21" t="n">
         <v>43894</v>
       </c>
-      <c r="AM1" s="20" t="n">
+      <c r="AM1" s="21" t="n">
         <v>43895</v>
       </c>
-      <c r="AN1" s="20" t="n">
+      <c r="AN1" s="21" t="n">
         <v>43896</v>
       </c>
-      <c r="AO1" s="20" t="n">
+      <c r="AO1" s="21" t="n">
         <v>43897</v>
       </c>
-      <c r="AP1" s="20" t="n">
+      <c r="AP1" s="21" t="n">
         <v>43898</v>
       </c>
-      <c r="AQ1" s="20" t="n">
+      <c r="AQ1" s="21" t="n">
         <v>43899</v>
       </c>
-      <c r="AR1" s="20" t="n">
+      <c r="AR1" s="21" t="n">
         <v>43900</v>
       </c>
-      <c r="AS1" s="20" t="n">
+      <c r="AS1" s="21" t="n">
         <v>43901</v>
       </c>
-      <c r="AT1" s="20" t="n">
+      <c r="AT1" s="21" t="n">
         <v>43902</v>
       </c>
-      <c r="AU1" s="20" t="n">
+      <c r="AU1" s="21" t="n">
         <v>43903</v>
       </c>
-      <c r="AV1" s="20" t="n">
+      <c r="AV1" s="21" t="n">
         <v>43904</v>
       </c>
-      <c r="AW1" s="20" t="n">
+      <c r="AW1" s="21" t="n">
         <v>43905</v>
       </c>
-      <c r="AX1" s="20" t="n">
+      <c r="AX1" s="21" t="n">
         <v>43906</v>
       </c>
-      <c r="AY1" s="20" t="n">
+      <c r="AY1" s="21" t="n">
         <v>43907</v>
       </c>
-      <c r="AZ1" s="20" t="n">
+      <c r="AZ1" s="21" t="n">
         <v>43908</v>
       </c>
-      <c r="BA1" s="20" t="n">
+      <c r="BA1" s="21" t="n">
         <v>43909</v>
       </c>
-      <c r="BB1" s="20" t="n">
+      <c r="BB1" s="21" t="n">
         <v>43910</v>
       </c>
-      <c r="BC1" s="20" t="n">
+      <c r="BC1" s="21" t="n">
         <v>43911</v>
       </c>
-      <c r="BD1" s="20" t="n">
+      <c r="BD1" s="21" t="n">
         <v>43912</v>
       </c>
-      <c r="BE1" s="20" t="n">
+      <c r="BE1" s="21" t="n">
         <v>43913</v>
       </c>
-      <c r="BF1" s="20" t="n">
+      <c r="BF1" s="21" t="n">
         <v>43914</v>
       </c>
-      <c r="BG1" s="20" t="n">
+      <c r="BG1" s="21" t="n">
         <v>43915</v>
       </c>
-      <c r="BH1" s="20" t="n">
+      <c r="BH1" s="21" t="n">
         <v>43916</v>
       </c>
-      <c r="BI1" s="20" t="n">
+      <c r="BI1" s="21" t="n">
         <v>43917</v>
       </c>
-      <c r="BJ1" s="20" t="n">
+      <c r="BJ1" s="21" t="n">
         <v>43918</v>
       </c>
-      <c r="BK1" s="20" t="n">
+      <c r="BK1" s="21" t="n">
         <v>43919</v>
       </c>
-      <c r="BL1" s="20" t="n">
+      <c r="BL1" s="21" t="n">
         <v>43920</v>
       </c>
-      <c r="BM1" s="20" t="n">
+      <c r="BM1" s="21" t="n">
         <v>43921</v>
       </c>
-      <c r="BN1" s="20" t="n">
+      <c r="BN1" s="21" t="n">
         <v>43922</v>
       </c>
-      <c r="BO1" s="20" t="n">
+      <c r="BO1" s="21" t="n">
         <v>43923</v>
       </c>
-      <c r="BP1" s="20" t="n">
+      <c r="BP1" s="21" t="n">
         <v>43924</v>
       </c>
-      <c r="BQ1" s="20" t="n">
+      <c r="BQ1" s="21" t="n">
         <v>43925</v>
       </c>
-      <c r="BR1" s="20" t="n">
+      <c r="BR1" s="21" t="n">
         <v>43926</v>
       </c>
-      <c r="BS1" s="20" t="n">
+      <c r="BS1" s="21" t="n">
         <v>43927</v>
       </c>
-      <c r="BT1" s="20" t="n">
+      <c r="BT1" s="21" t="n">
         <v>43928</v>
       </c>
-      <c r="BU1" s="20" t="n">
+      <c r="BU1" s="21" t="n">
         <v>43929</v>
       </c>
-      <c r="BV1" s="20" t="n">
+      <c r="BV1" s="21" t="n">
         <v>43930</v>
       </c>
-      <c r="BW1" s="20" t="n">
+      <c r="BW1" s="21" t="n">
         <v>43931</v>
       </c>
-      <c r="BX1" s="20" t="n">
+      <c r="BX1" s="21" t="n">
         <v>43932</v>
       </c>
-      <c r="BY1" s="20" t="n">
+      <c r="BY1" s="21" t="n">
         <v>43933</v>
       </c>
-      <c r="BZ1" s="20" t="n">
+      <c r="BZ1" s="21" t="n">
         <v>43934</v>
       </c>
-      <c r="CA1" s="20" t="n">
+      <c r="CA1" s="21" t="n">
         <v>43935</v>
       </c>
-      <c r="CB1" s="20" t="n">
+      <c r="CB1" s="21" t="n">
         <v>43936</v>
       </c>
-      <c r="CC1" s="20" t="n">
+      <c r="CC1" s="21" t="n">
         <v>43937</v>
       </c>
-      <c r="CD1" s="20" t="n">
+      <c r="CD1" s="21" t="n">
         <v>43938</v>
       </c>
-      <c r="CE1" s="20" t="n">
+      <c r="CE1" s="21" t="n">
         <v>43939</v>
       </c>
-      <c r="CF1" s="20" t="n">
+      <c r="CF1" s="21" t="n">
         <v>43940</v>
       </c>
-      <c r="CG1" s="20" t="n">
+      <c r="CG1" s="21" t="n">
         <v>43941</v>
       </c>
-      <c r="CH1" s="20" t="n">
+      <c r="CH1" s="21" t="n">
         <v>43942</v>
       </c>
-      <c r="CI1" s="20" t="n">
+      <c r="CI1" s="21" t="n">
         <v>43943</v>
       </c>
-      <c r="CJ1" s="20" t="n">
+      <c r="CJ1" s="21" t="n">
         <v>43944</v>
       </c>
-      <c r="CK1" s="20" t="n">
+      <c r="CK1" s="21" t="n">
         <v>43945</v>
       </c>
-      <c r="CL1" s="20" t="n">
+      <c r="CL1" s="21" t="n">
         <v>43946</v>
       </c>
-      <c r="CM1" s="20" t="n">
+      <c r="CM1" s="21" t="n">
         <v>43947</v>
       </c>
-      <c r="CN1" s="20" t="n">
+      <c r="CN1" s="21" t="n">
         <v>43948</v>
       </c>
-      <c r="CO1" s="20" t="n">
+      <c r="CO1" s="21" t="n">
         <v>43949</v>
       </c>
-      <c r="CP1" s="20" t="n">
+      <c r="CP1" s="21" t="n">
         <v>43950</v>
       </c>
-      <c r="CQ1" s="20" t="n">
+      <c r="CQ1" s="21" t="n">
         <v>43951</v>
       </c>
-      <c r="CR1" s="20" t="n">
+      <c r="CR1" s="21" t="n">
         <v>43952</v>
       </c>
-      <c r="CS1" s="20" t="n">
+      <c r="CS1" s="21" t="n">
         <v>43953</v>
       </c>
-      <c r="CT1" s="20" t="n">
+      <c r="CT1" s="21" t="n">
         <v>43954</v>
       </c>
-      <c r="CU1" s="20" t="n">
+      <c r="CU1" s="21" t="n">
         <v>43955</v>
       </c>
-      <c r="CV1" s="20" t="n">
+      <c r="CV1" s="21" t="n">
         <v>43956</v>
       </c>
-      <c r="CW1" s="20" t="n">
+      <c r="CW1" s="21" t="n">
         <v>43957</v>
       </c>
-      <c r="CX1" s="20" t="n">
+      <c r="CX1" s="21" t="n">
         <v>43958</v>
       </c>
-      <c r="CY1" s="20" t="n">
+      <c r="CY1" s="21" t="n">
         <v>43959</v>
       </c>
-      <c r="CZ1" s="20" t="n">
+      <c r="CZ1" s="21" t="n">
         <v>43960</v>
       </c>
-      <c r="DA1" s="20" t="n">
+      <c r="DA1" s="21" t="n">
         <v>43961</v>
       </c>
-      <c r="DB1" s="20" t="n">
+      <c r="DB1" s="21" t="n">
         <v>43962</v>
       </c>
-      <c r="DC1" s="20" t="n">
+      <c r="DC1" s="21" t="n">
         <v>43963</v>
       </c>
-      <c r="DD1" s="20" t="n">
+      <c r="DD1" s="21" t="n">
         <v>43964</v>
       </c>
-      <c r="DE1" s="20" t="n">
+      <c r="DE1" s="21" t="n">
         <v>43965</v>
       </c>
-      <c r="DF1" s="20" t="n">
+      <c r="DF1" s="21" t="n">
         <v>43966</v>
       </c>
-      <c r="DG1" s="20" t="n">
+      <c r="DG1" s="21" t="n">
         <v>43967</v>
       </c>
-      <c r="DH1" s="20" t="n">
+      <c r="DH1" s="21" t="n">
         <v>43968</v>
       </c>
-      <c r="DI1" s="20" t="n">
+      <c r="DI1" s="21" t="n">
         <v>43969</v>
       </c>
-      <c r="DJ1" s="20" t="n">
+      <c r="DJ1" s="21" t="n">
         <v>43970</v>
       </c>
-      <c r="DK1" s="20" t="n">
+      <c r="DK1" s="21" t="n">
         <v>43971</v>
       </c>
-      <c r="DL1" s="20" t="n">
+      <c r="DL1" s="21" t="n">
         <v>43972</v>
       </c>
-      <c r="DM1" s="20" t="n">
+      <c r="DM1" s="21" t="n">
         <v>43973</v>
       </c>
-      <c r="DN1" s="20" t="n">
+      <c r="DN1" s="21" t="n">
         <v>43974</v>
       </c>
-      <c r="DO1" s="20" t="n">
+      <c r="DO1" s="21" t="n">
         <v>43975</v>
       </c>
-      <c r="DP1" s="20" t="n">
+      <c r="DP1" s="21" t="n">
         <v>43976</v>
       </c>
-      <c r="DQ1" s="20" t="n">
+      <c r="DQ1" s="21" t="n">
         <v>43977</v>
       </c>
-      <c r="DR1" s="20" t="n">
+      <c r="DR1" s="21" t="n">
         <v>43978</v>
       </c>
-      <c r="DS1" s="20" t="n">
+      <c r="DS1" s="21" t="n">
         <v>43979</v>
       </c>
-      <c r="DT1" s="20" t="n">
+      <c r="DT1" s="21" t="n">
         <v>43980</v>
       </c>
-      <c r="DU1" s="20" t="n">
+      <c r="DU1" s="21" t="n">
         <v>43981</v>
       </c>
-      <c r="DV1" s="20" t="n">
+      <c r="DV1" s="21" t="n">
         <v>43982</v>
       </c>
-      <c r="DW1" s="20" t="n">
+      <c r="DW1" s="21" t="n">
         <v>43983</v>
       </c>
-      <c r="DX1" s="20" t="n">
+      <c r="DX1" s="21" t="n">
         <v>43984</v>
       </c>
-      <c r="DY1" s="20" t="n">
+      <c r="DY1" s="21" t="n">
         <v>43985</v>
       </c>
-      <c r="DZ1" s="20" t="n">
+      <c r="DZ1" s="21" t="n">
         <v>43986</v>
       </c>
-      <c r="EA1" s="20" t="n">
+      <c r="EA1" s="21" t="n">
         <v>43987</v>
       </c>
-      <c r="EB1" s="20" t="n">
+      <c r="EB1" s="21" t="n">
         <v>43988</v>
       </c>
-      <c r="EC1" s="20" t="n">
+      <c r="EC1" s="21" t="n">
         <v>43989</v>
       </c>
-      <c r="ED1" s="20" t="n">
+      <c r="ED1" s="21" t="n">
         <v>43990</v>
       </c>
-      <c r="EE1" s="20" t="n">
+      <c r="EE1" s="21" t="n">
         <v>43991</v>
       </c>
-      <c r="EF1" s="20" t="n">
+      <c r="EF1" s="21" t="n">
         <v>43992</v>
       </c>
-      <c r="EG1" s="20" t="n">
+      <c r="EG1" s="21" t="n">
         <v>43993</v>
       </c>
-      <c r="EH1" s="20" t="n">
+      <c r="EH1" s="21" t="n">
         <v>43994</v>
       </c>
-      <c r="EI1" s="20" t="n">
+      <c r="EI1" s="21" t="n">
         <v>43995</v>
       </c>
-      <c r="EJ1" s="20" t="n">
+      <c r="EJ1" s="21" t="n">
         <v>43996</v>
       </c>
-      <c r="EK1" s="20" t="n">
+      <c r="EK1" s="21" t="n">
         <v>43997</v>
       </c>
-      <c r="EL1" s="20" t="n">
+      <c r="EL1" s="21" t="n">
         <v>43998</v>
       </c>
-      <c r="EM1" s="20" t="n">
+      <c r="EM1" s="21" t="n">
         <v>43999</v>
       </c>
-      <c r="EN1" s="20" t="n">
+      <c r="EN1" s="21" t="n">
         <v>44000</v>
       </c>
-      <c r="EO1" s="20" t="n">
+      <c r="EO1" s="21" t="n">
         <v>44001</v>
       </c>
-      <c r="EP1" s="20" t="n">
+      <c r="EP1" s="21" t="n">
         <v>44002</v>
       </c>
-      <c r="EQ1" s="20" t="n">
+      <c r="EQ1" s="21" t="n">
         <v>44003</v>
       </c>
-      <c r="ER1" s="20" t="n">
+      <c r="ER1" s="21" t="n">
         <v>44004</v>
       </c>
-      <c r="ES1" s="20" t="n">
+      <c r="ES1" s="21" t="n">
         <v>44005</v>
       </c>
-      <c r="ET1" s="20" t="n">
+      <c r="ET1" s="21" t="n">
         <v>44006</v>
       </c>
-      <c r="EU1" s="20" t="n">
+      <c r="EU1" s="21" t="n">
         <v>44007</v>
       </c>
-      <c r="EV1" s="20" t="n">
+      <c r="EV1" s="21" t="n">
         <v>44008</v>
       </c>
-      <c r="EW1" s="20" t="n">
+      <c r="EW1" s="21" t="n">
         <v>44009</v>
       </c>
-      <c r="EX1" s="20" t="n">
+      <c r="EX1" s="21" t="n">
         <v>44010</v>
       </c>
-      <c r="EY1" s="20" t="n">
+      <c r="EY1" s="21" t="n">
         <v>44011</v>
       </c>
-      <c r="EZ1" s="20" t="n">
+      <c r="EZ1" s="21" t="n">
         <v>44012</v>
       </c>
-      <c r="FA1" s="20" t="n">
+      <c r="FA1" s="21" t="n">
         <v>44013</v>
       </c>
-      <c r="FB1" s="20" t="n">
+      <c r="FB1" s="21" t="n">
         <v>44014</v>
       </c>
-      <c r="FC1" s="20" t="n">
+      <c r="FC1" s="21" t="n">
         <v>44015</v>
       </c>
-      <c r="FD1" s="20" t="n">
+      <c r="FD1" s="21" t="n">
         <v>44016</v>
       </c>
-      <c r="FE1" s="20" t="n">
+      <c r="FE1" s="21" t="n">
         <v>44017</v>
       </c>
-      <c r="FF1" s="20" t="n">
+      <c r="FF1" s="21" t="n">
         <v>44018</v>
       </c>
-      <c r="FG1" s="20" t="n">
+      <c r="FG1" s="21" t="n">
         <v>44019</v>
       </c>
-      <c r="FH1" s="20" t="n">
+      <c r="FH1" s="21" t="n">
         <v>44020</v>
       </c>
-      <c r="FI1" s="20" t="n">
+      <c r="FI1" s="21" t="n">
         <v>44021</v>
       </c>
-      <c r="FJ1" s="20" t="n">
+      <c r="FJ1" s="21" t="n">
         <v>44022</v>
       </c>
-      <c r="FK1" s="20" t="n">
+      <c r="FK1" s="21" t="n">
         <v>44023</v>
       </c>
-      <c r="FL1" s="20" t="n">
+      <c r="FL1" s="21" t="n">
         <v>44024</v>
       </c>
-      <c r="FM1" s="20" t="n">
+      <c r="FM1" s="21" t="n">
         <v>44025</v>
       </c>
-      <c r="FN1" s="20" t="n">
+      <c r="FN1" s="21" t="n">
         <v>44026</v>
       </c>
-      <c r="FO1" s="20" t="n">
+      <c r="FO1" s="21" t="n">
         <v>44027</v>
       </c>
-      <c r="FP1" s="20" t="n">
+      <c r="FP1" s="21" t="n">
         <v>44028</v>
       </c>
-      <c r="FQ1" s="20" t="n">
+      <c r="FQ1" s="21" t="n">
         <v>44029</v>
       </c>
-      <c r="FR1" s="20" t="n">
+      <c r="FR1" s="21" t="n">
         <v>44030</v>
       </c>
-      <c r="FS1" s="20" t="n">
+      <c r="FS1" s="21" t="n">
         <v>44031</v>
       </c>
-      <c r="FT1" s="20" t="n">
+      <c r="FT1" s="21" t="n">
         <v>44032</v>
       </c>
-      <c r="FU1" s="20" t="n">
+      <c r="FU1" s="21" t="n">
         <v>44033</v>
       </c>
-      <c r="FV1" s="20" t="n">
+      <c r="FV1" s="21" t="n">
         <v>44034</v>
       </c>
-      <c r="FW1" s="20" t="n">
+      <c r="FW1" s="21" t="n">
         <v>44035</v>
       </c>
-      <c r="FX1" s="20" t="n">
+      <c r="FX1" s="21" t="n">
         <v>44036</v>
       </c>
-      <c r="FY1" s="20" t="n">
+      <c r="FY1" s="21" t="n">
         <v>44037</v>
       </c>
-      <c r="FZ1" s="20" t="n">
+      <c r="FZ1" s="21" t="n">
         <v>44038</v>
       </c>
-      <c r="GA1" s="20" t="n">
+      <c r="GA1" s="21" t="n">
         <v>44039</v>
       </c>
-      <c r="GB1" s="20" t="n">
+      <c r="GB1" s="21" t="n">
         <v>44040</v>
       </c>
-      <c r="GC1" s="20" t="n">
+      <c r="GC1" s="21" t="n">
         <v>44041</v>
       </c>
-      <c r="GD1" s="20" t="n">
+      <c r="GD1" s="21" t="n">
         <v>44042</v>
       </c>
-      <c r="GE1" s="20" t="n">
+      <c r="GE1" s="21" t="n">
         <v>44043</v>
       </c>
-      <c r="GF1" s="20" t="n">
+      <c r="GF1" s="21" t="n">
         <v>44044</v>
       </c>
-      <c r="GG1" s="20" t="n">
+      <c r="GG1" s="21" t="n">
         <v>44045</v>
       </c>
-      <c r="GH1" s="20" t="n">
+      <c r="GH1" s="21" t="n">
         <v>44046</v>
       </c>
-      <c r="GI1" s="20" t="n">
+      <c r="GI1" s="21" t="n">
         <v>44047</v>
       </c>
-      <c r="GJ1" s="20" t="n">
+      <c r="GJ1" s="21" t="n">
         <v>44048</v>
       </c>
-      <c r="GK1" s="20" t="n">
+      <c r="GK1" s="21" t="n">
         <v>44049</v>
       </c>
-      <c r="GL1" s="20" t="n">
+      <c r="GL1" s="21" t="n">
         <v>44050</v>
       </c>
-      <c r="GM1" s="20" t="n">
+      <c r="GM1" s="21" t="n">
         <v>44051</v>
       </c>
-      <c r="GN1" s="20" t="n">
+      <c r="GN1" s="21" t="n">
         <v>44052</v>
       </c>
-      <c r="GO1" s="20" t="n">
+      <c r="GO1" s="21" t="n">
         <v>44053</v>
       </c>
-      <c r="GP1" s="20" t="n">
+      <c r="GP1" s="21" t="n">
         <v>44054</v>
       </c>
-      <c r="GQ1" s="20" t="n">
+      <c r="GQ1" s="21" t="n">
         <v>44055</v>
       </c>
-      <c r="GR1" s="20" t="n">
+      <c r="GR1" s="21" t="n">
         <v>44056</v>
       </c>
-      <c r="GS1" s="20" t="n">
+      <c r="GS1" s="21" t="n">
         <v>44057</v>
       </c>
-      <c r="GT1" s="20" t="n">
+      <c r="GT1" s="21" t="n">
         <v>44058</v>
       </c>
-      <c r="GU1" s="20" t="n">
+      <c r="GU1" s="21" t="n">
         <v>44059</v>
       </c>
-      <c r="GV1" s="20" t="n">
+      <c r="GV1" s="21" t="n">
         <v>44060</v>
       </c>
-      <c r="GW1" s="20" t="n">
+      <c r="GW1" s="21" t="n">
         <v>44061</v>
       </c>
-      <c r="GX1" s="20" t="n">
+      <c r="GX1" s="21" t="n">
         <v>44062</v>
       </c>
-      <c r="GY1" s="20" t="n">
+      <c r="GY1" s="21" t="n">
         <v>44063</v>
       </c>
-      <c r="GZ1" s="20" t="n">
+      <c r="GZ1" s="21" t="n">
         <v>44064</v>
       </c>
-      <c r="HA1" s="20" t="n">
+      <c r="HA1" s="21" t="n">
         <v>44065</v>
       </c>
-      <c r="HB1" s="20" t="n">
+      <c r="HB1" s="21" t="n">
         <v>44066</v>
       </c>
-      <c r="HC1" s="20" t="n">
+      <c r="HC1" s="21" t="n">
         <v>44067</v>
       </c>
-      <c r="HD1" s="20" t="n">
+      <c r="HD1" s="21" t="n">
         <v>44068</v>
       </c>
-      <c r="HE1" s="20" t="n">
+      <c r="HE1" s="21" t="n">
         <v>44069</v>
       </c>
-      <c r="HF1" s="20" t="n">
+      <c r="HF1" s="21" t="n">
         <v>44070</v>
       </c>
-      <c r="HG1" s="20" t="n">
+      <c r="HG1" s="21" t="n">
         <v>44071</v>
       </c>
-      <c r="HH1" s="20" t="n">
+      <c r="HH1" s="21" t="n">
         <v>44072</v>
       </c>
-      <c r="HI1" s="20" t="n">
+      <c r="HI1" s="21" t="n">
         <v>44073</v>
       </c>
-      <c r="HJ1" s="20" t="n">
+      <c r="HJ1" s="21" t="n">
         <v>44074</v>
       </c>
-      <c r="HK1" s="20" t="n">
+      <c r="HK1" s="21" t="n">
         <v>44075</v>
       </c>
-      <c r="HL1" s="20" t="n">
+      <c r="HL1" s="21" t="n">
         <v>44076</v>
       </c>
-      <c r="HM1" s="20" t="n">
+      <c r="HM1" s="21" t="n">
         <v>44077</v>
       </c>
-      <c r="HN1" s="20" t="n">
+      <c r="HN1" s="21" t="n">
         <v>44078</v>
       </c>
-      <c r="HO1" s="20" t="n">
+      <c r="HO1" s="21" t="n">
         <v>44079</v>
       </c>
-      <c r="HP1" s="20" t="n">
+      <c r="HP1" s="21" t="n">
         <v>44080</v>
       </c>
-      <c r="HQ1" s="20" t="n">
+      <c r="HQ1" s="21" t="n">
         <v>44081</v>
       </c>
-      <c r="HR1" s="20" t="n">
+      <c r="HR1" s="21" t="n">
         <v>44082</v>
       </c>
-      <c r="HS1" s="20" t="n">
+      <c r="HS1" s="21" t="n">
         <v>44083</v>
       </c>
-      <c r="HT1" s="20" t="n">
+      <c r="HT1" s="21" t="n">
         <v>44084</v>
       </c>
-      <c r="HU1" s="20" t="n">
+      <c r="HU1" s="21" t="n">
         <v>44085</v>
       </c>
-      <c r="HV1" s="20" t="n">
+      <c r="HV1" s="21" t="n">
         <v>44086</v>
       </c>
-      <c r="HW1" s="20" t="n">
+      <c r="HW1" s="21" t="n">
         <v>44087</v>
       </c>
-      <c r="HX1" s="20" t="n">
+      <c r="HX1" s="21" t="n">
         <v>44088</v>
       </c>
-      <c r="HY1" s="20" t="n">
+      <c r="HY1" s="21" t="n">
         <v>44089</v>
       </c>
-      <c r="HZ1" s="20" t="n">
+      <c r="HZ1" s="21" t="n">
         <v>44090</v>
       </c>
-      <c r="IA1" s="20" t="n">
+      <c r="IA1" s="21" t="n">
         <v>44091</v>
       </c>
-      <c r="IB1" s="20" t="n">
+      <c r="IB1" s="21" t="n">
         <v>44092</v>
       </c>
-      <c r="IC1" s="20" t="n">
+      <c r="IC1" s="21" t="n">
         <v>44093</v>
       </c>
-      <c r="ID1" s="20" t="n">
+      <c r="ID1" s="21" t="n">
         <v>44094</v>
       </c>
-      <c r="IE1" s="20" t="n">
+      <c r="IE1" s="21" t="n">
         <v>44095</v>
       </c>
-      <c r="IF1" s="20" t="n">
+      <c r="IF1" s="21" t="n">
         <v>44096</v>
       </c>
-      <c r="IG1" s="20" t="n">
+      <c r="IG1" s="21" t="n">
         <v>44097</v>
       </c>
-      <c r="IH1" s="20" t="n">
+      <c r="IH1" s="21" t="n">
         <v>44098</v>
       </c>
-      <c r="II1" s="20" t="n">
+      <c r="II1" s="21" t="n">
         <v>44099</v>
       </c>
-      <c r="IJ1" s="20" t="n">
+      <c r="IJ1" s="21" t="n">
         <v>44100</v>
       </c>
-      <c r="IK1" s="20" t="n">
+      <c r="IK1" s="21" t="n">
         <v>44101</v>
       </c>
-      <c r="IL1" s="20" t="n">
+      <c r="IL1" s="21" t="n">
         <v>44102</v>
       </c>
-      <c r="IM1" s="20" t="n">
+      <c r="IM1" s="21" t="n">
         <v>44103</v>
       </c>
-      <c r="IN1" s="20" t="n">
+      <c r="IN1" s="21" t="n">
         <v>44104</v>
       </c>
-      <c r="IO1" s="20" t="n">
+      <c r="IO1" s="21" t="n">
         <v>44105</v>
       </c>
-      <c r="IP1" s="20" t="n">
+      <c r="IP1" s="21" t="n">
         <v>44106</v>
       </c>
-      <c r="IQ1" s="20" t="n">
+      <c r="IQ1" s="21" t="n">
         <v>44107</v>
       </c>
-      <c r="IR1" s="20" t="n">
+      <c r="IR1" s="21" t="n">
         <v>44108</v>
       </c>
-      <c r="IS1" s="20" t="n">
+      <c r="IS1" s="21" t="n">
         <v>44109</v>
       </c>
-      <c r="IT1" s="20" t="n">
+      <c r="IT1" s="21" t="n">
         <v>44110</v>
       </c>
-      <c r="IU1" s="20" t="n">
+      <c r="IU1" s="21" t="n">
         <v>44111</v>
       </c>
-      <c r="IV1" s="20" t="n">
+      <c r="IV1" s="21" t="n">
         <v>44112</v>
       </c>
-      <c r="IW1" s="20" t="n">
+      <c r="IW1" s="21" t="n">
         <v>44113</v>
       </c>
-      <c r="IX1" s="20" t="n">
+      <c r="IX1" s="21" t="n">
         <v>44114</v>
       </c>
-      <c r="IY1" s="20" t="n">
+      <c r="IY1" s="21" t="n">
         <v>44115</v>
       </c>
-      <c r="IZ1" s="20" t="n">
+      <c r="IZ1" s="21" t="n">
         <v>44116</v>
       </c>
-      <c r="JA1" s="20" t="n">
+      <c r="JA1" s="21" t="n">
         <v>44117</v>
       </c>
-      <c r="JB1" s="20" t="n">
+      <c r="JB1" s="21" t="n">
         <v>44118</v>
       </c>
-      <c r="JC1" s="20" t="n">
+      <c r="JC1" s="21" t="n">
         <v>44119</v>
       </c>
-      <c r="JD1" s="20" t="n">
+      <c r="JD1" s="21" t="n">
         <v>44120</v>
       </c>
-      <c r="JE1" s="20" t="n">
+      <c r="JE1" s="21" t="n">
         <v>44121</v>
       </c>
-      <c r="JF1" s="20" t="n">
+      <c r="JF1" s="21" t="n">
         <v>44122</v>
       </c>
-      <c r="JG1" s="20" t="n">
+      <c r="JG1" s="21" t="n">
         <v>44123</v>
       </c>
-      <c r="JH1" s="20" t="n">
+      <c r="JH1" s="21" t="n">
         <v>44124</v>
       </c>
-      <c r="JI1" s="20" t="n">
+      <c r="JI1" s="21" t="n">
         <v>44125</v>
       </c>
-      <c r="JJ1" s="20" t="n">
+      <c r="JJ1" s="21" t="n">
         <v>44126</v>
       </c>
-      <c r="JK1" s="20" t="n">
+      <c r="JK1" s="21" t="n">
         <v>44127</v>
       </c>
-      <c r="JL1" s="20" t="n">
+      <c r="JL1" s="21" t="n">
         <v>44128</v>
       </c>
-      <c r="JM1" s="20" t="n">
+      <c r="JM1" s="21" t="n">
         <v>44129</v>
       </c>
-      <c r="JN1" s="20" t="n">
+      <c r="JN1" s="21" t="n">
         <v>44130</v>
       </c>
-      <c r="JO1" s="20" t="n">
+      <c r="JO1" s="21" t="n">
         <v>44131</v>
       </c>
-      <c r="JP1" s="20" t="n">
+      <c r="JP1" s="21" t="n">
         <v>44132</v>
       </c>
-      <c r="JQ1" s="20" t="n">
+      <c r="JQ1" s="21" t="n">
         <v>44133</v>
       </c>
-      <c r="JR1" s="20" t="n">
+      <c r="JR1" s="21" t="n">
         <v>44134</v>
       </c>
-      <c r="JS1" s="20" t="n">
+      <c r="JS1" s="21" t="n">
         <v>44135</v>
       </c>
-      <c r="JT1" s="20" t="n">
+      <c r="JT1" s="21" t="n">
         <v>44136</v>
       </c>
-      <c r="JU1" s="20" t="n">
+      <c r="JU1" s="21" t="n">
         <v>44137</v>
       </c>
-      <c r="JV1" s="20" t="n">
+      <c r="JV1" s="21" t="n">
         <v>44138</v>
       </c>
-      <c r="JW1" s="20" t="n">
+      <c r="JW1" s="21" t="n">
         <v>44139</v>
       </c>
-      <c r="JX1" s="20" t="n">
+      <c r="JX1" s="21" t="n">
         <v>44140</v>
       </c>
-      <c r="JY1" s="20" t="n">
+      <c r="JY1" s="21" t="n">
         <v>44141</v>
       </c>
-      <c r="JZ1" s="20" t="n">
+      <c r="JZ1" s="21" t="n">
         <v>44142</v>
       </c>
-      <c r="KA1" s="20" t="n">
+      <c r="KA1" s="21" t="n">
         <v>44143</v>
       </c>
-      <c r="KB1" s="20" t="n">
+      <c r="KB1" s="21" t="n">
         <v>44144</v>
       </c>
-      <c r="KC1" s="20" t="n">
+      <c r="KC1" s="21" t="n">
         <v>44145</v>
       </c>
-      <c r="KD1" s="20" t="n">
+      <c r="KD1" s="21" t="n">
         <v>44146</v>
       </c>
-      <c r="KE1" s="20" t="n">
+      <c r="KE1" s="21" t="n">
         <v>44147</v>
       </c>
-      <c r="KF1" s="20" t="n">
+      <c r="KF1" s="21" t="n">
         <v>44148</v>
       </c>
-      <c r="KG1" s="20" t="n">
+      <c r="KG1" s="21" t="n">
         <v>44149</v>
       </c>
-      <c r="KH1" s="20" t="n">
+      <c r="KH1" s="21" t="n">
         <v>44150</v>
       </c>
-      <c r="KI1" s="20" t="n">
+      <c r="KI1" s="21" t="n">
         <v>44151</v>
       </c>
-      <c r="KJ1" s="20" t="n">
+      <c r="KJ1" s="21" t="n">
         <v>44152</v>
       </c>
-      <c r="KK1" s="20" t="n">
+      <c r="KK1" s="21" t="n">
         <v>44153</v>
       </c>
-      <c r="KL1" s="20" t="n">
+      <c r="KL1" s="21" t="n">
         <v>44154</v>
       </c>
-      <c r="KM1" s="20" t="n">
+      <c r="KM1" s="21" t="n">
         <v>44155</v>
       </c>
-      <c r="KN1" s="20" t="n">
+      <c r="KN1" s="21" t="n">
         <v>44156</v>
       </c>
-      <c r="KO1" s="20" t="n">
+      <c r="KO1" s="21" t="n">
         <v>44157</v>
       </c>
-      <c r="KP1" s="20" t="n">
+      <c r="KP1" s="21" t="n">
         <v>44158</v>
       </c>
-      <c r="KQ1" s="20" t="n">
+      <c r="KQ1" s="21" t="n">
         <v>44159</v>
       </c>
-      <c r="KR1" s="20" t="n">
+      <c r="KR1" s="21" t="n">
         <v>44160</v>
       </c>
-      <c r="KS1" s="20" t="n">
+      <c r="KS1" s="21" t="n">
         <v>44161</v>
       </c>
-      <c r="KT1" s="20" t="n">
+      <c r="KT1" s="21" t="n">
         <v>44162</v>
       </c>
-      <c r="KU1" s="20" t="n">
+      <c r="KU1" s="21" t="n">
         <v>44163</v>
       </c>
-      <c r="KV1" s="20" t="n">
+      <c r="KV1" s="21" t="n">
         <v>44164</v>
       </c>
-      <c r="KW1" s="20" t="n">
+      <c r="KW1" s="21" t="n">
         <v>44165</v>
       </c>
-      <c r="KX1" s="20" t="n">
+      <c r="KX1" s="21" t="n">
         <v>44166</v>
       </c>
-      <c r="KY1" s="20" t="n">
+      <c r="KY1" s="21" t="n">
         <v>44167</v>
       </c>
-      <c r="KZ1" s="20" t="n">
+      <c r="KZ1" s="21" t="n">
         <v>44168</v>
       </c>
-      <c r="LA1" s="20" t="n">
+      <c r="LA1" s="21" t="n">
         <v>44169</v>
       </c>
-      <c r="LB1" s="20" t="n">
+      <c r="LB1" s="21" t="n">
         <v>44170</v>
       </c>
-      <c r="LC1" s="20" t="n">
+      <c r="LC1" s="21" t="n">
         <v>44171</v>
       </c>
-      <c r="LD1" s="20" t="n">
+      <c r="LD1" s="21" t="n">
         <v>44172</v>
       </c>
-      <c r="LE1" s="20" t="n">
+      <c r="LE1" s="21" t="n">
         <v>44173</v>
       </c>
-      <c r="LF1" s="20" t="n">
+      <c r="LF1" s="21" t="n">
         <v>44174</v>
       </c>
-      <c r="LG1" s="20" t="n">
+      <c r="LG1" s="21" t="n">
         <v>44175</v>
       </c>
-      <c r="LH1" s="20" t="n">
+      <c r="LH1" s="21" t="n">
         <v>44176</v>
       </c>
-      <c r="LI1" s="20" t="n">
+      <c r="LI1" s="21" t="n">
         <v>44177</v>
       </c>
-      <c r="LJ1" s="20" t="n">
+      <c r="LJ1" s="21" t="n">
         <v>44178</v>
       </c>
-      <c r="LK1" s="20" t="n">
+      <c r="LK1" s="21" t="n">
         <v>44179</v>
       </c>
-      <c r="LL1" s="20" t="n">
+      <c r="LL1" s="21" t="n">
         <v>44180</v>
       </c>
-      <c r="LM1" s="20" t="n">
+      <c r="LM1" s="21" t="n">
         <v>44181</v>
       </c>
-      <c r="LN1" s="20" t="n">
+      <c r="LN1" s="21" t="n">
         <v>44182</v>
       </c>
-      <c r="LO1" s="20" t="n">
+      <c r="LO1" s="21" t="n">
         <v>44183</v>
       </c>
-      <c r="LP1" s="20" t="n">
+      <c r="LP1" s="21" t="n">
         <v>44184</v>
       </c>
-      <c r="LQ1" s="20" t="n">
+      <c r="LQ1" s="21" t="n">
         <v>44185</v>
       </c>
-      <c r="LR1" s="20" t="n">
+      <c r="LR1" s="21" t="n">
         <v>44186</v>
       </c>
-      <c r="LS1" s="20" t="n">
+      <c r="LS1" s="21" t="n">
         <v>44187</v>
       </c>
-      <c r="LT1" s="20" t="n">
+      <c r="LT1" s="21" t="n">
         <v>44188</v>
       </c>
-      <c r="LU1" s="20" t="n">
+      <c r="LU1" s="21" t="n">
         <v>44189</v>
       </c>
-      <c r="LV1" s="20" t="n">
+      <c r="LV1" s="21" t="n">
         <v>44190</v>
       </c>
-      <c r="LW1" s="20" t="n">
+      <c r="LW1" s="21" t="n">
         <v>44191</v>
       </c>
-      <c r="LX1" s="20" t="n">
+      <c r="LX1" s="21" t="n">
         <v>44192</v>
       </c>
-      <c r="LY1" s="20" t="n">
+      <c r="LY1" s="21" t="n">
         <v>44193</v>
       </c>
-      <c r="LZ1" s="20" t="n">
+      <c r="LZ1" s="21" t="n">
         <v>44194</v>
       </c>
-      <c r="MA1" s="20" t="n">
+      <c r="MA1" s="21" t="n">
         <v>44195</v>
       </c>
-      <c r="MB1" s="20" t="n">
+      <c r="MB1" s="21" t="n">
         <v>44196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
+      <c r="B2" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="C3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="D4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF3" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG4" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="21" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="21" t="s">
-        <v>17</v>
+      <c r="E6" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="21" t="s">
-        <v>17</v>
+      <c r="F7" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="21" t="s">
-        <v>17</v>
+      <c r="G8" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H9" s="21" t="s">
-        <v>17</v>
+      <c r="H9" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="21" t="s">
-        <v>17</v>
+      <c r="I10" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Concluido o capitulo sobre Manipulaçao de Arquivos
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Curva de ensino" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Andamento" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -80,6 +81,45 @@
   <si>
     <t xml:space="preserve">Python3 Completo</t>
   </si>
+  <si>
+    <t xml:space="preserve">dias para acabar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. cada módulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. estudados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quant dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. de lição por dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faltam – dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data prevista inicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dados planejados (alvo 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dados passados(alvo 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">média (alvo) 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 2</t>
+  </si>
 </sst>
 </file>
 
@@ -92,7 +132,7 @@
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,8 +168,47 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF00A933"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00A933"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,7 +236,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFDBB6"/>
-        <bgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -169,13 +248,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD7D7"/>
-        <bgColor rgb="FFFFDBB6"/>
+        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFFFD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFE8F2A1"/>
       </patternFill>
     </fill>
   </fills>
@@ -220,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +404,102 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,7 +512,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -342,8 +529,8 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFD7D7"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFFFD7"/>
+      <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -373,10 +560,10 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -392,15 +579,15 @@
   </sheetPr>
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -687,7 +874,9 @@
         <v>43869</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="9" t="n">
+        <v>0.129166666666667</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -3936,7 +4125,7 @@
       </c>
       <c r="D205" s="15" t="n">
         <f aca="false">SUM(D2:D204)</f>
-        <v>0.654861111111111</v>
+        <v>0.784027777777778</v>
       </c>
       <c r="E205" s="15" t="n">
         <f aca="false">SUM(E2:E204)</f>
@@ -3989,7 +4178,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4234,13 +4423,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:MB13"/>
+  <dimension ref="A1:MB14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5413,6 +5602,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5422,4 +5616,504 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="H1" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+    </row>
+    <row r="2" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="n">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="n">
+        <f aca="false">180+26</f>
+        <v>206</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="n">
+        <f aca="false">60+41</f>
+        <v>101</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="n">
+        <f aca="false">60+22</f>
+        <v>82</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="n">
+        <v>43</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="33" t="n">
+        <v>43869</v>
+      </c>
+      <c r="B11" s="34" t="n">
+        <v>47</v>
+      </c>
+      <c r="C11" s="35" t="n">
+        <f aca="false">SUM(B3:B11)</f>
+        <v>617</v>
+      </c>
+      <c r="D11" s="34" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="34" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C11/D11)</f>
+        <v>69</v>
+      </c>
+      <c r="F11" s="34" t="n">
+        <f aca="false">D$23-D11</f>
+        <v>22</v>
+      </c>
+      <c r="G11" s="33" t="n">
+        <f aca="false">$A11+F11</f>
+        <v>43891</v>
+      </c>
+      <c r="H11" s="36" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C11)/E$23)</f>
+        <v>19</v>
+      </c>
+      <c r="I11" s="37" t="n">
+        <f aca="false">$A11+H11</f>
+        <v>43888</v>
+      </c>
+      <c r="J11" s="38" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C11)/$E11)</f>
+        <v>14</v>
+      </c>
+      <c r="K11" s="39" t="n">
+        <f aca="false">$A11+J11</f>
+        <v>43883</v>
+      </c>
+      <c r="L11" s="40" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C11)/((E11+E$23)/2))</f>
+        <v>16</v>
+      </c>
+      <c r="M11" s="41" t="n">
+        <f aca="false">$A11+L11</f>
+        <v>43885</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="42" t="n">
+        <v>26</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="n">
+        <f aca="false">120+4</f>
+        <v>124</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="n">
+        <f aca="false">120+33</f>
+        <v>153</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="n">
+        <v>77</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="n">
+        <f aca="false">120+6</f>
+        <v>126</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="n">
+        <v>182</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="n">
+        <v>148</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="44" t="n">
+        <f aca="false">A11+(D23-D11)</f>
+        <v>43891</v>
+      </c>
+      <c r="B23" s="45" t="n">
+        <f aca="false">SUM(B3:B22)</f>
+        <v>1535</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45" t="n">
+        <v>31</v>
+      </c>
+      <c r="E23" s="45" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B23/D23)</f>
+        <v>50</v>
+      </c>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Terminei Capitulo sobre List e Dict Comprehension
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Faltam – dias</t>
   </si>
   <si>
-    <t xml:space="preserve">Data prevista inicial</t>
+    <t xml:space="preserve">Data térm. prevista inicial</t>
   </si>
   <si>
     <t xml:space="preserve">dados planejados (alvo 3)</t>
@@ -311,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,10 +484,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -587,7 +583,7 @@
       <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -4178,7 +4174,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4429,7 +4425,7 @@
       <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5626,10 +5622,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -5637,7 +5633,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.85"/>
@@ -5890,21 +5886,55 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
+      <c r="A12" s="33" t="n">
+        <v>43870</v>
+      </c>
       <c r="B12" s="42" t="n">
         <v>26</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
+      <c r="C12" s="35" t="n">
+        <f aca="false">C11+B12</f>
+        <v>643</v>
+      </c>
+      <c r="D12" s="34" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" s="34" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C12/D12)</f>
+        <v>65</v>
+      </c>
+      <c r="F12" s="34" t="n">
+        <f aca="false">D$23-D12</f>
+        <v>21</v>
+      </c>
+      <c r="G12" s="33" t="n">
+        <f aca="false">$A12+F12</f>
+        <v>43891</v>
+      </c>
+      <c r="H12" s="36" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C12)/E$23)</f>
+        <v>18</v>
+      </c>
+      <c r="I12" s="37" t="n">
+        <f aca="false">$A12+H12</f>
+        <v>43888</v>
+      </c>
+      <c r="J12" s="38" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C12)/$E12)</f>
+        <v>14</v>
+      </c>
+      <c r="K12" s="39" t="n">
+        <f aca="false">$A12+J12</f>
+        <v>43884</v>
+      </c>
+      <c r="L12" s="40" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C12)/((E12+E$23)/2))</f>
+        <v>16</v>
+      </c>
+      <c r="M12" s="41" t="n">
+        <f aca="false">$A12+L12</f>
+        <v>43886</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
@@ -6080,29 +6110,29 @@
       <c r="M22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44" t="n">
+      <c r="A23" s="43" t="n">
         <f aca="false">A11+(D23-D11)</f>
         <v>43891</v>
       </c>
-      <c r="B23" s="45" t="n">
+      <c r="B23" s="44" t="n">
         <f aca="false">SUM(B3:B22)</f>
         <v>1535</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45" t="n">
+      <c r="C23" s="44"/>
+      <c r="D23" s="44" t="n">
         <v>31</v>
       </c>
-      <c r="E23" s="45" t="n">
+      <c r="E23" s="44" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B23/D23)</f>
         <v>50</v>
       </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="46"/>
+      <c r="B24" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Concluido List comprehension e Iniciado Funçoes
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -575,15 +575,15 @@
   </sheetPr>
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -889,7 +889,9 @@
         <v>43870</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="10"/>
+      <c r="D15" s="9" t="n">
+        <v>0.1</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -4121,7 +4123,7 @@
       </c>
       <c r="D205" s="15" t="n">
         <f aca="false">SUM(D2:D204)</f>
-        <v>0.784027777777778</v>
+        <v>0.884027777777778</v>
       </c>
       <c r="E205" s="15" t="n">
         <f aca="false">SUM(E2:E204)</f>
@@ -4174,7 +4176,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4419,13 +4421,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:MB14"/>
+  <dimension ref="A1:MB16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5603,6 +5605,16 @@
         <v>18</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O16" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5621,11 +5633,11 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -5633,7 +5645,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.85"/>

</xml_diff>

<commit_message>
Continuando o capitulo de Funçoes
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -575,15 +575,15 @@
   </sheetPr>
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="D17" activeCellId="1" sqref="P17 D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -908,7 +908,9 @@
         <v>43871</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="9" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -4123,7 +4125,7 @@
       </c>
       <c r="D205" s="15" t="n">
         <f aca="false">SUM(D2:D204)</f>
-        <v>0.884027777777778</v>
+        <v>0.946527777777778</v>
       </c>
       <c r="E205" s="15" t="n">
         <f aca="false">SUM(E2:E204)</f>
@@ -4173,10 +4175,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="P17 D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4421,13 +4423,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:MB16"/>
+  <dimension ref="A1:MB17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5615,6 +5617,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P17" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5634,10 +5641,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="P17 C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>

</xml_diff>

<commit_message>
Exemplos da "Seçao 2 : Pacotes" inseridos
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -580,10 +580,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" activeCellId="1" sqref="P17 D17"/>
+      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -927,7 +927,9 @@
         <v>43872</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="10"/>
+      <c r="D17" s="9" t="n">
+        <v>0.0375</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -4125,7 +4127,7 @@
       </c>
       <c r="D205" s="15" t="n">
         <f aca="false">SUM(D2:D204)</f>
-        <v>0.946527777777778</v>
+        <v>0.984027777777778</v>
       </c>
       <c r="E205" s="15" t="n">
         <f aca="false">SUM(E2:E204)</f>
@@ -4175,10 +4177,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="P17 D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4423,13 +4425,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:MB17"/>
+  <dimension ref="A1:MB18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5622,6 +5624,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q18" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5640,11 +5647,11 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="P17 C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -5956,22 +5963,56 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
+      <c r="A13" s="33" t="n">
+        <v>43873</v>
+      </c>
       <c r="B13" s="4" t="n">
         <f aca="false">120+4</f>
         <v>124</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
+      <c r="C13" s="35" t="n">
+        <f aca="false">C12+B13</f>
+        <v>767</v>
+      </c>
+      <c r="D13" s="34" t="n">
+        <v>13</v>
+      </c>
+      <c r="E13" s="34" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C13/D13)</f>
+        <v>59</v>
+      </c>
+      <c r="F13" s="34" t="n">
+        <f aca="false">D$23-D13</f>
+        <v>18</v>
+      </c>
+      <c r="G13" s="33" t="n">
+        <f aca="false">$A13+F13</f>
+        <v>43891</v>
+      </c>
+      <c r="H13" s="36" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C13)/E$23)</f>
+        <v>16</v>
+      </c>
+      <c r="I13" s="37" t="n">
+        <f aca="false">$A13+H13</f>
+        <v>43889</v>
+      </c>
+      <c r="J13" s="38" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C13)/$E13)</f>
+        <v>14</v>
+      </c>
+      <c r="K13" s="39" t="n">
+        <f aca="false">$A13+J13</f>
+        <v>43887</v>
+      </c>
+      <c r="L13" s="40" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C13)/((E13+E$23)/2))</f>
+        <v>15</v>
+      </c>
+      <c r="M13" s="41" t="n">
+        <f aca="false">$A13+L13</f>
+        <v>43888</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>

</xml_diff>

<commit_message>
Testes de acesso a B3 e tetstes sobre pacotes
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -583,7 +583,7 @@
       <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -4180,7 +4180,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4431,7 +4431,7 @@
       <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5648,10 +5648,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -6015,21 +6015,55 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
+      <c r="A14" s="33" t="n">
+        <v>43873</v>
+      </c>
       <c r="B14" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
+      <c r="C14" s="35" t="n">
+        <f aca="false">C13+B14</f>
+        <v>799</v>
+      </c>
+      <c r="D14" s="34" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" s="34" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C14/D14)</f>
+        <v>62</v>
+      </c>
+      <c r="F14" s="34" t="n">
+        <f aca="false">D$23-D14</f>
+        <v>18</v>
+      </c>
+      <c r="G14" s="33" t="n">
+        <f aca="false">$A14+F14</f>
+        <v>43891</v>
+      </c>
+      <c r="H14" s="36" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C14)/E$23)</f>
+        <v>15</v>
+      </c>
+      <c r="I14" s="37" t="n">
+        <f aca="false">$A14+H14</f>
+        <v>43888</v>
+      </c>
+      <c r="J14" s="38" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C14)/$E14)</f>
+        <v>12</v>
+      </c>
+      <c r="K14" s="39" t="n">
+        <f aca="false">$A14+J14</f>
+        <v>43885</v>
+      </c>
+      <c r="L14" s="40" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C14)/((E14+E$23)/2))</f>
+        <v>14</v>
+      </c>
+      <c r="M14" s="41" t="n">
+        <f aca="false">$A14+L14</f>
+        <v>43887</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>

</xml_diff>

<commit_message>
Encerrando o modulo sobre POO
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -583,7 +583,7 @@
       <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -4180,7 +4180,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4431,7 +4431,7 @@
       <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5648,10 +5648,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -6066,22 +6066,57 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
+      <c r="A15" s="33" t="n">
+        <v>43880</v>
+      </c>
       <c r="B15" s="4" t="n">
         <f aca="false">120+33</f>
         <v>153</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
+      <c r="C15" s="35" t="n">
+        <f aca="false">C14+B15</f>
+        <v>952</v>
+      </c>
+      <c r="D15" s="34" t="n">
+        <f aca="false">D14+(A15-A14)</f>
+        <v>20</v>
+      </c>
+      <c r="E15" s="34" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C15/D15)</f>
+        <v>48</v>
+      </c>
+      <c r="F15" s="34" t="n">
+        <f aca="false">D$23-D15</f>
+        <v>11</v>
+      </c>
+      <c r="G15" s="33" t="n">
+        <f aca="false">$A15+F15</f>
+        <v>43891</v>
+      </c>
+      <c r="H15" s="36" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C15)/E$23)</f>
+        <v>12</v>
+      </c>
+      <c r="I15" s="37" t="n">
+        <f aca="false">$A15+H15</f>
+        <v>43892</v>
+      </c>
+      <c r="J15" s="38" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C15)/$E15)</f>
+        <v>13</v>
+      </c>
+      <c r="K15" s="39" t="n">
+        <f aca="false">$A15+J15</f>
+        <v>43893</v>
+      </c>
+      <c r="L15" s="40" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C15)/((E15+E$23)/2))</f>
+        <v>12</v>
+      </c>
+      <c r="M15" s="41" t="n">
+        <f aca="false">$A15+L15</f>
+        <v>43892</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>

</xml_diff>

<commit_message>
Iniciado modulo de Programaçao Funcional
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -132,7 +132,7 @@
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -157,6 +157,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -311,7 +318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -356,6 +363,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,7 +403,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,31 +415,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,39 +455,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -484,15 +495,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,15 +586,15 @@
   </sheetPr>
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -890,7 +901,7 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="9" t="n">
-        <v>0.1</v>
+        <v>0.0381944444444444</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -909,7 +920,7 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="9" t="n">
-        <v>0.0625</v>
+        <v>0.1</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -928,7 +939,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="9" t="n">
-        <v>0.0375</v>
+        <v>0.0625</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -946,7 +957,9 @@
         <v>43873</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="10"/>
+      <c r="D18" s="9" t="n">
+        <v>0.0590277777777778</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -963,7 +976,9 @@
         <v>43874</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -980,7 +995,9 @@
         <v>43875</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -997,7 +1014,9 @@
         <v>43876</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1014,7 +1033,9 @@
         <v>43877</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -1031,7 +1052,9 @@
         <v>43878</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="9" t="n">
+        <v>0.0548611111111111</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1048,7 +1071,9 @@
         <v>43879</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="10"/>
+      <c r="D24" s="9" t="n">
+        <v>0.03125</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -1065,7 +1090,9 @@
         <v>43880</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="10"/>
+      <c r="D25" s="9" t="n">
+        <v>0.115972222222222</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -1082,7 +1109,9 @@
         <v>43881</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="9" t="n">
+        <v>0.0361111111111111</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -1099,7 +1128,9 @@
         <v>43882</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="11" t="n">
+        <v>0.0208333333333333</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
@@ -1287,7 +1318,7 @@
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="11"/>
+      <c r="E38" s="12"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -1304,7 +1335,7 @@
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="11"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -1321,7 +1352,7 @@
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="11"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -1338,7 +1369,7 @@
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="11"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -1355,7 +1386,7 @@
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="11"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
@@ -1372,7 +1403,7 @@
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="11"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -1389,7 +1420,7 @@
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="11"/>
+      <c r="E44" s="12"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
@@ -1406,7 +1437,7 @@
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="11"/>
+      <c r="E45" s="12"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
@@ -1423,7 +1454,7 @@
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="11"/>
+      <c r="E46" s="12"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
@@ -1440,7 +1471,7 @@
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="11"/>
+      <c r="E47" s="12"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -1457,7 +1488,7 @@
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="11"/>
+      <c r="E48" s="12"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -1474,7 +1505,7 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="11"/>
+      <c r="E49" s="12"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -1491,7 +1522,7 @@
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="11"/>
+      <c r="E50" s="12"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -1508,7 +1539,7 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="11"/>
+      <c r="E51" s="12"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -1525,7 +1556,7 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
-      <c r="E52" s="11"/>
+      <c r="E52" s="12"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
@@ -1542,7 +1573,7 @@
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
-      <c r="E53" s="11"/>
+      <c r="E53" s="12"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
@@ -1559,7 +1590,7 @@
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="11"/>
+      <c r="E54" s="12"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -1576,7 +1607,7 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="11"/>
+      <c r="E55" s="12"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -1593,7 +1624,7 @@
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="11"/>
+      <c r="E56" s="12"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
@@ -1610,7 +1641,7 @@
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="11"/>
+      <c r="E57" s="12"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -1627,7 +1658,7 @@
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="11"/>
+      <c r="E58" s="12"/>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
@@ -1644,7 +1675,7 @@
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="11"/>
+      <c r="E59" s="12"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -1661,7 +1692,7 @@
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="11"/>
+      <c r="E60" s="12"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
@@ -1679,8 +1710,8 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -1696,8 +1727,8 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -1713,8 +1744,8 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -1730,8 +1761,8 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="7"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
@@ -1747,8 +1778,8 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
@@ -1764,8 +1795,8 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="7"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
@@ -1781,8 +1812,8 @@
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="7"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -1798,8 +1829,8 @@
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="7"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
@@ -1815,8 +1846,8 @@
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="7"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
@@ -1832,8 +1863,8 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="7"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
@@ -1849,8 +1880,8 @@
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="7"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
@@ -1866,8 +1897,8 @@
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="7"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
@@ -1883,8 +1914,8 @@
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="7"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
@@ -1900,8 +1931,8 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="7"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
@@ -1917,8 +1948,8 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="7"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
@@ -1934,8 +1965,8 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="7"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
@@ -1951,8 +1982,8 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="7"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -1968,8 +1999,8 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="7"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
@@ -1985,8 +2016,8 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="7"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
@@ -2002,8 +2033,8 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="7"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
@@ -2019,8 +2050,8 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="7"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
@@ -2036,8 +2067,8 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="7"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -2053,8 +2084,8 @@
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="7"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
@@ -2070,8 +2101,8 @@
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="7"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
@@ -2087,8 +2118,8 @@
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="7"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
@@ -2104,8 +2135,8 @@
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
       <c r="E86" s="7"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
@@ -2121,8 +2152,8 @@
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="7"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
@@ -2138,8 +2169,8 @@
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="7"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
@@ -2155,8 +2186,8 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="7"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="12"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
@@ -2172,8 +2203,8 @@
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="7"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
@@ -2189,8 +2220,8 @@
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="7"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
@@ -2206,8 +2237,8 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="7"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
@@ -2223,8 +2254,8 @@
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="7"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
@@ -2240,8 +2271,8 @@
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="7"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
@@ -2257,8 +2288,8 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="7"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
@@ -2274,8 +2305,8 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="7"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
@@ -2291,8 +2322,8 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="7"/>
-      <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
@@ -2308,8 +2339,8 @@
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="7"/>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
@@ -2325,8 +2356,8 @@
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="7"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="12"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
@@ -2342,8 +2373,8 @@
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="7"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
@@ -2359,8 +2390,8 @@
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="7"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
@@ -2376,8 +2407,8 @@
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="7"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
@@ -2393,8 +2424,8 @@
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="7"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="12"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
@@ -2410,8 +2441,8 @@
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="7"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
@@ -2427,8 +2458,8 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="7"/>
-      <c r="F105" s="12"/>
-      <c r="G105" s="12"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
@@ -2444,8 +2475,8 @@
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="7"/>
-      <c r="F106" s="12"/>
-      <c r="G106" s="12"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
@@ -2461,8 +2492,8 @@
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="7"/>
-      <c r="F107" s="12"/>
-      <c r="G107" s="12"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
@@ -2480,8 +2511,8 @@
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
     </row>
@@ -2497,8 +2528,8 @@
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
-      <c r="H109" s="13"/>
-      <c r="I109" s="13"/>
+      <c r="H109" s="14"/>
+      <c r="I109" s="14"/>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
     </row>
@@ -2514,8 +2545,8 @@
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="13"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="14"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
     </row>
@@ -2531,8 +2562,8 @@
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="14"/>
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
     </row>
@@ -2548,8 +2579,8 @@
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
     </row>
@@ -2565,8 +2596,8 @@
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
-      <c r="H113" s="13"/>
-      <c r="I113" s="13"/>
+      <c r="H113" s="14"/>
+      <c r="I113" s="14"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
     </row>
@@ -2582,8 +2613,8 @@
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
+      <c r="H114" s="14"/>
+      <c r="I114" s="14"/>
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
     </row>
@@ -2599,8 +2630,8 @@
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
+      <c r="H115" s="14"/>
+      <c r="I115" s="14"/>
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
     </row>
@@ -2616,8 +2647,8 @@
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
+      <c r="H116" s="14"/>
+      <c r="I116" s="14"/>
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
     </row>
@@ -2633,8 +2664,8 @@
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
     </row>
@@ -2650,8 +2681,8 @@
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
+      <c r="H118" s="14"/>
+      <c r="I118" s="14"/>
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
     </row>
@@ -2667,8 +2698,8 @@
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
+      <c r="H119" s="14"/>
+      <c r="I119" s="14"/>
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
     </row>
@@ -2684,8 +2715,8 @@
       <c r="E120" s="7"/>
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
     </row>
@@ -2701,8 +2732,8 @@
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
+      <c r="H121" s="14"/>
+      <c r="I121" s="14"/>
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
     </row>
@@ -2718,8 +2749,8 @@
       <c r="E122" s="7"/>
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
+      <c r="H122" s="14"/>
+      <c r="I122" s="14"/>
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
     </row>
@@ -2735,8 +2766,8 @@
       <c r="E123" s="7"/>
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
+      <c r="H123" s="14"/>
+      <c r="I123" s="14"/>
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
     </row>
@@ -2752,8 +2783,8 @@
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
+      <c r="H124" s="14"/>
+      <c r="I124" s="14"/>
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
     </row>
@@ -2769,8 +2800,8 @@
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
+      <c r="H125" s="14"/>
+      <c r="I125" s="14"/>
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
     </row>
@@ -2786,8 +2817,8 @@
       <c r="E126" s="7"/>
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
-      <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
+      <c r="H126" s="14"/>
+      <c r="I126" s="14"/>
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
     </row>
@@ -2803,8 +2834,8 @@
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
+      <c r="H127" s="14"/>
+      <c r="I127" s="14"/>
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
     </row>
@@ -2820,8 +2851,8 @@
       <c r="E128" s="7"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
+      <c r="H128" s="14"/>
+      <c r="I128" s="14"/>
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
     </row>
@@ -2837,8 +2868,8 @@
       <c r="E129" s="7"/>
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
+      <c r="H129" s="14"/>
+      <c r="I129" s="14"/>
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
     </row>
@@ -2854,8 +2885,8 @@
       <c r="E130" s="7"/>
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
-      <c r="H130" s="13"/>
-      <c r="I130" s="13"/>
+      <c r="H130" s="14"/>
+      <c r="I130" s="14"/>
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
     </row>
@@ -2871,8 +2902,8 @@
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
+      <c r="H131" s="14"/>
+      <c r="I131" s="14"/>
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
     </row>
@@ -2888,8 +2919,8 @@
       <c r="E132" s="7"/>
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
+      <c r="H132" s="14"/>
+      <c r="I132" s="14"/>
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
     </row>
@@ -2905,8 +2936,8 @@
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
-      <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
+      <c r="H133" s="14"/>
+      <c r="I133" s="14"/>
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
     </row>
@@ -2922,8 +2953,8 @@
       <c r="E134" s="7"/>
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
-      <c r="H134" s="13"/>
-      <c r="I134" s="13"/>
+      <c r="H134" s="14"/>
+      <c r="I134" s="14"/>
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
     </row>
@@ -2939,8 +2970,8 @@
       <c r="E135" s="7"/>
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="13"/>
+      <c r="H135" s="14"/>
+      <c r="I135" s="14"/>
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
     </row>
@@ -2956,8 +2987,8 @@
       <c r="E136" s="7"/>
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
-      <c r="H136" s="13"/>
-      <c r="I136" s="13"/>
+      <c r="H136" s="14"/>
+      <c r="I136" s="14"/>
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
     </row>
@@ -2973,8 +3004,8 @@
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
-      <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
+      <c r="H137" s="14"/>
+      <c r="I137" s="14"/>
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
     </row>
@@ -2990,8 +3021,8 @@
       <c r="E138" s="7"/>
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
+      <c r="H138" s="14"/>
+      <c r="I138" s="14"/>
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
     </row>
@@ -3007,8 +3038,8 @@
       <c r="E139" s="7"/>
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
-      <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
+      <c r="H139" s="14"/>
+      <c r="I139" s="14"/>
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
     </row>
@@ -3024,8 +3055,8 @@
       <c r="E140" s="7"/>
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
+      <c r="H140" s="14"/>
+      <c r="I140" s="14"/>
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
     </row>
@@ -3041,8 +3072,8 @@
       <c r="E141" s="7"/>
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
+      <c r="H141" s="14"/>
+      <c r="I141" s="14"/>
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
     </row>
@@ -3058,8 +3089,8 @@
       <c r="E142" s="7"/>
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
+      <c r="H142" s="14"/>
+      <c r="I142" s="14"/>
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
     </row>
@@ -3075,8 +3106,8 @@
       <c r="E143" s="7"/>
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
-      <c r="H143" s="13"/>
-      <c r="I143" s="13"/>
+      <c r="H143" s="14"/>
+      <c r="I143" s="14"/>
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
     </row>
@@ -3092,8 +3123,8 @@
       <c r="E144" s="7"/>
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="13"/>
+      <c r="H144" s="14"/>
+      <c r="I144" s="14"/>
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
     </row>
@@ -3109,8 +3140,8 @@
       <c r="E145" s="7"/>
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
-      <c r="H145" s="13"/>
-      <c r="I145" s="13"/>
+      <c r="H145" s="14"/>
+      <c r="I145" s="14"/>
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
     </row>
@@ -3126,8 +3157,8 @@
       <c r="E146" s="7"/>
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
-      <c r="H146" s="13"/>
-      <c r="I146" s="13"/>
+      <c r="H146" s="14"/>
+      <c r="I146" s="14"/>
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
     </row>
@@ -3143,8 +3174,8 @@
       <c r="E147" s="7"/>
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
-      <c r="H147" s="13"/>
-      <c r="I147" s="13"/>
+      <c r="H147" s="14"/>
+      <c r="I147" s="14"/>
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
     </row>
@@ -3160,8 +3191,8 @@
       <c r="E148" s="7"/>
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
-      <c r="H148" s="13"/>
-      <c r="I148" s="13"/>
+      <c r="H148" s="14"/>
+      <c r="I148" s="14"/>
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
     </row>
@@ -3177,8 +3208,8 @@
       <c r="E149" s="7"/>
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
-      <c r="H149" s="13"/>
-      <c r="I149" s="13"/>
+      <c r="H149" s="14"/>
+      <c r="I149" s="14"/>
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
     </row>
@@ -3194,8 +3225,8 @@
       <c r="E150" s="7"/>
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
-      <c r="H150" s="13"/>
-      <c r="I150" s="13"/>
+      <c r="H150" s="14"/>
+      <c r="I150" s="14"/>
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
     </row>
@@ -3211,8 +3242,8 @@
       <c r="E151" s="7"/>
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
-      <c r="H151" s="13"/>
-      <c r="I151" s="13"/>
+      <c r="H151" s="14"/>
+      <c r="I151" s="14"/>
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
     </row>
@@ -3228,8 +3259,8 @@
       <c r="E152" s="7"/>
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
-      <c r="H152" s="13"/>
-      <c r="I152" s="13"/>
+      <c r="H152" s="14"/>
+      <c r="I152" s="14"/>
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
     </row>
@@ -3245,8 +3276,8 @@
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
-      <c r="H153" s="13"/>
-      <c r="I153" s="13"/>
+      <c r="H153" s="14"/>
+      <c r="I153" s="14"/>
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
     </row>
@@ -3262,8 +3293,8 @@
       <c r="E154" s="7"/>
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
-      <c r="H154" s="13"/>
-      <c r="I154" s="13"/>
+      <c r="H154" s="14"/>
+      <c r="I154" s="14"/>
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
     </row>
@@ -3279,8 +3310,8 @@
       <c r="E155" s="7"/>
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
-      <c r="H155" s="13"/>
-      <c r="I155" s="13"/>
+      <c r="H155" s="14"/>
+      <c r="I155" s="14"/>
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
     </row>
@@ -3296,8 +3327,8 @@
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
-      <c r="H156" s="13"/>
-      <c r="I156" s="13"/>
+      <c r="H156" s="14"/>
+      <c r="I156" s="14"/>
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
     </row>
@@ -3315,8 +3346,8 @@
       <c r="G157" s="7"/>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
-      <c r="J157" s="14"/>
-      <c r="K157" s="14"/>
+      <c r="J157" s="15"/>
+      <c r="K157" s="15"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="n">
@@ -3332,8 +3363,8 @@
       <c r="G158" s="7"/>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
-      <c r="J158" s="14"/>
-      <c r="K158" s="14"/>
+      <c r="J158" s="15"/>
+      <c r="K158" s="15"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="4" t="n">
@@ -3349,8 +3380,8 @@
       <c r="G159" s="7"/>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
-      <c r="J159" s="14"/>
-      <c r="K159" s="14"/>
+      <c r="J159" s="15"/>
+      <c r="K159" s="15"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="4" t="n">
@@ -3366,8 +3397,8 @@
       <c r="G160" s="7"/>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
-      <c r="J160" s="14"/>
-      <c r="K160" s="14"/>
+      <c r="J160" s="15"/>
+      <c r="K160" s="15"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="4" t="n">
@@ -3383,8 +3414,8 @@
       <c r="G161" s="7"/>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
-      <c r="J161" s="14"/>
-      <c r="K161" s="14"/>
+      <c r="J161" s="15"/>
+      <c r="K161" s="15"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="4" t="n">
@@ -3400,8 +3431,8 @@
       <c r="G162" s="7"/>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
-      <c r="J162" s="14"/>
-      <c r="K162" s="14"/>
+      <c r="J162" s="15"/>
+      <c r="K162" s="15"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="4" t="n">
@@ -3417,8 +3448,8 @@
       <c r="G163" s="7"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
-      <c r="J163" s="14"/>
-      <c r="K163" s="14"/>
+      <c r="J163" s="15"/>
+      <c r="K163" s="15"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="n">
@@ -3434,8 +3465,8 @@
       <c r="G164" s="7"/>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
-      <c r="J164" s="14"/>
-      <c r="K164" s="14"/>
+      <c r="J164" s="15"/>
+      <c r="K164" s="15"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="n">
@@ -3451,8 +3482,8 @@
       <c r="G165" s="7"/>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
-      <c r="J165" s="14"/>
-      <c r="K165" s="14"/>
+      <c r="J165" s="15"/>
+      <c r="K165" s="15"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="n">
@@ -3468,8 +3499,8 @@
       <c r="G166" s="7"/>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
-      <c r="J166" s="14"/>
-      <c r="K166" s="14"/>
+      <c r="J166" s="15"/>
+      <c r="K166" s="15"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="4" t="n">
@@ -3485,8 +3516,8 @@
       <c r="G167" s="7"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
-      <c r="J167" s="14"/>
-      <c r="K167" s="14"/>
+      <c r="J167" s="15"/>
+      <c r="K167" s="15"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="4" t="n">
@@ -3502,8 +3533,8 @@
       <c r="G168" s="7"/>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
-      <c r="J168" s="14"/>
-      <c r="K168" s="14"/>
+      <c r="J168" s="15"/>
+      <c r="K168" s="15"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="4" t="n">
@@ -3519,8 +3550,8 @@
       <c r="G169" s="7"/>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
-      <c r="J169" s="14"/>
-      <c r="K169" s="14"/>
+      <c r="J169" s="15"/>
+      <c r="K169" s="15"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="4" t="n">
@@ -3536,8 +3567,8 @@
       <c r="G170" s="7"/>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
-      <c r="J170" s="14"/>
-      <c r="K170" s="14"/>
+      <c r="J170" s="15"/>
+      <c r="K170" s="15"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="4" t="n">
@@ -3553,8 +3584,8 @@
       <c r="G171" s="7"/>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
-      <c r="J171" s="14"/>
-      <c r="K171" s="14"/>
+      <c r="J171" s="15"/>
+      <c r="K171" s="15"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="4" t="n">
@@ -3570,8 +3601,8 @@
       <c r="G172" s="7"/>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
-      <c r="J172" s="14"/>
-      <c r="K172" s="14"/>
+      <c r="J172" s="15"/>
+      <c r="K172" s="15"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="4" t="n">
@@ -3587,8 +3618,8 @@
       <c r="G173" s="7"/>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
-      <c r="J173" s="14"/>
-      <c r="K173" s="14"/>
+      <c r="J173" s="15"/>
+      <c r="K173" s="15"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="4" t="n">
@@ -3604,8 +3635,8 @@
       <c r="G174" s="7"/>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
-      <c r="J174" s="14"/>
-      <c r="K174" s="14"/>
+      <c r="J174" s="15"/>
+      <c r="K174" s="15"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="4" t="n">
@@ -3621,8 +3652,8 @@
       <c r="G175" s="7"/>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
-      <c r="J175" s="14"/>
-      <c r="K175" s="14"/>
+      <c r="J175" s="15"/>
+      <c r="K175" s="15"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="4" t="n">
@@ -3638,8 +3669,8 @@
       <c r="G176" s="7"/>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
-      <c r="J176" s="14"/>
-      <c r="K176" s="14"/>
+      <c r="J176" s="15"/>
+      <c r="K176" s="15"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="4" t="n">
@@ -3655,8 +3686,8 @@
       <c r="G177" s="7"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
-      <c r="J177" s="14"/>
-      <c r="K177" s="14"/>
+      <c r="J177" s="15"/>
+      <c r="K177" s="15"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="4" t="n">
@@ -3672,8 +3703,8 @@
       <c r="G178" s="7"/>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
-      <c r="J178" s="14"/>
-      <c r="K178" s="14"/>
+      <c r="J178" s="15"/>
+      <c r="K178" s="15"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="4" t="n">
@@ -3689,8 +3720,8 @@
       <c r="G179" s="7"/>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
-      <c r="J179" s="14"/>
-      <c r="K179" s="14"/>
+      <c r="J179" s="15"/>
+      <c r="K179" s="15"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="4" t="n">
@@ -3706,8 +3737,8 @@
       <c r="G180" s="7"/>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
-      <c r="J180" s="14"/>
-      <c r="K180" s="14"/>
+      <c r="J180" s="15"/>
+      <c r="K180" s="15"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="4" t="n">
@@ -3723,8 +3754,8 @@
       <c r="G181" s="7"/>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
-      <c r="J181" s="14"/>
-      <c r="K181" s="14"/>
+      <c r="J181" s="15"/>
+      <c r="K181" s="15"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="4" t="n">
@@ -3740,8 +3771,8 @@
       <c r="G182" s="7"/>
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
-      <c r="J182" s="14"/>
-      <c r="K182" s="14"/>
+      <c r="J182" s="15"/>
+      <c r="K182" s="15"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="4" t="n">
@@ -3757,8 +3788,8 @@
       <c r="G183" s="7"/>
       <c r="H183" s="7"/>
       <c r="I183" s="7"/>
-      <c r="J183" s="14"/>
-      <c r="K183" s="14"/>
+      <c r="J183" s="15"/>
+      <c r="K183" s="15"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="4" t="n">
@@ -3774,8 +3805,8 @@
       <c r="G184" s="7"/>
       <c r="H184" s="7"/>
       <c r="I184" s="7"/>
-      <c r="J184" s="14"/>
-      <c r="K184" s="14"/>
+      <c r="J184" s="15"/>
+      <c r="K184" s="15"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="4" t="n">
@@ -3791,8 +3822,8 @@
       <c r="G185" s="7"/>
       <c r="H185" s="7"/>
       <c r="I185" s="7"/>
-      <c r="J185" s="14"/>
-      <c r="K185" s="14"/>
+      <c r="J185" s="15"/>
+      <c r="K185" s="15"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="4" t="n">
@@ -3808,8 +3839,8 @@
       <c r="G186" s="7"/>
       <c r="H186" s="7"/>
       <c r="I186" s="7"/>
-      <c r="J186" s="14"/>
-      <c r="K186" s="14"/>
+      <c r="J186" s="15"/>
+      <c r="K186" s="15"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="4" t="n">
@@ -3825,8 +3856,8 @@
       <c r="G187" s="7"/>
       <c r="H187" s="7"/>
       <c r="I187" s="7"/>
-      <c r="J187" s="14"/>
-      <c r="K187" s="14"/>
+      <c r="J187" s="15"/>
+      <c r="K187" s="15"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="4" t="n">
@@ -3842,8 +3873,8 @@
       <c r="G188" s="7"/>
       <c r="H188" s="7"/>
       <c r="I188" s="7"/>
-      <c r="J188" s="14"/>
-      <c r="K188" s="14"/>
+      <c r="J188" s="15"/>
+      <c r="K188" s="15"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="4" t="n">
@@ -3859,8 +3890,8 @@
       <c r="G189" s="7"/>
       <c r="H189" s="7"/>
       <c r="I189" s="7"/>
-      <c r="J189" s="14"/>
-      <c r="K189" s="14"/>
+      <c r="J189" s="15"/>
+      <c r="K189" s="15"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="4" t="n">
@@ -3876,8 +3907,8 @@
       <c r="G190" s="7"/>
       <c r="H190" s="7"/>
       <c r="I190" s="7"/>
-      <c r="J190" s="14"/>
-      <c r="K190" s="14"/>
+      <c r="J190" s="15"/>
+      <c r="K190" s="15"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="4" t="n">
@@ -3893,8 +3924,8 @@
       <c r="G191" s="7"/>
       <c r="H191" s="7"/>
       <c r="I191" s="7"/>
-      <c r="J191" s="14"/>
-      <c r="K191" s="14"/>
+      <c r="J191" s="15"/>
+      <c r="K191" s="15"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="4" t="n">
@@ -3910,8 +3941,8 @@
       <c r="G192" s="7"/>
       <c r="H192" s="7"/>
       <c r="I192" s="7"/>
-      <c r="J192" s="14"/>
-      <c r="K192" s="14"/>
+      <c r="J192" s="15"/>
+      <c r="K192" s="15"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="4" t="n">
@@ -3927,8 +3958,8 @@
       <c r="G193" s="7"/>
       <c r="H193" s="7"/>
       <c r="I193" s="7"/>
-      <c r="J193" s="14"/>
-      <c r="K193" s="14"/>
+      <c r="J193" s="15"/>
+      <c r="K193" s="15"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="4" t="n">
@@ -3944,8 +3975,8 @@
       <c r="G194" s="7"/>
       <c r="H194" s="7"/>
       <c r="I194" s="7"/>
-      <c r="J194" s="14"/>
-      <c r="K194" s="14"/>
+      <c r="J194" s="15"/>
+      <c r="K194" s="15"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="4" t="n">
@@ -3961,8 +3992,8 @@
       <c r="G195" s="7"/>
       <c r="H195" s="7"/>
       <c r="I195" s="7"/>
-      <c r="J195" s="14"/>
-      <c r="K195" s="14"/>
+      <c r="J195" s="15"/>
+      <c r="K195" s="15"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="4" t="n">
@@ -3978,8 +4009,8 @@
       <c r="G196" s="7"/>
       <c r="H196" s="7"/>
       <c r="I196" s="7"/>
-      <c r="J196" s="14"/>
-      <c r="K196" s="14"/>
+      <c r="J196" s="15"/>
+      <c r="K196" s="15"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="4" t="n">
@@ -3995,8 +4026,8 @@
       <c r="G197" s="7"/>
       <c r="H197" s="7"/>
       <c r="I197" s="7"/>
-      <c r="J197" s="14"/>
-      <c r="K197" s="14"/>
+      <c r="J197" s="15"/>
+      <c r="K197" s="15"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="4" t="n">
@@ -4012,8 +4043,8 @@
       <c r="G198" s="7"/>
       <c r="H198" s="7"/>
       <c r="I198" s="7"/>
-      <c r="J198" s="14"/>
-      <c r="K198" s="14"/>
+      <c r="J198" s="15"/>
+      <c r="K198" s="15"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="4" t="n">
@@ -4029,8 +4060,8 @@
       <c r="G199" s="7"/>
       <c r="H199" s="7"/>
       <c r="I199" s="7"/>
-      <c r="J199" s="14"/>
-      <c r="K199" s="14"/>
+      <c r="J199" s="15"/>
+      <c r="K199" s="15"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="4" t="n">
@@ -4046,8 +4077,8 @@
       <c r="G200" s="7"/>
       <c r="H200" s="7"/>
       <c r="I200" s="7"/>
-      <c r="J200" s="14"/>
-      <c r="K200" s="14"/>
+      <c r="J200" s="15"/>
+      <c r="K200" s="15"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="4" t="n">
@@ -4063,8 +4094,8 @@
       <c r="G201" s="7"/>
       <c r="H201" s="7"/>
       <c r="I201" s="7"/>
-      <c r="J201" s="14"/>
-      <c r="K201" s="14"/>
+      <c r="J201" s="15"/>
+      <c r="K201" s="15"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="4" t="n">
@@ -4080,8 +4111,8 @@
       <c r="G202" s="7"/>
       <c r="H202" s="7"/>
       <c r="I202" s="7"/>
-      <c r="J202" s="14"/>
-      <c r="K202" s="14"/>
+      <c r="J202" s="15"/>
+      <c r="K202" s="15"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="4" t="n">
@@ -4097,8 +4128,8 @@
       <c r="G203" s="7"/>
       <c r="H203" s="7"/>
       <c r="I203" s="7"/>
-      <c r="J203" s="14"/>
-      <c r="K203" s="14"/>
+      <c r="J203" s="15"/>
+      <c r="K203" s="15"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="4" t="n">
@@ -4114,46 +4145,46 @@
       <c r="G204" s="7"/>
       <c r="H204" s="7"/>
       <c r="I204" s="7"/>
-      <c r="J204" s="14"/>
-      <c r="K204" s="14"/>
+      <c r="J204" s="15"/>
+      <c r="K204" s="15"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C205" s="15" t="n">
+      <c r="C205" s="16" t="n">
         <f aca="false">SUM(C2:C204)</f>
         <v>0.424305555555556</v>
       </c>
-      <c r="D205" s="15" t="n">
+      <c r="D205" s="16" t="n">
         <f aca="false">SUM(D2:D204)</f>
-        <v>0.984027777777778</v>
-      </c>
-      <c r="E205" s="15" t="n">
+        <v>1.30277777777778</v>
+      </c>
+      <c r="E205" s="16" t="n">
         <f aca="false">SUM(E2:E204)</f>
         <v>0</v>
       </c>
-      <c r="F205" s="15" t="n">
+      <c r="F205" s="16" t="n">
         <f aca="false">SUM(F2:F204)</f>
         <v>0</v>
       </c>
-      <c r="G205" s="15" t="n">
+      <c r="G205" s="16" t="n">
         <f aca="false">SUM(G2:G204)</f>
         <v>0</v>
       </c>
-      <c r="H205" s="15" t="n">
+      <c r="H205" s="16" t="n">
         <f aca="false">SUM(H2:H204)</f>
         <v>0</v>
       </c>
-      <c r="I205" s="15" t="n">
+      <c r="I205" s="16" t="n">
         <f aca="false">SUM(I2:I204)</f>
         <v>0</v>
       </c>
-      <c r="J205" s="15" t="n">
+      <c r="J205" s="16" t="n">
         <f aca="false">SUM(J2:J204)</f>
         <v>0</v>
       </c>
-      <c r="K205" s="15" t="n">
+      <c r="K205" s="16" t="n">
         <f aca="false">SUM(K2:K204)</f>
         <v>0</v>
       </c>
@@ -4180,27 +4211,27 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
   </cols>
   <sheetData>
-    <row r="1" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="16" t="n">
+      <c r="C1" s="18"/>
+      <c r="D1" s="17" t="n">
         <v>200</v>
       </c>
-      <c r="E1" s="16" t="n">
+      <c r="E1" s="17" t="n">
         <v>300</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4211,7 +4242,7 @@
       <c r="B2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="19" t="n">
+      <c r="C2" s="20" t="n">
         <f aca="false">B2/$B$11</f>
         <v>0.0207715133531157</v>
       </c>
@@ -4226,7 +4257,7 @@
       <c r="F2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="20" t="n">
+      <c r="G2" s="21" t="n">
         <f aca="false">D2-F2</f>
         <v>1</v>
       </c>
@@ -4238,7 +4269,7 @@
       <c r="B3" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="C3" s="19" t="n">
+      <c r="C3" s="20" t="n">
         <f aca="false">B3/$B$11</f>
         <v>0.154302670623145</v>
       </c>
@@ -4258,7 +4289,7 @@
       <c r="B4" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="C4" s="19" t="n">
+      <c r="C4" s="20" t="n">
         <f aca="false">B4/$B$11</f>
         <v>0.112759643916914</v>
       </c>
@@ -4278,7 +4309,7 @@
       <c r="B5" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C5" s="19" t="n">
+      <c r="C5" s="20" t="n">
         <f aca="false">B5/$B$11</f>
         <v>0.106824925816024</v>
       </c>
@@ -4298,7 +4329,7 @@
       <c r="B6" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C6" s="19" t="n">
+      <c r="C6" s="20" t="n">
         <f aca="false">B6/$B$11</f>
         <v>0.124629080118694</v>
       </c>
@@ -4318,7 +4349,7 @@
       <c r="B7" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C7" s="19" t="n">
+      <c r="C7" s="20" t="n">
         <f aca="false">B7/$B$11</f>
         <v>0.0534124629080119</v>
       </c>
@@ -4338,7 +4369,7 @@
       <c r="B8" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="C8" s="19" t="n">
+      <c r="C8" s="20" t="n">
         <f aca="false">B8/$B$11</f>
         <v>0.189910979228487</v>
       </c>
@@ -4358,7 +4389,7 @@
       <c r="B9" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C9" s="19" t="n">
+      <c r="C9" s="20" t="n">
         <f aca="false">B9/$B$11</f>
         <v>0.0949554896142433</v>
       </c>
@@ -4378,7 +4409,7 @@
       <c r="B10" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="C10" s="19" t="n">
+      <c r="C10" s="20" t="n">
         <f aca="false">B10/$B$11</f>
         <v>0.142433234421365</v>
       </c>
@@ -4392,19 +4423,19 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="16" t="n">
+      <c r="B11" s="17" t="n">
         <f aca="false">SUM(B2:B10)</f>
         <v>337</v>
       </c>
-      <c r="C11" s="17" t="n">
+      <c r="C11" s="18" t="n">
         <f aca="false">B11/$B$11</f>
         <v>1</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="17" t="n">
         <f aca="false">SUM(D2:D10)</f>
         <v>203</v>
       </c>
-      <c r="E11" s="16" t="n">
+      <c r="E11" s="17" t="n">
         <f aca="false">SUM(E2:E10)</f>
         <v>305</v>
       </c>
@@ -4431,7 +4462,7 @@
       <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -4487,1032 +4518,1032 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="n">
+      <c r="A1" s="22" t="n">
         <v>43857</v>
       </c>
-      <c r="B1" s="21" t="n">
+      <c r="B1" s="22" t="n">
         <v>43858</v>
       </c>
-      <c r="C1" s="21" t="n">
+      <c r="C1" s="22" t="n">
         <v>43859</v>
       </c>
-      <c r="D1" s="21" t="n">
+      <c r="D1" s="22" t="n">
         <v>43860</v>
       </c>
-      <c r="E1" s="21" t="n">
+      <c r="E1" s="22" t="n">
         <v>43861</v>
       </c>
-      <c r="F1" s="21" t="n">
+      <c r="F1" s="22" t="n">
         <v>43862</v>
       </c>
-      <c r="G1" s="21" t="n">
+      <c r="G1" s="22" t="n">
         <v>43863</v>
       </c>
-      <c r="H1" s="21" t="n">
+      <c r="H1" s="22" t="n">
         <v>43864</v>
       </c>
-      <c r="I1" s="21" t="n">
+      <c r="I1" s="22" t="n">
         <v>43865</v>
       </c>
-      <c r="J1" s="21" t="n">
+      <c r="J1" s="22" t="n">
         <v>43866</v>
       </c>
-      <c r="K1" s="21" t="n">
+      <c r="K1" s="22" t="n">
         <v>43867</v>
       </c>
-      <c r="L1" s="21" t="n">
+      <c r="L1" s="22" t="n">
         <v>43868</v>
       </c>
-      <c r="M1" s="21" t="n">
+      <c r="M1" s="22" t="n">
         <v>43869</v>
       </c>
-      <c r="N1" s="21" t="n">
+      <c r="N1" s="22" t="n">
         <v>43870</v>
       </c>
-      <c r="O1" s="21" t="n">
+      <c r="O1" s="22" t="n">
         <v>43871</v>
       </c>
-      <c r="P1" s="21" t="n">
+      <c r="P1" s="22" t="n">
         <v>43872</v>
       </c>
-      <c r="Q1" s="21" t="n">
+      <c r="Q1" s="22" t="n">
         <v>43873</v>
       </c>
-      <c r="R1" s="21" t="n">
+      <c r="R1" s="22" t="n">
         <v>43874</v>
       </c>
-      <c r="S1" s="21" t="n">
+      <c r="S1" s="22" t="n">
         <v>43875</v>
       </c>
-      <c r="T1" s="21" t="n">
+      <c r="T1" s="22" t="n">
         <v>43876</v>
       </c>
-      <c r="U1" s="21" t="n">
+      <c r="U1" s="22" t="n">
         <v>43877</v>
       </c>
-      <c r="V1" s="21" t="n">
+      <c r="V1" s="22" t="n">
         <v>43878</v>
       </c>
-      <c r="W1" s="21" t="n">
+      <c r="W1" s="22" t="n">
         <v>43879</v>
       </c>
-      <c r="X1" s="21" t="n">
+      <c r="X1" s="22" t="n">
         <v>43880</v>
       </c>
-      <c r="Y1" s="21" t="n">
+      <c r="Y1" s="22" t="n">
         <v>43881</v>
       </c>
-      <c r="Z1" s="21" t="n">
+      <c r="Z1" s="22" t="n">
         <v>43882</v>
       </c>
-      <c r="AA1" s="21" t="n">
+      <c r="AA1" s="22" t="n">
         <v>43883</v>
       </c>
-      <c r="AB1" s="21" t="n">
+      <c r="AB1" s="22" t="n">
         <v>43884</v>
       </c>
-      <c r="AC1" s="21" t="n">
+      <c r="AC1" s="22" t="n">
         <v>43885</v>
       </c>
-      <c r="AD1" s="21" t="n">
+      <c r="AD1" s="22" t="n">
         <v>43886</v>
       </c>
-      <c r="AE1" s="21" t="n">
+      <c r="AE1" s="22" t="n">
         <v>43887</v>
       </c>
-      <c r="AF1" s="21" t="n">
+      <c r="AF1" s="22" t="n">
         <v>43888</v>
       </c>
-      <c r="AG1" s="21" t="n">
+      <c r="AG1" s="22" t="n">
         <v>43889</v>
       </c>
-      <c r="AH1" s="21" t="n">
+      <c r="AH1" s="22" t="n">
         <v>43890</v>
       </c>
-      <c r="AI1" s="21" t="n">
+      <c r="AI1" s="22" t="n">
         <v>43891</v>
       </c>
-      <c r="AJ1" s="21" t="n">
+      <c r="AJ1" s="22" t="n">
         <v>43892</v>
       </c>
-      <c r="AK1" s="21" t="n">
+      <c r="AK1" s="22" t="n">
         <v>43893</v>
       </c>
-      <c r="AL1" s="21" t="n">
+      <c r="AL1" s="22" t="n">
         <v>43894</v>
       </c>
-      <c r="AM1" s="21" t="n">
+      <c r="AM1" s="22" t="n">
         <v>43895</v>
       </c>
-      <c r="AN1" s="21" t="n">
+      <c r="AN1" s="22" t="n">
         <v>43896</v>
       </c>
-      <c r="AO1" s="21" t="n">
+      <c r="AO1" s="22" t="n">
         <v>43897</v>
       </c>
-      <c r="AP1" s="21" t="n">
+      <c r="AP1" s="22" t="n">
         <v>43898</v>
       </c>
-      <c r="AQ1" s="21" t="n">
+      <c r="AQ1" s="22" t="n">
         <v>43899</v>
       </c>
-      <c r="AR1" s="21" t="n">
+      <c r="AR1" s="22" t="n">
         <v>43900</v>
       </c>
-      <c r="AS1" s="21" t="n">
+      <c r="AS1" s="22" t="n">
         <v>43901</v>
       </c>
-      <c r="AT1" s="21" t="n">
+      <c r="AT1" s="22" t="n">
         <v>43902</v>
       </c>
-      <c r="AU1" s="21" t="n">
+      <c r="AU1" s="22" t="n">
         <v>43903</v>
       </c>
-      <c r="AV1" s="21" t="n">
+      <c r="AV1" s="22" t="n">
         <v>43904</v>
       </c>
-      <c r="AW1" s="21" t="n">
+      <c r="AW1" s="22" t="n">
         <v>43905</v>
       </c>
-      <c r="AX1" s="21" t="n">
+      <c r="AX1" s="22" t="n">
         <v>43906</v>
       </c>
-      <c r="AY1" s="21" t="n">
+      <c r="AY1" s="22" t="n">
         <v>43907</v>
       </c>
-      <c r="AZ1" s="21" t="n">
+      <c r="AZ1" s="22" t="n">
         <v>43908</v>
       </c>
-      <c r="BA1" s="21" t="n">
+      <c r="BA1" s="22" t="n">
         <v>43909</v>
       </c>
-      <c r="BB1" s="21" t="n">
+      <c r="BB1" s="22" t="n">
         <v>43910</v>
       </c>
-      <c r="BC1" s="21" t="n">
+      <c r="BC1" s="22" t="n">
         <v>43911</v>
       </c>
-      <c r="BD1" s="21" t="n">
+      <c r="BD1" s="22" t="n">
         <v>43912</v>
       </c>
-      <c r="BE1" s="21" t="n">
+      <c r="BE1" s="22" t="n">
         <v>43913</v>
       </c>
-      <c r="BF1" s="21" t="n">
+      <c r="BF1" s="22" t="n">
         <v>43914</v>
       </c>
-      <c r="BG1" s="21" t="n">
+      <c r="BG1" s="22" t="n">
         <v>43915</v>
       </c>
-      <c r="BH1" s="21" t="n">
+      <c r="BH1" s="22" t="n">
         <v>43916</v>
       </c>
-      <c r="BI1" s="21" t="n">
+      <c r="BI1" s="22" t="n">
         <v>43917</v>
       </c>
-      <c r="BJ1" s="21" t="n">
+      <c r="BJ1" s="22" t="n">
         <v>43918</v>
       </c>
-      <c r="BK1" s="21" t="n">
+      <c r="BK1" s="22" t="n">
         <v>43919</v>
       </c>
-      <c r="BL1" s="21" t="n">
+      <c r="BL1" s="22" t="n">
         <v>43920</v>
       </c>
-      <c r="BM1" s="21" t="n">
+      <c r="BM1" s="22" t="n">
         <v>43921</v>
       </c>
-      <c r="BN1" s="21" t="n">
+      <c r="BN1" s="22" t="n">
         <v>43922</v>
       </c>
-      <c r="BO1" s="21" t="n">
+      <c r="BO1" s="22" t="n">
         <v>43923</v>
       </c>
-      <c r="BP1" s="21" t="n">
+      <c r="BP1" s="22" t="n">
         <v>43924</v>
       </c>
-      <c r="BQ1" s="21" t="n">
+      <c r="BQ1" s="22" t="n">
         <v>43925</v>
       </c>
-      <c r="BR1" s="21" t="n">
+      <c r="BR1" s="22" t="n">
         <v>43926</v>
       </c>
-      <c r="BS1" s="21" t="n">
+      <c r="BS1" s="22" t="n">
         <v>43927</v>
       </c>
-      <c r="BT1" s="21" t="n">
+      <c r="BT1" s="22" t="n">
         <v>43928</v>
       </c>
-      <c r="BU1" s="21" t="n">
+      <c r="BU1" s="22" t="n">
         <v>43929</v>
       </c>
-      <c r="BV1" s="21" t="n">
+      <c r="BV1" s="22" t="n">
         <v>43930</v>
       </c>
-      <c r="BW1" s="21" t="n">
+      <c r="BW1" s="22" t="n">
         <v>43931</v>
       </c>
-      <c r="BX1" s="21" t="n">
+      <c r="BX1" s="22" t="n">
         <v>43932</v>
       </c>
-      <c r="BY1" s="21" t="n">
+      <c r="BY1" s="22" t="n">
         <v>43933</v>
       </c>
-      <c r="BZ1" s="21" t="n">
+      <c r="BZ1" s="22" t="n">
         <v>43934</v>
       </c>
-      <c r="CA1" s="21" t="n">
+      <c r="CA1" s="22" t="n">
         <v>43935</v>
       </c>
-      <c r="CB1" s="21" t="n">
+      <c r="CB1" s="22" t="n">
         <v>43936</v>
       </c>
-      <c r="CC1" s="21" t="n">
+      <c r="CC1" s="22" t="n">
         <v>43937</v>
       </c>
-      <c r="CD1" s="21" t="n">
+      <c r="CD1" s="22" t="n">
         <v>43938</v>
       </c>
-      <c r="CE1" s="21" t="n">
+      <c r="CE1" s="22" t="n">
         <v>43939</v>
       </c>
-      <c r="CF1" s="21" t="n">
+      <c r="CF1" s="22" t="n">
         <v>43940</v>
       </c>
-      <c r="CG1" s="21" t="n">
+      <c r="CG1" s="22" t="n">
         <v>43941</v>
       </c>
-      <c r="CH1" s="21" t="n">
+      <c r="CH1" s="22" t="n">
         <v>43942</v>
       </c>
-      <c r="CI1" s="21" t="n">
+      <c r="CI1" s="22" t="n">
         <v>43943</v>
       </c>
-      <c r="CJ1" s="21" t="n">
+      <c r="CJ1" s="22" t="n">
         <v>43944</v>
       </c>
-      <c r="CK1" s="21" t="n">
+      <c r="CK1" s="22" t="n">
         <v>43945</v>
       </c>
-      <c r="CL1" s="21" t="n">
+      <c r="CL1" s="22" t="n">
         <v>43946</v>
       </c>
-      <c r="CM1" s="21" t="n">
+      <c r="CM1" s="22" t="n">
         <v>43947</v>
       </c>
-      <c r="CN1" s="21" t="n">
+      <c r="CN1" s="22" t="n">
         <v>43948</v>
       </c>
-      <c r="CO1" s="21" t="n">
+      <c r="CO1" s="22" t="n">
         <v>43949</v>
       </c>
-      <c r="CP1" s="21" t="n">
+      <c r="CP1" s="22" t="n">
         <v>43950</v>
       </c>
-      <c r="CQ1" s="21" t="n">
+      <c r="CQ1" s="22" t="n">
         <v>43951</v>
       </c>
-      <c r="CR1" s="21" t="n">
+      <c r="CR1" s="22" t="n">
         <v>43952</v>
       </c>
-      <c r="CS1" s="21" t="n">
+      <c r="CS1" s="22" t="n">
         <v>43953</v>
       </c>
-      <c r="CT1" s="21" t="n">
+      <c r="CT1" s="22" t="n">
         <v>43954</v>
       </c>
-      <c r="CU1" s="21" t="n">
+      <c r="CU1" s="22" t="n">
         <v>43955</v>
       </c>
-      <c r="CV1" s="21" t="n">
+      <c r="CV1" s="22" t="n">
         <v>43956</v>
       </c>
-      <c r="CW1" s="21" t="n">
+      <c r="CW1" s="22" t="n">
         <v>43957</v>
       </c>
-      <c r="CX1" s="21" t="n">
+      <c r="CX1" s="22" t="n">
         <v>43958</v>
       </c>
-      <c r="CY1" s="21" t="n">
+      <c r="CY1" s="22" t="n">
         <v>43959</v>
       </c>
-      <c r="CZ1" s="21" t="n">
+      <c r="CZ1" s="22" t="n">
         <v>43960</v>
       </c>
-      <c r="DA1" s="21" t="n">
+      <c r="DA1" s="22" t="n">
         <v>43961</v>
       </c>
-      <c r="DB1" s="21" t="n">
+      <c r="DB1" s="22" t="n">
         <v>43962</v>
       </c>
-      <c r="DC1" s="21" t="n">
+      <c r="DC1" s="22" t="n">
         <v>43963</v>
       </c>
-      <c r="DD1" s="21" t="n">
+      <c r="DD1" s="22" t="n">
         <v>43964</v>
       </c>
-      <c r="DE1" s="21" t="n">
+      <c r="DE1" s="22" t="n">
         <v>43965</v>
       </c>
-      <c r="DF1" s="21" t="n">
+      <c r="DF1" s="22" t="n">
         <v>43966</v>
       </c>
-      <c r="DG1" s="21" t="n">
+      <c r="DG1" s="22" t="n">
         <v>43967</v>
       </c>
-      <c r="DH1" s="21" t="n">
+      <c r="DH1" s="22" t="n">
         <v>43968</v>
       </c>
-      <c r="DI1" s="21" t="n">
+      <c r="DI1" s="22" t="n">
         <v>43969</v>
       </c>
-      <c r="DJ1" s="21" t="n">
+      <c r="DJ1" s="22" t="n">
         <v>43970</v>
       </c>
-      <c r="DK1" s="21" t="n">
+      <c r="DK1" s="22" t="n">
         <v>43971</v>
       </c>
-      <c r="DL1" s="21" t="n">
+      <c r="DL1" s="22" t="n">
         <v>43972</v>
       </c>
-      <c r="DM1" s="21" t="n">
+      <c r="DM1" s="22" t="n">
         <v>43973</v>
       </c>
-      <c r="DN1" s="21" t="n">
+      <c r="DN1" s="22" t="n">
         <v>43974</v>
       </c>
-      <c r="DO1" s="21" t="n">
+      <c r="DO1" s="22" t="n">
         <v>43975</v>
       </c>
-      <c r="DP1" s="21" t="n">
+      <c r="DP1" s="22" t="n">
         <v>43976</v>
       </c>
-      <c r="DQ1" s="21" t="n">
+      <c r="DQ1" s="22" t="n">
         <v>43977</v>
       </c>
-      <c r="DR1" s="21" t="n">
+      <c r="DR1" s="22" t="n">
         <v>43978</v>
       </c>
-      <c r="DS1" s="21" t="n">
+      <c r="DS1" s="22" t="n">
         <v>43979</v>
       </c>
-      <c r="DT1" s="21" t="n">
+      <c r="DT1" s="22" t="n">
         <v>43980</v>
       </c>
-      <c r="DU1" s="21" t="n">
+      <c r="DU1" s="22" t="n">
         <v>43981</v>
       </c>
-      <c r="DV1" s="21" t="n">
+      <c r="DV1" s="22" t="n">
         <v>43982</v>
       </c>
-      <c r="DW1" s="21" t="n">
+      <c r="DW1" s="22" t="n">
         <v>43983</v>
       </c>
-      <c r="DX1" s="21" t="n">
+      <c r="DX1" s="22" t="n">
         <v>43984</v>
       </c>
-      <c r="DY1" s="21" t="n">
+      <c r="DY1" s="22" t="n">
         <v>43985</v>
       </c>
-      <c r="DZ1" s="21" t="n">
+      <c r="DZ1" s="22" t="n">
         <v>43986</v>
       </c>
-      <c r="EA1" s="21" t="n">
+      <c r="EA1" s="22" t="n">
         <v>43987</v>
       </c>
-      <c r="EB1" s="21" t="n">
+      <c r="EB1" s="22" t="n">
         <v>43988</v>
       </c>
-      <c r="EC1" s="21" t="n">
+      <c r="EC1" s="22" t="n">
         <v>43989</v>
       </c>
-      <c r="ED1" s="21" t="n">
+      <c r="ED1" s="22" t="n">
         <v>43990</v>
       </c>
-      <c r="EE1" s="21" t="n">
+      <c r="EE1" s="22" t="n">
         <v>43991</v>
       </c>
-      <c r="EF1" s="21" t="n">
+      <c r="EF1" s="22" t="n">
         <v>43992</v>
       </c>
-      <c r="EG1" s="21" t="n">
+      <c r="EG1" s="22" t="n">
         <v>43993</v>
       </c>
-      <c r="EH1" s="21" t="n">
+      <c r="EH1" s="22" t="n">
         <v>43994</v>
       </c>
-      <c r="EI1" s="21" t="n">
+      <c r="EI1" s="22" t="n">
         <v>43995</v>
       </c>
-      <c r="EJ1" s="21" t="n">
+      <c r="EJ1" s="22" t="n">
         <v>43996</v>
       </c>
-      <c r="EK1" s="21" t="n">
+      <c r="EK1" s="22" t="n">
         <v>43997</v>
       </c>
-      <c r="EL1" s="21" t="n">
+      <c r="EL1" s="22" t="n">
         <v>43998</v>
       </c>
-      <c r="EM1" s="21" t="n">
+      <c r="EM1" s="22" t="n">
         <v>43999</v>
       </c>
-      <c r="EN1" s="21" t="n">
+      <c r="EN1" s="22" t="n">
         <v>44000</v>
       </c>
-      <c r="EO1" s="21" t="n">
+      <c r="EO1" s="22" t="n">
         <v>44001</v>
       </c>
-      <c r="EP1" s="21" t="n">
+      <c r="EP1" s="22" t="n">
         <v>44002</v>
       </c>
-      <c r="EQ1" s="21" t="n">
+      <c r="EQ1" s="22" t="n">
         <v>44003</v>
       </c>
-      <c r="ER1" s="21" t="n">
+      <c r="ER1" s="22" t="n">
         <v>44004</v>
       </c>
-      <c r="ES1" s="21" t="n">
+      <c r="ES1" s="22" t="n">
         <v>44005</v>
       </c>
-      <c r="ET1" s="21" t="n">
+      <c r="ET1" s="22" t="n">
         <v>44006</v>
       </c>
-      <c r="EU1" s="21" t="n">
+      <c r="EU1" s="22" t="n">
         <v>44007</v>
       </c>
-      <c r="EV1" s="21" t="n">
+      <c r="EV1" s="22" t="n">
         <v>44008</v>
       </c>
-      <c r="EW1" s="21" t="n">
+      <c r="EW1" s="22" t="n">
         <v>44009</v>
       </c>
-      <c r="EX1" s="21" t="n">
+      <c r="EX1" s="22" t="n">
         <v>44010</v>
       </c>
-      <c r="EY1" s="21" t="n">
+      <c r="EY1" s="22" t="n">
         <v>44011</v>
       </c>
-      <c r="EZ1" s="21" t="n">
+      <c r="EZ1" s="22" t="n">
         <v>44012</v>
       </c>
-      <c r="FA1" s="21" t="n">
+      <c r="FA1" s="22" t="n">
         <v>44013</v>
       </c>
-      <c r="FB1" s="21" t="n">
+      <c r="FB1" s="22" t="n">
         <v>44014</v>
       </c>
-      <c r="FC1" s="21" t="n">
+      <c r="FC1" s="22" t="n">
         <v>44015</v>
       </c>
-      <c r="FD1" s="21" t="n">
+      <c r="FD1" s="22" t="n">
         <v>44016</v>
       </c>
-      <c r="FE1" s="21" t="n">
+      <c r="FE1" s="22" t="n">
         <v>44017</v>
       </c>
-      <c r="FF1" s="21" t="n">
+      <c r="FF1" s="22" t="n">
         <v>44018</v>
       </c>
-      <c r="FG1" s="21" t="n">
+      <c r="FG1" s="22" t="n">
         <v>44019</v>
       </c>
-      <c r="FH1" s="21" t="n">
+      <c r="FH1" s="22" t="n">
         <v>44020</v>
       </c>
-      <c r="FI1" s="21" t="n">
+      <c r="FI1" s="22" t="n">
         <v>44021</v>
       </c>
-      <c r="FJ1" s="21" t="n">
+      <c r="FJ1" s="22" t="n">
         <v>44022</v>
       </c>
-      <c r="FK1" s="21" t="n">
+      <c r="FK1" s="22" t="n">
         <v>44023</v>
       </c>
-      <c r="FL1" s="21" t="n">
+      <c r="FL1" s="22" t="n">
         <v>44024</v>
       </c>
-      <c r="FM1" s="21" t="n">
+      <c r="FM1" s="22" t="n">
         <v>44025</v>
       </c>
-      <c r="FN1" s="21" t="n">
+      <c r="FN1" s="22" t="n">
         <v>44026</v>
       </c>
-      <c r="FO1" s="21" t="n">
+      <c r="FO1" s="22" t="n">
         <v>44027</v>
       </c>
-      <c r="FP1" s="21" t="n">
+      <c r="FP1" s="22" t="n">
         <v>44028</v>
       </c>
-      <c r="FQ1" s="21" t="n">
+      <c r="FQ1" s="22" t="n">
         <v>44029</v>
       </c>
-      <c r="FR1" s="21" t="n">
+      <c r="FR1" s="22" t="n">
         <v>44030</v>
       </c>
-      <c r="FS1" s="21" t="n">
+      <c r="FS1" s="22" t="n">
         <v>44031</v>
       </c>
-      <c r="FT1" s="21" t="n">
+      <c r="FT1" s="22" t="n">
         <v>44032</v>
       </c>
-      <c r="FU1" s="21" t="n">
+      <c r="FU1" s="22" t="n">
         <v>44033</v>
       </c>
-      <c r="FV1" s="21" t="n">
+      <c r="FV1" s="22" t="n">
         <v>44034</v>
       </c>
-      <c r="FW1" s="21" t="n">
+      <c r="FW1" s="22" t="n">
         <v>44035</v>
       </c>
-      <c r="FX1" s="21" t="n">
+      <c r="FX1" s="22" t="n">
         <v>44036</v>
       </c>
-      <c r="FY1" s="21" t="n">
+      <c r="FY1" s="22" t="n">
         <v>44037</v>
       </c>
-      <c r="FZ1" s="21" t="n">
+      <c r="FZ1" s="22" t="n">
         <v>44038</v>
       </c>
-      <c r="GA1" s="21" t="n">
+      <c r="GA1" s="22" t="n">
         <v>44039</v>
       </c>
-      <c r="GB1" s="21" t="n">
+      <c r="GB1" s="22" t="n">
         <v>44040</v>
       </c>
-      <c r="GC1" s="21" t="n">
+      <c r="GC1" s="22" t="n">
         <v>44041</v>
       </c>
-      <c r="GD1" s="21" t="n">
+      <c r="GD1" s="22" t="n">
         <v>44042</v>
       </c>
-      <c r="GE1" s="21" t="n">
+      <c r="GE1" s="22" t="n">
         <v>44043</v>
       </c>
-      <c r="GF1" s="21" t="n">
+      <c r="GF1" s="22" t="n">
         <v>44044</v>
       </c>
-      <c r="GG1" s="21" t="n">
+      <c r="GG1" s="22" t="n">
         <v>44045</v>
       </c>
-      <c r="GH1" s="21" t="n">
+      <c r="GH1" s="22" t="n">
         <v>44046</v>
       </c>
-      <c r="GI1" s="21" t="n">
+      <c r="GI1" s="22" t="n">
         <v>44047</v>
       </c>
-      <c r="GJ1" s="21" t="n">
+      <c r="GJ1" s="22" t="n">
         <v>44048</v>
       </c>
-      <c r="GK1" s="21" t="n">
+      <c r="GK1" s="22" t="n">
         <v>44049</v>
       </c>
-      <c r="GL1" s="21" t="n">
+      <c r="GL1" s="22" t="n">
         <v>44050</v>
       </c>
-      <c r="GM1" s="21" t="n">
+      <c r="GM1" s="22" t="n">
         <v>44051</v>
       </c>
-      <c r="GN1" s="21" t="n">
+      <c r="GN1" s="22" t="n">
         <v>44052</v>
       </c>
-      <c r="GO1" s="21" t="n">
+      <c r="GO1" s="22" t="n">
         <v>44053</v>
       </c>
-      <c r="GP1" s="21" t="n">
+      <c r="GP1" s="22" t="n">
         <v>44054</v>
       </c>
-      <c r="GQ1" s="21" t="n">
+      <c r="GQ1" s="22" t="n">
         <v>44055</v>
       </c>
-      <c r="GR1" s="21" t="n">
+      <c r="GR1" s="22" t="n">
         <v>44056</v>
       </c>
-      <c r="GS1" s="21" t="n">
+      <c r="GS1" s="22" t="n">
         <v>44057</v>
       </c>
-      <c r="GT1" s="21" t="n">
+      <c r="GT1" s="22" t="n">
         <v>44058</v>
       </c>
-      <c r="GU1" s="21" t="n">
+      <c r="GU1" s="22" t="n">
         <v>44059</v>
       </c>
-      <c r="GV1" s="21" t="n">
+      <c r="GV1" s="22" t="n">
         <v>44060</v>
       </c>
-      <c r="GW1" s="21" t="n">
+      <c r="GW1" s="22" t="n">
         <v>44061</v>
       </c>
-      <c r="GX1" s="21" t="n">
+      <c r="GX1" s="22" t="n">
         <v>44062</v>
       </c>
-      <c r="GY1" s="21" t="n">
+      <c r="GY1" s="22" t="n">
         <v>44063</v>
       </c>
-      <c r="GZ1" s="21" t="n">
+      <c r="GZ1" s="22" t="n">
         <v>44064</v>
       </c>
-      <c r="HA1" s="21" t="n">
+      <c r="HA1" s="22" t="n">
         <v>44065</v>
       </c>
-      <c r="HB1" s="21" t="n">
+      <c r="HB1" s="22" t="n">
         <v>44066</v>
       </c>
-      <c r="HC1" s="21" t="n">
+      <c r="HC1" s="22" t="n">
         <v>44067</v>
       </c>
-      <c r="HD1" s="21" t="n">
+      <c r="HD1" s="22" t="n">
         <v>44068</v>
       </c>
-      <c r="HE1" s="21" t="n">
+      <c r="HE1" s="22" t="n">
         <v>44069</v>
       </c>
-      <c r="HF1" s="21" t="n">
+      <c r="HF1" s="22" t="n">
         <v>44070</v>
       </c>
-      <c r="HG1" s="21" t="n">
+      <c r="HG1" s="22" t="n">
         <v>44071</v>
       </c>
-      <c r="HH1" s="21" t="n">
+      <c r="HH1" s="22" t="n">
         <v>44072</v>
       </c>
-      <c r="HI1" s="21" t="n">
+      <c r="HI1" s="22" t="n">
         <v>44073</v>
       </c>
-      <c r="HJ1" s="21" t="n">
+      <c r="HJ1" s="22" t="n">
         <v>44074</v>
       </c>
-      <c r="HK1" s="21" t="n">
+      <c r="HK1" s="22" t="n">
         <v>44075</v>
       </c>
-      <c r="HL1" s="21" t="n">
+      <c r="HL1" s="22" t="n">
         <v>44076</v>
       </c>
-      <c r="HM1" s="21" t="n">
+      <c r="HM1" s="22" t="n">
         <v>44077</v>
       </c>
-      <c r="HN1" s="21" t="n">
+      <c r="HN1" s="22" t="n">
         <v>44078</v>
       </c>
-      <c r="HO1" s="21" t="n">
+      <c r="HO1" s="22" t="n">
         <v>44079</v>
       </c>
-      <c r="HP1" s="21" t="n">
+      <c r="HP1" s="22" t="n">
         <v>44080</v>
       </c>
-      <c r="HQ1" s="21" t="n">
+      <c r="HQ1" s="22" t="n">
         <v>44081</v>
       </c>
-      <c r="HR1" s="21" t="n">
+      <c r="HR1" s="22" t="n">
         <v>44082</v>
       </c>
-      <c r="HS1" s="21" t="n">
+      <c r="HS1" s="22" t="n">
         <v>44083</v>
       </c>
-      <c r="HT1" s="21" t="n">
+      <c r="HT1" s="22" t="n">
         <v>44084</v>
       </c>
-      <c r="HU1" s="21" t="n">
+      <c r="HU1" s="22" t="n">
         <v>44085</v>
       </c>
-      <c r="HV1" s="21" t="n">
+      <c r="HV1" s="22" t="n">
         <v>44086</v>
       </c>
-      <c r="HW1" s="21" t="n">
+      <c r="HW1" s="22" t="n">
         <v>44087</v>
       </c>
-      <c r="HX1" s="21" t="n">
+      <c r="HX1" s="22" t="n">
         <v>44088</v>
       </c>
-      <c r="HY1" s="21" t="n">
+      <c r="HY1" s="22" t="n">
         <v>44089</v>
       </c>
-      <c r="HZ1" s="21" t="n">
+      <c r="HZ1" s="22" t="n">
         <v>44090</v>
       </c>
-      <c r="IA1" s="21" t="n">
+      <c r="IA1" s="22" t="n">
         <v>44091</v>
       </c>
-      <c r="IB1" s="21" t="n">
+      <c r="IB1" s="22" t="n">
         <v>44092</v>
       </c>
-      <c r="IC1" s="21" t="n">
+      <c r="IC1" s="22" t="n">
         <v>44093</v>
       </c>
-      <c r="ID1" s="21" t="n">
+      <c r="ID1" s="22" t="n">
         <v>44094</v>
       </c>
-      <c r="IE1" s="21" t="n">
+      <c r="IE1" s="22" t="n">
         <v>44095</v>
       </c>
-      <c r="IF1" s="21" t="n">
+      <c r="IF1" s="22" t="n">
         <v>44096</v>
       </c>
-      <c r="IG1" s="21" t="n">
+      <c r="IG1" s="22" t="n">
         <v>44097</v>
       </c>
-      <c r="IH1" s="21" t="n">
+      <c r="IH1" s="22" t="n">
         <v>44098</v>
       </c>
-      <c r="II1" s="21" t="n">
+      <c r="II1" s="22" t="n">
         <v>44099</v>
       </c>
-      <c r="IJ1" s="21" t="n">
+      <c r="IJ1" s="22" t="n">
         <v>44100</v>
       </c>
-      <c r="IK1" s="21" t="n">
+      <c r="IK1" s="22" t="n">
         <v>44101</v>
       </c>
-      <c r="IL1" s="21" t="n">
+      <c r="IL1" s="22" t="n">
         <v>44102</v>
       </c>
-      <c r="IM1" s="21" t="n">
+      <c r="IM1" s="22" t="n">
         <v>44103</v>
       </c>
-      <c r="IN1" s="21" t="n">
+      <c r="IN1" s="22" t="n">
         <v>44104</v>
       </c>
-      <c r="IO1" s="21" t="n">
+      <c r="IO1" s="22" t="n">
         <v>44105</v>
       </c>
-      <c r="IP1" s="21" t="n">
+      <c r="IP1" s="22" t="n">
         <v>44106</v>
       </c>
-      <c r="IQ1" s="21" t="n">
+      <c r="IQ1" s="22" t="n">
         <v>44107</v>
       </c>
-      <c r="IR1" s="21" t="n">
+      <c r="IR1" s="22" t="n">
         <v>44108</v>
       </c>
-      <c r="IS1" s="21" t="n">
+      <c r="IS1" s="22" t="n">
         <v>44109</v>
       </c>
-      <c r="IT1" s="21" t="n">
+      <c r="IT1" s="22" t="n">
         <v>44110</v>
       </c>
-      <c r="IU1" s="21" t="n">
+      <c r="IU1" s="22" t="n">
         <v>44111</v>
       </c>
-      <c r="IV1" s="21" t="n">
+      <c r="IV1" s="22" t="n">
         <v>44112</v>
       </c>
-      <c r="IW1" s="21" t="n">
+      <c r="IW1" s="22" t="n">
         <v>44113</v>
       </c>
-      <c r="IX1" s="21" t="n">
+      <c r="IX1" s="22" t="n">
         <v>44114</v>
       </c>
-      <c r="IY1" s="21" t="n">
+      <c r="IY1" s="22" t="n">
         <v>44115</v>
       </c>
-      <c r="IZ1" s="21" t="n">
+      <c r="IZ1" s="22" t="n">
         <v>44116</v>
       </c>
-      <c r="JA1" s="21" t="n">
+      <c r="JA1" s="22" t="n">
         <v>44117</v>
       </c>
-      <c r="JB1" s="21" t="n">
+      <c r="JB1" s="22" t="n">
         <v>44118</v>
       </c>
-      <c r="JC1" s="21" t="n">
+      <c r="JC1" s="22" t="n">
         <v>44119</v>
       </c>
-      <c r="JD1" s="21" t="n">
+      <c r="JD1" s="22" t="n">
         <v>44120</v>
       </c>
-      <c r="JE1" s="21" t="n">
+      <c r="JE1" s="22" t="n">
         <v>44121</v>
       </c>
-      <c r="JF1" s="21" t="n">
+      <c r="JF1" s="22" t="n">
         <v>44122</v>
       </c>
-      <c r="JG1" s="21" t="n">
+      <c r="JG1" s="22" t="n">
         <v>44123</v>
       </c>
-      <c r="JH1" s="21" t="n">
+      <c r="JH1" s="22" t="n">
         <v>44124</v>
       </c>
-      <c r="JI1" s="21" t="n">
+      <c r="JI1" s="22" t="n">
         <v>44125</v>
       </c>
-      <c r="JJ1" s="21" t="n">
+      <c r="JJ1" s="22" t="n">
         <v>44126</v>
       </c>
-      <c r="JK1" s="21" t="n">
+      <c r="JK1" s="22" t="n">
         <v>44127</v>
       </c>
-      <c r="JL1" s="21" t="n">
+      <c r="JL1" s="22" t="n">
         <v>44128</v>
       </c>
-      <c r="JM1" s="21" t="n">
+      <c r="JM1" s="22" t="n">
         <v>44129</v>
       </c>
-      <c r="JN1" s="21" t="n">
+      <c r="JN1" s="22" t="n">
         <v>44130</v>
       </c>
-      <c r="JO1" s="21" t="n">
+      <c r="JO1" s="22" t="n">
         <v>44131</v>
       </c>
-      <c r="JP1" s="21" t="n">
+      <c r="JP1" s="22" t="n">
         <v>44132</v>
       </c>
-      <c r="JQ1" s="21" t="n">
+      <c r="JQ1" s="22" t="n">
         <v>44133</v>
       </c>
-      <c r="JR1" s="21" t="n">
+      <c r="JR1" s="22" t="n">
         <v>44134</v>
       </c>
-      <c r="JS1" s="21" t="n">
+      <c r="JS1" s="22" t="n">
         <v>44135</v>
       </c>
-      <c r="JT1" s="21" t="n">
+      <c r="JT1" s="22" t="n">
         <v>44136</v>
       </c>
-      <c r="JU1" s="21" t="n">
+      <c r="JU1" s="22" t="n">
         <v>44137</v>
       </c>
-      <c r="JV1" s="21" t="n">
+      <c r="JV1" s="22" t="n">
         <v>44138</v>
       </c>
-      <c r="JW1" s="21" t="n">
+      <c r="JW1" s="22" t="n">
         <v>44139</v>
       </c>
-      <c r="JX1" s="21" t="n">
+      <c r="JX1" s="22" t="n">
         <v>44140</v>
       </c>
-      <c r="JY1" s="21" t="n">
+      <c r="JY1" s="22" t="n">
         <v>44141</v>
       </c>
-      <c r="JZ1" s="21" t="n">
+      <c r="JZ1" s="22" t="n">
         <v>44142</v>
       </c>
-      <c r="KA1" s="21" t="n">
+      <c r="KA1" s="22" t="n">
         <v>44143</v>
       </c>
-      <c r="KB1" s="21" t="n">
+      <c r="KB1" s="22" t="n">
         <v>44144</v>
       </c>
-      <c r="KC1" s="21" t="n">
+      <c r="KC1" s="22" t="n">
         <v>44145</v>
       </c>
-      <c r="KD1" s="21" t="n">
+      <c r="KD1" s="22" t="n">
         <v>44146</v>
       </c>
-      <c r="KE1" s="21" t="n">
+      <c r="KE1" s="22" t="n">
         <v>44147</v>
       </c>
-      <c r="KF1" s="21" t="n">
+      <c r="KF1" s="22" t="n">
         <v>44148</v>
       </c>
-      <c r="KG1" s="21" t="n">
+      <c r="KG1" s="22" t="n">
         <v>44149</v>
       </c>
-      <c r="KH1" s="21" t="n">
+      <c r="KH1" s="22" t="n">
         <v>44150</v>
       </c>
-      <c r="KI1" s="21" t="n">
+      <c r="KI1" s="22" t="n">
         <v>44151</v>
       </c>
-      <c r="KJ1" s="21" t="n">
+      <c r="KJ1" s="22" t="n">
         <v>44152</v>
       </c>
-      <c r="KK1" s="21" t="n">
+      <c r="KK1" s="22" t="n">
         <v>44153</v>
       </c>
-      <c r="KL1" s="21" t="n">
+      <c r="KL1" s="22" t="n">
         <v>44154</v>
       </c>
-      <c r="KM1" s="21" t="n">
+      <c r="KM1" s="22" t="n">
         <v>44155</v>
       </c>
-      <c r="KN1" s="21" t="n">
+      <c r="KN1" s="22" t="n">
         <v>44156</v>
       </c>
-      <c r="KO1" s="21" t="n">
+      <c r="KO1" s="22" t="n">
         <v>44157</v>
       </c>
-      <c r="KP1" s="21" t="n">
+      <c r="KP1" s="22" t="n">
         <v>44158</v>
       </c>
-      <c r="KQ1" s="21" t="n">
+      <c r="KQ1" s="22" t="n">
         <v>44159</v>
       </c>
-      <c r="KR1" s="21" t="n">
+      <c r="KR1" s="22" t="n">
         <v>44160</v>
       </c>
-      <c r="KS1" s="21" t="n">
+      <c r="KS1" s="22" t="n">
         <v>44161</v>
       </c>
-      <c r="KT1" s="21" t="n">
+      <c r="KT1" s="22" t="n">
         <v>44162</v>
       </c>
-      <c r="KU1" s="21" t="n">
+      <c r="KU1" s="22" t="n">
         <v>44163</v>
       </c>
-      <c r="KV1" s="21" t="n">
+      <c r="KV1" s="22" t="n">
         <v>44164</v>
       </c>
-      <c r="KW1" s="21" t="n">
+      <c r="KW1" s="22" t="n">
         <v>44165</v>
       </c>
-      <c r="KX1" s="21" t="n">
+      <c r="KX1" s="22" t="n">
         <v>44166</v>
       </c>
-      <c r="KY1" s="21" t="n">
+      <c r="KY1" s="22" t="n">
         <v>44167</v>
       </c>
-      <c r="KZ1" s="21" t="n">
+      <c r="KZ1" s="22" t="n">
         <v>44168</v>
       </c>
-      <c r="LA1" s="21" t="n">
+      <c r="LA1" s="22" t="n">
         <v>44169</v>
       </c>
-      <c r="LB1" s="21" t="n">
+      <c r="LB1" s="22" t="n">
         <v>44170</v>
       </c>
-      <c r="LC1" s="21" t="n">
+      <c r="LC1" s="22" t="n">
         <v>44171</v>
       </c>
-      <c r="LD1" s="21" t="n">
+      <c r="LD1" s="22" t="n">
         <v>44172</v>
       </c>
-      <c r="LE1" s="21" t="n">
+      <c r="LE1" s="22" t="n">
         <v>44173</v>
       </c>
-      <c r="LF1" s="21" t="n">
+      <c r="LF1" s="22" t="n">
         <v>44174</v>
       </c>
-      <c r="LG1" s="21" t="n">
+      <c r="LG1" s="22" t="n">
         <v>44175</v>
       </c>
-      <c r="LH1" s="21" t="n">
+      <c r="LH1" s="22" t="n">
         <v>44176</v>
       </c>
-      <c r="LI1" s="21" t="n">
+      <c r="LI1" s="22" t="n">
         <v>44177</v>
       </c>
-      <c r="LJ1" s="21" t="n">
+      <c r="LJ1" s="22" t="n">
         <v>44178</v>
       </c>
-      <c r="LK1" s="21" t="n">
+      <c r="LK1" s="22" t="n">
         <v>44179</v>
       </c>
-      <c r="LL1" s="21" t="n">
+      <c r="LL1" s="22" t="n">
         <v>44180</v>
       </c>
-      <c r="LM1" s="21" t="n">
+      <c r="LM1" s="22" t="n">
         <v>44181</v>
       </c>
-      <c r="LN1" s="21" t="n">
+      <c r="LN1" s="22" t="n">
         <v>44182</v>
       </c>
-      <c r="LO1" s="21" t="n">
+      <c r="LO1" s="22" t="n">
         <v>44183</v>
       </c>
-      <c r="LP1" s="21" t="n">
+      <c r="LP1" s="22" t="n">
         <v>44184</v>
       </c>
-      <c r="LQ1" s="21" t="n">
+      <c r="LQ1" s="22" t="n">
         <v>44185</v>
       </c>
-      <c r="LR1" s="21" t="n">
+      <c r="LR1" s="22" t="n">
         <v>44186</v>
       </c>
-      <c r="LS1" s="21" t="n">
+      <c r="LS1" s="22" t="n">
         <v>44187</v>
       </c>
-      <c r="LT1" s="21" t="n">
+      <c r="LT1" s="22" t="n">
         <v>44188</v>
       </c>
-      <c r="LU1" s="21" t="n">
+      <c r="LU1" s="22" t="n">
         <v>44189</v>
       </c>
-      <c r="LV1" s="21" t="n">
+      <c r="LV1" s="22" t="n">
         <v>44190</v>
       </c>
-      <c r="LW1" s="21" t="n">
+      <c r="LW1" s="22" t="n">
         <v>44191</v>
       </c>
-      <c r="LX1" s="21" t="n">
+      <c r="LX1" s="22" t="n">
         <v>44192</v>
       </c>
-      <c r="LY1" s="21" t="n">
+      <c r="LY1" s="22" t="n">
         <v>44193</v>
       </c>
-      <c r="LZ1" s="21" t="n">
+      <c r="LZ1" s="22" t="n">
         <v>44194</v>
       </c>
-      <c r="MA1" s="21" t="n">
+      <c r="MA1" s="22" t="n">
         <v>44195</v>
       </c>
-      <c r="MB1" s="21" t="n">
+      <c r="MB1" s="22" t="n">
         <v>44196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -5523,10 +5554,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="0" t="s">
@@ -5537,10 +5568,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="0" t="s">
@@ -5551,7 +5582,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -5565,67 +5596,67 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L13" s="22" t="s">
+      <c r="L13" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N15" s="22" t="s">
+      <c r="N15" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O16" s="22" t="s">
+      <c r="O16" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P17" s="22" t="s">
+      <c r="P17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q18" s="22" t="s">
+      <c r="Q18" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5647,11 +5678,11 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -5668,56 +5699,56 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.13"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="H1" s="25" t="s">
+    <row r="1" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="H1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-    </row>
-    <row r="2" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+    </row>
+    <row r="2" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="30" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5731,12 +5762,12 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
@@ -5748,12 +5779,12 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
@@ -5765,12 +5796,12 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
@@ -5782,12 +5813,12 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
@@ -5800,12 +5831,12 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -5818,12 +5849,12 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
@@ -5836,12 +5867,12 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
@@ -5853,287 +5884,322 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33" t="n">
+      <c r="A11" s="34" t="n">
         <v>43869</v>
       </c>
-      <c r="B11" s="34" t="n">
+      <c r="B11" s="35" t="n">
         <v>47</v>
       </c>
-      <c r="C11" s="35" t="n">
+      <c r="C11" s="36" t="n">
         <f aca="false">SUM(B3:B11)</f>
         <v>617</v>
       </c>
-      <c r="D11" s="34" t="n">
+      <c r="D11" s="35" t="n">
         <v>9</v>
       </c>
-      <c r="E11" s="34" t="n">
+      <c r="E11" s="35" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C11/D11)</f>
         <v>69</v>
       </c>
-      <c r="F11" s="34" t="n">
+      <c r="F11" s="35" t="n">
         <f aca="false">D$23-D11</f>
         <v>22</v>
       </c>
-      <c r="G11" s="33" t="n">
+      <c r="G11" s="34" t="n">
         <f aca="false">$A11+F11</f>
         <v>43891</v>
       </c>
-      <c r="H11" s="36" t="n">
+      <c r="H11" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C11)/E$23)</f>
         <v>19</v>
       </c>
-      <c r="I11" s="37" t="n">
+      <c r="I11" s="38" t="n">
         <f aca="false">$A11+H11</f>
         <v>43888</v>
       </c>
-      <c r="J11" s="38" t="n">
+      <c r="J11" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C11)/$E11)</f>
         <v>14</v>
       </c>
-      <c r="K11" s="39" t="n">
+      <c r="K11" s="40" t="n">
         <f aca="false">$A11+J11</f>
         <v>43883</v>
       </c>
-      <c r="L11" s="40" t="n">
+      <c r="L11" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C11)/((E11+E$23)/2))</f>
         <v>16</v>
       </c>
-      <c r="M11" s="41" t="n">
+      <c r="M11" s="42" t="n">
         <f aca="false">$A11+L11</f>
         <v>43885</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="n">
+      <c r="A12" s="34" t="n">
         <v>43870</v>
       </c>
-      <c r="B12" s="42" t="n">
+      <c r="B12" s="43" t="n">
         <v>26</v>
       </c>
-      <c r="C12" s="35" t="n">
+      <c r="C12" s="36" t="n">
         <f aca="false">C11+B12</f>
         <v>643</v>
       </c>
-      <c r="D12" s="34" t="n">
+      <c r="D12" s="35" t="n">
         <v>10</v>
       </c>
-      <c r="E12" s="34" t="n">
+      <c r="E12" s="35" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C12/D12)</f>
         <v>65</v>
       </c>
-      <c r="F12" s="34" t="n">
+      <c r="F12" s="35" t="n">
         <f aca="false">D$23-D12</f>
         <v>21</v>
       </c>
-      <c r="G12" s="33" t="n">
+      <c r="G12" s="34" t="n">
         <f aca="false">$A12+F12</f>
         <v>43891</v>
       </c>
-      <c r="H12" s="36" t="n">
+      <c r="H12" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C12)/E$23)</f>
         <v>18</v>
       </c>
-      <c r="I12" s="37" t="n">
+      <c r="I12" s="38" t="n">
         <f aca="false">$A12+H12</f>
         <v>43888</v>
       </c>
-      <c r="J12" s="38" t="n">
+      <c r="J12" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C12)/$E12)</f>
         <v>14</v>
       </c>
-      <c r="K12" s="39" t="n">
+      <c r="K12" s="40" t="n">
         <f aca="false">$A12+J12</f>
         <v>43884</v>
       </c>
-      <c r="L12" s="40" t="n">
+      <c r="L12" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C12)/((E12+E$23)/2))</f>
         <v>16</v>
       </c>
-      <c r="M12" s="41" t="n">
+      <c r="M12" s="42" t="n">
         <f aca="false">$A12+L12</f>
         <v>43886</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="n">
+      <c r="A13" s="34" t="n">
         <v>43873</v>
       </c>
       <c r="B13" s="4" t="n">
         <f aca="false">120+4</f>
         <v>124</v>
       </c>
-      <c r="C13" s="35" t="n">
+      <c r="C13" s="36" t="n">
         <f aca="false">C12+B13</f>
         <v>767</v>
       </c>
-      <c r="D13" s="34" t="n">
+      <c r="D13" s="35" t="n">
         <v>13</v>
       </c>
-      <c r="E13" s="34" t="n">
+      <c r="E13" s="35" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C13/D13)</f>
         <v>59</v>
       </c>
-      <c r="F13" s="34" t="n">
+      <c r="F13" s="35" t="n">
         <f aca="false">D$23-D13</f>
         <v>18</v>
       </c>
-      <c r="G13" s="33" t="n">
+      <c r="G13" s="34" t="n">
         <f aca="false">$A13+F13</f>
         <v>43891</v>
       </c>
-      <c r="H13" s="36" t="n">
+      <c r="H13" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C13)/E$23)</f>
         <v>16</v>
       </c>
-      <c r="I13" s="37" t="n">
+      <c r="I13" s="38" t="n">
         <f aca="false">$A13+H13</f>
         <v>43889</v>
       </c>
-      <c r="J13" s="38" t="n">
+      <c r="J13" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C13)/$E13)</f>
         <v>14</v>
       </c>
-      <c r="K13" s="39" t="n">
+      <c r="K13" s="40" t="n">
         <f aca="false">$A13+J13</f>
         <v>43887</v>
       </c>
-      <c r="L13" s="40" t="n">
+      <c r="L13" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C13)/((E13+E$23)/2))</f>
         <v>15</v>
       </c>
-      <c r="M13" s="41" t="n">
+      <c r="M13" s="42" t="n">
         <f aca="false">$A13+L13</f>
         <v>43888</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33" t="n">
+      <c r="A14" s="34" t="n">
         <v>43873</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C14" s="35" t="n">
+      <c r="C14" s="36" t="n">
         <f aca="false">C13+B14</f>
         <v>799</v>
       </c>
-      <c r="D14" s="34" t="n">
+      <c r="D14" s="35" t="n">
         <v>13</v>
       </c>
-      <c r="E14" s="34" t="n">
+      <c r="E14" s="35" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C14/D14)</f>
         <v>62</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="35" t="n">
         <f aca="false">D$23-D14</f>
         <v>18</v>
       </c>
-      <c r="G14" s="33" t="n">
+      <c r="G14" s="34" t="n">
         <f aca="false">$A14+F14</f>
         <v>43891</v>
       </c>
-      <c r="H14" s="36" t="n">
+      <c r="H14" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C14)/E$23)</f>
         <v>15</v>
       </c>
-      <c r="I14" s="37" t="n">
+      <c r="I14" s="38" t="n">
         <f aca="false">$A14+H14</f>
         <v>43888</v>
       </c>
-      <c r="J14" s="38" t="n">
+      <c r="J14" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C14)/$E14)</f>
         <v>12</v>
       </c>
-      <c r="K14" s="39" t="n">
+      <c r="K14" s="40" t="n">
         <f aca="false">$A14+J14</f>
         <v>43885</v>
       </c>
-      <c r="L14" s="40" t="n">
+      <c r="L14" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C14)/((E14+E$23)/2))</f>
         <v>14</v>
       </c>
-      <c r="M14" s="41" t="n">
+      <c r="M14" s="42" t="n">
         <f aca="false">$A14+L14</f>
         <v>43887</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="33" t="n">
+      <c r="A15" s="34" t="n">
         <v>43880</v>
       </c>
       <c r="B15" s="4" t="n">
         <f aca="false">120+33</f>
         <v>153</v>
       </c>
-      <c r="C15" s="35" t="n">
+      <c r="C15" s="36" t="n">
         <f aca="false">C14+B15</f>
         <v>952</v>
       </c>
-      <c r="D15" s="34" t="n">
+      <c r="D15" s="35" t="n">
         <f aca="false">D14+(A15-A14)</f>
         <v>20</v>
       </c>
-      <c r="E15" s="34" t="n">
+      <c r="E15" s="35" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C15/D15)</f>
         <v>48</v>
       </c>
-      <c r="F15" s="34" t="n">
+      <c r="F15" s="35" t="n">
         <f aca="false">D$23-D15</f>
         <v>11</v>
       </c>
-      <c r="G15" s="33" t="n">
+      <c r="G15" s="34" t="n">
         <f aca="false">$A15+F15</f>
         <v>43891</v>
       </c>
-      <c r="H15" s="36" t="n">
+      <c r="H15" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C15)/E$23)</f>
         <v>12</v>
       </c>
-      <c r="I15" s="37" t="n">
+      <c r="I15" s="38" t="n">
         <f aca="false">$A15+H15</f>
         <v>43892</v>
       </c>
-      <c r="J15" s="38" t="n">
+      <c r="J15" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C15)/$E15)</f>
         <v>13</v>
       </c>
-      <c r="K15" s="39" t="n">
+      <c r="K15" s="40" t="n">
         <f aca="false">$A15+J15</f>
         <v>43893</v>
       </c>
-      <c r="L15" s="40" t="n">
+      <c r="L15" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C15)/((E15+E$23)/2))</f>
         <v>12</v>
       </c>
-      <c r="M15" s="41" t="n">
+      <c r="M15" s="42" t="n">
         <f aca="false">$A15+L15</f>
         <v>43892</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
+      <c r="A16" s="34" t="n">
+        <v>43882</v>
+      </c>
       <c r="B16" s="4" t="n">
         <v>77</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="C16" s="36" t="n">
+        <f aca="false">C15+B16</f>
+        <v>1029</v>
+      </c>
+      <c r="D16" s="35" t="n">
+        <f aca="false">D15+(A16-A15)</f>
+        <v>22</v>
+      </c>
+      <c r="E16" s="35" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C16/D16)</f>
+        <v>47</v>
+      </c>
+      <c r="F16" s="35" t="n">
+        <f aca="false">D$23-D16</f>
+        <v>9</v>
+      </c>
+      <c r="G16" s="34" t="n">
+        <f aca="false">$A16+F16</f>
+        <v>43891</v>
+      </c>
+      <c r="H16" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C16)/E$23)</f>
+        <v>11</v>
+      </c>
+      <c r="I16" s="38" t="n">
+        <f aca="false">$A16+H16</f>
+        <v>43893</v>
+      </c>
+      <c r="J16" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C16)/$E16)</f>
+        <v>11</v>
+      </c>
+      <c r="K16" s="40" t="n">
+        <f aca="false">$A16+J16</f>
+        <v>43893</v>
+      </c>
+      <c r="L16" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C16)/((E16+E$23)/2))</f>
+        <v>11</v>
+      </c>
+      <c r="M16" s="42" t="n">
+        <f aca="false">$A16+L16</f>
+        <v>43893</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
@@ -6146,12 +6212,12 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
@@ -6163,12 +6229,12 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
@@ -6180,12 +6246,12 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
@@ -6197,12 +6263,12 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
@@ -6214,12 +6280,12 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
@@ -6231,37 +6297,37 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="43" t="n">
+      <c r="A23" s="44" t="n">
         <f aca="false">A11+(D23-D11)</f>
         <v>43891</v>
       </c>
-      <c r="B23" s="44" t="n">
+      <c r="B23" s="45" t="n">
         <f aca="false">SUM(B3:B22)</f>
         <v>1535</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44" t="n">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45" t="n">
         <v>31</v>
       </c>
-      <c r="E23" s="44" t="n">
+      <c r="E23" s="45" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B23/D23)</f>
         <v>50</v>
       </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="45"/>
+      <c r="B24" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Restante dos exemplos de Programaçao Funcional
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
@@ -586,15 +586,15 @@
   </sheetPr>
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
       <selection pane="bottomRight" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -1147,7 +1147,9 @@
         <v>43883</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="10"/>
+      <c r="D28" s="9" t="n">
+        <v>0.0229166666666667</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -1164,7 +1166,9 @@
         <v>43884</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -1181,7 +1185,9 @@
         <v>43885</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="10"/>
+      <c r="D30" s="9" t="n">
+        <v>0.0819444444444444</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -1198,7 +1204,9 @@
         <v>43886</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="9" t="n">
+        <v>0.05</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -4158,7 +4166,7 @@
       </c>
       <c r="D205" s="16" t="n">
         <f aca="false">SUM(D2:D204)</f>
-        <v>1.30277777777778</v>
+        <v>1.45763888888889</v>
       </c>
       <c r="E205" s="16" t="n">
         <f aca="false">SUM(E2:E204)</f>
@@ -4211,7 +4219,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4462,7 +4470,7 @@
       <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5678,11 +5686,11 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -6202,22 +6210,57 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
+      <c r="A17" s="34" t="n">
+        <v>43886</v>
+      </c>
       <c r="B17" s="4" t="n">
         <f aca="false">120+6</f>
         <v>126</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
+      <c r="C17" s="36" t="n">
+        <f aca="false">C16+B17</f>
+        <v>1155</v>
+      </c>
+      <c r="D17" s="35" t="n">
+        <f aca="false">D16+(A17-A16)</f>
+        <v>26</v>
+      </c>
+      <c r="E17" s="35" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C17/D17)</f>
+        <v>45</v>
+      </c>
+      <c r="F17" s="35" t="n">
+        <f aca="false">D$23-D17</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="34" t="n">
+        <f aca="false">$A17+F17</f>
+        <v>43891</v>
+      </c>
+      <c r="H17" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C17)/E$23)</f>
+        <v>8</v>
+      </c>
+      <c r="I17" s="38" t="n">
+        <f aca="false">$A17+H17</f>
+        <v>43894</v>
+      </c>
+      <c r="J17" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C17)/$E17)</f>
+        <v>9</v>
+      </c>
+      <c r="K17" s="40" t="n">
+        <f aca="false">$A17+J17</f>
+        <v>43895</v>
+      </c>
+      <c r="L17" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C17)/((E17+E$23)/2))</f>
+        <v>8</v>
+      </c>
+      <c r="M17" s="42" t="n">
+        <f aca="false">$A17+L17</f>
+        <v>43894</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>

</xml_diff>

<commit_message>
Modulo de BD encerrado
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -594,7 +594,7 @@
       <selection pane="bottomRight" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -4219,7 +4219,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4470,7 +4470,7 @@
       <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -5687,10 +5687,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
@@ -6263,55 +6263,160 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
+      <c r="A18" s="34" t="n">
+        <v>43887</v>
+      </c>
       <c r="B18" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
+      <c r="C18" s="36" t="n">
+        <f aca="false">C17+B18</f>
+        <v>1186</v>
+      </c>
+      <c r="D18" s="35" t="n">
+        <f aca="false">D17+(A18-A17)</f>
+        <v>27</v>
+      </c>
+      <c r="E18" s="35" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C18/D18)</f>
+        <v>44</v>
+      </c>
+      <c r="F18" s="35" t="n">
+        <f aca="false">D$23-D18</f>
+        <v>4</v>
+      </c>
+      <c r="G18" s="34" t="n">
+        <f aca="false">$A18+F18</f>
+        <v>43891</v>
+      </c>
+      <c r="H18" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C18)/E$23)</f>
+        <v>7</v>
+      </c>
+      <c r="I18" s="38" t="n">
+        <f aca="false">$A18+H18</f>
+        <v>43894</v>
+      </c>
+      <c r="J18" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C18)/$E18)</f>
+        <v>8</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <f aca="false">$A18+J18</f>
+        <v>43895</v>
+      </c>
+      <c r="L18" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C18)/((E18+E$23)/2))</f>
+        <v>8</v>
+      </c>
+      <c r="M18" s="42" t="n">
+        <f aca="false">$A18+L18</f>
+        <v>43895</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
+      <c r="A19" s="34" t="n">
+        <v>43887</v>
+      </c>
       <c r="B19" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
+      <c r="C19" s="36" t="n">
+        <f aca="false">C18+B19</f>
+        <v>1204</v>
+      </c>
+      <c r="D19" s="35" t="n">
+        <f aca="false">D18+(A19-A18)</f>
+        <v>27</v>
+      </c>
+      <c r="E19" s="35" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C19/D19)</f>
+        <v>45</v>
+      </c>
+      <c r="F19" s="35" t="n">
+        <f aca="false">D$23-D19</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="34" t="n">
+        <f aca="false">$A19+F19</f>
+        <v>43891</v>
+      </c>
+      <c r="H19" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C19)/E$23)</f>
+        <v>7</v>
+      </c>
+      <c r="I19" s="38" t="n">
+        <f aca="false">$A19+H19</f>
+        <v>43894</v>
+      </c>
+      <c r="J19" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C19)/$E19)</f>
+        <v>8</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <f aca="false">$A19+J19</f>
+        <v>43895</v>
+      </c>
+      <c r="L19" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C19)/((E19+E$23)/2))</f>
+        <v>7</v>
+      </c>
+      <c r="M19" s="42" t="n">
+        <f aca="false">$A19+L19</f>
+        <v>43894</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
+      <c r="A20" s="34" t="n">
+        <v>43889</v>
+      </c>
       <c r="B20" s="4" t="n">
         <v>182</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
+      <c r="C20" s="36" t="n">
+        <f aca="false">C19+B20</f>
+        <v>1386</v>
+      </c>
+      <c r="D20" s="35" t="n">
+        <f aca="false">D19+(A20-A19)</f>
+        <v>29</v>
+      </c>
+      <c r="E20" s="35" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C20/D20)</f>
+        <v>48</v>
+      </c>
+      <c r="F20" s="35" t="n">
+        <f aca="false">D$23-D20</f>
+        <v>2</v>
+      </c>
+      <c r="G20" s="34" t="n">
+        <f aca="false">$A20+F20</f>
+        <v>43891</v>
+      </c>
+      <c r="H20" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C20)/E$23)</f>
+        <v>3</v>
+      </c>
+      <c r="I20" s="38" t="n">
+        <f aca="false">$A20+H20</f>
+        <v>43892</v>
+      </c>
+      <c r="J20" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C20)/$E20)</f>
+        <v>4</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <f aca="false">$A20+J20</f>
+        <v>43893</v>
+      </c>
+      <c r="L20" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C20)/((E20+E$23)/2))</f>
+        <v>4</v>
+      </c>
+      <c r="M20" s="42" t="n">
+        <f aca="false">$A20+L20</f>
+        <v>43893</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>

</xml_diff>

<commit_message>
Finalizando o modulo de BD com Python e o curos Python3 Completo
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
   <si>
     <t xml:space="preserve">dia</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">Python3 Completo</t>
   </si>
   <si>
+    <t xml:space="preserve">Curso Python3</t>
+  </si>
+  <si>
     <t xml:space="preserve">dias para acabar</t>
   </si>
   <si>
@@ -120,19 +123,55 @@
   <si>
     <t xml:space="preserve">Data 2</t>
   </si>
+  <si>
+    <t xml:space="preserve">Livro WebScraping com Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capítulos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">págs do capítulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. cada Capítulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total de dias por capítulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total de horas por capítulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data de Início</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livro Pense Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ap A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ap B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D&quot;. &quot;MMM"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="169" formatCode="DD/MMM"/>
+    <numFmt numFmtId="170" formatCode="0"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,8 +253,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF2A6099"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,7 +284,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB3CAC7"/>
-        <bgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFB4C7DC"/>
       </patternFill>
     </fill>
     <fill>
@@ -256,6 +303,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD7D7"/>
         <bgColor rgb="FFFFD8CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFB3CAC7"/>
       </patternFill>
     </fill>
     <fill>
@@ -318,7 +371,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -399,7 +452,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,7 +472,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -431,11 +492,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,11 +504,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,19 +528,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,6 +565,50 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +645,7 @@
       <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFDEDCE6"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -554,7 +659,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFDDE8CB"/>
       <rgbColor rgb="FFE8F2A1"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFDBB6"/>
@@ -591,10 +696,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="D27" activeCellId="1" sqref="H27:H44 D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
@@ -4213,13 +4318,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="H27:H44 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
@@ -4242,19 +4347,20 @@
       <c r="G1" s="19" t="s">
         <v>15</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="20" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="20" t="n">
+      <c r="C2" s="21" t="n">
         <f aca="false">B2/$B$11</f>
-        <v>0.0207715133531157</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>0.0205278592375367</v>
+      </c>
+      <c r="D2" s="22" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C2*$D$1)</f>
         <v>5</v>
       </c>
@@ -4265,29 +4371,29 @@
       <c r="F2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="21" t="n">
+      <c r="G2" s="23" t="n">
         <f aca="false">D2-F2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="20" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="C3" s="20" t="n">
+      <c r="C3" s="21" t="n">
         <f aca="false">B3/$B$11</f>
-        <v>0.154302670623145</v>
-      </c>
-      <c r="D3" s="0" t="n">
+        <v>0.152492668621701</v>
+      </c>
+      <c r="D3" s="22" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C3*$D$1)</f>
         <v>31</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C3*$E$1)</f>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4295,19 +4401,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="C4" s="20" t="n">
+        <v>42</v>
+      </c>
+      <c r="C4" s="21" t="n">
         <f aca="false">B4/$B$11</f>
-        <v>0.112759643916914</v>
+        <v>0.12316715542522</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C4*$D$1)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C4*$E$1)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4317,9 +4423,9 @@
       <c r="B5" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="C5" s="20" t="n">
+      <c r="C5" s="21" t="n">
         <f aca="false">B5/$B$11</f>
-        <v>0.106824925816024</v>
+        <v>0.105571847507331</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C5*$D$1)</f>
@@ -4327,7 +4433,7 @@
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C5*$E$1)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4337,9 +4443,9 @@
       <c r="B6" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C6" s="20" t="n">
+      <c r="C6" s="21" t="n">
         <f aca="false">B6/$B$11</f>
-        <v>0.124629080118694</v>
+        <v>0.12316715542522</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C6*$D$1)</f>
@@ -4347,7 +4453,7 @@
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C6*$E$1)</f>
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4357,9 +4463,9 @@
       <c r="B7" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="21" t="n">
         <f aca="false">B7/$B$11</f>
-        <v>0.0534124629080119</v>
+        <v>0.0527859237536657</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C7*$D$1)</f>
@@ -4367,7 +4473,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C7*$E$1)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4377,9 +4483,9 @@
       <c r="B8" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="C8" s="20" t="n">
+      <c r="C8" s="21" t="n">
         <f aca="false">B8/$B$11</f>
-        <v>0.189910979228487</v>
+        <v>0.187683284457478</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C8*$D$1)</f>
@@ -4397,9 +4503,9 @@
       <c r="B9" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C9" s="20" t="n">
+      <c r="C9" s="21" t="n">
         <f aca="false">B9/$B$11</f>
-        <v>0.0949554896142433</v>
+        <v>0.093841642228739</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C9*$D$1)</f>
@@ -4417,9 +4523,9 @@
       <c r="B10" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="21" t="n">
         <f aca="false">B10/$B$11</f>
-        <v>0.142433234421365</v>
+        <v>0.140762463343109</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C10*$D$1)</f>
@@ -4433,7 +4539,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="17" t="n">
         <f aca="false">SUM(B2:B10)</f>
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C11" s="18" t="n">
         <f aca="false">B11/$B$11</f>
@@ -4441,11 +4547,11 @@
       </c>
       <c r="D11" s="17" t="n">
         <f aca="false">SUM(D2:D10)</f>
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E11" s="17" t="n">
         <f aca="false">SUM(E2:E10)</f>
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4467,10 +4573,10 @@
   <dimension ref="A1:MB18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
+      <selection pane="topLeft" activeCell="Q18" activeCellId="1" sqref="H27:H44 Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.88"/>
@@ -4526,1032 +4632,1032 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="n">
+      <c r="A1" s="24" t="n">
         <v>43857</v>
       </c>
-      <c r="B1" s="22" t="n">
+      <c r="B1" s="24" t="n">
         <v>43858</v>
       </c>
-      <c r="C1" s="22" t="n">
+      <c r="C1" s="24" t="n">
         <v>43859</v>
       </c>
-      <c r="D1" s="22" t="n">
+      <c r="D1" s="24" t="n">
         <v>43860</v>
       </c>
-      <c r="E1" s="22" t="n">
+      <c r="E1" s="24" t="n">
         <v>43861</v>
       </c>
-      <c r="F1" s="22" t="n">
+      <c r="F1" s="24" t="n">
         <v>43862</v>
       </c>
-      <c r="G1" s="22" t="n">
+      <c r="G1" s="24" t="n">
         <v>43863</v>
       </c>
-      <c r="H1" s="22" t="n">
+      <c r="H1" s="24" t="n">
         <v>43864</v>
       </c>
-      <c r="I1" s="22" t="n">
+      <c r="I1" s="24" t="n">
         <v>43865</v>
       </c>
-      <c r="J1" s="22" t="n">
+      <c r="J1" s="24" t="n">
         <v>43866</v>
       </c>
-      <c r="K1" s="22" t="n">
+      <c r="K1" s="24" t="n">
         <v>43867</v>
       </c>
-      <c r="L1" s="22" t="n">
+      <c r="L1" s="24" t="n">
         <v>43868</v>
       </c>
-      <c r="M1" s="22" t="n">
+      <c r="M1" s="24" t="n">
         <v>43869</v>
       </c>
-      <c r="N1" s="22" t="n">
+      <c r="N1" s="24" t="n">
         <v>43870</v>
       </c>
-      <c r="O1" s="22" t="n">
+      <c r="O1" s="24" t="n">
         <v>43871</v>
       </c>
-      <c r="P1" s="22" t="n">
+      <c r="P1" s="24" t="n">
         <v>43872</v>
       </c>
-      <c r="Q1" s="22" t="n">
+      <c r="Q1" s="24" t="n">
         <v>43873</v>
       </c>
-      <c r="R1" s="22" t="n">
+      <c r="R1" s="24" t="n">
         <v>43874</v>
       </c>
-      <c r="S1" s="22" t="n">
+      <c r="S1" s="24" t="n">
         <v>43875</v>
       </c>
-      <c r="T1" s="22" t="n">
+      <c r="T1" s="24" t="n">
         <v>43876</v>
       </c>
-      <c r="U1" s="22" t="n">
+      <c r="U1" s="24" t="n">
         <v>43877</v>
       </c>
-      <c r="V1" s="22" t="n">
+      <c r="V1" s="24" t="n">
         <v>43878</v>
       </c>
-      <c r="W1" s="22" t="n">
+      <c r="W1" s="24" t="n">
         <v>43879</v>
       </c>
-      <c r="X1" s="22" t="n">
+      <c r="X1" s="24" t="n">
         <v>43880</v>
       </c>
-      <c r="Y1" s="22" t="n">
+      <c r="Y1" s="24" t="n">
         <v>43881</v>
       </c>
-      <c r="Z1" s="22" t="n">
+      <c r="Z1" s="24" t="n">
         <v>43882</v>
       </c>
-      <c r="AA1" s="22" t="n">
+      <c r="AA1" s="24" t="n">
         <v>43883</v>
       </c>
-      <c r="AB1" s="22" t="n">
+      <c r="AB1" s="24" t="n">
         <v>43884</v>
       </c>
-      <c r="AC1" s="22" t="n">
+      <c r="AC1" s="24" t="n">
         <v>43885</v>
       </c>
-      <c r="AD1" s="22" t="n">
+      <c r="AD1" s="24" t="n">
         <v>43886</v>
       </c>
-      <c r="AE1" s="22" t="n">
+      <c r="AE1" s="24" t="n">
         <v>43887</v>
       </c>
-      <c r="AF1" s="22" t="n">
+      <c r="AF1" s="24" t="n">
         <v>43888</v>
       </c>
-      <c r="AG1" s="22" t="n">
+      <c r="AG1" s="24" t="n">
         <v>43889</v>
       </c>
-      <c r="AH1" s="22" t="n">
+      <c r="AH1" s="24" t="n">
         <v>43890</v>
       </c>
-      <c r="AI1" s="22" t="n">
+      <c r="AI1" s="24" t="n">
         <v>43891</v>
       </c>
-      <c r="AJ1" s="22" t="n">
+      <c r="AJ1" s="24" t="n">
         <v>43892</v>
       </c>
-      <c r="AK1" s="22" t="n">
+      <c r="AK1" s="24" t="n">
         <v>43893</v>
       </c>
-      <c r="AL1" s="22" t="n">
+      <c r="AL1" s="24" t="n">
         <v>43894</v>
       </c>
-      <c r="AM1" s="22" t="n">
+      <c r="AM1" s="24" t="n">
         <v>43895</v>
       </c>
-      <c r="AN1" s="22" t="n">
+      <c r="AN1" s="24" t="n">
         <v>43896</v>
       </c>
-      <c r="AO1" s="22" t="n">
+      <c r="AO1" s="24" t="n">
         <v>43897</v>
       </c>
-      <c r="AP1" s="22" t="n">
+      <c r="AP1" s="24" t="n">
         <v>43898</v>
       </c>
-      <c r="AQ1" s="22" t="n">
+      <c r="AQ1" s="24" t="n">
         <v>43899</v>
       </c>
-      <c r="AR1" s="22" t="n">
+      <c r="AR1" s="24" t="n">
         <v>43900</v>
       </c>
-      <c r="AS1" s="22" t="n">
+      <c r="AS1" s="24" t="n">
         <v>43901</v>
       </c>
-      <c r="AT1" s="22" t="n">
+      <c r="AT1" s="24" t="n">
         <v>43902</v>
       </c>
-      <c r="AU1" s="22" t="n">
+      <c r="AU1" s="24" t="n">
         <v>43903</v>
       </c>
-      <c r="AV1" s="22" t="n">
+      <c r="AV1" s="24" t="n">
         <v>43904</v>
       </c>
-      <c r="AW1" s="22" t="n">
+      <c r="AW1" s="24" t="n">
         <v>43905</v>
       </c>
-      <c r="AX1" s="22" t="n">
+      <c r="AX1" s="24" t="n">
         <v>43906</v>
       </c>
-      <c r="AY1" s="22" t="n">
+      <c r="AY1" s="24" t="n">
         <v>43907</v>
       </c>
-      <c r="AZ1" s="22" t="n">
+      <c r="AZ1" s="24" t="n">
         <v>43908</v>
       </c>
-      <c r="BA1" s="22" t="n">
+      <c r="BA1" s="24" t="n">
         <v>43909</v>
       </c>
-      <c r="BB1" s="22" t="n">
+      <c r="BB1" s="24" t="n">
         <v>43910</v>
       </c>
-      <c r="BC1" s="22" t="n">
+      <c r="BC1" s="24" t="n">
         <v>43911</v>
       </c>
-      <c r="BD1" s="22" t="n">
+      <c r="BD1" s="24" t="n">
         <v>43912</v>
       </c>
-      <c r="BE1" s="22" t="n">
+      <c r="BE1" s="24" t="n">
         <v>43913</v>
       </c>
-      <c r="BF1" s="22" t="n">
+      <c r="BF1" s="24" t="n">
         <v>43914</v>
       </c>
-      <c r="BG1" s="22" t="n">
+      <c r="BG1" s="24" t="n">
         <v>43915</v>
       </c>
-      <c r="BH1" s="22" t="n">
+      <c r="BH1" s="24" t="n">
         <v>43916</v>
       </c>
-      <c r="BI1" s="22" t="n">
+      <c r="BI1" s="24" t="n">
         <v>43917</v>
       </c>
-      <c r="BJ1" s="22" t="n">
+      <c r="BJ1" s="24" t="n">
         <v>43918</v>
       </c>
-      <c r="BK1" s="22" t="n">
+      <c r="BK1" s="24" t="n">
         <v>43919</v>
       </c>
-      <c r="BL1" s="22" t="n">
+      <c r="BL1" s="24" t="n">
         <v>43920</v>
       </c>
-      <c r="BM1" s="22" t="n">
+      <c r="BM1" s="24" t="n">
         <v>43921</v>
       </c>
-      <c r="BN1" s="22" t="n">
+      <c r="BN1" s="24" t="n">
         <v>43922</v>
       </c>
-      <c r="BO1" s="22" t="n">
+      <c r="BO1" s="24" t="n">
         <v>43923</v>
       </c>
-      <c r="BP1" s="22" t="n">
+      <c r="BP1" s="24" t="n">
         <v>43924</v>
       </c>
-      <c r="BQ1" s="22" t="n">
+      <c r="BQ1" s="24" t="n">
         <v>43925</v>
       </c>
-      <c r="BR1" s="22" t="n">
+      <c r="BR1" s="24" t="n">
         <v>43926</v>
       </c>
-      <c r="BS1" s="22" t="n">
+      <c r="BS1" s="24" t="n">
         <v>43927</v>
       </c>
-      <c r="BT1" s="22" t="n">
+      <c r="BT1" s="24" t="n">
         <v>43928</v>
       </c>
-      <c r="BU1" s="22" t="n">
+      <c r="BU1" s="24" t="n">
         <v>43929</v>
       </c>
-      <c r="BV1" s="22" t="n">
+      <c r="BV1" s="24" t="n">
         <v>43930</v>
       </c>
-      <c r="BW1" s="22" t="n">
+      <c r="BW1" s="24" t="n">
         <v>43931</v>
       </c>
-      <c r="BX1" s="22" t="n">
+      <c r="BX1" s="24" t="n">
         <v>43932</v>
       </c>
-      <c r="BY1" s="22" t="n">
+      <c r="BY1" s="24" t="n">
         <v>43933</v>
       </c>
-      <c r="BZ1" s="22" t="n">
+      <c r="BZ1" s="24" t="n">
         <v>43934</v>
       </c>
-      <c r="CA1" s="22" t="n">
+      <c r="CA1" s="24" t="n">
         <v>43935</v>
       </c>
-      <c r="CB1" s="22" t="n">
+      <c r="CB1" s="24" t="n">
         <v>43936</v>
       </c>
-      <c r="CC1" s="22" t="n">
+      <c r="CC1" s="24" t="n">
         <v>43937</v>
       </c>
-      <c r="CD1" s="22" t="n">
+      <c r="CD1" s="24" t="n">
         <v>43938</v>
       </c>
-      <c r="CE1" s="22" t="n">
+      <c r="CE1" s="24" t="n">
         <v>43939</v>
       </c>
-      <c r="CF1" s="22" t="n">
+      <c r="CF1" s="24" t="n">
         <v>43940</v>
       </c>
-      <c r="CG1" s="22" t="n">
+      <c r="CG1" s="24" t="n">
         <v>43941</v>
       </c>
-      <c r="CH1" s="22" t="n">
+      <c r="CH1" s="24" t="n">
         <v>43942</v>
       </c>
-      <c r="CI1" s="22" t="n">
+      <c r="CI1" s="24" t="n">
         <v>43943</v>
       </c>
-      <c r="CJ1" s="22" t="n">
+      <c r="CJ1" s="24" t="n">
         <v>43944</v>
       </c>
-      <c r="CK1" s="22" t="n">
+      <c r="CK1" s="24" t="n">
         <v>43945</v>
       </c>
-      <c r="CL1" s="22" t="n">
+      <c r="CL1" s="24" t="n">
         <v>43946</v>
       </c>
-      <c r="CM1" s="22" t="n">
+      <c r="CM1" s="24" t="n">
         <v>43947</v>
       </c>
-      <c r="CN1" s="22" t="n">
+      <c r="CN1" s="24" t="n">
         <v>43948</v>
       </c>
-      <c r="CO1" s="22" t="n">
+      <c r="CO1" s="24" t="n">
         <v>43949</v>
       </c>
-      <c r="CP1" s="22" t="n">
+      <c r="CP1" s="24" t="n">
         <v>43950</v>
       </c>
-      <c r="CQ1" s="22" t="n">
+      <c r="CQ1" s="24" t="n">
         <v>43951</v>
       </c>
-      <c r="CR1" s="22" t="n">
+      <c r="CR1" s="24" t="n">
         <v>43952</v>
       </c>
-      <c r="CS1" s="22" t="n">
+      <c r="CS1" s="24" t="n">
         <v>43953</v>
       </c>
-      <c r="CT1" s="22" t="n">
+      <c r="CT1" s="24" t="n">
         <v>43954</v>
       </c>
-      <c r="CU1" s="22" t="n">
+      <c r="CU1" s="24" t="n">
         <v>43955</v>
       </c>
-      <c r="CV1" s="22" t="n">
+      <c r="CV1" s="24" t="n">
         <v>43956</v>
       </c>
-      <c r="CW1" s="22" t="n">
+      <c r="CW1" s="24" t="n">
         <v>43957</v>
       </c>
-      <c r="CX1" s="22" t="n">
+      <c r="CX1" s="24" t="n">
         <v>43958</v>
       </c>
-      <c r="CY1" s="22" t="n">
+      <c r="CY1" s="24" t="n">
         <v>43959</v>
       </c>
-      <c r="CZ1" s="22" t="n">
+      <c r="CZ1" s="24" t="n">
         <v>43960</v>
       </c>
-      <c r="DA1" s="22" t="n">
+      <c r="DA1" s="24" t="n">
         <v>43961</v>
       </c>
-      <c r="DB1" s="22" t="n">
+      <c r="DB1" s="24" t="n">
         <v>43962</v>
       </c>
-      <c r="DC1" s="22" t="n">
+      <c r="DC1" s="24" t="n">
         <v>43963</v>
       </c>
-      <c r="DD1" s="22" t="n">
+      <c r="DD1" s="24" t="n">
         <v>43964</v>
       </c>
-      <c r="DE1" s="22" t="n">
+      <c r="DE1" s="24" t="n">
         <v>43965</v>
       </c>
-      <c r="DF1" s="22" t="n">
+      <c r="DF1" s="24" t="n">
         <v>43966</v>
       </c>
-      <c r="DG1" s="22" t="n">
+      <c r="DG1" s="24" t="n">
         <v>43967</v>
       </c>
-      <c r="DH1" s="22" t="n">
+      <c r="DH1" s="24" t="n">
         <v>43968</v>
       </c>
-      <c r="DI1" s="22" t="n">
+      <c r="DI1" s="24" t="n">
         <v>43969</v>
       </c>
-      <c r="DJ1" s="22" t="n">
+      <c r="DJ1" s="24" t="n">
         <v>43970</v>
       </c>
-      <c r="DK1" s="22" t="n">
+      <c r="DK1" s="24" t="n">
         <v>43971</v>
       </c>
-      <c r="DL1" s="22" t="n">
+      <c r="DL1" s="24" t="n">
         <v>43972</v>
       </c>
-      <c r="DM1" s="22" t="n">
+      <c r="DM1" s="24" t="n">
         <v>43973</v>
       </c>
-      <c r="DN1" s="22" t="n">
+      <c r="DN1" s="24" t="n">
         <v>43974</v>
       </c>
-      <c r="DO1" s="22" t="n">
+      <c r="DO1" s="24" t="n">
         <v>43975</v>
       </c>
-      <c r="DP1" s="22" t="n">
+      <c r="DP1" s="24" t="n">
         <v>43976</v>
       </c>
-      <c r="DQ1" s="22" t="n">
+      <c r="DQ1" s="24" t="n">
         <v>43977</v>
       </c>
-      <c r="DR1" s="22" t="n">
+      <c r="DR1" s="24" t="n">
         <v>43978</v>
       </c>
-      <c r="DS1" s="22" t="n">
+      <c r="DS1" s="24" t="n">
         <v>43979</v>
       </c>
-      <c r="DT1" s="22" t="n">
+      <c r="DT1" s="24" t="n">
         <v>43980</v>
       </c>
-      <c r="DU1" s="22" t="n">
+      <c r="DU1" s="24" t="n">
         <v>43981</v>
       </c>
-      <c r="DV1" s="22" t="n">
+      <c r="DV1" s="24" t="n">
         <v>43982</v>
       </c>
-      <c r="DW1" s="22" t="n">
+      <c r="DW1" s="24" t="n">
         <v>43983</v>
       </c>
-      <c r="DX1" s="22" t="n">
+      <c r="DX1" s="24" t="n">
         <v>43984</v>
       </c>
-      <c r="DY1" s="22" t="n">
+      <c r="DY1" s="24" t="n">
         <v>43985</v>
       </c>
-      <c r="DZ1" s="22" t="n">
+      <c r="DZ1" s="24" t="n">
         <v>43986</v>
       </c>
-      <c r="EA1" s="22" t="n">
+      <c r="EA1" s="24" t="n">
         <v>43987</v>
       </c>
-      <c r="EB1" s="22" t="n">
+      <c r="EB1" s="24" t="n">
         <v>43988</v>
       </c>
-      <c r="EC1" s="22" t="n">
+      <c r="EC1" s="24" t="n">
         <v>43989</v>
       </c>
-      <c r="ED1" s="22" t="n">
+      <c r="ED1" s="24" t="n">
         <v>43990</v>
       </c>
-      <c r="EE1" s="22" t="n">
+      <c r="EE1" s="24" t="n">
         <v>43991</v>
       </c>
-      <c r="EF1" s="22" t="n">
+      <c r="EF1" s="24" t="n">
         <v>43992</v>
       </c>
-      <c r="EG1" s="22" t="n">
+      <c r="EG1" s="24" t="n">
         <v>43993</v>
       </c>
-      <c r="EH1" s="22" t="n">
+      <c r="EH1" s="24" t="n">
         <v>43994</v>
       </c>
-      <c r="EI1" s="22" t="n">
+      <c r="EI1" s="24" t="n">
         <v>43995</v>
       </c>
-      <c r="EJ1" s="22" t="n">
+      <c r="EJ1" s="24" t="n">
         <v>43996</v>
       </c>
-      <c r="EK1" s="22" t="n">
+      <c r="EK1" s="24" t="n">
         <v>43997</v>
       </c>
-      <c r="EL1" s="22" t="n">
+      <c r="EL1" s="24" t="n">
         <v>43998</v>
       </c>
-      <c r="EM1" s="22" t="n">
+      <c r="EM1" s="24" t="n">
         <v>43999</v>
       </c>
-      <c r="EN1" s="22" t="n">
+      <c r="EN1" s="24" t="n">
         <v>44000</v>
       </c>
-      <c r="EO1" s="22" t="n">
+      <c r="EO1" s="24" t="n">
         <v>44001</v>
       </c>
-      <c r="EP1" s="22" t="n">
+      <c r="EP1" s="24" t="n">
         <v>44002</v>
       </c>
-      <c r="EQ1" s="22" t="n">
+      <c r="EQ1" s="24" t="n">
         <v>44003</v>
       </c>
-      <c r="ER1" s="22" t="n">
+      <c r="ER1" s="24" t="n">
         <v>44004</v>
       </c>
-      <c r="ES1" s="22" t="n">
+      <c r="ES1" s="24" t="n">
         <v>44005</v>
       </c>
-      <c r="ET1" s="22" t="n">
+      <c r="ET1" s="24" t="n">
         <v>44006</v>
       </c>
-      <c r="EU1" s="22" t="n">
+      <c r="EU1" s="24" t="n">
         <v>44007</v>
       </c>
-      <c r="EV1" s="22" t="n">
+      <c r="EV1" s="24" t="n">
         <v>44008</v>
       </c>
-      <c r="EW1" s="22" t="n">
+      <c r="EW1" s="24" t="n">
         <v>44009</v>
       </c>
-      <c r="EX1" s="22" t="n">
+      <c r="EX1" s="24" t="n">
         <v>44010</v>
       </c>
-      <c r="EY1" s="22" t="n">
+      <c r="EY1" s="24" t="n">
         <v>44011</v>
       </c>
-      <c r="EZ1" s="22" t="n">
+      <c r="EZ1" s="24" t="n">
         <v>44012</v>
       </c>
-      <c r="FA1" s="22" t="n">
+      <c r="FA1" s="24" t="n">
         <v>44013</v>
       </c>
-      <c r="FB1" s="22" t="n">
+      <c r="FB1" s="24" t="n">
         <v>44014</v>
       </c>
-      <c r="FC1" s="22" t="n">
+      <c r="FC1" s="24" t="n">
         <v>44015</v>
       </c>
-      <c r="FD1" s="22" t="n">
+      <c r="FD1" s="24" t="n">
         <v>44016</v>
       </c>
-      <c r="FE1" s="22" t="n">
+      <c r="FE1" s="24" t="n">
         <v>44017</v>
       </c>
-      <c r="FF1" s="22" t="n">
+      <c r="FF1" s="24" t="n">
         <v>44018</v>
       </c>
-      <c r="FG1" s="22" t="n">
+      <c r="FG1" s="24" t="n">
         <v>44019</v>
       </c>
-      <c r="FH1" s="22" t="n">
+      <c r="FH1" s="24" t="n">
         <v>44020</v>
       </c>
-      <c r="FI1" s="22" t="n">
+      <c r="FI1" s="24" t="n">
         <v>44021</v>
       </c>
-      <c r="FJ1" s="22" t="n">
+      <c r="FJ1" s="24" t="n">
         <v>44022</v>
       </c>
-      <c r="FK1" s="22" t="n">
+      <c r="FK1" s="24" t="n">
         <v>44023</v>
       </c>
-      <c r="FL1" s="22" t="n">
+      <c r="FL1" s="24" t="n">
         <v>44024</v>
       </c>
-      <c r="FM1" s="22" t="n">
+      <c r="FM1" s="24" t="n">
         <v>44025</v>
       </c>
-      <c r="FN1" s="22" t="n">
+      <c r="FN1" s="24" t="n">
         <v>44026</v>
       </c>
-      <c r="FO1" s="22" t="n">
+      <c r="FO1" s="24" t="n">
         <v>44027</v>
       </c>
-      <c r="FP1" s="22" t="n">
+      <c r="FP1" s="24" t="n">
         <v>44028</v>
       </c>
-      <c r="FQ1" s="22" t="n">
+      <c r="FQ1" s="24" t="n">
         <v>44029</v>
       </c>
-      <c r="FR1" s="22" t="n">
+      <c r="FR1" s="24" t="n">
         <v>44030</v>
       </c>
-      <c r="FS1" s="22" t="n">
+      <c r="FS1" s="24" t="n">
         <v>44031</v>
       </c>
-      <c r="FT1" s="22" t="n">
+      <c r="FT1" s="24" t="n">
         <v>44032</v>
       </c>
-      <c r="FU1" s="22" t="n">
+      <c r="FU1" s="24" t="n">
         <v>44033</v>
       </c>
-      <c r="FV1" s="22" t="n">
+      <c r="FV1" s="24" t="n">
         <v>44034</v>
       </c>
-      <c r="FW1" s="22" t="n">
+      <c r="FW1" s="24" t="n">
         <v>44035</v>
       </c>
-      <c r="FX1" s="22" t="n">
+      <c r="FX1" s="24" t="n">
         <v>44036</v>
       </c>
-      <c r="FY1" s="22" t="n">
+      <c r="FY1" s="24" t="n">
         <v>44037</v>
       </c>
-      <c r="FZ1" s="22" t="n">
+      <c r="FZ1" s="24" t="n">
         <v>44038</v>
       </c>
-      <c r="GA1" s="22" t="n">
+      <c r="GA1" s="24" t="n">
         <v>44039</v>
       </c>
-      <c r="GB1" s="22" t="n">
+      <c r="GB1" s="24" t="n">
         <v>44040</v>
       </c>
-      <c r="GC1" s="22" t="n">
+      <c r="GC1" s="24" t="n">
         <v>44041</v>
       </c>
-      <c r="GD1" s="22" t="n">
+      <c r="GD1" s="24" t="n">
         <v>44042</v>
       </c>
-      <c r="GE1" s="22" t="n">
+      <c r="GE1" s="24" t="n">
         <v>44043</v>
       </c>
-      <c r="GF1" s="22" t="n">
+      <c r="GF1" s="24" t="n">
         <v>44044</v>
       </c>
-      <c r="GG1" s="22" t="n">
+      <c r="GG1" s="24" t="n">
         <v>44045</v>
       </c>
-      <c r="GH1" s="22" t="n">
+      <c r="GH1" s="24" t="n">
         <v>44046</v>
       </c>
-      <c r="GI1" s="22" t="n">
+      <c r="GI1" s="24" t="n">
         <v>44047</v>
       </c>
-      <c r="GJ1" s="22" t="n">
+      <c r="GJ1" s="24" t="n">
         <v>44048</v>
       </c>
-      <c r="GK1" s="22" t="n">
+      <c r="GK1" s="24" t="n">
         <v>44049</v>
       </c>
-      <c r="GL1" s="22" t="n">
+      <c r="GL1" s="24" t="n">
         <v>44050</v>
       </c>
-      <c r="GM1" s="22" t="n">
+      <c r="GM1" s="24" t="n">
         <v>44051</v>
       </c>
-      <c r="GN1" s="22" t="n">
+      <c r="GN1" s="24" t="n">
         <v>44052</v>
       </c>
-      <c r="GO1" s="22" t="n">
+      <c r="GO1" s="24" t="n">
         <v>44053</v>
       </c>
-      <c r="GP1" s="22" t="n">
+      <c r="GP1" s="24" t="n">
         <v>44054</v>
       </c>
-      <c r="GQ1" s="22" t="n">
+      <c r="GQ1" s="24" t="n">
         <v>44055</v>
       </c>
-      <c r="GR1" s="22" t="n">
+      <c r="GR1" s="24" t="n">
         <v>44056</v>
       </c>
-      <c r="GS1" s="22" t="n">
+      <c r="GS1" s="24" t="n">
         <v>44057</v>
       </c>
-      <c r="GT1" s="22" t="n">
+      <c r="GT1" s="24" t="n">
         <v>44058</v>
       </c>
-      <c r="GU1" s="22" t="n">
+      <c r="GU1" s="24" t="n">
         <v>44059</v>
       </c>
-      <c r="GV1" s="22" t="n">
+      <c r="GV1" s="24" t="n">
         <v>44060</v>
       </c>
-      <c r="GW1" s="22" t="n">
+      <c r="GW1" s="24" t="n">
         <v>44061</v>
       </c>
-      <c r="GX1" s="22" t="n">
+      <c r="GX1" s="24" t="n">
         <v>44062</v>
       </c>
-      <c r="GY1" s="22" t="n">
+      <c r="GY1" s="24" t="n">
         <v>44063</v>
       </c>
-      <c r="GZ1" s="22" t="n">
+      <c r="GZ1" s="24" t="n">
         <v>44064</v>
       </c>
-      <c r="HA1" s="22" t="n">
+      <c r="HA1" s="24" t="n">
         <v>44065</v>
       </c>
-      <c r="HB1" s="22" t="n">
+      <c r="HB1" s="24" t="n">
         <v>44066</v>
       </c>
-      <c r="HC1" s="22" t="n">
+      <c r="HC1" s="24" t="n">
         <v>44067</v>
       </c>
-      <c r="HD1" s="22" t="n">
+      <c r="HD1" s="24" t="n">
         <v>44068</v>
       </c>
-      <c r="HE1" s="22" t="n">
+      <c r="HE1" s="24" t="n">
         <v>44069</v>
       </c>
-      <c r="HF1" s="22" t="n">
+      <c r="HF1" s="24" t="n">
         <v>44070</v>
       </c>
-      <c r="HG1" s="22" t="n">
+      <c r="HG1" s="24" t="n">
         <v>44071</v>
       </c>
-      <c r="HH1" s="22" t="n">
+      <c r="HH1" s="24" t="n">
         <v>44072</v>
       </c>
-      <c r="HI1" s="22" t="n">
+      <c r="HI1" s="24" t="n">
         <v>44073</v>
       </c>
-      <c r="HJ1" s="22" t="n">
+      <c r="HJ1" s="24" t="n">
         <v>44074</v>
       </c>
-      <c r="HK1" s="22" t="n">
+      <c r="HK1" s="24" t="n">
         <v>44075</v>
       </c>
-      <c r="HL1" s="22" t="n">
+      <c r="HL1" s="24" t="n">
         <v>44076</v>
       </c>
-      <c r="HM1" s="22" t="n">
+      <c r="HM1" s="24" t="n">
         <v>44077</v>
       </c>
-      <c r="HN1" s="22" t="n">
+      <c r="HN1" s="24" t="n">
         <v>44078</v>
       </c>
-      <c r="HO1" s="22" t="n">
+      <c r="HO1" s="24" t="n">
         <v>44079</v>
       </c>
-      <c r="HP1" s="22" t="n">
+      <c r="HP1" s="24" t="n">
         <v>44080</v>
       </c>
-      <c r="HQ1" s="22" t="n">
+      <c r="HQ1" s="24" t="n">
         <v>44081</v>
       </c>
-      <c r="HR1" s="22" t="n">
+      <c r="HR1" s="24" t="n">
         <v>44082</v>
       </c>
-      <c r="HS1" s="22" t="n">
+      <c r="HS1" s="24" t="n">
         <v>44083</v>
       </c>
-      <c r="HT1" s="22" t="n">
+      <c r="HT1" s="24" t="n">
         <v>44084</v>
       </c>
-      <c r="HU1" s="22" t="n">
+      <c r="HU1" s="24" t="n">
         <v>44085</v>
       </c>
-      <c r="HV1" s="22" t="n">
+      <c r="HV1" s="24" t="n">
         <v>44086</v>
       </c>
-      <c r="HW1" s="22" t="n">
+      <c r="HW1" s="24" t="n">
         <v>44087</v>
       </c>
-      <c r="HX1" s="22" t="n">
+      <c r="HX1" s="24" t="n">
         <v>44088</v>
       </c>
-      <c r="HY1" s="22" t="n">
+      <c r="HY1" s="24" t="n">
         <v>44089</v>
       </c>
-      <c r="HZ1" s="22" t="n">
+      <c r="HZ1" s="24" t="n">
         <v>44090</v>
       </c>
-      <c r="IA1" s="22" t="n">
+      <c r="IA1" s="24" t="n">
         <v>44091</v>
       </c>
-      <c r="IB1" s="22" t="n">
+      <c r="IB1" s="24" t="n">
         <v>44092</v>
       </c>
-      <c r="IC1" s="22" t="n">
+      <c r="IC1" s="24" t="n">
         <v>44093</v>
       </c>
-      <c r="ID1" s="22" t="n">
+      <c r="ID1" s="24" t="n">
         <v>44094</v>
       </c>
-      <c r="IE1" s="22" t="n">
+      <c r="IE1" s="24" t="n">
         <v>44095</v>
       </c>
-      <c r="IF1" s="22" t="n">
+      <c r="IF1" s="24" t="n">
         <v>44096</v>
       </c>
-      <c r="IG1" s="22" t="n">
+      <c r="IG1" s="24" t="n">
         <v>44097</v>
       </c>
-      <c r="IH1" s="22" t="n">
+      <c r="IH1" s="24" t="n">
         <v>44098</v>
       </c>
-      <c r="II1" s="22" t="n">
+      <c r="II1" s="24" t="n">
         <v>44099</v>
       </c>
-      <c r="IJ1" s="22" t="n">
+      <c r="IJ1" s="24" t="n">
         <v>44100</v>
       </c>
-      <c r="IK1" s="22" t="n">
+      <c r="IK1" s="24" t="n">
         <v>44101</v>
       </c>
-      <c r="IL1" s="22" t="n">
+      <c r="IL1" s="24" t="n">
         <v>44102</v>
       </c>
-      <c r="IM1" s="22" t="n">
+      <c r="IM1" s="24" t="n">
         <v>44103</v>
       </c>
-      <c r="IN1" s="22" t="n">
+      <c r="IN1" s="24" t="n">
         <v>44104</v>
       </c>
-      <c r="IO1" s="22" t="n">
+      <c r="IO1" s="24" t="n">
         <v>44105</v>
       </c>
-      <c r="IP1" s="22" t="n">
+      <c r="IP1" s="24" t="n">
         <v>44106</v>
       </c>
-      <c r="IQ1" s="22" t="n">
+      <c r="IQ1" s="24" t="n">
         <v>44107</v>
       </c>
-      <c r="IR1" s="22" t="n">
+      <c r="IR1" s="24" t="n">
         <v>44108</v>
       </c>
-      <c r="IS1" s="22" t="n">
+      <c r="IS1" s="24" t="n">
         <v>44109</v>
       </c>
-      <c r="IT1" s="22" t="n">
+      <c r="IT1" s="24" t="n">
         <v>44110</v>
       </c>
-      <c r="IU1" s="22" t="n">
+      <c r="IU1" s="24" t="n">
         <v>44111</v>
       </c>
-      <c r="IV1" s="22" t="n">
+      <c r="IV1" s="24" t="n">
         <v>44112</v>
       </c>
-      <c r="IW1" s="22" t="n">
+      <c r="IW1" s="24" t="n">
         <v>44113</v>
       </c>
-      <c r="IX1" s="22" t="n">
+      <c r="IX1" s="24" t="n">
         <v>44114</v>
       </c>
-      <c r="IY1" s="22" t="n">
+      <c r="IY1" s="24" t="n">
         <v>44115</v>
       </c>
-      <c r="IZ1" s="22" t="n">
+      <c r="IZ1" s="24" t="n">
         <v>44116</v>
       </c>
-      <c r="JA1" s="22" t="n">
+      <c r="JA1" s="24" t="n">
         <v>44117</v>
       </c>
-      <c r="JB1" s="22" t="n">
+      <c r="JB1" s="24" t="n">
         <v>44118</v>
       </c>
-      <c r="JC1" s="22" t="n">
+      <c r="JC1" s="24" t="n">
         <v>44119</v>
       </c>
-      <c r="JD1" s="22" t="n">
+      <c r="JD1" s="24" t="n">
         <v>44120</v>
       </c>
-      <c r="JE1" s="22" t="n">
+      <c r="JE1" s="24" t="n">
         <v>44121</v>
       </c>
-      <c r="JF1" s="22" t="n">
+      <c r="JF1" s="24" t="n">
         <v>44122</v>
       </c>
-      <c r="JG1" s="22" t="n">
+      <c r="JG1" s="24" t="n">
         <v>44123</v>
       </c>
-      <c r="JH1" s="22" t="n">
+      <c r="JH1" s="24" t="n">
         <v>44124</v>
       </c>
-      <c r="JI1" s="22" t="n">
+      <c r="JI1" s="24" t="n">
         <v>44125</v>
       </c>
-      <c r="JJ1" s="22" t="n">
+      <c r="JJ1" s="24" t="n">
         <v>44126</v>
       </c>
-      <c r="JK1" s="22" t="n">
+      <c r="JK1" s="24" t="n">
         <v>44127</v>
       </c>
-      <c r="JL1" s="22" t="n">
+      <c r="JL1" s="24" t="n">
         <v>44128</v>
       </c>
-      <c r="JM1" s="22" t="n">
+      <c r="JM1" s="24" t="n">
         <v>44129</v>
       </c>
-      <c r="JN1" s="22" t="n">
+      <c r="JN1" s="24" t="n">
         <v>44130</v>
       </c>
-      <c r="JO1" s="22" t="n">
+      <c r="JO1" s="24" t="n">
         <v>44131</v>
       </c>
-      <c r="JP1" s="22" t="n">
+      <c r="JP1" s="24" t="n">
         <v>44132</v>
       </c>
-      <c r="JQ1" s="22" t="n">
+      <c r="JQ1" s="24" t="n">
         <v>44133</v>
       </c>
-      <c r="JR1" s="22" t="n">
+      <c r="JR1" s="24" t="n">
         <v>44134</v>
       </c>
-      <c r="JS1" s="22" t="n">
+      <c r="JS1" s="24" t="n">
         <v>44135</v>
       </c>
-      <c r="JT1" s="22" t="n">
+      <c r="JT1" s="24" t="n">
         <v>44136</v>
       </c>
-      <c r="JU1" s="22" t="n">
+      <c r="JU1" s="24" t="n">
         <v>44137</v>
       </c>
-      <c r="JV1" s="22" t="n">
+      <c r="JV1" s="24" t="n">
         <v>44138</v>
       </c>
-      <c r="JW1" s="22" t="n">
+      <c r="JW1" s="24" t="n">
         <v>44139</v>
       </c>
-      <c r="JX1" s="22" t="n">
+      <c r="JX1" s="24" t="n">
         <v>44140</v>
       </c>
-      <c r="JY1" s="22" t="n">
+      <c r="JY1" s="24" t="n">
         <v>44141</v>
       </c>
-      <c r="JZ1" s="22" t="n">
+      <c r="JZ1" s="24" t="n">
         <v>44142</v>
       </c>
-      <c r="KA1" s="22" t="n">
+      <c r="KA1" s="24" t="n">
         <v>44143</v>
       </c>
-      <c r="KB1" s="22" t="n">
+      <c r="KB1" s="24" t="n">
         <v>44144</v>
       </c>
-      <c r="KC1" s="22" t="n">
+      <c r="KC1" s="24" t="n">
         <v>44145</v>
       </c>
-      <c r="KD1" s="22" t="n">
+      <c r="KD1" s="24" t="n">
         <v>44146</v>
       </c>
-      <c r="KE1" s="22" t="n">
+      <c r="KE1" s="24" t="n">
         <v>44147</v>
       </c>
-      <c r="KF1" s="22" t="n">
+      <c r="KF1" s="24" t="n">
         <v>44148</v>
       </c>
-      <c r="KG1" s="22" t="n">
+      <c r="KG1" s="24" t="n">
         <v>44149</v>
       </c>
-      <c r="KH1" s="22" t="n">
+      <c r="KH1" s="24" t="n">
         <v>44150</v>
       </c>
-      <c r="KI1" s="22" t="n">
+      <c r="KI1" s="24" t="n">
         <v>44151</v>
       </c>
-      <c r="KJ1" s="22" t="n">
+      <c r="KJ1" s="24" t="n">
         <v>44152</v>
       </c>
-      <c r="KK1" s="22" t="n">
+      <c r="KK1" s="24" t="n">
         <v>44153</v>
       </c>
-      <c r="KL1" s="22" t="n">
+      <c r="KL1" s="24" t="n">
         <v>44154</v>
       </c>
-      <c r="KM1" s="22" t="n">
+      <c r="KM1" s="24" t="n">
         <v>44155</v>
       </c>
-      <c r="KN1" s="22" t="n">
+      <c r="KN1" s="24" t="n">
         <v>44156</v>
       </c>
-      <c r="KO1" s="22" t="n">
+      <c r="KO1" s="24" t="n">
         <v>44157</v>
       </c>
-      <c r="KP1" s="22" t="n">
+      <c r="KP1" s="24" t="n">
         <v>44158</v>
       </c>
-      <c r="KQ1" s="22" t="n">
+      <c r="KQ1" s="24" t="n">
         <v>44159</v>
       </c>
-      <c r="KR1" s="22" t="n">
+      <c r="KR1" s="24" t="n">
         <v>44160</v>
       </c>
-      <c r="KS1" s="22" t="n">
+      <c r="KS1" s="24" t="n">
         <v>44161</v>
       </c>
-      <c r="KT1" s="22" t="n">
+      <c r="KT1" s="24" t="n">
         <v>44162</v>
       </c>
-      <c r="KU1" s="22" t="n">
+      <c r="KU1" s="24" t="n">
         <v>44163</v>
       </c>
-      <c r="KV1" s="22" t="n">
+      <c r="KV1" s="24" t="n">
         <v>44164</v>
       </c>
-      <c r="KW1" s="22" t="n">
+      <c r="KW1" s="24" t="n">
         <v>44165</v>
       </c>
-      <c r="KX1" s="22" t="n">
+      <c r="KX1" s="24" t="n">
         <v>44166</v>
       </c>
-      <c r="KY1" s="22" t="n">
+      <c r="KY1" s="24" t="n">
         <v>44167</v>
       </c>
-      <c r="KZ1" s="22" t="n">
+      <c r="KZ1" s="24" t="n">
         <v>44168</v>
       </c>
-      <c r="LA1" s="22" t="n">
+      <c r="LA1" s="24" t="n">
         <v>44169</v>
       </c>
-      <c r="LB1" s="22" t="n">
+      <c r="LB1" s="24" t="n">
         <v>44170</v>
       </c>
-      <c r="LC1" s="22" t="n">
+      <c r="LC1" s="24" t="n">
         <v>44171</v>
       </c>
-      <c r="LD1" s="22" t="n">
+      <c r="LD1" s="24" t="n">
         <v>44172</v>
       </c>
-      <c r="LE1" s="22" t="n">
+      <c r="LE1" s="24" t="n">
         <v>44173</v>
       </c>
-      <c r="LF1" s="22" t="n">
+      <c r="LF1" s="24" t="n">
         <v>44174</v>
       </c>
-      <c r="LG1" s="22" t="n">
+      <c r="LG1" s="24" t="n">
         <v>44175</v>
       </c>
-      <c r="LH1" s="22" t="n">
+      <c r="LH1" s="24" t="n">
         <v>44176</v>
       </c>
-      <c r="LI1" s="22" t="n">
+      <c r="LI1" s="24" t="n">
         <v>44177</v>
       </c>
-      <c r="LJ1" s="22" t="n">
+      <c r="LJ1" s="24" t="n">
         <v>44178</v>
       </c>
-      <c r="LK1" s="22" t="n">
+      <c r="LK1" s="24" t="n">
         <v>44179</v>
       </c>
-      <c r="LL1" s="22" t="n">
+      <c r="LL1" s="24" t="n">
         <v>44180</v>
       </c>
-      <c r="LM1" s="22" t="n">
+      <c r="LM1" s="24" t="n">
         <v>44181</v>
       </c>
-      <c r="LN1" s="22" t="n">
+      <c r="LN1" s="24" t="n">
         <v>44182</v>
       </c>
-      <c r="LO1" s="22" t="n">
+      <c r="LO1" s="24" t="n">
         <v>44183</v>
       </c>
-      <c r="LP1" s="22" t="n">
+      <c r="LP1" s="24" t="n">
         <v>44184</v>
       </c>
-      <c r="LQ1" s="22" t="n">
+      <c r="LQ1" s="24" t="n">
         <v>44185</v>
       </c>
-      <c r="LR1" s="22" t="n">
+      <c r="LR1" s="24" t="n">
         <v>44186</v>
       </c>
-      <c r="LS1" s="22" t="n">
+      <c r="LS1" s="24" t="n">
         <v>44187</v>
       </c>
-      <c r="LT1" s="22" t="n">
+      <c r="LT1" s="24" t="n">
         <v>44188</v>
       </c>
-      <c r="LU1" s="22" t="n">
+      <c r="LU1" s="24" t="n">
         <v>44189</v>
       </c>
-      <c r="LV1" s="22" t="n">
+      <c r="LV1" s="24" t="n">
         <v>44190</v>
       </c>
-      <c r="LW1" s="22" t="n">
+      <c r="LW1" s="24" t="n">
         <v>44191</v>
       </c>
-      <c r="LX1" s="22" t="n">
+      <c r="LX1" s="24" t="n">
         <v>44192</v>
       </c>
-      <c r="LY1" s="22" t="n">
+      <c r="LY1" s="24" t="n">
         <v>44193</v>
       </c>
-      <c r="LZ1" s="22" t="n">
+      <c r="LZ1" s="24" t="n">
         <v>44194</v>
       </c>
-      <c r="MA1" s="22" t="n">
+      <c r="MA1" s="24" t="n">
         <v>44195</v>
       </c>
-      <c r="MB1" s="22" t="n">
+      <c r="MB1" s="24" t="n">
         <v>44196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -5562,10 +5668,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="25" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="0" t="s">
@@ -5576,10 +5682,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="0" t="s">
@@ -5590,7 +5696,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -5604,67 +5710,67 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="23" t="s">
+      <c r="M14" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N15" s="23" t="s">
+      <c r="N15" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P17" s="23" t="s">
+      <c r="P17" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q18" s="23" t="s">
+      <c r="Q18" s="25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5684,80 +5790,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:AMJ71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27:H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.13"/>
   </cols>
   <sheetData>
-    <row r="1" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="H1" s="26" t="s">
+    <row r="1" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-    </row>
-    <row r="2" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="B1" s="26"/>
+      <c r="H1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+    </row>
+    <row r="2" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="E2" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="H2" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="J2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="L2" s="32" t="s">
         <v>31</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,12 +5878,12 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
@@ -5787,12 +5895,12 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
@@ -5804,12 +5912,12 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
@@ -5821,12 +5929,12 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
@@ -5839,12 +5947,12 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -5857,12 +5965,12 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
@@ -5875,12 +5983,12 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
@@ -5892,594 +6000,1928 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="n">
+      <c r="A11" s="36" t="n">
         <v>43869</v>
       </c>
-      <c r="B11" s="35" t="n">
+      <c r="B11" s="37" t="n">
         <v>47</v>
       </c>
-      <c r="C11" s="36" t="n">
+      <c r="C11" s="38" t="n">
         <f aca="false">SUM(B3:B11)</f>
         <v>617</v>
       </c>
-      <c r="D11" s="35" t="n">
+      <c r="D11" s="37" t="n">
         <v>9</v>
       </c>
-      <c r="E11" s="35" t="n">
+      <c r="E11" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C11/D11)</f>
         <v>69</v>
       </c>
-      <c r="F11" s="35" t="n">
+      <c r="F11" s="37" t="n">
         <f aca="false">D$23-D11</f>
         <v>22</v>
       </c>
-      <c r="G11" s="34" t="n">
+      <c r="G11" s="36" t="n">
         <f aca="false">$A11+F11</f>
         <v>43891</v>
       </c>
-      <c r="H11" s="37" t="n">
+      <c r="H11" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C11)/E$23)</f>
         <v>19</v>
       </c>
-      <c r="I11" s="38" t="n">
+      <c r="I11" s="40" t="n">
         <f aca="false">$A11+H11</f>
         <v>43888</v>
       </c>
-      <c r="J11" s="39" t="n">
+      <c r="J11" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C11)/$E11)</f>
         <v>14</v>
       </c>
-      <c r="K11" s="40" t="n">
+      <c r="K11" s="42" t="n">
         <f aca="false">$A11+J11</f>
         <v>43883</v>
       </c>
-      <c r="L11" s="41" t="n">
+      <c r="L11" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C11)/((E11+E$23)/2))</f>
         <v>16</v>
       </c>
-      <c r="M11" s="42" t="n">
+      <c r="M11" s="44" t="n">
         <f aca="false">$A11+L11</f>
         <v>43885</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="n">
+      <c r="A12" s="36" t="n">
         <v>43870</v>
       </c>
-      <c r="B12" s="43" t="n">
+      <c r="B12" s="45" t="n">
         <v>26</v>
       </c>
-      <c r="C12" s="36" t="n">
+      <c r="C12" s="38" t="n">
         <f aca="false">C11+B12</f>
         <v>643</v>
       </c>
-      <c r="D12" s="35" t="n">
+      <c r="D12" s="37" t="n">
         <v>10</v>
       </c>
-      <c r="E12" s="35" t="n">
+      <c r="E12" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C12/D12)</f>
         <v>65</v>
       </c>
-      <c r="F12" s="35" t="n">
+      <c r="F12" s="37" t="n">
         <f aca="false">D$23-D12</f>
         <v>21</v>
       </c>
-      <c r="G12" s="34" t="n">
+      <c r="G12" s="36" t="n">
         <f aca="false">$A12+F12</f>
         <v>43891</v>
       </c>
-      <c r="H12" s="37" t="n">
+      <c r="H12" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C12)/E$23)</f>
         <v>18</v>
       </c>
-      <c r="I12" s="38" t="n">
+      <c r="I12" s="40" t="n">
         <f aca="false">$A12+H12</f>
         <v>43888</v>
       </c>
-      <c r="J12" s="39" t="n">
+      <c r="J12" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C12)/$E12)</f>
         <v>14</v>
       </c>
-      <c r="K12" s="40" t="n">
+      <c r="K12" s="42" t="n">
         <f aca="false">$A12+J12</f>
         <v>43884</v>
       </c>
-      <c r="L12" s="41" t="n">
+      <c r="L12" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C12)/((E12+E$23)/2))</f>
         <v>16</v>
       </c>
-      <c r="M12" s="42" t="n">
+      <c r="M12" s="44" t="n">
         <f aca="false">$A12+L12</f>
         <v>43886</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="n">
+      <c r="A13" s="36" t="n">
         <v>43873</v>
       </c>
       <c r="B13" s="4" t="n">
         <f aca="false">120+4</f>
         <v>124</v>
       </c>
-      <c r="C13" s="36" t="n">
+      <c r="C13" s="38" t="n">
         <f aca="false">C12+B13</f>
         <v>767</v>
       </c>
-      <c r="D13" s="35" t="n">
+      <c r="D13" s="37" t="n">
         <v>13</v>
       </c>
-      <c r="E13" s="35" t="n">
+      <c r="E13" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C13/D13)</f>
         <v>59</v>
       </c>
-      <c r="F13" s="35" t="n">
+      <c r="F13" s="37" t="n">
         <f aca="false">D$23-D13</f>
         <v>18</v>
       </c>
-      <c r="G13" s="34" t="n">
+      <c r="G13" s="36" t="n">
         <f aca="false">$A13+F13</f>
         <v>43891</v>
       </c>
-      <c r="H13" s="37" t="n">
+      <c r="H13" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C13)/E$23)</f>
         <v>16</v>
       </c>
-      <c r="I13" s="38" t="n">
+      <c r="I13" s="40" t="n">
         <f aca="false">$A13+H13</f>
         <v>43889</v>
       </c>
-      <c r="J13" s="39" t="n">
+      <c r="J13" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C13)/$E13)</f>
         <v>14</v>
       </c>
-      <c r="K13" s="40" t="n">
+      <c r="K13" s="42" t="n">
         <f aca="false">$A13+J13</f>
         <v>43887</v>
       </c>
-      <c r="L13" s="41" t="n">
+      <c r="L13" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C13)/((E13+E$23)/2))</f>
         <v>15</v>
       </c>
-      <c r="M13" s="42" t="n">
+      <c r="M13" s="44" t="n">
         <f aca="false">$A13+L13</f>
         <v>43888</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="34" t="n">
+      <c r="A14" s="36" t="n">
         <v>43873</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C14" s="36" t="n">
+      <c r="C14" s="38" t="n">
         <f aca="false">C13+B14</f>
         <v>799</v>
       </c>
-      <c r="D14" s="35" t="n">
+      <c r="D14" s="37" t="n">
         <v>13</v>
       </c>
-      <c r="E14" s="35" t="n">
+      <c r="E14" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C14/D14)</f>
         <v>62</v>
       </c>
-      <c r="F14" s="35" t="n">
+      <c r="F14" s="37" t="n">
         <f aca="false">D$23-D14</f>
         <v>18</v>
       </c>
-      <c r="G14" s="34" t="n">
+      <c r="G14" s="36" t="n">
         <f aca="false">$A14+F14</f>
         <v>43891</v>
       </c>
-      <c r="H14" s="37" t="n">
+      <c r="H14" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C14)/E$23)</f>
         <v>15</v>
       </c>
-      <c r="I14" s="38" t="n">
+      <c r="I14" s="40" t="n">
         <f aca="false">$A14+H14</f>
         <v>43888</v>
       </c>
-      <c r="J14" s="39" t="n">
+      <c r="J14" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C14)/$E14)</f>
         <v>12</v>
       </c>
-      <c r="K14" s="40" t="n">
+      <c r="K14" s="42" t="n">
         <f aca="false">$A14+J14</f>
         <v>43885</v>
       </c>
-      <c r="L14" s="41" t="n">
+      <c r="L14" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C14)/((E14+E$23)/2))</f>
         <v>14</v>
       </c>
-      <c r="M14" s="42" t="n">
+      <c r="M14" s="44" t="n">
         <f aca="false">$A14+L14</f>
         <v>43887</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34" t="n">
+      <c r="A15" s="36" t="n">
         <v>43880</v>
       </c>
       <c r="B15" s="4" t="n">
         <f aca="false">120+33</f>
         <v>153</v>
       </c>
-      <c r="C15" s="36" t="n">
+      <c r="C15" s="38" t="n">
         <f aca="false">C14+B15</f>
         <v>952</v>
       </c>
-      <c r="D15" s="35" t="n">
+      <c r="D15" s="37" t="n">
         <f aca="false">D14+(A15-A14)</f>
         <v>20</v>
       </c>
-      <c r="E15" s="35" t="n">
+      <c r="E15" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C15/D15)</f>
         <v>48</v>
       </c>
-      <c r="F15" s="35" t="n">
+      <c r="F15" s="37" t="n">
         <f aca="false">D$23-D15</f>
         <v>11</v>
       </c>
-      <c r="G15" s="34" t="n">
+      <c r="G15" s="36" t="n">
         <f aca="false">$A15+F15</f>
         <v>43891</v>
       </c>
-      <c r="H15" s="37" t="n">
+      <c r="H15" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C15)/E$23)</f>
         <v>12</v>
       </c>
-      <c r="I15" s="38" t="n">
+      <c r="I15" s="40" t="n">
         <f aca="false">$A15+H15</f>
         <v>43892</v>
       </c>
-      <c r="J15" s="39" t="n">
+      <c r="J15" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C15)/$E15)</f>
         <v>13</v>
       </c>
-      <c r="K15" s="40" t="n">
+      <c r="K15" s="42" t="n">
         <f aca="false">$A15+J15</f>
         <v>43893</v>
       </c>
-      <c r="L15" s="41" t="n">
+      <c r="L15" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C15)/((E15+E$23)/2))</f>
         <v>12</v>
       </c>
-      <c r="M15" s="42" t="n">
+      <c r="M15" s="44" t="n">
         <f aca="false">$A15+L15</f>
         <v>43892</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="n">
+      <c r="A16" s="36" t="n">
         <v>43882</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>77</v>
       </c>
-      <c r="C16" s="36" t="n">
+      <c r="C16" s="38" t="n">
         <f aca="false">C15+B16</f>
         <v>1029</v>
       </c>
-      <c r="D16" s="35" t="n">
+      <c r="D16" s="37" t="n">
         <f aca="false">D15+(A16-A15)</f>
         <v>22</v>
       </c>
-      <c r="E16" s="35" t="n">
+      <c r="E16" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C16/D16)</f>
         <v>47</v>
       </c>
-      <c r="F16" s="35" t="n">
+      <c r="F16" s="37" t="n">
         <f aca="false">D$23-D16</f>
         <v>9</v>
       </c>
-      <c r="G16" s="34" t="n">
+      <c r="G16" s="36" t="n">
         <f aca="false">$A16+F16</f>
         <v>43891</v>
       </c>
-      <c r="H16" s="37" t="n">
+      <c r="H16" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C16)/E$23)</f>
         <v>11</v>
       </c>
-      <c r="I16" s="38" t="n">
+      <c r="I16" s="40" t="n">
         <f aca="false">$A16+H16</f>
         <v>43893</v>
       </c>
-      <c r="J16" s="39" t="n">
+      <c r="J16" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C16)/$E16)</f>
         <v>11</v>
       </c>
-      <c r="K16" s="40" t="n">
+      <c r="K16" s="42" t="n">
         <f aca="false">$A16+J16</f>
         <v>43893</v>
       </c>
-      <c r="L16" s="41" t="n">
+      <c r="L16" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C16)/((E16+E$23)/2))</f>
         <v>11</v>
       </c>
-      <c r="M16" s="42" t="n">
+      <c r="M16" s="44" t="n">
         <f aca="false">$A16+L16</f>
         <v>43893</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="n">
+      <c r="A17" s="36" t="n">
         <v>43886</v>
       </c>
       <c r="B17" s="4" t="n">
         <f aca="false">120+6</f>
         <v>126</v>
       </c>
-      <c r="C17" s="36" t="n">
+      <c r="C17" s="38" t="n">
         <f aca="false">C16+B17</f>
         <v>1155</v>
       </c>
-      <c r="D17" s="35" t="n">
+      <c r="D17" s="37" t="n">
         <f aca="false">D16+(A17-A16)</f>
         <v>26</v>
       </c>
-      <c r="E17" s="35" t="n">
+      <c r="E17" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C17/D17)</f>
         <v>45</v>
       </c>
-      <c r="F17" s="35" t="n">
+      <c r="F17" s="37" t="n">
         <f aca="false">D$23-D17</f>
         <v>5</v>
       </c>
-      <c r="G17" s="34" t="n">
+      <c r="G17" s="36" t="n">
         <f aca="false">$A17+F17</f>
         <v>43891</v>
       </c>
-      <c r="H17" s="37" t="n">
+      <c r="H17" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C17)/E$23)</f>
         <v>8</v>
       </c>
-      <c r="I17" s="38" t="n">
+      <c r="I17" s="40" t="n">
         <f aca="false">$A17+H17</f>
         <v>43894</v>
       </c>
-      <c r="J17" s="39" t="n">
+      <c r="J17" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C17)/$E17)</f>
         <v>9</v>
       </c>
-      <c r="K17" s="40" t="n">
+      <c r="K17" s="42" t="n">
         <f aca="false">$A17+J17</f>
         <v>43895</v>
       </c>
-      <c r="L17" s="41" t="n">
+      <c r="L17" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C17)/((E17+E$23)/2))</f>
         <v>8</v>
       </c>
-      <c r="M17" s="42" t="n">
+      <c r="M17" s="44" t="n">
         <f aca="false">$A17+L17</f>
         <v>43894</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="n">
+      <c r="A18" s="36" t="n">
         <v>43887</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="C18" s="36" t="n">
+      <c r="C18" s="38" t="n">
         <f aca="false">C17+B18</f>
         <v>1186</v>
       </c>
-      <c r="D18" s="35" t="n">
+      <c r="D18" s="37" t="n">
         <f aca="false">D17+(A18-A17)</f>
         <v>27</v>
       </c>
-      <c r="E18" s="35" t="n">
+      <c r="E18" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C18/D18)</f>
         <v>44</v>
       </c>
-      <c r="F18" s="35" t="n">
+      <c r="F18" s="37" t="n">
         <f aca="false">D$23-D18</f>
         <v>4</v>
       </c>
-      <c r="G18" s="34" t="n">
+      <c r="G18" s="36" t="n">
         <f aca="false">$A18+F18</f>
         <v>43891</v>
       </c>
-      <c r="H18" s="37" t="n">
+      <c r="H18" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C18)/E$23)</f>
         <v>7</v>
       </c>
-      <c r="I18" s="38" t="n">
+      <c r="I18" s="40" t="n">
         <f aca="false">$A18+H18</f>
         <v>43894</v>
       </c>
-      <c r="J18" s="39" t="n">
+      <c r="J18" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C18)/$E18)</f>
         <v>8</v>
       </c>
-      <c r="K18" s="40" t="n">
+      <c r="K18" s="42" t="n">
         <f aca="false">$A18+J18</f>
         <v>43895</v>
       </c>
-      <c r="L18" s="41" t="n">
+      <c r="L18" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C18)/((E18+E$23)/2))</f>
         <v>8</v>
       </c>
-      <c r="M18" s="42" t="n">
+      <c r="M18" s="44" t="n">
         <f aca="false">$A18+L18</f>
         <v>43895</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="n">
+      <c r="A19" s="36" t="n">
         <v>43887</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="36" t="n">
+      <c r="C19" s="38" t="n">
         <f aca="false">C18+B19</f>
         <v>1204</v>
       </c>
-      <c r="D19" s="35" t="n">
+      <c r="D19" s="37" t="n">
         <f aca="false">D18+(A19-A18)</f>
         <v>27</v>
       </c>
-      <c r="E19" s="35" t="n">
+      <c r="E19" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C19/D19)</f>
         <v>45</v>
       </c>
-      <c r="F19" s="35" t="n">
+      <c r="F19" s="37" t="n">
         <f aca="false">D$23-D19</f>
         <v>4</v>
       </c>
-      <c r="G19" s="34" t="n">
+      <c r="G19" s="36" t="n">
         <f aca="false">$A19+F19</f>
         <v>43891</v>
       </c>
-      <c r="H19" s="37" t="n">
+      <c r="H19" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C19)/E$23)</f>
         <v>7</v>
       </c>
-      <c r="I19" s="38" t="n">
+      <c r="I19" s="40" t="n">
         <f aca="false">$A19+H19</f>
         <v>43894</v>
       </c>
-      <c r="J19" s="39" t="n">
+      <c r="J19" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C19)/$E19)</f>
         <v>8</v>
       </c>
-      <c r="K19" s="40" t="n">
+      <c r="K19" s="42" t="n">
         <f aca="false">$A19+J19</f>
         <v>43895</v>
       </c>
-      <c r="L19" s="41" t="n">
+      <c r="L19" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C19)/((E19+E$23)/2))</f>
         <v>7</v>
       </c>
-      <c r="M19" s="42" t="n">
+      <c r="M19" s="44" t="n">
         <f aca="false">$A19+L19</f>
         <v>43894</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="n">
+      <c r="A20" s="36" t="n">
         <v>43889</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>182</v>
       </c>
-      <c r="C20" s="36" t="n">
+      <c r="C20" s="38" t="n">
         <f aca="false">C19+B20</f>
         <v>1386</v>
       </c>
-      <c r="D20" s="35" t="n">
+      <c r="D20" s="37" t="n">
         <f aca="false">D19+(A20-A19)</f>
         <v>29</v>
       </c>
-      <c r="E20" s="35" t="n">
+      <c r="E20" s="37" t="n">
         <f aca="false">_xlfn.CEILING.MATH(C20/D20)</f>
         <v>48</v>
       </c>
-      <c r="F20" s="35" t="n">
+      <c r="F20" s="37" t="n">
         <f aca="false">D$23-D20</f>
         <v>2</v>
       </c>
-      <c r="G20" s="34" t="n">
+      <c r="G20" s="36" t="n">
         <f aca="false">$A20+F20</f>
         <v>43891</v>
       </c>
-      <c r="H20" s="37" t="n">
+      <c r="H20" s="39" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C20)/E$23)</f>
         <v>3</v>
       </c>
-      <c r="I20" s="38" t="n">
+      <c r="I20" s="40" t="n">
         <f aca="false">$A20+H20</f>
         <v>43892</v>
       </c>
-      <c r="J20" s="39" t="n">
+      <c r="J20" s="41" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-$C20)/$E20)</f>
         <v>4</v>
       </c>
-      <c r="K20" s="40" t="n">
+      <c r="K20" s="42" t="n">
         <f aca="false">$A20+J20</f>
         <v>43893</v>
       </c>
-      <c r="L20" s="41" t="n">
+      <c r="L20" s="43" t="n">
         <f aca="false">_xlfn.CEILING.MATH((B$23-C20)/((E20+E$23)/2))</f>
         <v>4</v>
       </c>
-      <c r="M20" s="42" t="n">
+      <c r="M20" s="44" t="n">
         <f aca="false">$A20+L20</f>
         <v>43893</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
+      <c r="A21" s="36" t="n">
+        <v>43891</v>
+      </c>
       <c r="B21" s="4" t="n">
         <v>148</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
+      <c r="C21" s="38" t="n">
+        <f aca="false">C20+B21</f>
+        <v>1534</v>
+      </c>
+      <c r="D21" s="37" t="n">
+        <f aca="false">D20+(A21-A20)</f>
+        <v>31</v>
+      </c>
+      <c r="E21" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C21/D21)</f>
+        <v>50</v>
+      </c>
+      <c r="F21" s="37" t="n">
+        <f aca="false">D$23-D21</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="36" t="n">
+        <f aca="false">$A21+F21</f>
+        <v>43891</v>
+      </c>
+      <c r="H21" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C21)/E$23)</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="40" t="n">
+        <f aca="false">$A21+H21</f>
+        <v>43892</v>
+      </c>
+      <c r="J21" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C21)/$E21)</f>
+        <v>1</v>
+      </c>
+      <c r="K21" s="42" t="n">
+        <f aca="false">$A21+J21</f>
+        <v>43892</v>
+      </c>
+      <c r="L21" s="43" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C21)/((E21+E$23)/2))</f>
+        <v>1</v>
+      </c>
+      <c r="M21" s="44" t="n">
+        <f aca="false">$A21+L21</f>
+        <v>43892</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
+      <c r="A22" s="36" t="n">
+        <v>43891</v>
+      </c>
       <c r="B22" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
+      <c r="C22" s="38" t="n">
+        <f aca="false">C21+B22</f>
+        <v>1535</v>
+      </c>
+      <c r="D22" s="37" t="n">
+        <f aca="false">D21+(A22-A21)</f>
+        <v>31</v>
+      </c>
+      <c r="E22" s="37" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(C22/D22)</f>
+        <v>50</v>
+      </c>
+      <c r="F22" s="37" t="n">
+        <f aca="false">D$23-D22</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="36" t="n">
+        <f aca="false">$A22+F22</f>
+        <v>43891</v>
+      </c>
+      <c r="H22" s="39" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C22)/E$23)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="40" t="n">
+        <f aca="false">$A22+H22</f>
+        <v>43891</v>
+      </c>
+      <c r="J22" s="41" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-$C22)/$E22)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="42" t="n">
+        <f aca="false">$A22+J22</f>
+        <v>43891</v>
+      </c>
+      <c r="L22" s="43" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((B$23-C22)/((E22+E$23)/2))</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="44" t="n">
+        <f aca="false">$A22+L22</f>
+        <v>43891</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44" t="n">
+      <c r="A23" s="46" t="n">
         <f aca="false">A11+(D23-D11)</f>
         <v>43891</v>
       </c>
-      <c r="B23" s="45" t="n">
+      <c r="B23" s="47" t="n">
         <f aca="false">SUM(B3:B22)</f>
         <v>1535</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45" t="n">
+      <c r="C23" s="47"/>
+      <c r="D23" s="47" t="n">
         <v>31</v>
       </c>
-      <c r="E23" s="45" t="n">
+      <c r="E23" s="47" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B23/D23)</f>
         <v>50</v>
       </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="46"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AMJ26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="49" t="n">
+        <v>22</v>
+      </c>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E27" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="53" t="n">
+        <f aca="false">IF((B27-A33)&lt;0,0,B27-A33)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="51"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="51" t="n">
+        <v>19</v>
+      </c>
+      <c r="E28" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="53" t="n">
+        <f aca="false">IF((B28-B27)&lt;0,0,B28-B27)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="51"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="54" t="n">
+        <f aca="false">(A27/18)</f>
+        <v>1.22222222222222</v>
+      </c>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" s="51" t="n">
+        <v>16</v>
+      </c>
+      <c r="E29" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="53" t="n">
+        <f aca="false">IF((B29-B28)&lt;0,0,B29-B28)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="51"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" s="51" t="n">
+        <v>21</v>
+      </c>
+      <c r="E30" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="53" t="n">
+        <f aca="false">IF((B30-B29)&lt;0,0,B30-B29)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="51"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="55" t="n">
+        <f aca="false">120*A29</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="D31" s="51" t="n">
+        <v>17</v>
+      </c>
+      <c r="E31" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="53" t="n">
+        <f aca="false">IF((B31-B30)&lt;0,0,B31-B30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="51"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="50"/>
+      <c r="C32" s="51" t="n">
+        <v>6</v>
+      </c>
+      <c r="D32" s="51" t="n">
+        <v>25</v>
+      </c>
+      <c r="E32" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="53" t="n">
+        <f aca="false">IF((B32-B31)&lt;0,0,B32-B31)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="51"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="50" t="n">
+        <v>43892</v>
+      </c>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51" t="n">
+        <v>7</v>
+      </c>
+      <c r="D33" s="51" t="n">
+        <v>17</v>
+      </c>
+      <c r="E33" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="53" t="n">
+        <f aca="false">IF((B33-B32)&lt;0,0,B33-B32)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="51"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="50"/>
+      <c r="C34" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E34" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="53" t="n">
+        <f aca="false">IF((B34-B33)&lt;0,0,B34-B33)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="51"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="50"/>
+      <c r="C35" s="51" t="n">
+        <v>9</v>
+      </c>
+      <c r="D35" s="51" t="n">
+        <v>22</v>
+      </c>
+      <c r="E35" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="53" t="n">
+        <f aca="false">IF((B35-B34)&lt;0,0,B35-B34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="51"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="50"/>
+      <c r="C36" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="D36" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E36" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="53" t="n">
+        <f aca="false">IF((B36-B35)&lt;0,0,B36-B35)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="51"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="50"/>
+      <c r="C37" s="51" t="n">
+        <v>11</v>
+      </c>
+      <c r="D37" s="51" t="n">
+        <v>16</v>
+      </c>
+      <c r="E37" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="53" t="n">
+        <f aca="false">IF((B37-B36)&lt;0,0,B37-B36)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="51"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="50"/>
+      <c r="C38" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="D38" s="51" t="n">
+        <v>19</v>
+      </c>
+      <c r="E38" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="53" t="n">
+        <f aca="false">IF((B38-B37)&lt;0,0,B38-B37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="51"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="50"/>
+      <c r="C39" s="51" t="n">
+        <v>13</v>
+      </c>
+      <c r="D39" s="51" t="n">
+        <v>25</v>
+      </c>
+      <c r="E39" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="53" t="n">
+        <f aca="false">IF((B39-B38)&lt;0,0,B39-B38)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="51"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="50"/>
+      <c r="C40" s="51" t="n">
+        <v>14</v>
+      </c>
+      <c r="D40" s="51" t="n">
+        <v>13</v>
+      </c>
+      <c r="E40" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="53" t="n">
+        <f aca="false">IF((B40-B39)&lt;0,0,B40-B39)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="51"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="51" t="n">
+        <v>15</v>
+      </c>
+      <c r="D41" s="51" t="n">
+        <v>13</v>
+      </c>
+      <c r="E41" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="53" t="n">
+        <f aca="false">IF((B41-B40)&lt;0,0,B41-B40)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="51"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="51" t="n">
+        <v>16</v>
+      </c>
+      <c r="D42" s="51" t="n">
+        <v>19</v>
+      </c>
+      <c r="E42" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="53" t="n">
+        <f aca="false">IF((B42-B41)&lt;0,0,B42-B41)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="51"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="51" t="n">
+        <v>17</v>
+      </c>
+      <c r="D43" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E43" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="53" t="n">
+        <f aca="false">IF((B43-B42)&lt;0,0,B43-B42)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="51"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="51" t="n">
+        <v>18</v>
+      </c>
+      <c r="D44" s="51" t="n">
+        <v>18</v>
+      </c>
+      <c r="E44" s="52" t="n">
+        <f aca="false">$A$31</f>
+        <v>146.666666666667</v>
+      </c>
+      <c r="F44" s="38"/>
+      <c r="G44" s="53" t="n">
+        <f aca="false">IF((B44-B43)&lt;0,0,B44-B43)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="51"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="44"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="57" t="n">
+        <f aca="false">B27+A27-1</f>
+        <v>21</v>
+      </c>
+      <c r="C45" s="57"/>
+      <c r="D45" s="58" t="n">
+        <f aca="false">SUM(D27:D44)</f>
+        <v>304</v>
+      </c>
+      <c r="E45" s="47" t="n">
+        <f aca="false">SUM(E27:E44)</f>
+        <v>2640</v>
+      </c>
+      <c r="F45" s="59" t="n">
+        <f aca="false">SUM(F27:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="59" t="n">
+        <f aca="false">SUM(G27:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="19"/>
+    </row>
+    <row r="48" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I48" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J48" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K48" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="N48" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O48" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AMJ48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="49" t="n">
+        <v>25</v>
+      </c>
+      <c r="B49" s="50"/>
+      <c r="C49" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E49" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="53" t="n">
+        <f aca="false">IF((B49-A55)&lt;0,0,B49-A55)</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="35"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="50"/>
+      <c r="C50" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E50" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="53" t="n">
+        <f aca="false">B50-B49</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="35"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="54" t="n">
+        <f aca="false">(A49/21)</f>
+        <v>1.19047619047619</v>
+      </c>
+      <c r="B51" s="50"/>
+      <c r="C51" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="D51" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E51" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="53" t="n">
+        <f aca="false">B51-B50</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="50"/>
+      <c r="C52" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E52" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="53" t="n">
+        <f aca="false">B52-B51</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="34"/>
+      <c r="M52" s="34"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="35"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="55" t="n">
+        <f aca="false">120*A51</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="B53" s="50"/>
+      <c r="C53" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="D53" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E53" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="53" t="n">
+        <f aca="false">B53-B52</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="50"/>
+      <c r="C54" s="51" t="n">
+        <v>6</v>
+      </c>
+      <c r="D54" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E54" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="53" t="n">
+        <f aca="false">B54-B53</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="34"/>
+      <c r="M54" s="34"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="50" t="n">
+        <v>43892</v>
+      </c>
+      <c r="B55" s="50"/>
+      <c r="C55" s="51" t="n">
+        <v>7</v>
+      </c>
+      <c r="D55" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E55" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="53" t="n">
+        <f aca="false">B55-B54</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="34"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="50"/>
+      <c r="C56" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="D56" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E56" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="53" t="n">
+        <f aca="false">B56-B55</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="34"/>
+      <c r="M56" s="34"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="35"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="50"/>
+      <c r="C57" s="51" t="n">
+        <v>9</v>
+      </c>
+      <c r="D57" s="51" t="n">
+        <v>6</v>
+      </c>
+      <c r="E57" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="53" t="n">
+        <f aca="false">B57-B56</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="35"/>
+      <c r="O57" s="35"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="50"/>
+      <c r="C58" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="D58" s="51" t="n">
+        <v>14</v>
+      </c>
+      <c r="E58" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="53" t="n">
+        <f aca="false">B58-B57</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="34"/>
+      <c r="M58" s="34"/>
+      <c r="N58" s="35"/>
+      <c r="O58" s="35"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="50"/>
+      <c r="C59" s="51" t="n">
+        <v>11</v>
+      </c>
+      <c r="D59" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E59" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="53" t="n">
+        <f aca="false">B59-B58</f>
+        <v>0</v>
+      </c>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="34"/>
+      <c r="M59" s="34"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="35"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="50"/>
+      <c r="C60" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="D60" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E60" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="53" t="n">
+        <f aca="false">B60-B59</f>
+        <v>0</v>
+      </c>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="34"/>
+      <c r="N60" s="35"/>
+      <c r="O60" s="35"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="50"/>
+      <c r="C61" s="51" t="n">
+        <v>13</v>
+      </c>
+      <c r="D61" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E61" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="53" t="n">
+        <f aca="false">B61-B60</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="35"/>
+      <c r="O61" s="35"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="50"/>
+      <c r="C62" s="51" t="n">
+        <v>14</v>
+      </c>
+      <c r="D62" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E62" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="53" t="n">
+        <f aca="false">B62-B61</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="34"/>
+      <c r="M62" s="34"/>
+      <c r="N62" s="35"/>
+      <c r="O62" s="35"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="50"/>
+      <c r="C63" s="51" t="n">
+        <v>15</v>
+      </c>
+      <c r="D63" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E63" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="53" t="n">
+        <f aca="false">B63-B62</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="33"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="34"/>
+      <c r="M63" s="34"/>
+      <c r="N63" s="35"/>
+      <c r="O63" s="35"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="50"/>
+      <c r="C64" s="51" t="n">
+        <v>16</v>
+      </c>
+      <c r="D64" s="51" t="n">
+        <v>6</v>
+      </c>
+      <c r="E64" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="53" t="n">
+        <f aca="false">B64-B63</f>
+        <v>0</v>
+      </c>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="35"/>
+      <c r="O64" s="35"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="50"/>
+      <c r="C65" s="51" t="n">
+        <v>17</v>
+      </c>
+      <c r="D65" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E65" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="53" t="n">
+        <f aca="false">B65-B64</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
+      <c r="L65" s="34"/>
+      <c r="M65" s="34"/>
+      <c r="N65" s="35"/>
+      <c r="O65" s="35"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="50"/>
+      <c r="C66" s="51" t="n">
+        <v>18</v>
+      </c>
+      <c r="D66" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="E66" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="53" t="n">
+        <f aca="false">B66-B65</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
+      <c r="L66" s="34"/>
+      <c r="M66" s="34"/>
+      <c r="N66" s="35"/>
+      <c r="O66" s="35"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="50"/>
+      <c r="C67" s="51" t="n">
+        <v>19</v>
+      </c>
+      <c r="D67" s="51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E67" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="53" t="n">
+        <f aca="false">B67-B66</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="34"/>
+      <c r="M67" s="34"/>
+      <c r="N67" s="35"/>
+      <c r="O67" s="35"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="50"/>
+      <c r="C68" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E68" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="53" t="n">
+        <f aca="false">B68-B67</f>
+        <v>0</v>
+      </c>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="34"/>
+      <c r="M68" s="34"/>
+      <c r="N68" s="35"/>
+      <c r="O68" s="35"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="50"/>
+      <c r="C69" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="51" t="n">
+        <v>9</v>
+      </c>
+      <c r="E69" s="52" t="n">
+        <f aca="false">$A$53</f>
+        <v>142.857142857143</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="53" t="n">
+        <f aca="false">B69-B68</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="33"/>
+      <c r="K69" s="33"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="35"/>
+      <c r="O69" s="35"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0"/>
+      <c r="B70" s="57" t="n">
+        <f aca="false">B49+A49-1</f>
+        <v>24</v>
+      </c>
+      <c r="C70" s="57"/>
+      <c r="D70" s="58" t="n">
+        <f aca="false">SUM(D49:D69)</f>
+        <v>209</v>
+      </c>
+      <c r="E70" s="47" t="n">
+        <f aca="false">SUM(E49:E69)</f>
+        <v>3000</v>
+      </c>
+      <c r="F70" s="59" t="n">
+        <f aca="false">SUM(F49:F69)</f>
+        <v>0</v>
+      </c>
+      <c r="G70" s="59" t="n">
+        <f aca="false">SUM(G49:G69)</f>
+        <v>0</v>
+      </c>
+      <c r="H70" s="48"/>
+      <c r="I70" s="48"/>
+      <c r="J70" s="48"/>
+      <c r="K70" s="48"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="47"/>
+      <c r="H71" s="48"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A47:B47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Inserido o README.md e alterado o planejamento.xlxs
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projeto-200-dias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC3FF96-2431-4082-90A5-0219D8C27DDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6388A9-DFDD-4262-9C9A-99B31EC9C3DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="70">
   <si>
     <t>dia</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>Livro Python Fluente</t>
+  </si>
+  <si>
+    <t>início:</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -665,15 +668,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -689,6 +683,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,21 +1111,21 @@
       <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="27.42578125" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1"/>
+    <col min="4" max="4" width="15.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1148,7 +1179,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1167,7 +1198,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1186,7 +1217,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1205,7 +1236,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1226,7 +1257,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1245,7 +1276,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1264,7 +1295,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1283,7 +1314,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1302,7 +1333,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1321,7 +1352,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1340,7 +1371,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1359,7 +1390,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1378,7 +1409,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1397,7 +1428,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1416,7 +1447,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1435,7 +1466,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1454,7 +1485,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1473,7 +1504,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1492,7 +1523,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1511,7 +1542,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1530,7 +1561,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1549,7 +1580,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1568,7 +1599,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1587,7 +1618,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1606,7 +1637,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1625,7 +1656,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1644,7 +1675,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1663,7 +1694,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1682,7 +1713,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1701,7 +1732,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1718,7 +1749,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1735,7 +1766,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1752,7 +1783,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1769,7 +1800,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1786,7 +1817,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1803,7 +1834,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1820,7 +1851,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1837,7 +1868,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1854,7 +1885,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -1871,7 +1902,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -1888,7 +1919,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -1905,7 +1936,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -1922,7 +1953,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -1939,7 +1970,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -1956,7 +1987,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -1973,7 +2004,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -1990,7 +2021,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2007,7 +2038,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2024,7 +2055,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2041,7 +2072,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -2058,7 +2089,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2075,7 +2106,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -2092,7 +2123,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -2109,7 +2140,7 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -2126,7 +2157,7 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -2143,7 +2174,7 @@
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -2160,7 +2191,7 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -2177,7 +2208,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -2194,7 +2225,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -2211,7 +2242,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -2228,7 +2259,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -2245,7 +2276,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -2262,7 +2293,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -2279,7 +2310,7 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -2296,7 +2327,7 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -2313,7 +2344,7 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -2330,7 +2361,7 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -2347,7 +2378,7 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -2364,7 +2395,7 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -2381,7 +2412,7 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -2398,7 +2429,7 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -2415,7 +2446,7 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -2432,7 +2463,7 @@
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -2449,7 +2480,7 @@
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -2466,7 +2497,7 @@
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -2483,7 +2514,7 @@
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -2500,7 +2531,7 @@
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -2517,7 +2548,7 @@
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -2534,7 +2565,7 @@
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -2551,7 +2582,7 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -2568,7 +2599,7 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -2585,7 +2616,7 @@
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -2602,7 +2633,7 @@
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -2619,7 +2650,7 @@
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -2636,7 +2667,7 @@
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -2653,7 +2684,7 @@
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -2670,7 +2701,7 @@
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -2687,7 +2718,7 @@
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -2704,7 +2735,7 @@
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -2721,7 +2752,7 @@
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -2738,7 +2769,7 @@
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -2755,7 +2786,7 @@
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -2772,7 +2803,7 @@
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -2789,7 +2820,7 @@
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -2806,7 +2837,7 @@
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -2823,7 +2854,7 @@
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -2840,7 +2871,7 @@
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -2857,7 +2888,7 @@
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -2874,7 +2905,7 @@
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -2891,7 +2922,7 @@
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -2908,7 +2939,7 @@
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -2925,7 +2956,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -2942,7 +2973,7 @@
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -2959,7 +2990,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -2976,7 +3007,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -2993,7 +3024,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -3010,7 +3041,7 @@
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -3027,7 +3058,7 @@
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -3044,7 +3075,7 @@
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -3061,7 +3092,7 @@
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -3078,7 +3109,7 @@
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -3095,7 +3126,7 @@
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -3112,7 +3143,7 @@
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -3129,7 +3160,7 @@
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -3146,7 +3177,7 @@
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -3163,7 +3194,7 @@
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -3180,7 +3211,7 @@
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -3197,7 +3228,7 @@
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -3214,7 +3245,7 @@
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -3231,7 +3262,7 @@
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -3248,7 +3279,7 @@
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -3265,7 +3296,7 @@
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -3282,7 +3313,7 @@
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -3299,7 +3330,7 @@
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -3316,7 +3347,7 @@
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -3333,7 +3364,7 @@
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -3350,7 +3381,7 @@
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -3367,7 +3398,7 @@
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -3384,7 +3415,7 @@
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -3401,7 +3432,7 @@
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -3418,7 +3449,7 @@
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -3435,7 +3466,7 @@
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -3452,7 +3483,7 @@
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -3469,7 +3500,7 @@
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -3486,7 +3517,7 @@
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -3503,7 +3534,7 @@
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -3520,7 +3551,7 @@
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -3537,7 +3568,7 @@
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -3554,7 +3585,7 @@
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -3571,7 +3602,7 @@
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -3588,7 +3619,7 @@
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -3605,7 +3636,7 @@
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -3622,7 +3653,7 @@
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -3639,7 +3670,7 @@
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -3656,7 +3687,7 @@
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -3673,7 +3704,7 @@
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -3690,7 +3721,7 @@
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -3707,7 +3738,7 @@
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -3724,7 +3755,7 @@
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -3741,7 +3772,7 @@
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -3758,7 +3789,7 @@
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -3775,7 +3806,7 @@
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -3792,7 +3823,7 @@
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -3809,7 +3840,7 @@
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -3826,7 +3857,7 @@
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -3843,7 +3874,7 @@
       <c r="J157" s="15"/>
       <c r="K157" s="15"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -3860,7 +3891,7 @@
       <c r="J158" s="15"/>
       <c r="K158" s="15"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -3877,7 +3908,7 @@
       <c r="J159" s="15"/>
       <c r="K159" s="15"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -3894,7 +3925,7 @@
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -3911,7 +3942,7 @@
       <c r="J161" s="15"/>
       <c r="K161" s="15"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -3928,7 +3959,7 @@
       <c r="J162" s="15"/>
       <c r="K162" s="15"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -3945,7 +3976,7 @@
       <c r="J163" s="15"/>
       <c r="K163" s="15"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -3962,7 +3993,7 @@
       <c r="J164" s="15"/>
       <c r="K164" s="15"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -3979,7 +4010,7 @@
       <c r="J165" s="15"/>
       <c r="K165" s="15"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -3996,7 +4027,7 @@
       <c r="J166" s="15"/>
       <c r="K166" s="15"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -4013,7 +4044,7 @@
       <c r="J167" s="15"/>
       <c r="K167" s="15"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -4030,7 +4061,7 @@
       <c r="J168" s="15"/>
       <c r="K168" s="15"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -4047,7 +4078,7 @@
       <c r="J169" s="15"/>
       <c r="K169" s="15"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -4064,7 +4095,7 @@
       <c r="J170" s="15"/>
       <c r="K170" s="15"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -4081,7 +4112,7 @@
       <c r="J171" s="15"/>
       <c r="K171" s="15"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -4098,7 +4129,7 @@
       <c r="J172" s="15"/>
       <c r="K172" s="15"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>172</v>
       </c>
@@ -4115,7 +4146,7 @@
       <c r="J173" s="15"/>
       <c r="K173" s="15"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -4132,7 +4163,7 @@
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -4149,7 +4180,7 @@
       <c r="J175" s="15"/>
       <c r="K175" s="15"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -4166,7 +4197,7 @@
       <c r="J176" s="15"/>
       <c r="K176" s="15"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -4183,7 +4214,7 @@
       <c r="J177" s="15"/>
       <c r="K177" s="15"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -4200,7 +4231,7 @@
       <c r="J178" s="15"/>
       <c r="K178" s="15"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>178</v>
       </c>
@@ -4217,7 +4248,7 @@
       <c r="J179" s="15"/>
       <c r="K179" s="15"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>179</v>
       </c>
@@ -4234,7 +4265,7 @@
       <c r="J180" s="15"/>
       <c r="K180" s="15"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>180</v>
       </c>
@@ -4251,7 +4282,7 @@
       <c r="J181" s="15"/>
       <c r="K181" s="15"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>181</v>
       </c>
@@ -4268,7 +4299,7 @@
       <c r="J182" s="15"/>
       <c r="K182" s="15"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>182</v>
       </c>
@@ -4285,7 +4316,7 @@
       <c r="J183" s="15"/>
       <c r="K183" s="15"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>183</v>
       </c>
@@ -4302,7 +4333,7 @@
       <c r="J184" s="15"/>
       <c r="K184" s="15"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>184</v>
       </c>
@@ -4319,7 +4350,7 @@
       <c r="J185" s="15"/>
       <c r="K185" s="15"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>185</v>
       </c>
@@ -4336,7 +4367,7 @@
       <c r="J186" s="15"/>
       <c r="K186" s="15"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>186</v>
       </c>
@@ -4353,7 +4384,7 @@
       <c r="J187" s="15"/>
       <c r="K187" s="15"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>187</v>
       </c>
@@ -4370,7 +4401,7 @@
       <c r="J188" s="15"/>
       <c r="K188" s="15"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>188</v>
       </c>
@@ -4387,7 +4418,7 @@
       <c r="J189" s="15"/>
       <c r="K189" s="15"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>189</v>
       </c>
@@ -4404,7 +4435,7 @@
       <c r="J190" s="15"/>
       <c r="K190" s="15"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>190</v>
       </c>
@@ -4421,7 +4452,7 @@
       <c r="J191" s="15"/>
       <c r="K191" s="15"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>191</v>
       </c>
@@ -4438,7 +4469,7 @@
       <c r="J192" s="15"/>
       <c r="K192" s="15"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>192</v>
       </c>
@@ -4455,7 +4486,7 @@
       <c r="J193" s="15"/>
       <c r="K193" s="15"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>193</v>
       </c>
@@ -4472,7 +4503,7 @@
       <c r="J194" s="15"/>
       <c r="K194" s="15"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>194</v>
       </c>
@@ -4489,7 +4520,7 @@
       <c r="J195" s="15"/>
       <c r="K195" s="15"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>195</v>
       </c>
@@ -4506,7 +4537,7 @@
       <c r="J196" s="15"/>
       <c r="K196" s="15"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>196</v>
       </c>
@@ -4523,7 +4554,7 @@
       <c r="J197" s="15"/>
       <c r="K197" s="15"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>197</v>
       </c>
@@ -4540,7 +4571,7 @@
       <c r="J198" s="15"/>
       <c r="K198" s="15"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>198</v>
       </c>
@@ -4557,7 +4588,7 @@
       <c r="J199" s="15"/>
       <c r="K199" s="15"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>199</v>
       </c>
@@ -4574,7 +4605,7 @@
       <c r="J200" s="15"/>
       <c r="K200" s="15"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>200</v>
       </c>
@@ -4591,7 +4622,7 @@
       <c r="J201" s="15"/>
       <c r="K201" s="15"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>201</v>
       </c>
@@ -4608,7 +4639,7 @@
       <c r="J202" s="15"/>
       <c r="K202" s="15"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>202</v>
       </c>
@@ -4625,7 +4656,7 @@
       <c r="J203" s="15"/>
       <c r="K203" s="15"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>203</v>
       </c>
@@ -4642,7 +4673,7 @@
       <c r="J204" s="15"/>
       <c r="K204" s="15"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>12</v>
       </c>
@@ -4695,19 +4726,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ11"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12 1025:1025" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
@@ -4724,9 +4758,9 @@
       <c r="G1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="AMJ1"/>
-    </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="AMK1"/>
+    </row>
+    <row r="2" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>0</v>
       </c>
@@ -4755,8 +4789,17 @@
       <c r="H2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="I2" s="92">
+        <f>A14</f>
+        <v>43864</v>
+      </c>
+      <c r="J2" s="92">
+        <f>A14+D2-1</f>
+        <v>43868</v>
+      </c>
+      <c r="L2" s="88"/>
+    </row>
+    <row r="3" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -4778,169 +4821,217 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:1024" s="80" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="79">
+      <c r="I3" s="92">
+        <f>J2+1</f>
+        <v>43869</v>
+      </c>
+      <c r="J3" s="92">
+        <f>I3+D3-1</f>
+        <v>43899</v>
+      </c>
+      <c r="L3" s="88"/>
+    </row>
+    <row r="4" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="76">
         <v>2</v>
       </c>
-      <c r="B4" s="80">
+      <c r="B4" s="77">
         <v>42</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="78">
         <f t="shared" si="0"/>
         <v>0.12316715542521994</v>
       </c>
-      <c r="D4" s="80">
+      <c r="D4" s="77">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="E4" s="80">
+      <c r="E4" s="77">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="77" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1024" s="80" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79">
+      <c r="I4" s="99">
+        <f>J3+1</f>
+        <v>43900</v>
+      </c>
+      <c r="J4" s="93">
+        <f>I4+D4+D5+D6-1</f>
+        <v>43971</v>
+      </c>
+      <c r="L4" s="89"/>
+    </row>
+    <row r="5" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="76">
         <v>3</v>
       </c>
-      <c r="B5" s="80">
+      <c r="B5" s="77">
         <v>36</v>
       </c>
-      <c r="C5" s="81">
+      <c r="C5" s="78">
         <f t="shared" si="0"/>
         <v>0.10557184750733138</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="77">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="E5" s="80">
+      <c r="E5" s="77">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="77" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:1024" s="80" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="79">
+      <c r="I5" s="99"/>
+      <c r="J5" s="94"/>
+      <c r="L5" s="89"/>
+    </row>
+    <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="76">
         <v>4</v>
       </c>
-      <c r="B6" s="80">
+      <c r="B6" s="77">
         <v>42</v>
       </c>
-      <c r="C6" s="81">
+      <c r="C6" s="78">
         <f t="shared" si="0"/>
         <v>0.12316715542521994</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="77">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="E6" s="80">
+      <c r="E6" s="77">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="77" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:1024" s="83" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="82">
+      <c r="I6" s="99"/>
+      <c r="J6" s="94"/>
+      <c r="L6" s="89"/>
+    </row>
+    <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="79">
         <v>5</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="80">
         <v>18</v>
       </c>
-      <c r="C7" s="84">
+      <c r="C7" s="81">
         <f t="shared" si="0"/>
         <v>5.2785923753665691E-2</v>
       </c>
-      <c r="D7" s="83">
+      <c r="D7" s="80">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="E7" s="83">
+      <c r="E7" s="80">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="H7" s="83" t="s">
+      <c r="H7" s="80" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:1024" s="83" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="82">
+      <c r="I7" s="99">
+        <f>J4+1</f>
+        <v>43972</v>
+      </c>
+      <c r="J7" s="95">
+        <f>I7+D7+D8-1</f>
+        <v>44020</v>
+      </c>
+      <c r="L7" s="90"/>
+    </row>
+    <row r="8" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="79">
         <v>6</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="80">
         <v>64</v>
       </c>
-      <c r="C8" s="84">
+      <c r="C8" s="81">
         <f t="shared" si="0"/>
         <v>0.18768328445747801</v>
       </c>
-      <c r="D8" s="83">
+      <c r="D8" s="80">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="80">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="80" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:1024" s="86" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="85">
+      <c r="I8" s="99"/>
+      <c r="J8" s="96"/>
+      <c r="L8" s="90"/>
+    </row>
+    <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="82">
         <v>7</v>
       </c>
-      <c r="B9" s="86">
+      <c r="B9" s="83">
         <v>32</v>
       </c>
-      <c r="C9" s="87">
+      <c r="C9" s="84">
         <f t="shared" si="0"/>
         <v>9.3841642228739003E-2</v>
       </c>
-      <c r="D9" s="86">
+      <c r="D9" s="83">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="83">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H9" s="86" t="s">
+      <c r="H9" s="83" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:1024" s="86" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="85">
+      <c r="I9" s="99">
+        <f>J7+1</f>
+        <v>44021</v>
+      </c>
+      <c r="J9" s="97">
+        <f>I9+D9+D10-1</f>
+        <v>44068</v>
+      </c>
+      <c r="L9" s="91"/>
+    </row>
+    <row r="10" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="82">
         <v>8</v>
       </c>
-      <c r="B10" s="86">
+      <c r="B10" s="83">
         <v>48</v>
       </c>
-      <c r="C10" s="87">
+      <c r="C10" s="84">
         <f t="shared" si="0"/>
         <v>0.14076246334310852</v>
       </c>
-      <c r="D10" s="86">
+      <c r="D10" s="83">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="E10" s="86">
+      <c r="E10" s="83">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="H10" s="86" t="s">
+      <c r="H10" s="83" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="I10" s="99"/>
+      <c r="J10" s="98"/>
+      <c r="L10" s="91"/>
+    </row>
+    <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <f>SUM(B2:B10)</f>
         <v>341</v>
@@ -4957,8 +5048,41 @@
         <f>SUM(E2:E10)</f>
         <v>304</v>
       </c>
+      <c r="J11" s="88">
+        <f>A14+D11</f>
+        <v>44069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+      <c r="A14" s="88">
+        <v>43864</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+      <c r="D15" s="88">
+        <v>43869</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+      <c r="D16" s="88">
+        <f>D15+D11</f>
+        <v>44074</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -4976,62 +5100,62 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="15" width="7.140625" customWidth="1"/>
-    <col min="16" max="24" width="6.7109375" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" customWidth="1"/>
-    <col min="26" max="26" width="7.5703125" customWidth="1"/>
-    <col min="27" max="30" width="7.7109375" customWidth="1"/>
-    <col min="31" max="34" width="10.85546875" customWidth="1"/>
-    <col min="35" max="43" width="6.7109375" customWidth="1"/>
-    <col min="44" max="44" width="7.7109375" customWidth="1"/>
-    <col min="45" max="45" width="7.5703125" customWidth="1"/>
-    <col min="46" max="65" width="7.7109375" customWidth="1"/>
-    <col min="66" max="74" width="6.140625" customWidth="1"/>
-    <col min="75" max="75" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="11" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="15" width="7.109375" customWidth="1"/>
+    <col min="16" max="24" width="6.6640625" customWidth="1"/>
+    <col min="25" max="25" width="7.6640625" customWidth="1"/>
+    <col min="26" max="26" width="7.5546875" customWidth="1"/>
+    <col min="27" max="30" width="7.6640625" customWidth="1"/>
+    <col min="31" max="34" width="10.88671875" customWidth="1"/>
+    <col min="35" max="43" width="6.6640625" customWidth="1"/>
+    <col min="44" max="44" width="7.6640625" customWidth="1"/>
+    <col min="45" max="45" width="7.5546875" customWidth="1"/>
+    <col min="46" max="65" width="7.6640625" customWidth="1"/>
+    <col min="66" max="74" width="6.109375" customWidth="1"/>
+    <col min="75" max="75" width="7.109375" customWidth="1"/>
     <col min="76" max="76" width="7" customWidth="1"/>
-    <col min="77" max="95" width="7.140625" customWidth="1"/>
-    <col min="96" max="104" width="6.5703125" customWidth="1"/>
-    <col min="105" max="105" width="7.5703125" customWidth="1"/>
-    <col min="106" max="106" width="7.42578125" customWidth="1"/>
-    <col min="107" max="126" width="7.5703125" customWidth="1"/>
+    <col min="77" max="95" width="7.109375" customWidth="1"/>
+    <col min="96" max="104" width="6.5546875" customWidth="1"/>
+    <col min="105" max="105" width="7.5546875" customWidth="1"/>
+    <col min="106" max="106" width="7.44140625" customWidth="1"/>
+    <col min="107" max="126" width="7.5546875" customWidth="1"/>
     <col min="127" max="135" width="6" customWidth="1"/>
     <col min="136" max="136" width="7" customWidth="1"/>
-    <col min="137" max="137" width="6.85546875" customWidth="1"/>
+    <col min="137" max="137" width="6.88671875" customWidth="1"/>
     <col min="138" max="156" width="7" customWidth="1"/>
-    <col min="157" max="165" width="5.42578125" customWidth="1"/>
-    <col min="166" max="166" width="6.42578125" customWidth="1"/>
-    <col min="167" max="167" width="6.28515625" customWidth="1"/>
-    <col min="168" max="187" width="6.42578125" customWidth="1"/>
-    <col min="188" max="196" width="6.5703125" customWidth="1"/>
-    <col min="197" max="197" width="7.5703125" customWidth="1"/>
-    <col min="198" max="198" width="7.42578125" customWidth="1"/>
-    <col min="199" max="218" width="7.5703125" customWidth="1"/>
-    <col min="219" max="227" width="6.140625" customWidth="1"/>
-    <col min="228" max="228" width="7.140625" customWidth="1"/>
+    <col min="157" max="165" width="5.44140625" customWidth="1"/>
+    <col min="166" max="166" width="6.44140625" customWidth="1"/>
+    <col min="167" max="167" width="6.33203125" customWidth="1"/>
+    <col min="168" max="187" width="6.44140625" customWidth="1"/>
+    <col min="188" max="196" width="6.5546875" customWidth="1"/>
+    <col min="197" max="197" width="7.5546875" customWidth="1"/>
+    <col min="198" max="198" width="7.44140625" customWidth="1"/>
+    <col min="199" max="218" width="7.5546875" customWidth="1"/>
+    <col min="219" max="227" width="6.109375" customWidth="1"/>
+    <col min="228" max="228" width="7.109375" customWidth="1"/>
     <col min="229" max="229" width="7" customWidth="1"/>
-    <col min="230" max="248" width="7.140625" customWidth="1"/>
-    <col min="249" max="257" width="6.140625" customWidth="1"/>
-    <col min="258" max="258" width="7.140625" customWidth="1"/>
+    <col min="230" max="248" width="7.109375" customWidth="1"/>
+    <col min="249" max="257" width="6.109375" customWidth="1"/>
+    <col min="258" max="258" width="7.109375" customWidth="1"/>
     <col min="259" max="259" width="7" customWidth="1"/>
-    <col min="260" max="279" width="7.140625" customWidth="1"/>
-    <col min="280" max="288" width="6.5703125" customWidth="1"/>
-    <col min="289" max="289" width="7.5703125" customWidth="1"/>
-    <col min="290" max="290" width="7.42578125" customWidth="1"/>
-    <col min="291" max="309" width="7.5703125" customWidth="1"/>
-    <col min="310" max="318" width="6.5703125" customWidth="1"/>
-    <col min="319" max="319" width="7.5703125" customWidth="1"/>
-    <col min="320" max="320" width="7.42578125" customWidth="1"/>
-    <col min="321" max="340" width="7.5703125" customWidth="1"/>
+    <col min="260" max="279" width="7.109375" customWidth="1"/>
+    <col min="280" max="288" width="6.5546875" customWidth="1"/>
+    <col min="289" max="289" width="7.5546875" customWidth="1"/>
+    <col min="290" max="290" width="7.44140625" customWidth="1"/>
+    <col min="291" max="309" width="7.5546875" customWidth="1"/>
+    <col min="310" max="318" width="6.5546875" customWidth="1"/>
+    <col min="319" max="319" width="7.5546875" customWidth="1"/>
+    <col min="320" max="320" width="7.44140625" customWidth="1"/>
+    <col min="321" max="340" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A1" s="24">
         <v>43857</v>
       </c>
@@ -6053,7 +6177,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="2" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
@@ -6067,7 +6191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:340" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>19</v>
       </c>
@@ -6081,7 +6205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:340" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
         <v>19</v>
       </c>
@@ -6095,7 +6219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:340" x14ac:dyDescent="0.25">
       <c r="D5" s="25" t="s">
         <v>19</v>
       </c>
@@ -6109,67 +6233,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:340" x14ac:dyDescent="0.25">
       <c r="E6" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:340" x14ac:dyDescent="0.25">
       <c r="F7" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:340" x14ac:dyDescent="0.25">
       <c r="G8" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:340" x14ac:dyDescent="0.25">
       <c r="H9" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:340" x14ac:dyDescent="0.25">
       <c r="I10" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:340" x14ac:dyDescent="0.25">
       <c r="J11" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:340" x14ac:dyDescent="0.25">
       <c r="K12" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:340" x14ac:dyDescent="0.25">
       <c r="L13" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:340" x14ac:dyDescent="0.25">
       <c r="M14" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:340" x14ac:dyDescent="0.25">
       <c r="N15" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:340" x14ac:dyDescent="0.25">
       <c r="O16" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P17" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="16:17" x14ac:dyDescent="0.25">
       <c r="Q18" s="25" t="s">
         <v>16</v>
       </c>
@@ -6188,43 +6312,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="H1" s="77" t="s">
+      <c r="B1" s="85"/>
+      <c r="H1" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-    </row>
-    <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+    </row>
+    <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -6265,7 +6389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>14</v>
@@ -6282,7 +6406,7 @@
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>52</v>
@@ -6299,7 +6423,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>46</v>
@@ -6316,7 +6440,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>26</v>
@@ -6333,7 +6457,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <f>180+26</f>
@@ -6351,7 +6475,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4">
         <f>60+41</f>
@@ -6369,7 +6493,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4">
         <f>60+22</f>
@@ -6387,7 +6511,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4">
         <v>43</v>
@@ -6404,7 +6528,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>43869</v>
       </c>
@@ -6455,7 +6579,7 @@
         <v>43885</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>43870</v>
       </c>
@@ -6506,7 +6630,7 @@
         <v>43886</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>43873</v>
       </c>
@@ -6558,7 +6682,7 @@
         <v>43888</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>43873</v>
       </c>
@@ -6609,7 +6733,7 @@
         <v>43887</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>43880</v>
       </c>
@@ -6662,7 +6786,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>43882</v>
       </c>
@@ -6714,7 +6838,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>43886</v>
       </c>
@@ -6767,7 +6891,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>43887</v>
       </c>
@@ -6819,7 +6943,7 @@
         <v>43895</v>
       </c>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>43887</v>
       </c>
@@ -6871,7 +6995,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>43889</v>
       </c>
@@ -6923,7 +7047,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>43891</v>
       </c>
@@ -6975,7 +7099,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>43891</v>
       </c>
@@ -7027,7 +7151,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A23" s="45">
         <f>A11+(D23-D11)</f>
         <v>43891</v>
@@ -7049,7 +7173,7 @@
       <c r="H23" s="47"/>
       <c r="I23" s="47"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
@@ -7060,13 +7184,13 @@
       <c r="H24" s="47"/>
       <c r="I24" s="47"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A25" s="78" t="s">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A25" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="78"/>
-    </row>
-    <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="87"/>
+    </row>
+    <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>36</v>
       </c>
@@ -7114,7 +7238,7 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49">
         <v>72</v>
       </c>
@@ -7169,7 +7293,7 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>47</v>
       </c>
@@ -7221,7 +7345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A29" s="55">
         <f>ROUND(A27/A35,0)</f>
         <v>3</v>
@@ -7274,7 +7398,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>48</v>
       </c>
@@ -7326,7 +7450,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A31" s="56">
         <f>A37*A29</f>
         <v>300</v>
@@ -7379,7 +7503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>50</v>
       </c>
@@ -7430,7 +7554,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="64">
         <v>43898</v>
       </c>
@@ -7481,7 +7605,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>51</v>
       </c>
@@ -7532,7 +7656,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>21</v>
       </c>
@@ -7583,7 +7707,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>52</v>
       </c>
@@ -7634,7 +7758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>100</v>
       </c>
@@ -7685,7 +7809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="57">
         <f t="shared" si="17"/>
         <v>43931</v>
@@ -7733,7 +7857,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="57">
         <f t="shared" si="17"/>
         <v>43934</v>
@@ -7781,7 +7905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="57">
         <f t="shared" si="17"/>
         <v>43937</v>
@@ -7829,7 +7953,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="57">
         <f t="shared" si="17"/>
         <v>43940</v>
@@ -7877,7 +8001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="57">
         <f t="shared" si="17"/>
         <v>43943</v>
@@ -7925,7 +8049,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="57">
         <f t="shared" si="17"/>
         <v>43946</v>
@@ -7973,7 +8097,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="57">
         <f t="shared" si="17"/>
         <v>43949</v>
@@ -8021,7 +8145,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="57">
         <f t="shared" si="17"/>
         <v>43952</v>
@@ -8069,7 +8193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="57">
         <f t="shared" si="17"/>
         <v>43955</v>
@@ -8117,7 +8241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" s="65">
         <f>A33+A27-1</f>
         <v>43969</v>
@@ -8165,7 +8289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48" s="65">
         <f>B47</f>
@@ -8199,7 +8323,7 @@
       <c r="M48" s="47"/>
       <c r="N48" s="47"/>
     </row>
-    <row r="49" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49" s="65"/>
       <c r="C49" s="65"/>
@@ -8213,14 +8337,14 @@
       <c r="K49" s="47"/>
       <c r="L49" s="47"/>
     </row>
-    <row r="51" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A51" s="78" t="s">
+    <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A51" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="78"/>
-      <c r="C51" s="78"/>
-    </row>
-    <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="87"/>
+      <c r="C51" s="87"/>
+    </row>
+    <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>36</v>
       </c>
@@ -8268,7 +8392,7 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49">
         <v>72</v>
       </c>
@@ -8323,7 +8447,7 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>47</v>
       </c>
@@ -8375,7 +8499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A55" s="55">
         <f>ROUND(A53/A61,0)</f>
         <v>4</v>
@@ -8428,7 +8552,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>48</v>
       </c>
@@ -8479,7 +8603,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A57" s="56">
         <f>A63*A55</f>
         <v>400</v>
@@ -8531,7 +8655,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>50</v>
       </c>
@@ -8582,7 +8706,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A59" s="64">
         <v>43898</v>
       </c>
@@ -8633,7 +8757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>51</v>
       </c>
@@ -8684,7 +8808,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>18</v>
       </c>
@@ -8735,7 +8859,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>52</v>
       </c>
@@ -8786,7 +8910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>100</v>
       </c>
@@ -8837,7 +8961,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B64" s="57">
         <f t="shared" si="25"/>
         <v>43942</v>
@@ -8885,7 +9009,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B65" s="57">
         <f t="shared" si="25"/>
         <v>43946</v>
@@ -8933,7 +9057,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B66" s="57">
         <f t="shared" si="25"/>
         <v>43950</v>
@@ -8981,7 +9105,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B67" s="57">
         <f t="shared" si="25"/>
         <v>43954</v>
@@ -9029,7 +9153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B68" s="57">
         <f t="shared" si="25"/>
         <v>43958</v>
@@ -9077,7 +9201,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B69" s="57">
         <f t="shared" si="25"/>
         <v>43962</v>
@@ -9125,7 +9249,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B70" s="65">
         <f>A59+A53-1</f>
         <v>43969</v>
@@ -9173,7 +9297,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71" s="65">
         <f>B70</f>
@@ -9207,19 +9331,19 @@
       <c r="M71" s="71"/>
       <c r="N71" s="71"/>
     </row>
-    <row r="72" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="K72" s="71"/>
       <c r="L72" s="71"/>
     </row>
-    <row r="73" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A73" s="78" t="s">
+    <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A73" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="78"/>
+      <c r="B73" s="87"/>
       <c r="K73" s="71"/>
       <c r="L73" s="71"/>
     </row>
-    <row r="74" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>36</v>
       </c>
@@ -9267,7 +9391,7 @@
       <c r="AMI74"/>
       <c r="AMJ74"/>
     </row>
-    <row r="75" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49">
         <v>72</v>
       </c>
@@ -9322,7 +9446,7 @@
       <c r="AMI75"/>
       <c r="AMJ75"/>
     </row>
-    <row r="76" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>47</v>
       </c>
@@ -9374,7 +9498,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="77" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A77" s="55">
         <f>ROUND(A75/A83,0)</f>
         <v>3</v>
@@ -9427,7 +9551,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="78" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>48</v>
       </c>
@@ -9479,7 +9603,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="79" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A79" s="56">
         <f>A85*A77</f>
         <v>300</v>
@@ -9531,7 +9655,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="80" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>50</v>
       </c>
@@ -9582,7 +9706,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="64">
         <v>43898</v>
       </c>
@@ -9633,7 +9757,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>51</v>
       </c>
@@ -9684,7 +9808,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>23</v>
       </c>
@@ -9735,7 +9859,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>52</v>
       </c>
@@ -9786,7 +9910,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>100</v>
       </c>
@@ -9837,7 +9961,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B86" s="57">
         <f t="shared" si="35"/>
         <v>43931</v>
@@ -9885,7 +10009,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B87" s="57">
         <f t="shared" si="35"/>
         <v>43934</v>
@@ -9933,7 +10057,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B88" s="57">
         <f t="shared" si="35"/>
         <v>43937</v>
@@ -9981,7 +10105,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B89" s="57">
         <f t="shared" si="35"/>
         <v>43940</v>
@@ -10029,7 +10153,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B90" s="57">
         <f t="shared" si="35"/>
         <v>43943</v>
@@ -10077,7 +10201,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B91" s="57">
         <f t="shared" si="35"/>
         <v>43946</v>
@@ -10125,7 +10249,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B92" s="57">
         <f t="shared" si="35"/>
         <v>43949</v>
@@ -10173,7 +10297,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B93" s="57">
         <f t="shared" si="35"/>
         <v>43952</v>
@@ -10221,7 +10345,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B94" s="57">
         <f t="shared" si="35"/>
         <v>43955</v>
@@ -10269,7 +10393,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B95" s="57">
         <f t="shared" si="35"/>
         <v>43958</v>
@@ -10317,7 +10441,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B96" s="65">
         <f>A81+A75-1</f>
         <v>43969</v>
@@ -10365,7 +10489,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97" s="65">
         <f>B96</f>
@@ -10399,7 +10523,7 @@
       <c r="M97" s="47"/>
       <c r="N97" s="47"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98"/>
       <c r="B98" s="65"/>
       <c r="C98" s="65"/>
@@ -10436,12 +10560,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -10449,7 +10573,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10461,7 +10585,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -10473,7 +10597,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -10485,7 +10609,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -10497,7 +10621,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -10509,7 +10633,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -10521,7 +10645,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -10533,7 +10657,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -10545,7 +10669,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -10557,7 +10681,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -10569,7 +10693,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -10581,7 +10705,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -10593,7 +10717,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -10605,7 +10729,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -10617,7 +10741,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -10629,7 +10753,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -10641,7 +10765,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -10653,7 +10777,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -10665,7 +10789,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -10677,7 +10801,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -10689,7 +10813,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -10701,7 +10825,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
atualizada a planilha de planejamento e inserido o arquivo referente ao teste do Capítulo 5, titTacToe.py/updated the planning spreadsheet and inserted the file for the Chapter 5 test, titTacToe.py
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6388A9-DFDD-4262-9C9A-99B31EC9C3DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF235262-6AA1-4E3C-9905-A2BD2EADE148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -683,15 +685,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -719,6 +712,15 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4728,7 +4730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -4789,15 +4791,15 @@
       <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="92">
+      <c r="I2" s="89">
         <f>A14</f>
         <v>43864</v>
       </c>
-      <c r="J2" s="92">
+      <c r="J2" s="89">
         <f>A14+D2-1</f>
         <v>43868</v>
       </c>
-      <c r="L2" s="88"/>
+      <c r="L2" s="85"/>
     </row>
     <row r="3" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
@@ -4821,15 +4823,15 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="92">
+      <c r="I3" s="89">
         <f>J2+1</f>
         <v>43869</v>
       </c>
-      <c r="J3" s="92">
+      <c r="J3" s="89">
         <f>I3+D3-1</f>
         <v>43899</v>
       </c>
-      <c r="L3" s="88"/>
+      <c r="L3" s="85"/>
     </row>
     <row r="4" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76">
@@ -4853,15 +4855,15 @@
       <c r="H4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="99">
+      <c r="I4" s="96">
         <f>J3+1</f>
         <v>43900</v>
       </c>
-      <c r="J4" s="93">
+      <c r="J4" s="90">
         <f>I4+D4+D5+D6-1</f>
         <v>43971</v>
       </c>
-      <c r="L4" s="89"/>
+      <c r="L4" s="86"/>
     </row>
     <row r="5" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="76">
@@ -4885,9 +4887,9 @@
       <c r="H5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="99"/>
-      <c r="J5" s="94"/>
-      <c r="L5" s="89"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="91"/>
+      <c r="L5" s="86"/>
     </row>
     <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
@@ -4911,9 +4913,9 @@
       <c r="H6" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="94"/>
-      <c r="L6" s="89"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="91"/>
+      <c r="L6" s="86"/>
     </row>
     <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79">
@@ -4937,15 +4939,15 @@
       <c r="H7" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="99">
+      <c r="I7" s="96">
         <f>J4+1</f>
         <v>43972</v>
       </c>
-      <c r="J7" s="95">
+      <c r="J7" s="92">
         <f>I7+D7+D8-1</f>
         <v>44020</v>
       </c>
-      <c r="L7" s="90"/>
+      <c r="L7" s="87"/>
     </row>
     <row r="8" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79">
@@ -4969,9 +4971,9 @@
       <c r="H8" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="99"/>
-      <c r="J8" s="96"/>
-      <c r="L8" s="90"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="93"/>
+      <c r="L8" s="87"/>
     </row>
     <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="82">
@@ -4995,15 +4997,15 @@
       <c r="H9" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="99">
+      <c r="I9" s="96">
         <f>J7+1</f>
         <v>44021</v>
       </c>
-      <c r="J9" s="97">
+      <c r="J9" s="94">
         <f>I9+D9+D10-1</f>
         <v>44068</v>
       </c>
-      <c r="L9" s="91"/>
+      <c r="L9" s="88"/>
     </row>
     <row r="10" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82">
@@ -5027,9 +5029,9 @@
       <c r="H10" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="99"/>
-      <c r="J10" s="98"/>
-      <c r="L10" s="91"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="95"/>
+      <c r="L10" s="88"/>
     </row>
     <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
@@ -5048,7 +5050,7 @@
         <f>SUM(E2:E10)</f>
         <v>304</v>
       </c>
-      <c r="J11" s="88">
+      <c r="J11" s="85">
         <f>A14+D11</f>
         <v>44069</v>
       </c>
@@ -5059,17 +5061,17 @@
       </c>
     </row>
     <row r="14" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
-      <c r="A14" s="88">
+      <c r="A14" s="85">
         <v>43864</v>
       </c>
     </row>
     <row r="15" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
-      <c r="D15" s="88">
+      <c r="D15" s="85">
         <v>43869</v>
       </c>
     </row>
     <row r="16" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
-      <c r="D16" s="88">
+      <c r="D16" s="85">
         <f>D15+D11</f>
         <v>44074</v>
       </c>
@@ -6312,8 +6314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6335,18 +6337,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="H1" s="86" t="s">
+      <c r="B1" s="97"/>
+      <c r="H1" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
     </row>
     <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -7185,10 +7187,10 @@
       <c r="I24" s="47"/>
     </row>
     <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A25" s="87" t="s">
+      <c r="A25" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="87"/>
+      <c r="B25" s="99"/>
     </row>
     <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -8338,11 +8340,11 @@
       <c r="L49" s="47"/>
     </row>
     <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A51" s="87" t="s">
+      <c r="A51" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="87"/>
-      <c r="C51" s="87"/>
+      <c r="B51" s="99"/>
+      <c r="C51" s="99"/>
     </row>
     <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
@@ -8556,51 +8558,52 @@
       <c r="A56" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="57">
+      <c r="B56" s="72">
         <f t="shared" si="25"/>
         <v>43910</v>
       </c>
-      <c r="C56" s="57"/>
-      <c r="D56" s="58">
+      <c r="C56" s="72">
+        <v>43921</v>
+      </c>
+      <c r="D56" s="73">
         <f t="shared" ref="D56:D70" si="28">IF(C56="",D55,C56-B56)</f>
+        <v>11</v>
+      </c>
+      <c r="E56" s="73">
         <v>4</v>
       </c>
-      <c r="E56" s="4">
-        <v>4</v>
-      </c>
-      <c r="F56" s="4">
+      <c r="F56" s="73">
         <v>21</v>
       </c>
-      <c r="G56" s="60">
+      <c r="G56" s="74">
         <f t="shared" si="20"/>
         <v>400</v>
       </c>
-      <c r="H56" s="69">
-        <f t="shared" ref="H56:H70" si="29">G56</f>
-        <v>400</v>
-      </c>
-      <c r="I56" s="69">
+      <c r="H56" s="74">
+        <v>404</v>
+      </c>
+      <c r="I56" s="74">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="J56" s="61">
+        <v>-4</v>
+      </c>
+      <c r="J56" s="73">
         <f t="shared" si="22"/>
         <v>13</v>
       </c>
-      <c r="K56" s="61">
+      <c r="K56" s="73">
         <f t="shared" si="23"/>
         <v>59</v>
       </c>
-      <c r="L56" s="57">
+      <c r="L56" s="72">
         <f t="shared" si="24"/>
-        <v>43973</v>
-      </c>
-      <c r="M56" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N56" s="63">
+        <v>43980</v>
+      </c>
+      <c r="M56" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N56" s="75">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8615,7 +8618,7 @@
       <c r="C57" s="57"/>
       <c r="D57" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E57" s="4">
         <v>5</v>
@@ -8628,7 +8631,7 @@
         <v>400</v>
       </c>
       <c r="H57" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="H57:H70" si="29">G57</f>
         <v>400</v>
       </c>
       <c r="I57" s="69">
@@ -8645,14 +8648,14 @@
       </c>
       <c r="L57" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M57" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N57" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8666,7 +8669,7 @@
       <c r="C58" s="57"/>
       <c r="D58" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E58" s="4">
         <v>6</v>
@@ -8696,14 +8699,14 @@
       </c>
       <c r="L58" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M58" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N58" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8717,7 +8720,7 @@
       <c r="C59" s="57"/>
       <c r="D59" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E59" s="4">
         <v>7</v>
@@ -8747,14 +8750,14 @@
       </c>
       <c r="L59" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M59" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N59" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8768,7 +8771,7 @@
       <c r="C60" s="57"/>
       <c r="D60" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -8798,14 +8801,14 @@
       </c>
       <c r="L60" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M60" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N60" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8819,7 +8822,7 @@
       <c r="C61" s="57"/>
       <c r="D61" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -8849,14 +8852,14 @@
       </c>
       <c r="L61" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N61" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8870,7 +8873,7 @@
       <c r="C62" s="57"/>
       <c r="D62" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -8900,14 +8903,14 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N62" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8921,7 +8924,7 @@
       <c r="C63" s="57"/>
       <c r="D63" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -8951,14 +8954,14 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N63" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8969,7 +8972,7 @@
       <c r="C64" s="57"/>
       <c r="D64" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -8999,14 +9002,14 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N64" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9017,7 +9020,7 @@
       <c r="C65" s="57"/>
       <c r="D65" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -9047,14 +9050,14 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N65" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9065,7 +9068,7 @@
       <c r="C66" s="57"/>
       <c r="D66" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -9095,14 +9098,14 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N66" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9113,7 +9116,7 @@
       <c r="C67" s="57"/>
       <c r="D67" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -9143,14 +9146,14 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N67" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9161,7 +9164,7 @@
       <c r="C68" s="57"/>
       <c r="D68" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -9191,14 +9194,14 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N68" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9209,7 +9212,7 @@
       <c r="C69" s="57"/>
       <c r="D69" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9239,14 +9242,14 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9257,7 +9260,7 @@
       <c r="C70" s="65"/>
       <c r="D70" s="58">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9287,14 +9290,14 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" si="24"/>
-        <v>43973</v>
+        <v>43980</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
         <f t="shared" si="27"/>
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9316,11 +9319,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>6570</v>
+        <v>6574</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>
@@ -9336,10 +9339,10 @@
       <c r="L72" s="71"/>
     </row>
     <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A73" s="87" t="s">
+      <c r="A73" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="87"/>
+      <c r="B73" s="99"/>
       <c r="K73" s="71"/>
       <c r="L73" s="71"/>
     </row>
@@ -9608,102 +9611,104 @@
         <f>A85*A77</f>
         <v>300</v>
       </c>
-      <c r="B79" s="57">
+      <c r="B79" s="72">
         <f t="shared" si="35"/>
         <v>43910</v>
       </c>
-      <c r="C79" s="57"/>
-      <c r="D79" s="61">
+      <c r="C79" s="72">
+        <v>43922</v>
+      </c>
+      <c r="D79" s="73">
         <f t="shared" ref="D79:D96" si="38">IF(C79="",D78,C79-B79)</f>
-        <v>6</v>
-      </c>
-      <c r="E79" s="4">
+        <v>12</v>
+      </c>
+      <c r="E79" s="73">
         <v>4</v>
       </c>
-      <c r="F79" s="4">
+      <c r="F79" s="73">
         <v>743</v>
       </c>
-      <c r="G79" s="60">
+      <c r="G79" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H79" s="60">
-        <f t="shared" ref="H79:H96" si="39">G79</f>
-        <v>300</v>
-      </c>
-      <c r="I79" s="60">
+      <c r="H79" s="74">
+        <v>30</v>
+      </c>
+      <c r="I79" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J79" s="61">
+        <v>270</v>
+      </c>
+      <c r="J79" s="73">
         <f t="shared" si="32"/>
         <v>13</v>
       </c>
-      <c r="K79" s="61">
+      <c r="K79" s="73">
         <f t="shared" si="33"/>
         <v>59</v>
       </c>
-      <c r="L79" s="57">
+      <c r="L79" s="72">
         <f t="shared" si="34"/>
-        <v>43975</v>
-      </c>
-      <c r="M79" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N79" s="63">
+        <v>43981</v>
+      </c>
+      <c r="M79" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N79" s="75">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B80" s="57">
+      <c r="B80" s="72">
         <f t="shared" si="35"/>
         <v>43913</v>
       </c>
-      <c r="C80" s="57"/>
-      <c r="D80" s="61">
+      <c r="C80" s="72">
+        <v>43922</v>
+      </c>
+      <c r="D80" s="73">
         <f t="shared" si="38"/>
-        <v>6</v>
-      </c>
-      <c r="E80" s="4">
+        <v>9</v>
+      </c>
+      <c r="E80" s="73">
         <v>5</v>
       </c>
-      <c r="F80" s="4">
+      <c r="F80" s="73">
         <v>498</v>
       </c>
-      <c r="G80" s="60">
+      <c r="G80" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H80" s="60">
-        <f t="shared" si="39"/>
-        <v>300</v>
-      </c>
-      <c r="I80" s="60">
+      <c r="H80" s="74">
+        <v>56</v>
+      </c>
+      <c r="I80" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J80" s="61">
+        <v>244</v>
+      </c>
+      <c r="J80" s="73">
         <f t="shared" si="32"/>
         <v>16</v>
       </c>
-      <c r="K80" s="61">
+      <c r="K80" s="73">
         <f t="shared" si="33"/>
         <v>56</v>
       </c>
-      <c r="L80" s="57">
+      <c r="L80" s="72">
         <f t="shared" si="34"/>
-        <v>43975</v>
-      </c>
-      <c r="M80" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N80" s="63">
+        <v>43978</v>
+      </c>
+      <c r="M80" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N80" s="75">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -9717,7 +9722,7 @@
       <c r="C81" s="57"/>
       <c r="D81" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E81" s="4">
         <v>6</v>
@@ -9730,7 +9735,7 @@
         <v>300</v>
       </c>
       <c r="H81" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="H80:H96" si="39">G81</f>
         <v>300</v>
       </c>
       <c r="I81" s="60">
@@ -9747,14 +9752,14 @@
       </c>
       <c r="L81" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M81" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N81" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -9768,7 +9773,7 @@
       <c r="C82" s="57"/>
       <c r="D82" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E82" s="4">
         <v>7</v>
@@ -9798,14 +9803,14 @@
       </c>
       <c r="L82" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M82" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N82" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -9819,7 +9824,7 @@
       <c r="C83" s="57"/>
       <c r="D83" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E83" s="4">
         <v>8</v>
@@ -9849,14 +9854,14 @@
       </c>
       <c r="L83" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M83" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N83" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -9870,7 +9875,7 @@
       <c r="C84" s="57"/>
       <c r="D84" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E84" s="4">
         <v>9</v>
@@ -9900,14 +9905,14 @@
       </c>
       <c r="L84" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M84" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N84" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -9921,7 +9926,7 @@
       <c r="C85" s="57"/>
       <c r="D85" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E85" s="4">
         <v>10</v>
@@ -9951,14 +9956,14 @@
       </c>
       <c r="L85" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M85" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N85" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -9969,7 +9974,7 @@
       <c r="C86" s="57"/>
       <c r="D86" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E86" s="4">
         <v>11</v>
@@ -9999,14 +10004,14 @@
       </c>
       <c r="L86" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M86" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N86" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -10017,7 +10022,7 @@
       <c r="C87" s="57"/>
       <c r="D87" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E87" s="4">
         <v>12</v>
@@ -10047,14 +10052,14 @@
       </c>
       <c r="L87" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M87" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N87" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -10065,7 +10070,7 @@
       <c r="C88" s="57"/>
       <c r="D88" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E88" s="4">
         <v>13</v>
@@ -10095,14 +10100,14 @@
       </c>
       <c r="L88" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M88" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N88" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -10113,7 +10118,7 @@
       <c r="C89" s="57"/>
       <c r="D89" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E89" s="4">
         <v>14</v>
@@ -10143,14 +10148,14 @@
       </c>
       <c r="L89" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M89" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N89" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -10161,7 +10166,7 @@
       <c r="C90" s="57"/>
       <c r="D90" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E90" s="4">
         <v>15</v>
@@ -10191,14 +10196,14 @@
       </c>
       <c r="L90" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -10209,7 +10214,7 @@
       <c r="C91" s="57"/>
       <c r="D91" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E91" s="4">
         <v>16</v>
@@ -10239,14 +10244,14 @@
       </c>
       <c r="L91" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -10257,7 +10262,7 @@
       <c r="C92" s="57"/>
       <c r="D92" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E92" s="4">
         <v>17</v>
@@ -10287,14 +10292,14 @@
       </c>
       <c r="L92" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -10305,7 +10310,7 @@
       <c r="C93" s="57"/>
       <c r="D93" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E93" s="4">
         <v>18</v>
@@ -10335,14 +10340,14 @@
       </c>
       <c r="L93" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -10353,7 +10358,7 @@
       <c r="C94" s="57"/>
       <c r="D94" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>53</v>
@@ -10383,14 +10388,14 @@
       </c>
       <c r="L94" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -10401,7 +10406,7 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>54</v>
@@ -10431,14 +10436,14 @@
       </c>
       <c r="L95" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -10449,7 +10454,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10479,14 +10484,14 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43975</v>
+        <v>43978</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>1869</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -10508,11 +10513,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>5601</v>
+        <v>5087</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>999</v>
+        <v>1513</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>

</xml_diff>

<commit_message>
inseridos arquivos do capítulo 6 sobre manipulação de strings, atualizado o arquivo de planejamento e o arquivo .gitignore
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF235262-6AA1-4E3C-9905-A2BD2EADE148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB328B14-80CC-4C0C-BD4E-072158CE35F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -6312,10 +6312,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ98"/>
+  <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M81" sqref="M81"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104:G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6323,17 +6323,17 @@
     <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5546875" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -9715,51 +9715,52 @@
       <c r="A81" s="64">
         <v>43898</v>
       </c>
-      <c r="B81" s="57">
+      <c r="B81" s="72">
         <f t="shared" si="35"/>
         <v>43916</v>
       </c>
-      <c r="C81" s="57"/>
-      <c r="D81" s="61">
+      <c r="C81" s="72">
+        <v>43923</v>
+      </c>
+      <c r="D81" s="73">
         <f t="shared" si="38"/>
-        <v>9</v>
-      </c>
-      <c r="E81" s="4">
-        <v>6</v>
-      </c>
-      <c r="F81" s="4">
-        <v>633</v>
-      </c>
-      <c r="G81" s="60">
+        <v>7</v>
+      </c>
+      <c r="E81" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F81" s="73">
+        <v>57</v>
+      </c>
+      <c r="G81" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H81" s="60">
-        <f t="shared" ref="H80:H96" si="39">G81</f>
-        <v>300</v>
-      </c>
-      <c r="I81" s="60">
+      <c r="H81" s="74">
+        <v>15</v>
+      </c>
+      <c r="I81" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J81" s="61">
+        <v>285</v>
+      </c>
+      <c r="J81" s="73">
         <f t="shared" si="32"/>
         <v>19</v>
       </c>
-      <c r="K81" s="61">
+      <c r="K81" s="73">
         <f t="shared" si="33"/>
         <v>53</v>
       </c>
-      <c r="L81" s="57">
+      <c r="L81" s="72">
         <f t="shared" si="34"/>
-        <v>43978</v>
-      </c>
-      <c r="M81" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N81" s="63">
+        <v>43976</v>
+      </c>
+      <c r="M81" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N81" s="75">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -9773,20 +9774,20 @@
       <c r="C82" s="57"/>
       <c r="D82" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E82" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" s="4">
-        <v>820</v>
+        <v>633</v>
       </c>
       <c r="G82" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H82" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="H81:H96" si="39">G82</f>
         <v>300</v>
       </c>
       <c r="I82" s="60">
@@ -9803,14 +9804,14 @@
       </c>
       <c r="L82" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M82" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N82" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -9824,13 +9825,13 @@
       <c r="C83" s="57"/>
       <c r="D83" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E83" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" s="4">
-        <v>707</v>
+        <v>820</v>
       </c>
       <c r="G83" s="60">
         <f t="shared" si="30"/>
@@ -9854,14 +9855,14 @@
       </c>
       <c r="L83" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M83" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N83" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -9875,13 +9876,13 @@
       <c r="C84" s="57"/>
       <c r="D84" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E84" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" s="4">
-        <v>567</v>
+        <v>707</v>
       </c>
       <c r="G84" s="60">
         <f t="shared" si="30"/>
@@ -9905,14 +9906,14 @@
       </c>
       <c r="L84" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M84" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N84" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -9926,13 +9927,13 @@
       <c r="C85" s="57"/>
       <c r="D85" s="61">
         <f t="shared" si="38"/>
+        <v>7</v>
+      </c>
+      <c r="E85" s="4">
         <v>9</v>
       </c>
-      <c r="E85" s="4">
-        <v>10</v>
-      </c>
       <c r="F85" s="4">
-        <v>506</v>
+        <v>567</v>
       </c>
       <c r="G85" s="60">
         <f t="shared" si="30"/>
@@ -9956,14 +9957,14 @@
       </c>
       <c r="L85" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M85" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N85" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -9974,13 +9975,13 @@
       <c r="C86" s="57"/>
       <c r="D86" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E86" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F86" s="4">
-        <v>924</v>
+        <v>506</v>
       </c>
       <c r="G86" s="60">
         <f t="shared" si="30"/>
@@ -10004,14 +10005,14 @@
       </c>
       <c r="L86" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M86" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N86" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -10022,13 +10023,13 @@
       <c r="C87" s="57"/>
       <c r="D87" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E87" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F87" s="4">
-        <v>876</v>
+        <v>924</v>
       </c>
       <c r="G87" s="60">
         <f t="shared" si="30"/>
@@ -10052,14 +10053,14 @@
       </c>
       <c r="L87" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M87" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N87" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -10070,13 +10071,13 @@
       <c r="C88" s="57"/>
       <c r="D88" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E88" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F88" s="4">
-        <v>699</v>
+        <v>876</v>
       </c>
       <c r="G88" s="60">
         <f t="shared" si="30"/>
@@ -10100,14 +10101,14 @@
       </c>
       <c r="L88" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M88" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N88" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -10118,13 +10119,13 @@
       <c r="C89" s="57"/>
       <c r="D89" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E89" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F89" s="4">
-        <v>498</v>
+        <v>699</v>
       </c>
       <c r="G89" s="60">
         <f t="shared" si="30"/>
@@ -10148,14 +10149,14 @@
       </c>
       <c r="L89" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M89" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N89" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -10166,13 +10167,13 @@
       <c r="C90" s="57"/>
       <c r="D90" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E90" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F90" s="4">
-        <v>820</v>
+        <v>498</v>
       </c>
       <c r="G90" s="60">
         <f t="shared" si="30"/>
@@ -10196,14 +10197,14 @@
       </c>
       <c r="L90" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -10214,13 +10215,13 @@
       <c r="C91" s="57"/>
       <c r="D91" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E91" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F91" s="4">
-        <v>791</v>
+        <v>820</v>
       </c>
       <c r="G91" s="60">
         <f t="shared" si="30"/>
@@ -10244,14 +10245,14 @@
       </c>
       <c r="L91" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -10262,13 +10263,13 @@
       <c r="C92" s="57"/>
       <c r="D92" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E92" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F92" s="4">
-        <v>717</v>
+        <v>791</v>
       </c>
       <c r="G92" s="60">
         <f t="shared" si="30"/>
@@ -10292,14 +10293,14 @@
       </c>
       <c r="L92" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -10310,13 +10311,13 @@
       <c r="C93" s="57"/>
       <c r="D93" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E93" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F93" s="4">
-        <v>827</v>
+        <v>717</v>
       </c>
       <c r="G93" s="60">
         <f t="shared" si="30"/>
@@ -10340,14 +10341,14 @@
       </c>
       <c r="L93" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -10358,13 +10359,13 @@
       <c r="C94" s="57"/>
       <c r="D94" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>53</v>
+        <v>7</v>
+      </c>
+      <c r="E94" s="4">
+        <v>18</v>
       </c>
       <c r="F94" s="4">
-        <v>42</v>
+        <v>827</v>
       </c>
       <c r="G94" s="60">
         <f t="shared" si="30"/>
@@ -10388,14 +10389,14 @@
       </c>
       <c r="L94" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -10406,13 +10407,13 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F95" s="4">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G95" s="60">
         <f t="shared" si="30"/>
@@ -10436,14 +10437,14 @@
       </c>
       <c r="L95" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -10454,7 +10455,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10484,14 +10485,14 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43978</v>
+        <v>43976</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>3110</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -10513,11 +10514,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>5087</v>
+        <v>4802</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>1513</v>
+        <v>1798</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>
@@ -10539,6 +10540,10 @@
       <c r="H98" s="47"/>
       <c r="I98" s="47"/>
       <c r="J98" s="47"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
inserido dois exemplos do capítulo sobre Regex
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB328B14-80CC-4C0C-BD4E-072158CE35F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65146EE-9B67-4AA1-8BE6-1FB9B35632E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6315,7 +6315,7 @@
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104:G104"/>
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9767,51 +9767,52 @@
       <c r="A82" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B82" s="57">
+      <c r="B82" s="72">
         <f t="shared" si="35"/>
         <v>43919</v>
       </c>
-      <c r="C82" s="57"/>
-      <c r="D82" s="61">
+      <c r="C82" s="72">
+        <v>43923</v>
+      </c>
+      <c r="D82" s="73">
         <f t="shared" si="38"/>
-        <v>7</v>
-      </c>
-      <c r="E82" s="4">
+        <v>4</v>
+      </c>
+      <c r="E82" s="73">
         <v>6</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="73">
         <v>633</v>
       </c>
-      <c r="G82" s="60">
+      <c r="G82" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H82" s="60">
-        <f t="shared" ref="H81:H96" si="39">G82</f>
-        <v>300</v>
-      </c>
-      <c r="I82" s="60">
+      <c r="H82" s="74">
+        <v>223</v>
+      </c>
+      <c r="I82" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J82" s="61">
+        <v>77</v>
+      </c>
+      <c r="J82" s="73">
         <f t="shared" si="32"/>
         <v>22</v>
       </c>
-      <c r="K82" s="61">
+      <c r="K82" s="73">
         <f t="shared" si="33"/>
         <v>50</v>
       </c>
-      <c r="L82" s="57">
+      <c r="L82" s="72">
         <f t="shared" si="34"/>
-        <v>43976</v>
-      </c>
-      <c r="M82" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N82" s="63">
+        <v>43973</v>
+      </c>
+      <c r="M82" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N82" s="75">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -9825,7 +9826,7 @@
       <c r="C83" s="57"/>
       <c r="D83" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E83" s="4">
         <v>7</v>
@@ -9838,7 +9839,7 @@
         <v>300</v>
       </c>
       <c r="H83" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="H82:H96" si="39">G83</f>
         <v>300</v>
       </c>
       <c r="I83" s="60">
@@ -9855,14 +9856,14 @@
       </c>
       <c r="L83" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M83" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N83" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -9876,7 +9877,7 @@
       <c r="C84" s="57"/>
       <c r="D84" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E84" s="4">
         <v>8</v>
@@ -9906,14 +9907,14 @@
       </c>
       <c r="L84" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M84" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N84" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -9927,7 +9928,7 @@
       <c r="C85" s="57"/>
       <c r="D85" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E85" s="4">
         <v>9</v>
@@ -9957,14 +9958,14 @@
       </c>
       <c r="L85" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M85" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N85" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -9975,7 +9976,7 @@
       <c r="C86" s="57"/>
       <c r="D86" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E86" s="4">
         <v>10</v>
@@ -10005,14 +10006,14 @@
       </c>
       <c r="L86" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M86" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N86" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -10023,7 +10024,7 @@
       <c r="C87" s="57"/>
       <c r="D87" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E87" s="4">
         <v>11</v>
@@ -10053,14 +10054,14 @@
       </c>
       <c r="L87" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M87" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N87" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -10071,7 +10072,7 @@
       <c r="C88" s="57"/>
       <c r="D88" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E88" s="4">
         <v>12</v>
@@ -10101,14 +10102,14 @@
       </c>
       <c r="L88" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M88" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N88" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -10119,7 +10120,7 @@
       <c r="C89" s="57"/>
       <c r="D89" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E89" s="4">
         <v>13</v>
@@ -10149,14 +10150,14 @@
       </c>
       <c r="L89" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M89" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N89" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -10167,7 +10168,7 @@
       <c r="C90" s="57"/>
       <c r="D90" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E90" s="4">
         <v>14</v>
@@ -10197,14 +10198,14 @@
       </c>
       <c r="L90" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -10215,7 +10216,7 @@
       <c r="C91" s="57"/>
       <c r="D91" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E91" s="4">
         <v>15</v>
@@ -10245,14 +10246,14 @@
       </c>
       <c r="L91" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -10263,7 +10264,7 @@
       <c r="C92" s="57"/>
       <c r="D92" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E92" s="4">
         <v>16</v>
@@ -10293,14 +10294,14 @@
       </c>
       <c r="L92" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -10311,7 +10312,7 @@
       <c r="C93" s="57"/>
       <c r="D93" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E93" s="4">
         <v>17</v>
@@ -10341,14 +10342,14 @@
       </c>
       <c r="L93" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -10359,7 +10360,7 @@
       <c r="C94" s="57"/>
       <c r="D94" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E94" s="4">
         <v>18</v>
@@ -10389,14 +10390,14 @@
       </c>
       <c r="L94" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -10407,7 +10408,7 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>53</v>
@@ -10437,14 +10438,14 @@
       </c>
       <c r="L95" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -10455,7 +10456,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10485,14 +10486,14 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43976</v>
+        <v>43973</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>3167</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -10514,11 +10515,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>4802</v>
+        <v>4725</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>1798</v>
+        <v>1875</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>

</xml_diff>

<commit_message>
Inserido os arquivos referentes aos estudos de expressões regulares
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65146EE-9B67-4AA1-8BE6-1FB9B35632E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F6EF6-21AC-45D8-B7F2-A48B71B8B1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6314,8 +6314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9819,51 +9819,52 @@
       <c r="A83" s="1">
         <v>23</v>
       </c>
-      <c r="B83" s="57">
+      <c r="B83" s="72">
         <f t="shared" si="35"/>
         <v>43922</v>
       </c>
-      <c r="C83" s="57"/>
-      <c r="D83" s="61">
+      <c r="C83" s="72">
+        <v>43924</v>
+      </c>
+      <c r="D83" s="73">
         <f t="shared" si="38"/>
-        <v>4</v>
-      </c>
-      <c r="E83" s="4">
+        <v>2</v>
+      </c>
+      <c r="E83" s="73">
         <v>7</v>
       </c>
-      <c r="F83" s="4">
+      <c r="F83" s="73">
         <v>820</v>
       </c>
-      <c r="G83" s="60">
+      <c r="G83" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H83" s="60">
-        <f t="shared" ref="H82:H96" si="39">G83</f>
-        <v>300</v>
-      </c>
-      <c r="I83" s="60">
+      <c r="H83" s="74">
+        <v>201</v>
+      </c>
+      <c r="I83" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J83" s="61">
+        <v>99</v>
+      </c>
+      <c r="J83" s="73">
         <f t="shared" si="32"/>
         <v>25</v>
       </c>
-      <c r="K83" s="61">
+      <c r="K83" s="73">
         <f t="shared" si="33"/>
         <v>47</v>
       </c>
-      <c r="L83" s="57">
+      <c r="L83" s="72">
         <f t="shared" si="34"/>
-        <v>43973</v>
-      </c>
-      <c r="M83" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N83" s="63">
+        <v>43971</v>
+      </c>
+      <c r="M83" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N83" s="75">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -9877,7 +9878,7 @@
       <c r="C84" s="57"/>
       <c r="D84" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E84" s="4">
         <v>8</v>
@@ -9890,7 +9891,7 @@
         <v>300</v>
       </c>
       <c r="H84" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="H83:H96" si="39">G84</f>
         <v>300</v>
       </c>
       <c r="I84" s="60">
@@ -9907,14 +9908,14 @@
       </c>
       <c r="L84" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M84" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N84" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -9928,7 +9929,7 @@
       <c r="C85" s="57"/>
       <c r="D85" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E85" s="4">
         <v>9</v>
@@ -9958,14 +9959,14 @@
       </c>
       <c r="L85" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M85" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N85" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -9976,7 +9977,7 @@
       <c r="C86" s="57"/>
       <c r="D86" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E86" s="4">
         <v>10</v>
@@ -10006,14 +10007,14 @@
       </c>
       <c r="L86" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M86" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N86" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -10024,7 +10025,7 @@
       <c r="C87" s="57"/>
       <c r="D87" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E87" s="4">
         <v>11</v>
@@ -10054,14 +10055,14 @@
       </c>
       <c r="L87" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M87" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N87" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -10072,7 +10073,7 @@
       <c r="C88" s="57"/>
       <c r="D88" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E88" s="4">
         <v>12</v>
@@ -10102,14 +10103,14 @@
       </c>
       <c r="L88" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M88" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N88" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -10120,7 +10121,7 @@
       <c r="C89" s="57"/>
       <c r="D89" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E89" s="4">
         <v>13</v>
@@ -10150,14 +10151,14 @@
       </c>
       <c r="L89" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M89" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N89" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -10168,7 +10169,7 @@
       <c r="C90" s="57"/>
       <c r="D90" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E90" s="4">
         <v>14</v>
@@ -10198,14 +10199,14 @@
       </c>
       <c r="L90" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -10216,7 +10217,7 @@
       <c r="C91" s="57"/>
       <c r="D91" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E91" s="4">
         <v>15</v>
@@ -10246,14 +10247,14 @@
       </c>
       <c r="L91" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -10264,7 +10265,7 @@
       <c r="C92" s="57"/>
       <c r="D92" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E92" s="4">
         <v>16</v>
@@ -10294,14 +10295,14 @@
       </c>
       <c r="L92" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -10312,7 +10313,7 @@
       <c r="C93" s="57"/>
       <c r="D93" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E93" s="4">
         <v>17</v>
@@ -10342,14 +10343,14 @@
       </c>
       <c r="L93" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -10360,7 +10361,7 @@
       <c r="C94" s="57"/>
       <c r="D94" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E94" s="4">
         <v>18</v>
@@ -10390,14 +10391,14 @@
       </c>
       <c r="L94" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -10408,7 +10409,7 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>53</v>
@@ -10438,14 +10439,14 @@
       </c>
       <c r="L95" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -10456,7 +10457,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10486,14 +10487,14 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43973</v>
+        <v>43971</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>3800</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -10515,11 +10516,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>4725</v>
+        <v>4626</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>1875</v>
+        <v>1974</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>

</xml_diff>

<commit_message>
Inseridos os arquivos referentes ao capítulo 9 do livro, referentes a organização de arquivos
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F6EF6-21AC-45D8-B7F2-A48B71B8B1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C456FAB-5E86-4DCD-A9EB-441CBBBC31AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -1113,21 +1113,21 @@
       <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1"/>
-    <col min="4" max="4" width="15.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
-    <col min="9" max="9" width="26.88671875" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="27.44140625" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1487,7 +1487,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1601,7 +1601,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -1972,7 +1972,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -2210,7 +2210,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -2227,7 +2227,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -2465,7 +2465,7 @@
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -2499,7 +2499,7 @@
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -2550,7 +2550,7 @@
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -2601,7 +2601,7 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -2652,7 +2652,7 @@
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -2720,7 +2720,7 @@
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -2771,7 +2771,7 @@
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -2839,7 +2839,7 @@
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -2856,7 +2856,7 @@
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -2873,7 +2873,7 @@
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -2890,7 +2890,7 @@
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -2941,7 +2941,7 @@
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -2958,7 +2958,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -3043,7 +3043,7 @@
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -3111,7 +3111,7 @@
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -3145,7 +3145,7 @@
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -3179,7 +3179,7 @@
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -3213,7 +3213,7 @@
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -3230,7 +3230,7 @@
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -3247,7 +3247,7 @@
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -3281,7 +3281,7 @@
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -3315,7 +3315,7 @@
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -3349,7 +3349,7 @@
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -3417,7 +3417,7 @@
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -3434,7 +3434,7 @@
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -3451,7 +3451,7 @@
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -3502,7 +3502,7 @@
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -3570,7 +3570,7 @@
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -3604,7 +3604,7 @@
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -3621,7 +3621,7 @@
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -3672,7 +3672,7 @@
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -3774,7 +3774,7 @@
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -3808,7 +3808,7 @@
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -3825,7 +3825,7 @@
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -3859,7 +3859,7 @@
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="J157" s="15"/>
       <c r="K157" s="15"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -3893,7 +3893,7 @@
       <c r="J158" s="15"/>
       <c r="K158" s="15"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="J159" s="15"/>
       <c r="K159" s="15"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -3927,7 +3927,7 @@
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="J161" s="15"/>
       <c r="K161" s="15"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="J162" s="15"/>
       <c r="K162" s="15"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -3978,7 +3978,7 @@
       <c r="J163" s="15"/>
       <c r="K163" s="15"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -3995,7 +3995,7 @@
       <c r="J164" s="15"/>
       <c r="K164" s="15"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -4012,7 +4012,7 @@
       <c r="J165" s="15"/>
       <c r="K165" s="15"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -4029,7 +4029,7 @@
       <c r="J166" s="15"/>
       <c r="K166" s="15"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="J167" s="15"/>
       <c r="K167" s="15"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="J168" s="15"/>
       <c r="K168" s="15"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -4080,7 +4080,7 @@
       <c r="J169" s="15"/>
       <c r="K169" s="15"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -4097,7 +4097,7 @@
       <c r="J170" s="15"/>
       <c r="K170" s="15"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -4114,7 +4114,7 @@
       <c r="J171" s="15"/>
       <c r="K171" s="15"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="J172" s="15"/>
       <c r="K172" s="15"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="4">
         <v>172</v>
       </c>
@@ -4148,7 +4148,7 @@
       <c r="J173" s="15"/>
       <c r="K173" s="15"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -4165,7 +4165,7 @@
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="J175" s="15"/>
       <c r="K175" s="15"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="J176" s="15"/>
       <c r="K176" s="15"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -4216,7 +4216,7 @@
       <c r="J177" s="15"/>
       <c r="K177" s="15"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="J178" s="15"/>
       <c r="K178" s="15"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>178</v>
       </c>
@@ -4250,7 +4250,7 @@
       <c r="J179" s="15"/>
       <c r="K179" s="15"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
         <v>179</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="J180" s="15"/>
       <c r="K180" s="15"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="4">
         <v>180</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="J181" s="15"/>
       <c r="K181" s="15"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="4">
         <v>181</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="J182" s="15"/>
       <c r="K182" s="15"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="4">
         <v>182</v>
       </c>
@@ -4318,7 +4318,7 @@
       <c r="J183" s="15"/>
       <c r="K183" s="15"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="4">
         <v>183</v>
       </c>
@@ -4335,7 +4335,7 @@
       <c r="J184" s="15"/>
       <c r="K184" s="15"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="4">
         <v>184</v>
       </c>
@@ -4352,7 +4352,7 @@
       <c r="J185" s="15"/>
       <c r="K185" s="15"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="4">
         <v>185</v>
       </c>
@@ -4369,7 +4369,7 @@
       <c r="J186" s="15"/>
       <c r="K186" s="15"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="4">
         <v>186</v>
       </c>
@@ -4386,7 +4386,7 @@
       <c r="J187" s="15"/>
       <c r="K187" s="15"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="4">
         <v>187</v>
       </c>
@@ -4403,7 +4403,7 @@
       <c r="J188" s="15"/>
       <c r="K188" s="15"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="4">
         <v>188</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="J189" s="15"/>
       <c r="K189" s="15"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="4">
         <v>189</v>
       </c>
@@ -4437,7 +4437,7 @@
       <c r="J190" s="15"/>
       <c r="K190" s="15"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
         <v>190</v>
       </c>
@@ -4454,7 +4454,7 @@
       <c r="J191" s="15"/>
       <c r="K191" s="15"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="4">
         <v>191</v>
       </c>
@@ -4471,7 +4471,7 @@
       <c r="J192" s="15"/>
       <c r="K192" s="15"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="4">
         <v>192</v>
       </c>
@@ -4488,7 +4488,7 @@
       <c r="J193" s="15"/>
       <c r="K193" s="15"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" s="4">
         <v>193</v>
       </c>
@@ -4505,7 +4505,7 @@
       <c r="J194" s="15"/>
       <c r="K194" s="15"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="4">
         <v>194</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="J195" s="15"/>
       <c r="K195" s="15"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
         <v>195</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="J196" s="15"/>
       <c r="K196" s="15"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="4">
         <v>196</v>
       </c>
@@ -4556,7 +4556,7 @@
       <c r="J197" s="15"/>
       <c r="K197" s="15"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" s="4">
         <v>197</v>
       </c>
@@ -4573,7 +4573,7 @@
       <c r="J198" s="15"/>
       <c r="K198" s="15"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" s="4">
         <v>198</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="J199" s="15"/>
       <c r="K199" s="15"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
         <v>199</v>
       </c>
@@ -4607,7 +4607,7 @@
       <c r="J200" s="15"/>
       <c r="K200" s="15"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" s="4">
         <v>200</v>
       </c>
@@ -4624,7 +4624,7 @@
       <c r="J201" s="15"/>
       <c r="K201" s="15"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" s="4">
         <v>201</v>
       </c>
@@ -4641,7 +4641,7 @@
       <c r="J202" s="15"/>
       <c r="K202" s="15"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" s="4">
         <v>202</v>
       </c>
@@ -4658,7 +4658,7 @@
       <c r="J203" s="15"/>
       <c r="K203" s="15"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" s="4">
         <v>203</v>
       </c>
@@ -4675,7 +4675,7 @@
       <c r="J204" s="15"/>
       <c r="K204" s="15"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>12</v>
       </c>
@@ -4734,16 +4734,16 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" customWidth="1"/>
-    <col min="8" max="8" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12 1025:1025" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12 1025:1025" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="AMK1"/>
     </row>
-    <row r="2" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
         <v>0</v>
       </c>
@@ -4801,7 +4801,7 @@
       </c>
       <c r="L2" s="85"/>
     </row>
-    <row r="3" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="L3" s="85"/>
     </row>
-    <row r="4" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="76">
         <v>2</v>
       </c>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="L4" s="86"/>
     </row>
-    <row r="5" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76">
         <v>3</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="J5" s="91"/>
       <c r="L5" s="86"/>
     </row>
-    <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -4917,7 +4917,7 @@
       <c r="J6" s="91"/>
       <c r="L6" s="86"/>
     </row>
-    <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="79">
         <v>5</v>
       </c>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="L7" s="87"/>
     </row>
-    <row r="8" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="79">
         <v>6</v>
       </c>
@@ -4975,7 +4975,7 @@
       <c r="J8" s="93"/>
       <c r="L8" s="87"/>
     </row>
-    <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="82">
         <v>7</v>
       </c>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="L9" s="88"/>
     </row>
-    <row r="10" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="82">
         <v>8</v>
       </c>
@@ -5033,7 +5033,7 @@
       <c r="J10" s="95"/>
       <c r="L10" s="88"/>
     </row>
-    <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="B11" s="17">
         <f>SUM(B2:B10)</f>
         <v>341</v>
@@ -5055,22 +5055,22 @@
         <v>44069</v>
       </c>
     </row>
-    <row r="13" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="A14" s="85">
         <v>43864</v>
       </c>
     </row>
-    <row r="15" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="D15" s="85">
         <v>43869</v>
       </c>
     </row>
-    <row r="16" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
       <c r="D16" s="85">
         <f>D15+D11</f>
         <v>44074</v>
@@ -5102,62 +5102,62 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="11" width="10.88671875" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" customWidth="1"/>
-    <col min="13" max="15" width="7.109375" customWidth="1"/>
-    <col min="16" max="24" width="6.6640625" customWidth="1"/>
-    <col min="25" max="25" width="7.6640625" customWidth="1"/>
-    <col min="26" max="26" width="7.5546875" customWidth="1"/>
-    <col min="27" max="30" width="7.6640625" customWidth="1"/>
-    <col min="31" max="34" width="10.88671875" customWidth="1"/>
-    <col min="35" max="43" width="6.6640625" customWidth="1"/>
-    <col min="44" max="44" width="7.6640625" customWidth="1"/>
-    <col min="45" max="45" width="7.5546875" customWidth="1"/>
-    <col min="46" max="65" width="7.6640625" customWidth="1"/>
-    <col min="66" max="74" width="6.109375" customWidth="1"/>
-    <col min="75" max="75" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="13" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="24" width="6.7109375" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" customWidth="1"/>
+    <col min="26" max="26" width="7.5703125" customWidth="1"/>
+    <col min="27" max="30" width="7.7109375" customWidth="1"/>
+    <col min="31" max="34" width="10.85546875" customWidth="1"/>
+    <col min="35" max="43" width="6.7109375" customWidth="1"/>
+    <col min="44" max="44" width="7.7109375" customWidth="1"/>
+    <col min="45" max="45" width="7.5703125" customWidth="1"/>
+    <col min="46" max="65" width="7.7109375" customWidth="1"/>
+    <col min="66" max="74" width="6.140625" customWidth="1"/>
+    <col min="75" max="75" width="7.140625" customWidth="1"/>
     <col min="76" max="76" width="7" customWidth="1"/>
-    <col min="77" max="95" width="7.109375" customWidth="1"/>
-    <col min="96" max="104" width="6.5546875" customWidth="1"/>
-    <col min="105" max="105" width="7.5546875" customWidth="1"/>
-    <col min="106" max="106" width="7.44140625" customWidth="1"/>
-    <col min="107" max="126" width="7.5546875" customWidth="1"/>
+    <col min="77" max="95" width="7.140625" customWidth="1"/>
+    <col min="96" max="104" width="6.5703125" customWidth="1"/>
+    <col min="105" max="105" width="7.5703125" customWidth="1"/>
+    <col min="106" max="106" width="7.42578125" customWidth="1"/>
+    <col min="107" max="126" width="7.5703125" customWidth="1"/>
     <col min="127" max="135" width="6" customWidth="1"/>
     <col min="136" max="136" width="7" customWidth="1"/>
-    <col min="137" max="137" width="6.88671875" customWidth="1"/>
+    <col min="137" max="137" width="6.85546875" customWidth="1"/>
     <col min="138" max="156" width="7" customWidth="1"/>
-    <col min="157" max="165" width="5.44140625" customWidth="1"/>
-    <col min="166" max="166" width="6.44140625" customWidth="1"/>
-    <col min="167" max="167" width="6.33203125" customWidth="1"/>
-    <col min="168" max="187" width="6.44140625" customWidth="1"/>
-    <col min="188" max="196" width="6.5546875" customWidth="1"/>
-    <col min="197" max="197" width="7.5546875" customWidth="1"/>
-    <col min="198" max="198" width="7.44140625" customWidth="1"/>
-    <col min="199" max="218" width="7.5546875" customWidth="1"/>
-    <col min="219" max="227" width="6.109375" customWidth="1"/>
-    <col min="228" max="228" width="7.109375" customWidth="1"/>
+    <col min="157" max="165" width="5.42578125" customWidth="1"/>
+    <col min="166" max="166" width="6.42578125" customWidth="1"/>
+    <col min="167" max="167" width="6.28515625" customWidth="1"/>
+    <col min="168" max="187" width="6.42578125" customWidth="1"/>
+    <col min="188" max="196" width="6.5703125" customWidth="1"/>
+    <col min="197" max="197" width="7.5703125" customWidth="1"/>
+    <col min="198" max="198" width="7.42578125" customWidth="1"/>
+    <col min="199" max="218" width="7.5703125" customWidth="1"/>
+    <col min="219" max="227" width="6.140625" customWidth="1"/>
+    <col min="228" max="228" width="7.140625" customWidth="1"/>
     <col min="229" max="229" width="7" customWidth="1"/>
-    <col min="230" max="248" width="7.109375" customWidth="1"/>
-    <col min="249" max="257" width="6.109375" customWidth="1"/>
-    <col min="258" max="258" width="7.109375" customWidth="1"/>
+    <col min="230" max="248" width="7.140625" customWidth="1"/>
+    <col min="249" max="257" width="6.140625" customWidth="1"/>
+    <col min="258" max="258" width="7.140625" customWidth="1"/>
     <col min="259" max="259" width="7" customWidth="1"/>
-    <col min="260" max="279" width="7.109375" customWidth="1"/>
-    <col min="280" max="288" width="6.5546875" customWidth="1"/>
-    <col min="289" max="289" width="7.5546875" customWidth="1"/>
-    <col min="290" max="290" width="7.44140625" customWidth="1"/>
-    <col min="291" max="309" width="7.5546875" customWidth="1"/>
-    <col min="310" max="318" width="6.5546875" customWidth="1"/>
-    <col min="319" max="319" width="7.5546875" customWidth="1"/>
-    <col min="320" max="320" width="7.44140625" customWidth="1"/>
-    <col min="321" max="340" width="7.5546875" customWidth="1"/>
+    <col min="260" max="279" width="7.140625" customWidth="1"/>
+    <col min="280" max="288" width="6.5703125" customWidth="1"/>
+    <col min="289" max="289" width="7.5703125" customWidth="1"/>
+    <col min="290" max="290" width="7.42578125" customWidth="1"/>
+    <col min="291" max="309" width="7.5703125" customWidth="1"/>
+    <col min="310" max="318" width="6.5703125" customWidth="1"/>
+    <col min="319" max="319" width="7.5703125" customWidth="1"/>
+    <col min="320" max="320" width="7.42578125" customWidth="1"/>
+    <col min="321" max="340" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:340" x14ac:dyDescent="0.2">
       <c r="A1" s="24">
         <v>43857</v>
       </c>
@@ -6179,7 +6179,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="2" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:340" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:340" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>19</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:340" x14ac:dyDescent="0.2">
       <c r="C4" s="25" t="s">
         <v>19</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:340" x14ac:dyDescent="0.2">
       <c r="D5" s="25" t="s">
         <v>19</v>
       </c>
@@ -6235,67 +6235,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:340" x14ac:dyDescent="0.2">
       <c r="E6" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:340" x14ac:dyDescent="0.2">
       <c r="F7" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:340" x14ac:dyDescent="0.2">
       <c r="G8" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:340" x14ac:dyDescent="0.2">
       <c r="H9" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:340" x14ac:dyDescent="0.2">
       <c r="I10" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:340" x14ac:dyDescent="0.2">
       <c r="J11" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:340" x14ac:dyDescent="0.2">
       <c r="K12" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:340" x14ac:dyDescent="0.2">
       <c r="L13" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:340" x14ac:dyDescent="0.2">
       <c r="M14" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:340" x14ac:dyDescent="0.2">
       <c r="N15" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:340" x14ac:dyDescent="0.2">
       <c r="O16" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="16:17" x14ac:dyDescent="0.2">
       <c r="P17" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="16:17" x14ac:dyDescent="0.2">
       <c r="Q18" s="25" t="s">
         <v>16</v>
       </c>
@@ -6314,29 +6314,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="97" t="s">
         <v>21</v>
       </c>
@@ -6350,7 +6350,7 @@
       <c r="L1" s="98"/>
       <c r="M1" s="98"/>
     </row>
-    <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>14</v>
@@ -6408,7 +6408,7 @@
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>52</v>
@@ -6425,7 +6425,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>46</v>
@@ -6442,7 +6442,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>26</v>
@@ -6459,7 +6459,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <f>180+26</f>
@@ -6477,7 +6477,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4">
         <f>60+41</f>
@@ -6495,7 +6495,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4">
         <f>60+22</f>
@@ -6513,7 +6513,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4">
         <v>43</v>
@@ -6530,7 +6530,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>43869</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>43885</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>43870</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>43886</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>43873</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>43888</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
         <v>43873</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>43887</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
         <v>43880</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
         <v>43882</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A17" s="35">
         <v>43886</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
         <v>43887</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>43895</v>
       </c>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
         <v>43887</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A20" s="35">
         <v>43889</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A21" s="35">
         <v>43891</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A22" s="35">
         <v>43891</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A23" s="45">
         <f>A11+(D23-D11)</f>
         <v>43891</v>
@@ -7175,7 +7175,7 @@
       <c r="H23" s="47"/>
       <c r="I23" s="47"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A24" s="45"/>
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
@@ -7186,13 +7186,13 @@
       <c r="H24" s="47"/>
       <c r="I24" s="47"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A25" s="99" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="99"/>
     </row>
-    <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>36</v>
       </c>
@@ -7240,7 +7240,7 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="49">
         <v>72</v>
       </c>
@@ -7295,7 +7295,7 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>47</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A29" s="55">
         <f>ROUND(A27/A35,0)</f>
         <v>3</v>
@@ -7400,7 +7400,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>48</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A31" s="56">
         <f>A37*A29</f>
         <v>300</v>
@@ -7505,7 +7505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>50</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="64">
         <v>43898</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>51</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>21</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>52</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>100</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B38" s="57">
         <f t="shared" si="17"/>
         <v>43931</v>
@@ -7859,7 +7859,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B39" s="57">
         <f t="shared" si="17"/>
         <v>43934</v>
@@ -7907,7 +7907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B40" s="57">
         <f t="shared" si="17"/>
         <v>43937</v>
@@ -7955,7 +7955,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B41" s="57">
         <f t="shared" si="17"/>
         <v>43940</v>
@@ -8003,7 +8003,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B42" s="57">
         <f t="shared" si="17"/>
         <v>43943</v>
@@ -8051,7 +8051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B43" s="57">
         <f t="shared" si="17"/>
         <v>43946</v>
@@ -8099,7 +8099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B44" s="57">
         <f t="shared" si="17"/>
         <v>43949</v>
@@ -8147,7 +8147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B45" s="57">
         <f t="shared" si="17"/>
         <v>43952</v>
@@ -8195,7 +8195,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B46" s="57">
         <f t="shared" si="17"/>
         <v>43955</v>
@@ -8243,7 +8243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B47" s="65">
         <f>A33+A27-1</f>
         <v>43969</v>
@@ -8291,7 +8291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="B48" s="65">
         <f>B47</f>
@@ -8325,7 +8325,7 @@
       <c r="M48" s="47"/>
       <c r="N48" s="47"/>
     </row>
-    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49" s="65"/>
       <c r="C49" s="65"/>
@@ -8339,14 +8339,14 @@
       <c r="K49" s="47"/>
       <c r="L49" s="47"/>
     </row>
-    <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A51" s="99" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="99"/>
       <c r="C51" s="99"/>
     </row>
-    <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>36</v>
       </c>
@@ -8394,7 +8394,7 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="49">
         <v>72</v>
       </c>
@@ -8449,7 +8449,7 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>47</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A55" s="55">
         <f>ROUND(A53/A61,0)</f>
         <v>4</v>
@@ -8554,7 +8554,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>48</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A57" s="56">
         <f>A63*A55</f>
         <v>400</v>
@@ -8658,7 +8658,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>50</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A59" s="64">
         <v>43898</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
         <v>51</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>18</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
         <v>52</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>100</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B64" s="57">
         <f t="shared" si="25"/>
         <v>43942</v>
@@ -9012,7 +9012,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B65" s="57">
         <f t="shared" si="25"/>
         <v>43946</v>
@@ -9060,7 +9060,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B66" s="57">
         <f t="shared" si="25"/>
         <v>43950</v>
@@ -9108,7 +9108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B67" s="57">
         <f t="shared" si="25"/>
         <v>43954</v>
@@ -9156,7 +9156,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B68" s="57">
         <f t="shared" si="25"/>
         <v>43958</v>
@@ -9204,7 +9204,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B69" s="57">
         <f t="shared" si="25"/>
         <v>43962</v>
@@ -9252,12 +9252,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="B70" s="65">
         <f>A59+A53-1</f>
         <v>43969</v>
       </c>
-      <c r="C70" s="65"/>
+      <c r="C70" s="57"/>
       <c r="D70" s="58">
         <f t="shared" si="28"/>
         <v>11</v>
@@ -9300,7 +9300,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A71"/>
       <c r="B71" s="65">
         <f>B70</f>
@@ -9334,11 +9334,11 @@
       <c r="M71" s="71"/>
       <c r="N71" s="71"/>
     </row>
-    <row r="72" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="K72" s="71"/>
       <c r="L72" s="71"/>
     </row>
-    <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A73" s="99" t="s">
         <v>18</v>
       </c>
@@ -9346,7 +9346,7 @@
       <c r="K73" s="71"/>
       <c r="L73" s="71"/>
     </row>
-    <row r="74" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
         <v>36</v>
       </c>
@@ -9394,7 +9394,7 @@
       <c r="AMI74"/>
       <c r="AMJ74"/>
     </row>
-    <row r="75" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="49">
         <v>72</v>
       </c>
@@ -9449,7 +9449,7 @@
       <c r="AMI75"/>
       <c r="AMJ75"/>
     </row>
-    <row r="76" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
         <v>47</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="77" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A77" s="55">
         <f>ROUND(A75/A83,0)</f>
         <v>3</v>
@@ -9554,7 +9554,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="78" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
         <v>48</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="79" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A79" s="56">
         <f>A85*A77</f>
         <v>300</v>
@@ -9659,7 +9659,7 @@
         <v>2612</v>
       </c>
     </row>
-    <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
         <v>50</v>
       </c>
@@ -9711,7 +9711,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="64">
         <v>43898</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
         <v>51</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>23</v>
       </c>
@@ -9867,589 +9867,591 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B84" s="57">
+      <c r="B84" s="72">
         <f t="shared" si="35"/>
         <v>43925</v>
       </c>
-      <c r="C84" s="57"/>
-      <c r="D84" s="61">
+      <c r="C84" s="72">
+        <v>43925</v>
+      </c>
+      <c r="D84" s="73">
         <f t="shared" si="38"/>
-        <v>2</v>
-      </c>
-      <c r="E84" s="4">
+        <v>0</v>
+      </c>
+      <c r="E84" s="73">
         <v>8</v>
       </c>
-      <c r="F84" s="4">
+      <c r="F84" s="73">
         <v>707</v>
       </c>
-      <c r="G84" s="60">
+      <c r="G84" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H84" s="60">
-        <f t="shared" ref="H83:H96" si="39">G84</f>
-        <v>300</v>
-      </c>
-      <c r="I84" s="60">
+      <c r="H84" s="74">
+        <v>214</v>
+      </c>
+      <c r="I84" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J84" s="61">
+        <v>86</v>
+      </c>
+      <c r="J84" s="73">
         <f t="shared" si="32"/>
         <v>28</v>
       </c>
-      <c r="K84" s="61">
+      <c r="K84" s="73">
         <f t="shared" si="33"/>
         <v>44</v>
       </c>
-      <c r="L84" s="57">
+      <c r="L84" s="72">
         <f t="shared" si="34"/>
-        <v>43971</v>
-      </c>
-      <c r="M84" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N84" s="63">
+        <v>43969</v>
+      </c>
+      <c r="M84" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N84" s="75">
         <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5327</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>100</v>
       </c>
-      <c r="B85" s="57">
+      <c r="B85" s="72">
         <f t="shared" si="35"/>
         <v>43928</v>
       </c>
-      <c r="C85" s="57"/>
-      <c r="D85" s="61">
+      <c r="C85" s="72">
+        <v>43926</v>
+      </c>
+      <c r="D85" s="73">
         <f t="shared" si="38"/>
-        <v>2</v>
-      </c>
-      <c r="E85" s="4">
-        <v>9</v>
-      </c>
-      <c r="F85" s="4">
-        <v>567</v>
-      </c>
-      <c r="G85" s="60">
+        <v>-2</v>
+      </c>
+      <c r="E85" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="F85" s="73">
+        <v>42</v>
+      </c>
+      <c r="G85" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H85" s="60">
-        <f t="shared" si="39"/>
-        <v>300</v>
-      </c>
-      <c r="I85" s="60">
+      <c r="H85" s="74">
+        <v>4</v>
+      </c>
+      <c r="I85" s="74">
         <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J85" s="61">
+        <v>296</v>
+      </c>
+      <c r="J85" s="73">
         <f t="shared" si="32"/>
         <v>31</v>
       </c>
-      <c r="K85" s="61">
+      <c r="K85" s="73">
         <f t="shared" si="33"/>
         <v>41</v>
       </c>
-      <c r="L85" s="57">
+      <c r="L85" s="72">
         <f t="shared" si="34"/>
-        <v>43971</v>
-      </c>
-      <c r="M85" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N85" s="63">
+        <v>43967</v>
+      </c>
+      <c r="M85" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N85" s="75">
         <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B86" s="57">
         <f t="shared" si="35"/>
         <v>43931</v>
       </c>
       <c r="C86" s="57"/>
       <c r="D86" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" ref="D86:D95" si="39">IF(C86="",D85,C86-B86)</f>
+        <v>-2</v>
       </c>
       <c r="E86" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" s="4">
-        <v>506</v>
+        <v>567</v>
       </c>
       <c r="G86" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H86" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="H86:H95" si="40">G86</f>
         <v>300</v>
       </c>
       <c r="I86" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="I86:I95" si="41">G86-H86</f>
         <v>0</v>
       </c>
       <c r="J86" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="J86:J95" si="42">$A$75-K86</f>
         <v>34</v>
       </c>
       <c r="K86" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="K86:K95" si="43">INT($B$97-B86)</f>
         <v>38</v>
       </c>
       <c r="L86" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" ref="L86:L95" si="44">B86+K86+D86</f>
+        <v>43967</v>
       </c>
       <c r="M86" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N86" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N86:N95" si="45">IF(M86&lt;&gt;"S",N85,N85+F86)</f>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B87" s="57">
         <f t="shared" si="35"/>
         <v>43934</v>
       </c>
       <c r="C87" s="57"/>
       <c r="D87" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E87" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F87" s="4">
-        <v>924</v>
+        <v>506</v>
       </c>
       <c r="G87" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H87" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I87" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J87" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>37</v>
       </c>
       <c r="K87" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>35</v>
       </c>
       <c r="L87" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M87" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N87" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B88" s="57">
         <f t="shared" si="35"/>
         <v>43937</v>
       </c>
       <c r="C88" s="57"/>
       <c r="D88" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E88" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F88" s="4">
-        <v>876</v>
+        <v>924</v>
       </c>
       <c r="G88" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H88" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I88" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J88" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>40</v>
       </c>
       <c r="K88" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>32</v>
       </c>
       <c r="L88" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M88" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N88" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B89" s="57">
         <f t="shared" si="35"/>
         <v>43940</v>
       </c>
       <c r="C89" s="57"/>
       <c r="D89" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E89" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F89" s="4">
-        <v>699</v>
+        <v>876</v>
       </c>
       <c r="G89" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H89" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I89" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J89" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>43</v>
       </c>
       <c r="K89" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>29</v>
       </c>
       <c r="L89" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M89" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N89" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B90" s="57">
         <f t="shared" si="35"/>
         <v>43943</v>
       </c>
       <c r="C90" s="57"/>
       <c r="D90" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E90" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F90" s="4">
-        <v>498</v>
+        <v>699</v>
       </c>
       <c r="G90" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H90" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I90" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J90" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>46</v>
       </c>
       <c r="K90" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>26</v>
       </c>
       <c r="L90" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B91" s="57">
         <f t="shared" si="35"/>
         <v>43946</v>
       </c>
       <c r="C91" s="57"/>
       <c r="D91" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E91" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F91" s="4">
-        <v>820</v>
+        <v>498</v>
       </c>
       <c r="G91" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H91" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I91" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J91" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>49</v>
       </c>
       <c r="K91" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>23</v>
       </c>
       <c r="L91" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B92" s="57">
         <f t="shared" si="35"/>
         <v>43949</v>
       </c>
       <c r="C92" s="57"/>
       <c r="D92" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E92" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F92" s="4">
-        <v>791</v>
+        <v>820</v>
       </c>
       <c r="G92" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H92" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I92" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J92" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>52</v>
       </c>
       <c r="K92" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>20</v>
       </c>
       <c r="L92" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B93" s="57">
         <f t="shared" si="35"/>
         <v>43952</v>
       </c>
       <c r="C93" s="57"/>
       <c r="D93" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E93" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F93" s="4">
-        <v>717</v>
+        <v>791</v>
       </c>
       <c r="G93" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H93" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I93" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J93" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>55</v>
       </c>
       <c r="K93" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>17</v>
       </c>
       <c r="L93" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B94" s="57">
         <f t="shared" si="35"/>
         <v>43955</v>
       </c>
       <c r="C94" s="57"/>
       <c r="D94" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
       </c>
       <c r="E94" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F94" s="4">
-        <v>827</v>
+        <v>717</v>
       </c>
       <c r="G94" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H94" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I94" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J94" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>58</v>
       </c>
       <c r="K94" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>14</v>
       </c>
       <c r="L94" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B95" s="57">
         <f t="shared" si="35"/>
         <v>43958</v>
       </c>
       <c r="C95" s="57"/>
       <c r="D95" s="61">
-        <f t="shared" si="38"/>
-        <v>2</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>53</v>
+        <f t="shared" si="39"/>
+        <v>-2</v>
+      </c>
+      <c r="E95" s="4">
+        <v>18</v>
       </c>
       <c r="F95" s="4">
-        <v>42</v>
+        <v>827</v>
       </c>
       <c r="G95" s="60">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
       <c r="H95" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>300</v>
       </c>
       <c r="I95" s="60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="J95" s="61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>61</v>
       </c>
       <c r="K95" s="61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>11</v>
       </c>
       <c r="L95" s="57">
-        <f t="shared" si="34"/>
-        <v>43971</v>
+        <f t="shared" si="44"/>
+        <v>43967</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
-        <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="45"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B96" s="65">
         <f>A81+A75-1</f>
         <v>43969</v>
@@ -10457,7 +10459,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10470,7 +10472,7 @@
         <v>300</v>
       </c>
       <c r="H96" s="60">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="H85:H96" si="46">G96</f>
         <v>300</v>
       </c>
       <c r="I96" s="60">
@@ -10487,17 +10489,17 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43971</v>
+        <v>43967</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>4620</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97"/>
       <c r="B97" s="65">
         <f>B96</f>
@@ -10516,11 +10518,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>4626</v>
+        <v>4244</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>1974</v>
+        <v>2356</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>
@@ -10531,7 +10533,7 @@
       <c r="M97" s="47"/>
       <c r="N97" s="47"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98"/>
       <c r="B98" s="65"/>
       <c r="C98" s="65"/>
@@ -10543,7 +10545,11 @@
       <c r="I98" s="47"/>
       <c r="J98" s="47"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E102" s="71"/>
+      <c r="F102" s="71"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
     </row>
@@ -10572,12 +10578,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -10585,7 +10591,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10597,7 +10603,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -10609,7 +10615,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -10621,7 +10627,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -10633,7 +10639,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -10645,7 +10651,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -10657,7 +10663,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -10669,7 +10675,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -10681,7 +10687,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -10693,7 +10699,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -10705,7 +10711,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -10717,7 +10723,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -10729,7 +10735,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -10741,7 +10747,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -10753,7 +10759,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -10765,7 +10771,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -10777,7 +10783,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -10789,7 +10795,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -10801,7 +10807,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -10813,7 +10819,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -10825,7 +10831,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -10837,7 +10843,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Inserido os arquivos restantes do capítulo 9 relativo a Debugging
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C456FAB-5E86-4DCD-A9EB-441CBBBC31AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36004EB6-585D-4810-AB14-AA9D0015A698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6314,8 +6314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9972,51 +9972,52 @@
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B86" s="57">
+      <c r="B86" s="72">
         <f t="shared" si="35"/>
         <v>43931</v>
       </c>
-      <c r="C86" s="57"/>
-      <c r="D86" s="61">
+      <c r="C86" s="72">
+        <v>43926</v>
+      </c>
+      <c r="D86" s="73">
         <f t="shared" ref="D86:D95" si="39">IF(C86="",D85,C86-B86)</f>
-        <v>-2</v>
-      </c>
-      <c r="E86" s="4">
+        <v>-5</v>
+      </c>
+      <c r="E86" s="73">
         <v>9</v>
       </c>
-      <c r="F86" s="4">
+      <c r="F86" s="73">
         <v>567</v>
       </c>
-      <c r="G86" s="60">
+      <c r="G86" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H86" s="60">
-        <f t="shared" ref="H86:H95" si="40">G86</f>
-        <v>300</v>
-      </c>
-      <c r="I86" s="60">
-        <f t="shared" ref="I86:I95" si="41">G86-H86</f>
-        <v>0</v>
-      </c>
-      <c r="J86" s="61">
-        <f t="shared" ref="J86:J95" si="42">$A$75-K86</f>
+      <c r="H86" s="74">
+        <v>225</v>
+      </c>
+      <c r="I86" s="74">
+        <f t="shared" ref="I86:I95" si="40">G86-H86</f>
+        <v>75</v>
+      </c>
+      <c r="J86" s="73">
+        <f t="shared" ref="J86:J95" si="41">$A$75-K86</f>
         <v>34</v>
       </c>
-      <c r="K86" s="61">
-        <f t="shared" ref="K86:K95" si="43">INT($B$97-B86)</f>
+      <c r="K86" s="73">
+        <f t="shared" ref="K86:K95" si="42">INT($B$97-B86)</f>
         <v>38</v>
       </c>
-      <c r="L86" s="57">
-        <f t="shared" ref="L86:L95" si="44">B86+K86+D86</f>
-        <v>43967</v>
-      </c>
-      <c r="M86" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N86" s="63">
-        <f t="shared" ref="N86:N95" si="45">IF(M86&lt;&gt;"S",N85,N85+F86)</f>
-        <v>5369</v>
+      <c r="L86" s="72">
+        <f t="shared" ref="L86:L95" si="43">B86+K86+D86</f>
+        <v>43964</v>
+      </c>
+      <c r="M86" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N86" s="75">
+        <f t="shared" ref="N86:N95" si="44">IF(M86&lt;&gt;"S",N85,N85+F86)</f>
+        <v>5936</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -10027,7 +10028,7 @@
       <c r="C87" s="57"/>
       <c r="D87" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E87" s="4">
         <v>10</v>
@@ -10040,31 +10041,31 @@
         <v>300</v>
       </c>
       <c r="H87" s="60">
+        <f t="shared" ref="H86:H95" si="45">G87</f>
+        <v>300</v>
+      </c>
+      <c r="I87" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I87" s="60">
+        <v>0</v>
+      </c>
+      <c r="J87" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J87" s="61">
+        <v>37</v>
+      </c>
+      <c r="K87" s="61">
         <f t="shared" si="42"/>
-        <v>37</v>
-      </c>
-      <c r="K87" s="61">
+        <v>35</v>
+      </c>
+      <c r="L87" s="57">
         <f t="shared" si="43"/>
-        <v>35</v>
-      </c>
-      <c r="L87" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M87" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N87" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -10075,7 +10076,7 @@
       <c r="C88" s="57"/>
       <c r="D88" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E88" s="4">
         <v>11</v>
@@ -10088,31 +10089,31 @@
         <v>300</v>
       </c>
       <c r="H88" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I88" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I88" s="60">
+        <v>0</v>
+      </c>
+      <c r="J88" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J88" s="61">
+        <v>40</v>
+      </c>
+      <c r="K88" s="61">
         <f t="shared" si="42"/>
-        <v>40</v>
-      </c>
-      <c r="K88" s="61">
+        <v>32</v>
+      </c>
+      <c r="L88" s="57">
         <f t="shared" si="43"/>
-        <v>32</v>
-      </c>
-      <c r="L88" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M88" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N88" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -10123,7 +10124,7 @@
       <c r="C89" s="57"/>
       <c r="D89" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E89" s="4">
         <v>12</v>
@@ -10136,31 +10137,31 @@
         <v>300</v>
       </c>
       <c r="H89" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I89" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I89" s="60">
+        <v>0</v>
+      </c>
+      <c r="J89" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J89" s="61">
+        <v>43</v>
+      </c>
+      <c r="K89" s="61">
         <f t="shared" si="42"/>
-        <v>43</v>
-      </c>
-      <c r="K89" s="61">
+        <v>29</v>
+      </c>
+      <c r="L89" s="57">
         <f t="shared" si="43"/>
-        <v>29</v>
-      </c>
-      <c r="L89" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M89" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N89" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -10171,7 +10172,7 @@
       <c r="C90" s="57"/>
       <c r="D90" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E90" s="4">
         <v>13</v>
@@ -10184,31 +10185,31 @@
         <v>300</v>
       </c>
       <c r="H90" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I90" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I90" s="60">
+        <v>0</v>
+      </c>
+      <c r="J90" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J90" s="61">
+        <v>46</v>
+      </c>
+      <c r="K90" s="61">
         <f t="shared" si="42"/>
-        <v>46</v>
-      </c>
-      <c r="K90" s="61">
+        <v>26</v>
+      </c>
+      <c r="L90" s="57">
         <f t="shared" si="43"/>
-        <v>26</v>
-      </c>
-      <c r="L90" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -10219,7 +10220,7 @@
       <c r="C91" s="57"/>
       <c r="D91" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E91" s="4">
         <v>14</v>
@@ -10232,31 +10233,31 @@
         <v>300</v>
       </c>
       <c r="H91" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I91" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I91" s="60">
+        <v>0</v>
+      </c>
+      <c r="J91" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J91" s="61">
+        <v>49</v>
+      </c>
+      <c r="K91" s="61">
         <f t="shared" si="42"/>
-        <v>49</v>
-      </c>
-      <c r="K91" s="61">
+        <v>23</v>
+      </c>
+      <c r="L91" s="57">
         <f t="shared" si="43"/>
-        <v>23</v>
-      </c>
-      <c r="L91" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -10267,7 +10268,7 @@
       <c r="C92" s="57"/>
       <c r="D92" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E92" s="4">
         <v>15</v>
@@ -10280,31 +10281,31 @@
         <v>300</v>
       </c>
       <c r="H92" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I92" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I92" s="60">
+        <v>0</v>
+      </c>
+      <c r="J92" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J92" s="61">
+        <v>52</v>
+      </c>
+      <c r="K92" s="61">
         <f t="shared" si="42"/>
-        <v>52</v>
-      </c>
-      <c r="K92" s="61">
+        <v>20</v>
+      </c>
+      <c r="L92" s="57">
         <f t="shared" si="43"/>
-        <v>20</v>
-      </c>
-      <c r="L92" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -10315,7 +10316,7 @@
       <c r="C93" s="57"/>
       <c r="D93" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E93" s="4">
         <v>16</v>
@@ -10328,31 +10329,31 @@
         <v>300</v>
       </c>
       <c r="H93" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I93" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I93" s="60">
+        <v>0</v>
+      </c>
+      <c r="J93" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="61">
+        <v>55</v>
+      </c>
+      <c r="K93" s="61">
         <f t="shared" si="42"/>
-        <v>55</v>
-      </c>
-      <c r="K93" s="61">
+        <v>17</v>
+      </c>
+      <c r="L93" s="57">
         <f t="shared" si="43"/>
-        <v>17</v>
-      </c>
-      <c r="L93" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -10363,7 +10364,7 @@
       <c r="C94" s="57"/>
       <c r="D94" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E94" s="4">
         <v>17</v>
@@ -10376,31 +10377,31 @@
         <v>300</v>
       </c>
       <c r="H94" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I94" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I94" s="60">
+        <v>0</v>
+      </c>
+      <c r="J94" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J94" s="61">
+        <v>58</v>
+      </c>
+      <c r="K94" s="61">
         <f t="shared" si="42"/>
-        <v>58</v>
-      </c>
-      <c r="K94" s="61">
+        <v>14</v>
+      </c>
+      <c r="L94" s="57">
         <f t="shared" si="43"/>
-        <v>14</v>
-      </c>
-      <c r="L94" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -10411,7 +10412,7 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="39"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E95" s="4">
         <v>18</v>
@@ -10424,31 +10425,31 @@
         <v>300</v>
       </c>
       <c r="H95" s="60">
+        <f t="shared" si="45"/>
+        <v>300</v>
+      </c>
+      <c r="I95" s="60">
         <f t="shared" si="40"/>
-        <v>300</v>
-      </c>
-      <c r="I95" s="60">
+        <v>0</v>
+      </c>
+      <c r="J95" s="61">
         <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="J95" s="61">
+        <v>61</v>
+      </c>
+      <c r="K95" s="61">
         <f t="shared" si="42"/>
-        <v>61</v>
-      </c>
-      <c r="K95" s="61">
+        <v>11</v>
+      </c>
+      <c r="L95" s="57">
         <f t="shared" si="43"/>
-        <v>11</v>
-      </c>
-      <c r="L95" s="57">
-        <f t="shared" si="44"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
-        <f t="shared" si="45"/>
-        <v>5369</v>
+        <f t="shared" si="44"/>
+        <v>5936</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -10459,7 +10460,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10489,14 +10490,14 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>5369</v>
+        <v>5936</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -10518,11 +10519,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>4244</v>
+        <v>4169</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>2356</v>
+        <v>2431</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>

</xml_diff>

<commit_message>
Inseridos os arquivos referentes aos capítulos 11 e 12, web scraping e trabalhando com planilhas do excel, respectivamente
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36004EB6-585D-4810-AB14-AA9D0015A698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93557A5E-8A72-46E3-8265-D46D0754C4D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="1110" windowWidth="19215" windowHeight="10410" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -6314,8 +6314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89:N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10021,147 +10021,150 @@
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B87" s="57">
+      <c r="B87" s="72">
         <f t="shared" si="35"/>
         <v>43934</v>
       </c>
-      <c r="C87" s="57"/>
-      <c r="D87" s="61">
+      <c r="C87" s="72">
+        <v>43927</v>
+      </c>
+      <c r="D87" s="73">
         <f t="shared" si="39"/>
-        <v>-5</v>
-      </c>
-      <c r="E87" s="4">
+        <v>-7</v>
+      </c>
+      <c r="E87" s="73">
         <v>10</v>
       </c>
-      <c r="F87" s="4">
+      <c r="F87" s="73">
         <v>506</v>
       </c>
-      <c r="G87" s="60">
+      <c r="G87" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H87" s="60">
-        <f t="shared" ref="H86:H95" si="45">G87</f>
-        <v>300</v>
-      </c>
-      <c r="I87" s="60">
+      <c r="H87" s="74">
+        <v>112</v>
+      </c>
+      <c r="I87" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J87" s="61">
+        <v>188</v>
+      </c>
+      <c r="J87" s="73">
         <f t="shared" si="41"/>
         <v>37</v>
       </c>
-      <c r="K87" s="61">
+      <c r="K87" s="73">
         <f t="shared" si="42"/>
         <v>35</v>
       </c>
-      <c r="L87" s="57">
+      <c r="L87" s="72">
         <f t="shared" si="43"/>
-        <v>43964</v>
-      </c>
-      <c r="M87" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N87" s="63">
+        <v>43962</v>
+      </c>
+      <c r="M87" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N87" s="75">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>6442</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B88" s="57">
+      <c r="B88" s="72">
         <f t="shared" si="35"/>
         <v>43937</v>
       </c>
-      <c r="C88" s="57"/>
-      <c r="D88" s="61">
+      <c r="C88" s="72">
+        <v>43928</v>
+      </c>
+      <c r="D88" s="73">
         <f t="shared" si="39"/>
-        <v>-5</v>
-      </c>
-      <c r="E88" s="4">
+        <v>-9</v>
+      </c>
+      <c r="E88" s="73">
         <v>11</v>
       </c>
-      <c r="F88" s="4">
+      <c r="F88" s="73">
         <v>924</v>
       </c>
-      <c r="G88" s="60">
+      <c r="G88" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H88" s="60">
-        <f t="shared" si="45"/>
-        <v>300</v>
-      </c>
-      <c r="I88" s="60">
+      <c r="H88" s="74">
+        <v>370</v>
+      </c>
+      <c r="I88" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J88" s="61">
+        <v>-70</v>
+      </c>
+      <c r="J88" s="73">
         <f t="shared" si="41"/>
         <v>40</v>
       </c>
-      <c r="K88" s="61">
+      <c r="K88" s="73">
         <f t="shared" si="42"/>
         <v>32</v>
       </c>
-      <c r="L88" s="57">
+      <c r="L88" s="72">
         <f t="shared" si="43"/>
-        <v>43964</v>
-      </c>
-      <c r="M88" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N88" s="63">
+        <v>43960</v>
+      </c>
+      <c r="M88" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N88" s="75">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>7366</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B89" s="57">
+      <c r="B89" s="72">
         <f t="shared" si="35"/>
         <v>43940</v>
       </c>
-      <c r="C89" s="57"/>
-      <c r="D89" s="61">
+      <c r="C89" s="72">
+        <v>43928</v>
+      </c>
+      <c r="D89" s="73">
         <f t="shared" si="39"/>
-        <v>-5</v>
-      </c>
-      <c r="E89" s="4">
+        <v>-12</v>
+      </c>
+      <c r="E89" s="73">
         <v>12</v>
       </c>
-      <c r="F89" s="4">
+      <c r="F89" s="73">
         <v>876</v>
       </c>
-      <c r="G89" s="60">
+      <c r="G89" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H89" s="60">
-        <f t="shared" si="45"/>
-        <v>300</v>
-      </c>
-      <c r="I89" s="60">
+      <c r="H89" s="74">
+        <v>278</v>
+      </c>
+      <c r="I89" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J89" s="61">
+        <v>22</v>
+      </c>
+      <c r="J89" s="73">
         <f t="shared" si="41"/>
         <v>43</v>
       </c>
-      <c r="K89" s="61">
+      <c r="K89" s="73">
         <f t="shared" si="42"/>
         <v>29</v>
       </c>
-      <c r="L89" s="57">
+      <c r="L89" s="72">
         <f t="shared" si="43"/>
-        <v>43964</v>
-      </c>
-      <c r="M89" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N89" s="63">
+        <v>43957</v>
+      </c>
+      <c r="M89" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N89" s="75">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -10172,7 +10175,7 @@
       <c r="C90" s="57"/>
       <c r="D90" s="61">
         <f t="shared" si="39"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E90" s="4">
         <v>13</v>
@@ -10185,7 +10188,7 @@
         <v>300</v>
       </c>
       <c r="H90" s="60">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="H89:H95" si="45">G90</f>
         <v>300</v>
       </c>
       <c r="I90" s="60">
@@ -10202,14 +10205,14 @@
       </c>
       <c r="L90" s="57">
         <f t="shared" si="43"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M90" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N90" s="63">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -10220,7 +10223,7 @@
       <c r="C91" s="57"/>
       <c r="D91" s="61">
         <f t="shared" si="39"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E91" s="4">
         <v>14</v>
@@ -10250,14 +10253,14 @@
       </c>
       <c r="L91" s="57">
         <f t="shared" si="43"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M91" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N91" s="63">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -10268,7 +10271,7 @@
       <c r="C92" s="57"/>
       <c r="D92" s="61">
         <f t="shared" si="39"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E92" s="4">
         <v>15</v>
@@ -10298,14 +10301,14 @@
       </c>
       <c r="L92" s="57">
         <f t="shared" si="43"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M92" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N92" s="63">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -10316,7 +10319,7 @@
       <c r="C93" s="57"/>
       <c r="D93" s="61">
         <f t="shared" si="39"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E93" s="4">
         <v>16</v>
@@ -10346,14 +10349,14 @@
       </c>
       <c r="L93" s="57">
         <f t="shared" si="43"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M93" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N93" s="63">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -10364,7 +10367,7 @@
       <c r="C94" s="57"/>
       <c r="D94" s="61">
         <f t="shared" si="39"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E94" s="4">
         <v>17</v>
@@ -10394,14 +10397,14 @@
       </c>
       <c r="L94" s="57">
         <f t="shared" si="43"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M94" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N94" s="63">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -10412,7 +10415,7 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="39"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E95" s="4">
         <v>18</v>
@@ -10442,14 +10445,14 @@
       </c>
       <c r="L95" s="57">
         <f t="shared" si="43"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
         <f t="shared" si="44"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -10460,7 +10463,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10473,7 +10476,7 @@
         <v>300</v>
       </c>
       <c r="H96" s="60">
-        <f t="shared" ref="H85:H96" si="46">G96</f>
+        <f t="shared" ref="H96" si="46">G96</f>
         <v>300</v>
       </c>
       <c r="I96" s="60">
@@ -10490,14 +10493,14 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43964</v>
+        <v>43957</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>5936</v>
+        <v>8242</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -10519,11 +10522,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>4169</v>
+        <v>4029</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>2431</v>
+        <v>2571</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>

</xml_diff>

<commit_message>
Inseridos os arquivos implementados do capítulo 17, sobre imagens
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93557A5E-8A72-46E3-8265-D46D0754C4D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23285794-08E3-44E3-8F62-A8878DB8A7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1110" windowWidth="19215" windowHeight="10410" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -1113,21 +1113,21 @@
       <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="27.42578125" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1"/>
+    <col min="4" max="4" width="15.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1487,7 +1487,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1601,7 +1601,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -1972,7 +1972,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -2210,7 +2210,7 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -2227,7 +2227,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -2465,7 +2465,7 @@
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -2499,7 +2499,7 @@
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -2550,7 +2550,7 @@
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -2601,7 +2601,7 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -2652,7 +2652,7 @@
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -2720,7 +2720,7 @@
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -2771,7 +2771,7 @@
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -2839,7 +2839,7 @@
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -2856,7 +2856,7 @@
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -2873,7 +2873,7 @@
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -2890,7 +2890,7 @@
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -2941,7 +2941,7 @@
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -2958,7 +2958,7 @@
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -3043,7 +3043,7 @@
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -3077,7 +3077,7 @@
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -3111,7 +3111,7 @@
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -3145,7 +3145,7 @@
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -3179,7 +3179,7 @@
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -3213,7 +3213,7 @@
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -3230,7 +3230,7 @@
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -3247,7 +3247,7 @@
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -3281,7 +3281,7 @@
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -3315,7 +3315,7 @@
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -3349,7 +3349,7 @@
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -3400,7 +3400,7 @@
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -3417,7 +3417,7 @@
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -3434,7 +3434,7 @@
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -3451,7 +3451,7 @@
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -3485,7 +3485,7 @@
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -3502,7 +3502,7 @@
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -3570,7 +3570,7 @@
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -3604,7 +3604,7 @@
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -3621,7 +3621,7 @@
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -3672,7 +3672,7 @@
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -3774,7 +3774,7 @@
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -3808,7 +3808,7 @@
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -3825,7 +3825,7 @@
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -3859,7 +3859,7 @@
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="J157" s="15"/>
       <c r="K157" s="15"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -3893,7 +3893,7 @@
       <c r="J158" s="15"/>
       <c r="K158" s="15"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="J159" s="15"/>
       <c r="K159" s="15"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -3927,7 +3927,7 @@
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="J161" s="15"/>
       <c r="K161" s="15"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="J162" s="15"/>
       <c r="K162" s="15"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -3978,7 +3978,7 @@
       <c r="J163" s="15"/>
       <c r="K163" s="15"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -3995,7 +3995,7 @@
       <c r="J164" s="15"/>
       <c r="K164" s="15"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -4012,7 +4012,7 @@
       <c r="J165" s="15"/>
       <c r="K165" s="15"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -4029,7 +4029,7 @@
       <c r="J166" s="15"/>
       <c r="K166" s="15"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="J167" s="15"/>
       <c r="K167" s="15"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="J168" s="15"/>
       <c r="K168" s="15"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -4080,7 +4080,7 @@
       <c r="J169" s="15"/>
       <c r="K169" s="15"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -4097,7 +4097,7 @@
       <c r="J170" s="15"/>
       <c r="K170" s="15"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -4114,7 +4114,7 @@
       <c r="J171" s="15"/>
       <c r="K171" s="15"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="J172" s="15"/>
       <c r="K172" s="15"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>172</v>
       </c>
@@ -4148,7 +4148,7 @@
       <c r="J173" s="15"/>
       <c r="K173" s="15"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -4165,7 +4165,7 @@
       <c r="J174" s="15"/>
       <c r="K174" s="15"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="J175" s="15"/>
       <c r="K175" s="15"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="J176" s="15"/>
       <c r="K176" s="15"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -4216,7 +4216,7 @@
       <c r="J177" s="15"/>
       <c r="K177" s="15"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="J178" s="15"/>
       <c r="K178" s="15"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>178</v>
       </c>
@@ -4250,7 +4250,7 @@
       <c r="J179" s="15"/>
       <c r="K179" s="15"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>179</v>
       </c>
@@ -4267,7 +4267,7 @@
       <c r="J180" s="15"/>
       <c r="K180" s="15"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>180</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="J181" s="15"/>
       <c r="K181" s="15"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>181</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="J182" s="15"/>
       <c r="K182" s="15"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>182</v>
       </c>
@@ -4318,7 +4318,7 @@
       <c r="J183" s="15"/>
       <c r="K183" s="15"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>183</v>
       </c>
@@ -4335,7 +4335,7 @@
       <c r="J184" s="15"/>
       <c r="K184" s="15"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>184</v>
       </c>
@@ -4352,7 +4352,7 @@
       <c r="J185" s="15"/>
       <c r="K185" s="15"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>185</v>
       </c>
@@ -4369,7 +4369,7 @@
       <c r="J186" s="15"/>
       <c r="K186" s="15"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>186</v>
       </c>
@@ -4386,7 +4386,7 @@
       <c r="J187" s="15"/>
       <c r="K187" s="15"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>187</v>
       </c>
@@ -4403,7 +4403,7 @@
       <c r="J188" s="15"/>
       <c r="K188" s="15"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>188</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="J189" s="15"/>
       <c r="K189" s="15"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>189</v>
       </c>
@@ -4437,7 +4437,7 @@
       <c r="J190" s="15"/>
       <c r="K190" s="15"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>190</v>
       </c>
@@ -4454,7 +4454,7 @@
       <c r="J191" s="15"/>
       <c r="K191" s="15"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>191</v>
       </c>
@@ -4471,7 +4471,7 @@
       <c r="J192" s="15"/>
       <c r="K192" s="15"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>192</v>
       </c>
@@ -4488,7 +4488,7 @@
       <c r="J193" s="15"/>
       <c r="K193" s="15"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>193</v>
       </c>
@@ -4505,7 +4505,7 @@
       <c r="J194" s="15"/>
       <c r="K194" s="15"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>194</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="J195" s="15"/>
       <c r="K195" s="15"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>195</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="J196" s="15"/>
       <c r="K196" s="15"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>196</v>
       </c>
@@ -4556,7 +4556,7 @@
       <c r="J197" s="15"/>
       <c r="K197" s="15"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>197</v>
       </c>
@@ -4573,7 +4573,7 @@
       <c r="J198" s="15"/>
       <c r="K198" s="15"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>198</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="J199" s="15"/>
       <c r="K199" s="15"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>199</v>
       </c>
@@ -4607,7 +4607,7 @@
       <c r="J200" s="15"/>
       <c r="K200" s="15"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>200</v>
       </c>
@@ -4624,7 +4624,7 @@
       <c r="J201" s="15"/>
       <c r="K201" s="15"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>201</v>
       </c>
@@ -4641,7 +4641,7 @@
       <c r="J202" s="15"/>
       <c r="K202" s="15"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>202</v>
       </c>
@@ -4658,7 +4658,7 @@
       <c r="J203" s="15"/>
       <c r="K203" s="15"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>203</v>
       </c>
@@ -4675,7 +4675,7 @@
       <c r="J204" s="15"/>
       <c r="K204" s="15"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>12</v>
       </c>
@@ -4734,16 +4734,16 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12 1025:1025" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12 1025:1025" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="AMK1"/>
     </row>
-    <row r="2" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>0</v>
       </c>
@@ -4801,7 +4801,7 @@
       </c>
       <c r="L2" s="85"/>
     </row>
-    <row r="3" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="L3" s="85"/>
     </row>
-    <row r="4" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76">
         <v>2</v>
       </c>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="L4" s="86"/>
     </row>
-    <row r="5" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="76">
         <v>3</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="J5" s="91"/>
       <c r="L5" s="86"/>
     </row>
-    <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="76">
         <v>4</v>
       </c>
@@ -4917,7 +4917,7 @@
       <c r="J6" s="91"/>
       <c r="L6" s="86"/>
     </row>
-    <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79">
         <v>5</v>
       </c>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="L7" s="87"/>
     </row>
-    <row r="8" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="79">
         <v>6</v>
       </c>
@@ -4975,7 +4975,7 @@
       <c r="J8" s="93"/>
       <c r="L8" s="87"/>
     </row>
-    <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="82">
         <v>7</v>
       </c>
@@ -5007,7 +5007,7 @@
       </c>
       <c r="L9" s="88"/>
     </row>
-    <row r="10" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82">
         <v>8</v>
       </c>
@@ -5033,7 +5033,7 @@
       <c r="J10" s="95"/>
       <c r="L10" s="88"/>
     </row>
-    <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="B11" s="17">
         <f>SUM(B2:B10)</f>
         <v>341</v>
@@ -5055,22 +5055,22 @@
         <v>44069</v>
       </c>
     </row>
-    <row r="13" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="A14" s="85">
         <v>43864</v>
       </c>
     </row>
-    <row r="15" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="D15" s="85">
         <v>43869</v>
       </c>
     </row>
-    <row r="16" spans="1:12 1025:1025" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
       <c r="D16" s="85">
         <f>D15+D11</f>
         <v>44074</v>
@@ -5102,62 +5102,62 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="15" width="7.140625" customWidth="1"/>
-    <col min="16" max="24" width="6.7109375" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" customWidth="1"/>
-    <col min="26" max="26" width="7.5703125" customWidth="1"/>
-    <col min="27" max="30" width="7.7109375" customWidth="1"/>
-    <col min="31" max="34" width="10.85546875" customWidth="1"/>
-    <col min="35" max="43" width="6.7109375" customWidth="1"/>
-    <col min="44" max="44" width="7.7109375" customWidth="1"/>
-    <col min="45" max="45" width="7.5703125" customWidth="1"/>
-    <col min="46" max="65" width="7.7109375" customWidth="1"/>
-    <col min="66" max="74" width="6.140625" customWidth="1"/>
-    <col min="75" max="75" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="11" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="15" width="7.109375" customWidth="1"/>
+    <col min="16" max="24" width="6.6640625" customWidth="1"/>
+    <col min="25" max="25" width="7.6640625" customWidth="1"/>
+    <col min="26" max="26" width="7.5546875" customWidth="1"/>
+    <col min="27" max="30" width="7.6640625" customWidth="1"/>
+    <col min="31" max="34" width="10.88671875" customWidth="1"/>
+    <col min="35" max="43" width="6.6640625" customWidth="1"/>
+    <col min="44" max="44" width="7.6640625" customWidth="1"/>
+    <col min="45" max="45" width="7.5546875" customWidth="1"/>
+    <col min="46" max="65" width="7.6640625" customWidth="1"/>
+    <col min="66" max="74" width="6.109375" customWidth="1"/>
+    <col min="75" max="75" width="7.109375" customWidth="1"/>
     <col min="76" max="76" width="7" customWidth="1"/>
-    <col min="77" max="95" width="7.140625" customWidth="1"/>
-    <col min="96" max="104" width="6.5703125" customWidth="1"/>
-    <col min="105" max="105" width="7.5703125" customWidth="1"/>
-    <col min="106" max="106" width="7.42578125" customWidth="1"/>
-    <col min="107" max="126" width="7.5703125" customWidth="1"/>
+    <col min="77" max="95" width="7.109375" customWidth="1"/>
+    <col min="96" max="104" width="6.5546875" customWidth="1"/>
+    <col min="105" max="105" width="7.5546875" customWidth="1"/>
+    <col min="106" max="106" width="7.44140625" customWidth="1"/>
+    <col min="107" max="126" width="7.5546875" customWidth="1"/>
     <col min="127" max="135" width="6" customWidth="1"/>
     <col min="136" max="136" width="7" customWidth="1"/>
-    <col min="137" max="137" width="6.85546875" customWidth="1"/>
+    <col min="137" max="137" width="6.88671875" customWidth="1"/>
     <col min="138" max="156" width="7" customWidth="1"/>
-    <col min="157" max="165" width="5.42578125" customWidth="1"/>
-    <col min="166" max="166" width="6.42578125" customWidth="1"/>
-    <col min="167" max="167" width="6.28515625" customWidth="1"/>
-    <col min="168" max="187" width="6.42578125" customWidth="1"/>
-    <col min="188" max="196" width="6.5703125" customWidth="1"/>
-    <col min="197" max="197" width="7.5703125" customWidth="1"/>
-    <col min="198" max="198" width="7.42578125" customWidth="1"/>
-    <col min="199" max="218" width="7.5703125" customWidth="1"/>
-    <col min="219" max="227" width="6.140625" customWidth="1"/>
-    <col min="228" max="228" width="7.140625" customWidth="1"/>
+    <col min="157" max="165" width="5.44140625" customWidth="1"/>
+    <col min="166" max="166" width="6.44140625" customWidth="1"/>
+    <col min="167" max="167" width="6.33203125" customWidth="1"/>
+    <col min="168" max="187" width="6.44140625" customWidth="1"/>
+    <col min="188" max="196" width="6.5546875" customWidth="1"/>
+    <col min="197" max="197" width="7.5546875" customWidth="1"/>
+    <col min="198" max="198" width="7.44140625" customWidth="1"/>
+    <col min="199" max="218" width="7.5546875" customWidth="1"/>
+    <col min="219" max="227" width="6.109375" customWidth="1"/>
+    <col min="228" max="228" width="7.109375" customWidth="1"/>
     <col min="229" max="229" width="7" customWidth="1"/>
-    <col min="230" max="248" width="7.140625" customWidth="1"/>
-    <col min="249" max="257" width="6.140625" customWidth="1"/>
-    <col min="258" max="258" width="7.140625" customWidth="1"/>
+    <col min="230" max="248" width="7.109375" customWidth="1"/>
+    <col min="249" max="257" width="6.109375" customWidth="1"/>
+    <col min="258" max="258" width="7.109375" customWidth="1"/>
     <col min="259" max="259" width="7" customWidth="1"/>
-    <col min="260" max="279" width="7.140625" customWidth="1"/>
-    <col min="280" max="288" width="6.5703125" customWidth="1"/>
-    <col min="289" max="289" width="7.5703125" customWidth="1"/>
-    <col min="290" max="290" width="7.42578125" customWidth="1"/>
-    <col min="291" max="309" width="7.5703125" customWidth="1"/>
-    <col min="310" max="318" width="6.5703125" customWidth="1"/>
-    <col min="319" max="319" width="7.5703125" customWidth="1"/>
-    <col min="320" max="320" width="7.42578125" customWidth="1"/>
-    <col min="321" max="340" width="7.5703125" customWidth="1"/>
+    <col min="260" max="279" width="7.109375" customWidth="1"/>
+    <col min="280" max="288" width="6.5546875" customWidth="1"/>
+    <col min="289" max="289" width="7.5546875" customWidth="1"/>
+    <col min="290" max="290" width="7.44140625" customWidth="1"/>
+    <col min="291" max="309" width="7.5546875" customWidth="1"/>
+    <col min="310" max="318" width="6.5546875" customWidth="1"/>
+    <col min="319" max="319" width="7.5546875" customWidth="1"/>
+    <col min="320" max="320" width="7.44140625" customWidth="1"/>
+    <col min="321" max="340" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A1" s="24">
         <v>43857</v>
       </c>
@@ -6179,7 +6179,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="2" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:340" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>19</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:340" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
         <v>19</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:340" x14ac:dyDescent="0.25">
       <c r="D5" s="25" t="s">
         <v>19</v>
       </c>
@@ -6235,67 +6235,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:340" x14ac:dyDescent="0.25">
       <c r="E6" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:340" x14ac:dyDescent="0.25">
       <c r="F7" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:340" x14ac:dyDescent="0.25">
       <c r="G8" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:340" x14ac:dyDescent="0.25">
       <c r="H9" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:340" x14ac:dyDescent="0.25">
       <c r="I10" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:340" x14ac:dyDescent="0.25">
       <c r="J11" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:340" x14ac:dyDescent="0.25">
       <c r="K12" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:340" x14ac:dyDescent="0.25">
       <c r="L13" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:340" x14ac:dyDescent="0.25">
       <c r="M14" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:340" x14ac:dyDescent="0.25">
       <c r="N15" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:340" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:340" x14ac:dyDescent="0.25">
       <c r="O16" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P17" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="16:17" x14ac:dyDescent="0.25">
       <c r="Q18" s="25" t="s">
         <v>16</v>
       </c>
@@ -6315,28 +6315,28 @@
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89:N89"/>
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
         <v>21</v>
       </c>
@@ -6350,7 +6350,7 @@
       <c r="L1" s="98"/>
       <c r="M1" s="98"/>
     </row>
-    <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>14</v>
@@ -6408,7 +6408,7 @@
       <c r="L3" s="34"/>
       <c r="M3" s="34"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>52</v>
@@ -6425,7 +6425,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>46</v>
@@ -6442,7 +6442,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>26</v>
@@ -6459,7 +6459,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="34"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <f>180+26</f>
@@ -6477,7 +6477,7 @@
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4">
         <f>60+41</f>
@@ -6495,7 +6495,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4">
         <f>60+22</f>
@@ -6513,7 +6513,7 @@
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4">
         <v>43</v>
@@ -6530,7 +6530,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>43869</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>43885</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>43870</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>43886</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>43873</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>43888</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>43873</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>43887</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>43880</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>43882</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>43886</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>43887</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>43895</v>
       </c>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>43887</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>43889</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>43891</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>43892</v>
       </c>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>43891</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A23" s="45">
         <f>A11+(D23-D11)</f>
         <v>43891</v>
@@ -7175,7 +7175,7 @@
       <c r="H23" s="47"/>
       <c r="I23" s="47"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
@@ -7186,13 +7186,13 @@
       <c r="H24" s="47"/>
       <c r="I24" s="47"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A25" s="99" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="99"/>
     </row>
-    <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>36</v>
       </c>
@@ -7240,7 +7240,7 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49">
         <v>72</v>
       </c>
@@ -7295,7 +7295,7 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>47</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A29" s="55">
         <f>ROUND(A27/A35,0)</f>
         <v>3</v>
@@ -7400,7 +7400,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>48</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A31" s="56">
         <f>A37*A29</f>
         <v>300</v>
@@ -7505,7 +7505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>50</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="64">
         <v>43898</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>51</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>21</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>52</v>
       </c>
@@ -7760,7 +7760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>100</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="57">
         <f t="shared" si="17"/>
         <v>43931</v>
@@ -7859,7 +7859,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="57">
         <f t="shared" si="17"/>
         <v>43934</v>
@@ -7907,7 +7907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="57">
         <f t="shared" si="17"/>
         <v>43937</v>
@@ -7955,7 +7955,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="57">
         <f t="shared" si="17"/>
         <v>43940</v>
@@ -8003,7 +8003,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="57">
         <f t="shared" si="17"/>
         <v>43943</v>
@@ -8051,7 +8051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="57">
         <f t="shared" si="17"/>
         <v>43946</v>
@@ -8099,7 +8099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="57">
         <f t="shared" si="17"/>
         <v>43949</v>
@@ -8147,7 +8147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="57">
         <f t="shared" si="17"/>
         <v>43952</v>
@@ -8195,7 +8195,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="57">
         <f t="shared" si="17"/>
         <v>43955</v>
@@ -8243,7 +8243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" s="65">
         <f>A33+A27-1</f>
         <v>43969</v>
@@ -8291,7 +8291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48" s="65">
         <f>B47</f>
@@ -8325,7 +8325,7 @@
       <c r="M48" s="47"/>
       <c r="N48" s="47"/>
     </row>
-    <row r="49" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49" s="65"/>
       <c r="C49" s="65"/>
@@ -8339,14 +8339,14 @@
       <c r="K49" s="47"/>
       <c r="L49" s="47"/>
     </row>
-    <row r="51" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A51" s="99" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="99"/>
       <c r="C51" s="99"/>
     </row>
-    <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>36</v>
       </c>
@@ -8394,7 +8394,7 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49">
         <v>72</v>
       </c>
@@ -8449,7 +8449,7 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>47</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A55" s="55">
         <f>ROUND(A53/A61,0)</f>
         <v>4</v>
@@ -8554,7 +8554,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>48</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A57" s="56">
         <f>A63*A55</f>
         <v>400</v>
@@ -8658,7 +8658,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>50</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A59" s="64">
         <v>43898</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>51</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>18</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>52</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>100</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B64" s="57">
         <f t="shared" si="25"/>
         <v>43942</v>
@@ -9012,7 +9012,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B65" s="57">
         <f t="shared" si="25"/>
         <v>43946</v>
@@ -9060,7 +9060,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B66" s="57">
         <f t="shared" si="25"/>
         <v>43950</v>
@@ -9108,7 +9108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B67" s="57">
         <f t="shared" si="25"/>
         <v>43954</v>
@@ -9156,7 +9156,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B68" s="57">
         <f t="shared" si="25"/>
         <v>43958</v>
@@ -9204,7 +9204,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B69" s="57">
         <f t="shared" si="25"/>
         <v>43962</v>
@@ -9252,7 +9252,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B70" s="65">
         <f>A59+A53-1</f>
         <v>43969</v>
@@ -9300,7 +9300,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71" s="65">
         <f>B70</f>
@@ -9334,11 +9334,11 @@
       <c r="M71" s="71"/>
       <c r="N71" s="71"/>
     </row>
-    <row r="72" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="K72" s="71"/>
       <c r="L72" s="71"/>
     </row>
-    <row r="73" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A73" s="99" t="s">
         <v>18</v>
       </c>
@@ -9346,7 +9346,7 @@
       <c r="K73" s="71"/>
       <c r="L73" s="71"/>
     </row>
-    <row r="74" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>36</v>
       </c>
@@ -9394,7 +9394,7 @@
       <c r="AMI74"/>
       <c r="AMJ74"/>
     </row>
-    <row r="75" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1024" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49">
         <v>72</v>
       </c>
@@ -9449,7 +9449,7 @@
       <c r="AMI75"/>
       <c r="AMJ75"/>
     </row>
-    <row r="76" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>47</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="77" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A77" s="55">
         <f>ROUND(A75/A83,0)</f>
         <v>3</v>
@@ -9554,7 +9554,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="78" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>48</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="79" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A79" s="56">
         <f>A85*A77</f>
         <v>300</v>
@@ -9659,7 +9659,7 @@
         <v>2612</v>
       </c>
     </row>
-    <row r="80" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>50</v>
       </c>
@@ -9711,7 +9711,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="64">
         <v>43898</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>51</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>23</v>
       </c>
@@ -9867,7 +9867,7 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>52</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>5327</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>100</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>5369</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B86" s="72">
         <f t="shared" si="35"/>
         <v>43931</v>
@@ -10020,7 +10020,7 @@
         <v>5936</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B87" s="72">
         <f t="shared" si="35"/>
         <v>43934</v>
@@ -10069,7 +10069,7 @@
         <v>6442</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B88" s="72">
         <f t="shared" si="35"/>
         <v>43937</v>
@@ -10118,7 +10118,7 @@
         <v>7366</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B89" s="72">
         <f t="shared" si="35"/>
         <v>43940</v>
@@ -10167,247 +10167,252 @@
         <v>8242</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B90" s="57">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B90" s="72">
         <f t="shared" si="35"/>
         <v>43943</v>
       </c>
-      <c r="C90" s="57"/>
-      <c r="D90" s="61">
+      <c r="C90" s="72">
+        <v>43929</v>
+      </c>
+      <c r="D90" s="73">
         <f t="shared" si="39"/>
-        <v>-12</v>
-      </c>
-      <c r="E90" s="4">
+        <v>-14</v>
+      </c>
+      <c r="E90" s="73">
         <v>13</v>
       </c>
-      <c r="F90" s="4">
+      <c r="F90" s="73">
         <v>699</v>
       </c>
-      <c r="G90" s="60">
+      <c r="G90" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H90" s="60">
-        <f t="shared" ref="H89:H95" si="45">G90</f>
-        <v>300</v>
-      </c>
-      <c r="I90" s="60">
+      <c r="H90" s="74">
+        <v>140</v>
+      </c>
+      <c r="I90" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J90" s="61">
+        <v>160</v>
+      </c>
+      <c r="J90" s="73">
         <f t="shared" si="41"/>
         <v>46</v>
       </c>
-      <c r="K90" s="61">
+      <c r="K90" s="73">
         <f t="shared" si="42"/>
         <v>26</v>
       </c>
-      <c r="L90" s="57">
+      <c r="L90" s="72">
         <f t="shared" si="43"/>
-        <v>43957</v>
-      </c>
-      <c r="M90" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N90" s="63">
+        <v>43955</v>
+      </c>
+      <c r="M90" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N90" s="75">
         <f t="shared" si="44"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B91" s="57">
+        <v>8941</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B91" s="72">
         <f t="shared" si="35"/>
         <v>43946</v>
       </c>
-      <c r="C91" s="57"/>
-      <c r="D91" s="61">
+      <c r="C91" s="72">
+        <v>43930</v>
+      </c>
+      <c r="D91" s="73">
         <f t="shared" si="39"/>
-        <v>-12</v>
-      </c>
-      <c r="E91" s="4">
+        <v>-16</v>
+      </c>
+      <c r="E91" s="73">
         <v>14</v>
       </c>
-      <c r="F91" s="4">
+      <c r="F91" s="73">
         <v>498</v>
       </c>
-      <c r="G91" s="60">
+      <c r="G91" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H91" s="60">
-        <f t="shared" si="45"/>
-        <v>300</v>
-      </c>
-      <c r="I91" s="60">
+      <c r="H91" s="74">
+        <v>69</v>
+      </c>
+      <c r="I91" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J91" s="61">
+        <v>231</v>
+      </c>
+      <c r="J91" s="73">
         <f t="shared" si="41"/>
         <v>49</v>
       </c>
-      <c r="K91" s="61">
+      <c r="K91" s="73">
         <f t="shared" si="42"/>
         <v>23</v>
       </c>
-      <c r="L91" s="57">
+      <c r="L91" s="72">
         <f t="shared" si="43"/>
-        <v>43957</v>
-      </c>
-      <c r="M91" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N91" s="63">
+        <v>43953</v>
+      </c>
+      <c r="M91" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N91" s="75">
         <f t="shared" si="44"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B92" s="57">
+        <v>9439</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B92" s="72">
         <f t="shared" si="35"/>
         <v>43949</v>
       </c>
-      <c r="C92" s="57"/>
-      <c r="D92" s="61">
+      <c r="C92" s="72">
+        <v>43931</v>
+      </c>
+      <c r="D92" s="73">
         <f t="shared" si="39"/>
-        <v>-12</v>
-      </c>
-      <c r="E92" s="4">
+        <v>-18</v>
+      </c>
+      <c r="E92" s="73">
         <v>15</v>
       </c>
-      <c r="F92" s="4">
+      <c r="F92" s="73">
         <v>820</v>
       </c>
-      <c r="G92" s="60">
+      <c r="G92" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H92" s="60">
-        <f t="shared" si="45"/>
-        <v>300</v>
-      </c>
-      <c r="I92" s="60">
+      <c r="H92" s="74">
+        <v>208</v>
+      </c>
+      <c r="I92" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J92" s="61">
+        <v>92</v>
+      </c>
+      <c r="J92" s="73">
         <f t="shared" si="41"/>
         <v>52</v>
       </c>
-      <c r="K92" s="61">
+      <c r="K92" s="73">
         <f t="shared" si="42"/>
         <v>20</v>
       </c>
-      <c r="L92" s="57">
+      <c r="L92" s="72">
         <f t="shared" si="43"/>
-        <v>43957</v>
-      </c>
-      <c r="M92" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N92" s="63">
+        <v>43951</v>
+      </c>
+      <c r="M92" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N92" s="75">
         <f t="shared" si="44"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B93" s="57">
+        <v>10259</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B93" s="72">
         <f t="shared" si="35"/>
         <v>43952</v>
       </c>
-      <c r="C93" s="57"/>
-      <c r="D93" s="61">
+      <c r="C93" s="72">
+        <v>43931</v>
+      </c>
+      <c r="D93" s="73">
         <f t="shared" si="39"/>
-        <v>-12</v>
-      </c>
-      <c r="E93" s="4">
+        <v>-21</v>
+      </c>
+      <c r="E93" s="73">
         <v>16</v>
       </c>
-      <c r="F93" s="4">
+      <c r="F93" s="73">
         <v>791</v>
       </c>
-      <c r="G93" s="60">
+      <c r="G93" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H93" s="60">
-        <f t="shared" si="45"/>
-        <v>300</v>
-      </c>
-      <c r="I93" s="60">
+      <c r="H93" s="74">
+        <v>184</v>
+      </c>
+      <c r="I93" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="61">
+        <v>116</v>
+      </c>
+      <c r="J93" s="73">
         <f t="shared" si="41"/>
         <v>55</v>
       </c>
-      <c r="K93" s="61">
+      <c r="K93" s="73">
         <f t="shared" si="42"/>
         <v>17</v>
       </c>
-      <c r="L93" s="57">
+      <c r="L93" s="72">
         <f t="shared" si="43"/>
-        <v>43957</v>
-      </c>
-      <c r="M93" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N93" s="63">
+        <v>43948</v>
+      </c>
+      <c r="M93" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N93" s="75">
         <f t="shared" si="44"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B94" s="57">
+        <v>11050</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B94" s="72">
         <f t="shared" si="35"/>
         <v>43955</v>
       </c>
-      <c r="C94" s="57"/>
-      <c r="D94" s="61">
+      <c r="C94" s="72">
+        <v>43932</v>
+      </c>
+      <c r="D94" s="73">
         <f t="shared" si="39"/>
-        <v>-12</v>
-      </c>
-      <c r="E94" s="4">
+        <v>-23</v>
+      </c>
+      <c r="E94" s="73">
         <v>17</v>
       </c>
-      <c r="F94" s="4">
+      <c r="F94" s="73">
         <v>717</v>
       </c>
-      <c r="G94" s="60">
+      <c r="G94" s="74">
         <f t="shared" si="30"/>
         <v>300</v>
       </c>
-      <c r="H94" s="60">
-        <f t="shared" si="45"/>
-        <v>300</v>
-      </c>
-      <c r="I94" s="60">
+      <c r="H94" s="74">
+        <v>161</v>
+      </c>
+      <c r="I94" s="74">
         <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J94" s="61">
+        <v>139</v>
+      </c>
+      <c r="J94" s="73">
         <f t="shared" si="41"/>
         <v>58</v>
       </c>
-      <c r="K94" s="61">
+      <c r="K94" s="73">
         <f t="shared" si="42"/>
         <v>14</v>
       </c>
-      <c r="L94" s="57">
+      <c r="L94" s="72">
         <f t="shared" si="43"/>
-        <v>43957</v>
-      </c>
-      <c r="M94" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N94" s="63">
+        <v>43946</v>
+      </c>
+      <c r="M94" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N94" s="75">
         <f t="shared" si="44"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+        <v>11767</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B95" s="57">
         <f t="shared" si="35"/>
         <v>43958</v>
@@ -10415,7 +10420,7 @@
       <c r="C95" s="57"/>
       <c r="D95" s="61">
         <f t="shared" si="39"/>
-        <v>-12</v>
+        <v>-23</v>
       </c>
       <c r="E95" s="4">
         <v>18</v>
@@ -10428,7 +10433,7 @@
         <v>300</v>
       </c>
       <c r="H95" s="60">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="H94:H95" si="45">G95</f>
         <v>300</v>
       </c>
       <c r="I95" s="60">
@@ -10445,17 +10450,17 @@
       </c>
       <c r="L95" s="57">
         <f t="shared" si="43"/>
-        <v>43957</v>
+        <v>43946</v>
       </c>
       <c r="M95" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N95" s="63">
         <f t="shared" si="44"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+        <v>11767</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B96" s="65">
         <f>A81+A75-1</f>
         <v>43969</v>
@@ -10463,7 +10468,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="61">
         <f t="shared" si="38"/>
-        <v>-12</v>
+        <v>-23</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10493,17 +10498,17 @@
       </c>
       <c r="L96" s="57">
         <f t="shared" si="34"/>
-        <v>43957</v>
+        <v>43946</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
         <f t="shared" si="37"/>
-        <v>8242</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+        <v>11767</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97" s="65">
         <f>B96</f>
@@ -10522,11 +10527,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>4029</v>
+        <v>3291</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>2571</v>
+        <v>3309</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>
@@ -10537,7 +10542,7 @@
       <c r="M97" s="47"/>
       <c r="N97" s="47"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98"/>
       <c r="B98" s="65"/>
       <c r="C98" s="65"/>
@@ -10549,11 +10554,11 @@
       <c r="I98" s="47"/>
       <c r="J98" s="47"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E102" s="71"/>
       <c r="F102" s="71"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
     </row>
@@ -10582,12 +10587,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -10595,7 +10600,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10607,7 +10612,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -10619,7 +10624,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -10631,7 +10636,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -10643,7 +10648,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -10655,7 +10660,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -10667,7 +10672,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -10679,7 +10684,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -10691,7 +10696,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -10703,7 +10708,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -10715,7 +10720,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -10727,7 +10732,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -10739,7 +10744,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -10751,7 +10756,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -10763,7 +10768,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -10775,7 +10780,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -10787,7 +10792,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -10799,7 +10804,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -10811,7 +10816,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -10823,7 +10828,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -10835,7 +10840,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -10847,7 +10852,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Inseridos arquivos do Cap 5 e 6 de Web Scraping
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23285794-08E3-44E3-8F62-A8878DB8A7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128372B1-B640-4C8B-B965-7A337209F1B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,6 +722,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6314,8 +6315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7513,10 +7514,13 @@
         <f t="shared" si="17"/>
         <v>43913</v>
       </c>
-      <c r="C32" s="57"/>
+      <c r="C32" s="57">
+        <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
+        <v>43938</v>
+      </c>
       <c r="D32" s="58">
-        <f t="shared" ref="D32:D47" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>3</v>
+        <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
+        <v>25</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -7545,8 +7549,8 @@
         <v>56</v>
       </c>
       <c r="L32" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43994</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -7564,10 +7568,13 @@
         <f t="shared" si="17"/>
         <v>43916</v>
       </c>
-      <c r="C33" s="57"/>
+      <c r="C33" s="57">
+        <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
+        <v>43942</v>
+      </c>
       <c r="D33" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>26</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -7596,8 +7603,8 @@
         <v>53</v>
       </c>
       <c r="L33" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43995</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -7615,10 +7622,13 @@
         <f t="shared" si="17"/>
         <v>43919</v>
       </c>
-      <c r="C34" s="57"/>
+      <c r="C34" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43946</v>
+      </c>
       <c r="D34" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>27</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -7647,8 +7657,8 @@
         <v>50</v>
       </c>
       <c r="L34" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43996</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -7666,10 +7676,13 @@
         <f t="shared" si="17"/>
         <v>43922</v>
       </c>
-      <c r="C35" s="57"/>
+      <c r="C35" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43950</v>
+      </c>
       <c r="D35" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>28</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -7698,8 +7711,8 @@
         <v>47</v>
       </c>
       <c r="L35" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43997</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -7717,10 +7730,13 @@
         <f t="shared" si="17"/>
         <v>43925</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43954</v>
+      </c>
       <c r="D36" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>29</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -7749,8 +7765,8 @@
         <v>44</v>
       </c>
       <c r="L36" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43998</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -7768,10 +7784,13 @@
         <f t="shared" si="17"/>
         <v>43928</v>
       </c>
-      <c r="C37" s="57"/>
+      <c r="C37" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43958</v>
+      </c>
       <c r="D37" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>30</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -7800,8 +7819,8 @@
         <v>41</v>
       </c>
       <c r="L37" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43999</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -7816,10 +7835,13 @@
         <f t="shared" si="17"/>
         <v>43931</v>
       </c>
-      <c r="C38" s="57"/>
+      <c r="C38" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43962</v>
+      </c>
       <c r="D38" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>31</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -7848,8 +7870,8 @@
         <v>38</v>
       </c>
       <c r="L38" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44000</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -7864,10 +7886,13 @@
         <f t="shared" si="17"/>
         <v>43934</v>
       </c>
-      <c r="C39" s="57"/>
+      <c r="C39" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43966</v>
+      </c>
       <c r="D39" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>32</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -7896,8 +7921,8 @@
         <v>35</v>
       </c>
       <c r="L39" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44001</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -7912,10 +7937,13 @@
         <f t="shared" si="17"/>
         <v>43937</v>
       </c>
-      <c r="C40" s="57"/>
+      <c r="C40" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43970</v>
+      </c>
       <c r="D40" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>33</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -7944,8 +7972,8 @@
         <v>32</v>
       </c>
       <c r="L40" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44002</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -7960,10 +7988,13 @@
         <f t="shared" si="17"/>
         <v>43940</v>
       </c>
-      <c r="C41" s="57"/>
+      <c r="C41" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43974</v>
+      </c>
       <c r="D41" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>34</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -7992,8 +8023,8 @@
         <v>29</v>
       </c>
       <c r="L41" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44003</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -8008,10 +8039,13 @@
         <f t="shared" si="17"/>
         <v>43943</v>
       </c>
-      <c r="C42" s="57"/>
+      <c r="C42" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43978</v>
+      </c>
       <c r="D42" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>35</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -8040,8 +8074,8 @@
         <v>26</v>
       </c>
       <c r="L42" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44004</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -8056,10 +8090,13 @@
         <f t="shared" si="17"/>
         <v>43946</v>
       </c>
-      <c r="C43" s="57"/>
+      <c r="C43" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43982</v>
+      </c>
       <c r="D43" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>36</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -8088,8 +8125,8 @@
         <v>23</v>
       </c>
       <c r="L43" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44005</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -8104,10 +8141,13 @@
         <f t="shared" si="17"/>
         <v>43949</v>
       </c>
-      <c r="C44" s="57"/>
+      <c r="C44" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43986</v>
+      </c>
       <c r="D44" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>37</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -8136,8 +8176,8 @@
         <v>20</v>
       </c>
       <c r="L44" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44006</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -8152,10 +8192,13 @@
         <f t="shared" si="17"/>
         <v>43952</v>
       </c>
-      <c r="C45" s="57"/>
+      <c r="C45" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43990</v>
+      </c>
       <c r="D45" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>38</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -8184,8 +8227,8 @@
         <v>17</v>
       </c>
       <c r="L45" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44007</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -8200,10 +8243,13 @@
         <f t="shared" si="17"/>
         <v>43955</v>
       </c>
-      <c r="C46" s="57"/>
+      <c r="C46" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43994</v>
+      </c>
       <c r="D46" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>39</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -8232,8 +8278,8 @@
         <v>14</v>
       </c>
       <c r="L46" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>44008</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -8248,10 +8294,13 @@
         <f>A33+A27-1</f>
         <v>43969</v>
       </c>
-      <c r="C47" s="65"/>
+      <c r="C47" s="57">
+        <f t="shared" ca="1" si="20"/>
+        <v>43998</v>
+      </c>
       <c r="D47" s="58">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>29</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -8280,8 +8329,8 @@
         <v>0</v>
       </c>
       <c r="L47" s="62">
-        <f t="shared" si="15"/>
-        <v>43972</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>43998</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -8415,26 +8464,26 @@
         <v>12</v>
       </c>
       <c r="G53" s="52">
-        <f t="shared" ref="G53:G70" si="20">$A$57</f>
+        <f t="shared" ref="G53:G70" si="21">$A$57</f>
         <v>400</v>
       </c>
       <c r="H53" s="36">
         <v>124</v>
       </c>
       <c r="I53" s="52">
-        <f t="shared" ref="I53:I70" si="21">G53-H53</f>
+        <f t="shared" ref="I53:I70" si="22">G53-H53</f>
         <v>276</v>
       </c>
       <c r="J53" s="36">
-        <f t="shared" ref="J53:J70" si="22">$A$53-K53</f>
+        <f t="shared" ref="J53:J70" si="23">$A$53-K53</f>
         <v>1</v>
       </c>
       <c r="K53" s="36">
-        <f t="shared" ref="K53:K70" si="23">INT($B$71-B53)</f>
+        <f t="shared" ref="K53:K70" si="24">INT($B$71-B53)</f>
         <v>71</v>
       </c>
       <c r="L53" s="50">
-        <f t="shared" ref="L53:L70" si="24">B53+K53+D53</f>
+        <f t="shared" ref="L53:L70" si="25">B53+K53+D53</f>
         <v>43969</v>
       </c>
       <c r="M53" s="53" t="s">
@@ -8454,14 +8503,14 @@
         <v>47</v>
       </c>
       <c r="B54" s="50">
-        <f t="shared" ref="B54:B69" si="25">B53+$A$55</f>
+        <f t="shared" ref="B54:B69" si="26">B53+$A$55</f>
         <v>43902</v>
       </c>
       <c r="C54" s="50">
         <v>43900</v>
       </c>
       <c r="D54" s="51">
-        <f t="shared" ref="D54" si="26">IF(C54="",D53,C54-B54+D53)</f>
+        <f t="shared" ref="D54" si="27">IF(C54="",D53,C54-B54+D53)</f>
         <v>-2</v>
       </c>
       <c r="E54" s="36">
@@ -8471,33 +8520,33 @@
         <v>19</v>
       </c>
       <c r="G54" s="52">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H54" s="52">
         <v>159</v>
       </c>
       <c r="I54" s="52">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>241</v>
       </c>
       <c r="J54" s="51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="K54" s="51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>67</v>
       </c>
       <c r="L54" s="50">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>43967</v>
       </c>
       <c r="M54" s="53" t="s">
         <v>46</v>
       </c>
       <c r="N54" s="53">
-        <f t="shared" ref="N54:N70" si="27">IF(M54&lt;&gt;"S",N53,N53+F54)</f>
+        <f t="shared" ref="N54:N70" si="28">IF(M54&lt;&gt;"S",N53,N53+F54)</f>
         <v>31</v>
       </c>
     </row>
@@ -8507,7 +8556,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="50">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43906</v>
       </c>
       <c r="C55" s="50">
@@ -8524,33 +8573,33 @@
         <v>16</v>
       </c>
       <c r="G55" s="52">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H55" s="52">
         <v>287</v>
       </c>
       <c r="I55" s="52">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>113</v>
       </c>
       <c r="J55" s="51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9</v>
       </c>
       <c r="K55" s="51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>63</v>
       </c>
       <c r="L55" s="50">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>43973</v>
       </c>
       <c r="M55" s="53" t="s">
         <v>46</v>
       </c>
       <c r="N55" s="53">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>47</v>
       </c>
     </row>
@@ -8559,14 +8608,14 @@
         <v>48</v>
       </c>
       <c r="B56" s="72">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43910</v>
       </c>
       <c r="C56" s="72">
         <v>43921</v>
       </c>
       <c r="D56" s="73">
-        <f t="shared" ref="D56:D70" si="28">IF(C56="",D55,C56-B56)</f>
+        <f t="shared" ref="D56:D70" si="29">IF(C56="",D55,C56-B56)</f>
         <v>11</v>
       </c>
       <c r="E56" s="73">
@@ -8576,33 +8625,33 @@
         <v>21</v>
       </c>
       <c r="G56" s="74">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H56" s="74">
         <v>404</v>
       </c>
       <c r="I56" s="74">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>-4</v>
       </c>
       <c r="J56" s="73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>13</v>
       </c>
       <c r="K56" s="73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>59</v>
       </c>
       <c r="L56" s="72">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>43980</v>
       </c>
       <c r="M56" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N56" s="75">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>68</v>
       </c>
     </row>
@@ -8611,65 +8660,70 @@
         <f>A63*A55</f>
         <v>400</v>
       </c>
-      <c r="B57" s="57">
+      <c r="B57" s="72">
+        <f t="shared" si="26"/>
+        <v>43914</v>
+      </c>
+      <c r="C57" s="72">
+        <v>43935</v>
+      </c>
+      <c r="D57" s="73">
+        <f t="shared" si="29"/>
+        <v>21</v>
+      </c>
+      <c r="E57" s="73">
+        <v>5</v>
+      </c>
+      <c r="F57" s="73">
+        <v>17</v>
+      </c>
+      <c r="G57" s="74">
+        <f t="shared" si="21"/>
+        <v>400</v>
+      </c>
+      <c r="H57" s="74">
+        <v>145</v>
+      </c>
+      <c r="I57" s="74">
+        <f t="shared" si="22"/>
+        <v>255</v>
+      </c>
+      <c r="J57" s="73">
+        <f t="shared" si="23"/>
+        <v>17</v>
+      </c>
+      <c r="K57" s="73">
+        <f t="shared" si="24"/>
+        <v>55</v>
+      </c>
+      <c r="L57" s="72">
         <f t="shared" si="25"/>
-        <v>43914</v>
-      </c>
-      <c r="C57" s="57"/>
-      <c r="D57" s="58">
+        <v>43990</v>
+      </c>
+      <c r="M57" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N57" s="75">
         <f t="shared" si="28"/>
-        <v>11</v>
-      </c>
-      <c r="E57" s="4">
-        <v>5</v>
-      </c>
-      <c r="F57" s="4">
-        <v>17</v>
-      </c>
-      <c r="G57" s="60">
-        <f t="shared" si="20"/>
-        <v>400</v>
-      </c>
-      <c r="H57" s="69">
-        <f t="shared" ref="H57:H70" si="29">G57</f>
-        <v>400</v>
-      </c>
-      <c r="I57" s="69">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="61">
-        <f t="shared" si="22"/>
-        <v>17</v>
-      </c>
-      <c r="K57" s="61">
-        <f t="shared" si="23"/>
-        <v>55</v>
-      </c>
-      <c r="L57" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
-      </c>
-      <c r="M57" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N57" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="P57" s="100"/>
     </row>
     <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B58" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43918</v>
       </c>
-      <c r="C58" s="57"/>
+      <c r="C58" s="57">
+        <f ca="1">IF(M57="S",TODAY()+A$55,C57+4)</f>
+        <v>43939</v>
+      </c>
       <c r="D58" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E58" s="4">
         <v>6</v>
@@ -8678,35 +8732,35 @@
         <v>25</v>
       </c>
       <c r="G58" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H58" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="H57:H70" si="30">G58</f>
         <v>400</v>
       </c>
       <c r="I58" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J58" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>21</v>
       </c>
       <c r="K58" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>51</v>
       </c>
       <c r="L58" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M58" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N58" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8714,13 +8768,16 @@
         <v>43898</v>
       </c>
       <c r="B59" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43922</v>
       </c>
-      <c r="C59" s="57"/>
+      <c r="C59" s="57">
+        <f t="shared" ref="C59:C70" ca="1" si="31">IF(M58="S",TODAY()+A$55,C58+4)</f>
+        <v>43943</v>
+      </c>
       <c r="D59" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E59" s="4">
         <v>7</v>
@@ -8729,35 +8786,35 @@
         <v>17</v>
       </c>
       <c r="G59" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H59" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I59" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J59" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>25</v>
       </c>
       <c r="K59" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="L59" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M59" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N59" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8765,13 +8822,16 @@
         <v>51</v>
       </c>
       <c r="B60" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43926</v>
       </c>
-      <c r="C60" s="57"/>
+      <c r="C60" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43947</v>
+      </c>
       <c r="D60" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -8780,35 +8840,35 @@
         <v>12</v>
       </c>
       <c r="G60" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H60" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I60" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J60" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>29</v>
       </c>
       <c r="K60" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>43</v>
       </c>
       <c r="L60" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M60" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N60" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8816,13 +8876,16 @@
         <v>18</v>
       </c>
       <c r="B61" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43930</v>
       </c>
-      <c r="C61" s="57"/>
+      <c r="C61" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43951</v>
+      </c>
       <c r="D61" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -8831,35 +8894,35 @@
         <v>22</v>
       </c>
       <c r="G61" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H61" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I61" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J61" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>33</v>
       </c>
       <c r="K61" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>39</v>
       </c>
       <c r="L61" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N61" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8867,13 +8930,16 @@
         <v>52</v>
       </c>
       <c r="B62" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43934</v>
       </c>
-      <c r="C62" s="57"/>
+      <c r="C62" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43955</v>
+      </c>
       <c r="D62" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -8882,35 +8948,35 @@
         <v>10</v>
       </c>
       <c r="G62" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H62" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I62" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J62" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>37</v>
       </c>
       <c r="K62" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>35</v>
       </c>
       <c r="L62" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N62" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8918,13 +8984,16 @@
         <v>100</v>
       </c>
       <c r="B63" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43938</v>
       </c>
-      <c r="C63" s="57"/>
+      <c r="C63" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43959</v>
+      </c>
       <c r="D63" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -8933,46 +9002,49 @@
         <v>16</v>
       </c>
       <c r="G63" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H63" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I63" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J63" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>41</v>
       </c>
       <c r="K63" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>31</v>
       </c>
       <c r="L63" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N63" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B64" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43942</v>
       </c>
-      <c r="C64" s="57"/>
+      <c r="C64" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43963</v>
+      </c>
       <c r="D64" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -8981,46 +9053,49 @@
         <v>19</v>
       </c>
       <c r="G64" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H64" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I64" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J64" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>45</v>
       </c>
       <c r="K64" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>27</v>
       </c>
       <c r="L64" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N64" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B65" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43946</v>
       </c>
-      <c r="C65" s="57"/>
+      <c r="C65" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43967</v>
+      </c>
       <c r="D65" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -9029,46 +9104,49 @@
         <v>25</v>
       </c>
       <c r="G65" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H65" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I65" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J65" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>49</v>
       </c>
       <c r="K65" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>23</v>
       </c>
       <c r="L65" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N65" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B66" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43950</v>
       </c>
-      <c r="C66" s="57"/>
+      <c r="C66" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43971</v>
+      </c>
       <c r="D66" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -9077,46 +9155,49 @@
         <v>13</v>
       </c>
       <c r="G66" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H66" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I66" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J66" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>53</v>
       </c>
       <c r="K66" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>19</v>
       </c>
       <c r="L66" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N66" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B67" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43954</v>
       </c>
-      <c r="C67" s="57"/>
+      <c r="C67" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43975</v>
+      </c>
       <c r="D67" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -9125,46 +9206,49 @@
         <v>13</v>
       </c>
       <c r="G67" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H67" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I67" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J67" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>57</v>
       </c>
       <c r="K67" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>15</v>
       </c>
       <c r="L67" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N67" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B68" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43958</v>
       </c>
-      <c r="C68" s="57"/>
+      <c r="C68" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43979</v>
+      </c>
       <c r="D68" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -9173,46 +9257,49 @@
         <v>19</v>
       </c>
       <c r="G68" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H68" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I68" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J68" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>61</v>
       </c>
       <c r="K68" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>11</v>
       </c>
       <c r="L68" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N68" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="B69" s="57">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>43962</v>
       </c>
-      <c r="C69" s="57"/>
+      <c r="C69" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43983</v>
+      </c>
       <c r="D69" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>21</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9221,35 +9308,35 @@
         <v>10</v>
       </c>
       <c r="G69" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H69" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I69" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J69" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>65</v>
       </c>
       <c r="K69" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="L69" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43990</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9257,10 +9344,13 @@
         <f>A59+A53-1</f>
         <v>43969</v>
       </c>
-      <c r="C70" s="57"/>
+      <c r="C70" s="57">
+        <f t="shared" ca="1" si="31"/>
+        <v>43987</v>
+      </c>
       <c r="D70" s="58">
-        <f t="shared" si="28"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="29"/>
+        <v>18</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9269,35 +9359,35 @@
         <v>18</v>
       </c>
       <c r="G70" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>400</v>
       </c>
       <c r="H70" s="69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>400</v>
       </c>
       <c r="I70" s="69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J70" s="61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>72</v>
       </c>
       <c r="K70" s="61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L70" s="57">
-        <f t="shared" si="24"/>
-        <v>43980</v>
+        <f t="shared" ca="1" si="25"/>
+        <v>43987</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
-        <f t="shared" si="27"/>
-        <v>68</v>
+        <f t="shared" si="28"/>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9319,11 +9409,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>6574</v>
+        <v>6319</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>626</v>
+        <v>881</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>
@@ -9415,26 +9505,26 @@
         <v>251</v>
       </c>
       <c r="G75" s="74">
-        <f t="shared" ref="G75:G96" si="30">$A$79</f>
+        <f t="shared" ref="G75:G96" si="32">$A$79</f>
         <v>300</v>
       </c>
       <c r="H75" s="73">
         <v>29</v>
       </c>
       <c r="I75" s="74">
-        <f t="shared" ref="I75:I96" si="31">G75-H75</f>
+        <f t="shared" ref="I75:I96" si="33">G75-H75</f>
         <v>271</v>
       </c>
       <c r="J75" s="73">
-        <f t="shared" ref="J75:J96" si="32">$A$75-K75</f>
+        <f t="shared" ref="J75:J96" si="34">$A$75-K75</f>
         <v>1</v>
       </c>
       <c r="K75" s="73">
-        <f t="shared" ref="K75:K96" si="33">INT($B$97-B75)</f>
+        <f t="shared" ref="K75:K96" si="35">INT($B$97-B75)</f>
         <v>71</v>
       </c>
       <c r="L75" s="72">
-        <f t="shared" ref="L75:L96" si="34">B75+K75+D75</f>
+        <f t="shared" ref="L75:L96" si="36">B75+K75+D75</f>
         <v>43969</v>
       </c>
       <c r="M75" s="75" t="s">
@@ -9454,14 +9544,14 @@
         <v>47</v>
       </c>
       <c r="B76" s="72">
-        <f t="shared" ref="B76:B95" si="35">B75+$A$77</f>
+        <f t="shared" ref="B76:B95" si="37">B75+$A$77</f>
         <v>43901</v>
       </c>
       <c r="C76" s="72">
         <v>43900</v>
       </c>
       <c r="D76" s="73">
-        <f t="shared" ref="D76" si="36">IF(C76="",D75,C76-B76+D75)</f>
+        <f t="shared" ref="D76" si="38">IF(C76="",D75,C76-B76+D75)</f>
         <v>-1</v>
       </c>
       <c r="E76" s="73">
@@ -9471,33 +9561,33 @@
         <v>478</v>
       </c>
       <c r="G76" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H76" s="74">
         <v>7</v>
       </c>
       <c r="I76" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>293</v>
       </c>
       <c r="J76" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="K76" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>68</v>
       </c>
       <c r="L76" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43968</v>
       </c>
       <c r="M76" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N76" s="75">
-        <f t="shared" ref="N76:N96" si="37">IF(M76&lt;&gt;"S",N75,N75+F76)</f>
+        <f t="shared" ref="N76:N96" si="39">IF(M76&lt;&gt;"S",N75,N75+F76)</f>
         <v>729</v>
       </c>
     </row>
@@ -9507,7 +9597,7 @@
         <v>3</v>
       </c>
       <c r="B77" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43904</v>
       </c>
       <c r="C77" s="72">
@@ -9524,33 +9614,33 @@
         <v>647</v>
       </c>
       <c r="G77" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H77" s="74">
         <v>77</v>
       </c>
       <c r="I77" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>223</v>
       </c>
       <c r="J77" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>7</v>
       </c>
       <c r="K77" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>65</v>
       </c>
       <c r="L77" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43976</v>
       </c>
       <c r="M77" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N77" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1376</v>
       </c>
     </row>
@@ -9559,7 +9649,7 @@
         <v>48</v>
       </c>
       <c r="B78" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43907</v>
       </c>
       <c r="C78" s="72">
@@ -9576,33 +9666,33 @@
         <v>493</v>
       </c>
       <c r="G78" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H78" s="74">
         <v>88</v>
       </c>
       <c r="I78" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>212</v>
       </c>
       <c r="J78" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>10</v>
       </c>
       <c r="K78" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>62</v>
       </c>
       <c r="L78" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43975</v>
       </c>
       <c r="M78" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N78" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1869</v>
       </c>
     </row>
@@ -9612,14 +9702,14 @@
         <v>300</v>
       </c>
       <c r="B79" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43910</v>
       </c>
       <c r="C79" s="72">
         <v>43922</v>
       </c>
       <c r="D79" s="73">
-        <f t="shared" ref="D79:D96" si="38">IF(C79="",D78,C79-B79)</f>
+        <f t="shared" ref="D79:D96" si="40">IF(C79="",D78,C79-B79)</f>
         <v>12</v>
       </c>
       <c r="E79" s="73">
@@ -9629,33 +9719,33 @@
         <v>743</v>
       </c>
       <c r="G79" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H79" s="74">
         <v>30</v>
       </c>
       <c r="I79" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>270</v>
       </c>
       <c r="J79" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>13</v>
       </c>
       <c r="K79" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>59</v>
       </c>
       <c r="L79" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43981</v>
       </c>
       <c r="M79" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N79" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>2612</v>
       </c>
     </row>
@@ -9664,14 +9754,14 @@
         <v>50</v>
       </c>
       <c r="B80" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43913</v>
       </c>
       <c r="C80" s="72">
         <v>43922</v>
       </c>
       <c r="D80" s="73">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>9</v>
       </c>
       <c r="E80" s="73">
@@ -9681,33 +9771,33 @@
         <v>498</v>
       </c>
       <c r="G80" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H80" s="74">
         <v>56</v>
       </c>
       <c r="I80" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>244</v>
       </c>
       <c r="J80" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>16</v>
       </c>
       <c r="K80" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>56</v>
       </c>
       <c r="L80" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43978</v>
       </c>
       <c r="M80" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N80" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>3110</v>
       </c>
     </row>
@@ -9716,14 +9806,14 @@
         <v>43898</v>
       </c>
       <c r="B81" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43916</v>
       </c>
       <c r="C81" s="72">
         <v>43923</v>
       </c>
       <c r="D81" s="73">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>7</v>
       </c>
       <c r="E81" s="73" t="s">
@@ -9733,33 +9823,33 @@
         <v>57</v>
       </c>
       <c r="G81" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H81" s="74">
         <v>15</v>
       </c>
       <c r="I81" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>285</v>
       </c>
       <c r="J81" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>19</v>
       </c>
       <c r="K81" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>53</v>
       </c>
       <c r="L81" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43976</v>
       </c>
       <c r="M81" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N81" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>3167</v>
       </c>
     </row>
@@ -9768,14 +9858,14 @@
         <v>51</v>
       </c>
       <c r="B82" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43919</v>
       </c>
       <c r="C82" s="72">
         <v>43923</v>
       </c>
       <c r="D82" s="73">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>4</v>
       </c>
       <c r="E82" s="73">
@@ -9785,33 +9875,33 @@
         <v>633</v>
       </c>
       <c r="G82" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H82" s="74">
         <v>223</v>
       </c>
       <c r="I82" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>77</v>
       </c>
       <c r="J82" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>22</v>
       </c>
       <c r="K82" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>50</v>
       </c>
       <c r="L82" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43973</v>
       </c>
       <c r="M82" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N82" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>3800</v>
       </c>
     </row>
@@ -9820,14 +9910,14 @@
         <v>23</v>
       </c>
       <c r="B83" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43922</v>
       </c>
       <c r="C83" s="72">
         <v>43924</v>
       </c>
       <c r="D83" s="73">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="E83" s="73">
@@ -9837,33 +9927,33 @@
         <v>820</v>
       </c>
       <c r="G83" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H83" s="74">
         <v>201</v>
       </c>
       <c r="I83" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>99</v>
       </c>
       <c r="J83" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>25</v>
       </c>
       <c r="K83" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>47</v>
       </c>
       <c r="L83" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43971</v>
       </c>
       <c r="M83" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N83" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>4620</v>
       </c>
     </row>
@@ -9872,14 +9962,14 @@
         <v>52</v>
       </c>
       <c r="B84" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43925</v>
       </c>
       <c r="C84" s="72">
         <v>43925</v>
       </c>
       <c r="D84" s="73">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="E84" s="73">
@@ -9889,33 +9979,33 @@
         <v>707</v>
       </c>
       <c r="G84" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H84" s="74">
         <v>214</v>
       </c>
       <c r="I84" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>86</v>
       </c>
       <c r="J84" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>28</v>
       </c>
       <c r="K84" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>44</v>
       </c>
       <c r="L84" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43969</v>
       </c>
       <c r="M84" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N84" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>5327</v>
       </c>
     </row>
@@ -9924,14 +10014,14 @@
         <v>100</v>
       </c>
       <c r="B85" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43928</v>
       </c>
       <c r="C85" s="72">
         <v>43926</v>
       </c>
       <c r="D85" s="73">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>-2</v>
       </c>
       <c r="E85" s="73" t="s">
@@ -9941,46 +10031,46 @@
         <v>42</v>
       </c>
       <c r="G85" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H85" s="74">
         <v>4</v>
       </c>
       <c r="I85" s="74">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>296</v>
       </c>
       <c r="J85" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>31</v>
       </c>
       <c r="K85" s="73">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>41</v>
       </c>
       <c r="L85" s="72">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>43967</v>
       </c>
       <c r="M85" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N85" s="75">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>5369</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B86" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43931</v>
       </c>
       <c r="C86" s="72">
         <v>43926</v>
       </c>
       <c r="D86" s="73">
-        <f t="shared" ref="D86:D95" si="39">IF(C86="",D85,C86-B86)</f>
+        <f t="shared" ref="D86:D95" si="41">IF(C86="",D85,C86-B86)</f>
         <v>-5</v>
       </c>
       <c r="E86" s="73">
@@ -9990,46 +10080,46 @@
         <v>567</v>
       </c>
       <c r="G86" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H86" s="74">
         <v>225</v>
       </c>
       <c r="I86" s="74">
-        <f t="shared" ref="I86:I95" si="40">G86-H86</f>
+        <f t="shared" ref="I86:I95" si="42">G86-H86</f>
         <v>75</v>
       </c>
       <c r="J86" s="73">
-        <f t="shared" ref="J86:J95" si="41">$A$75-K86</f>
+        <f t="shared" ref="J86:J95" si="43">$A$75-K86</f>
         <v>34</v>
       </c>
       <c r="K86" s="73">
-        <f t="shared" ref="K86:K95" si="42">INT($B$97-B86)</f>
+        <f t="shared" ref="K86:K95" si="44">INT($B$97-B86)</f>
         <v>38</v>
       </c>
       <c r="L86" s="72">
-        <f t="shared" ref="L86:L95" si="43">B86+K86+D86</f>
+        <f t="shared" ref="L86:L95" si="45">B86+K86+D86</f>
         <v>43964</v>
       </c>
       <c r="M86" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N86" s="75">
-        <f t="shared" ref="N86:N95" si="44">IF(M86&lt;&gt;"S",N85,N85+F86)</f>
+        <f t="shared" ref="N86:N95" si="46">IF(M86&lt;&gt;"S",N85,N85+F86)</f>
         <v>5936</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B87" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43934</v>
       </c>
       <c r="C87" s="72">
         <v>43927</v>
       </c>
       <c r="D87" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-7</v>
       </c>
       <c r="E87" s="73">
@@ -10039,46 +10129,46 @@
         <v>506</v>
       </c>
       <c r="G87" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H87" s="74">
         <v>112</v>
       </c>
       <c r="I87" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>188</v>
       </c>
       <c r="J87" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>37</v>
       </c>
       <c r="K87" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>35</v>
       </c>
       <c r="L87" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43962</v>
       </c>
       <c r="M87" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N87" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>6442</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B88" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43937</v>
       </c>
       <c r="C88" s="72">
         <v>43928</v>
       </c>
       <c r="D88" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-9</v>
       </c>
       <c r="E88" s="73">
@@ -10088,46 +10178,46 @@
         <v>924</v>
       </c>
       <c r="G88" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H88" s="74">
         <v>370</v>
       </c>
       <c r="I88" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>-70</v>
       </c>
       <c r="J88" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>40</v>
       </c>
       <c r="K88" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>32</v>
       </c>
       <c r="L88" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43960</v>
       </c>
       <c r="M88" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N88" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>7366</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B89" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43940</v>
       </c>
       <c r="C89" s="72">
         <v>43928</v>
       </c>
       <c r="D89" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-12</v>
       </c>
       <c r="E89" s="73">
@@ -10137,46 +10227,46 @@
         <v>876</v>
       </c>
       <c r="G89" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H89" s="74">
         <v>278</v>
       </c>
       <c r="I89" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>22</v>
       </c>
       <c r="J89" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>43</v>
       </c>
       <c r="K89" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>29</v>
       </c>
       <c r="L89" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43957</v>
       </c>
       <c r="M89" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N89" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>8242</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B90" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43943</v>
       </c>
       <c r="C90" s="72">
         <v>43929</v>
       </c>
       <c r="D90" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-14</v>
       </c>
       <c r="E90" s="73">
@@ -10186,46 +10276,46 @@
         <v>699</v>
       </c>
       <c r="G90" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H90" s="74">
         <v>140</v>
       </c>
       <c r="I90" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>160</v>
       </c>
       <c r="J90" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>46</v>
       </c>
       <c r="K90" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>26</v>
       </c>
       <c r="L90" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43955</v>
       </c>
       <c r="M90" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N90" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>8941</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B91" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43946</v>
       </c>
       <c r="C91" s="72">
         <v>43930</v>
       </c>
       <c r="D91" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-16</v>
       </c>
       <c r="E91" s="73">
@@ -10235,46 +10325,46 @@
         <v>498</v>
       </c>
       <c r="G91" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H91" s="74">
         <v>69</v>
       </c>
       <c r="I91" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>231</v>
       </c>
       <c r="J91" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>49</v>
       </c>
       <c r="K91" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>23</v>
       </c>
       <c r="L91" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43953</v>
       </c>
       <c r="M91" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N91" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>9439</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B92" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43949</v>
       </c>
       <c r="C92" s="72">
         <v>43931</v>
       </c>
       <c r="D92" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-18</v>
       </c>
       <c r="E92" s="73">
@@ -10284,46 +10374,46 @@
         <v>820</v>
       </c>
       <c r="G92" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H92" s="74">
         <v>208</v>
       </c>
       <c r="I92" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>92</v>
       </c>
       <c r="J92" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>52</v>
       </c>
       <c r="K92" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>20</v>
       </c>
       <c r="L92" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43951</v>
       </c>
       <c r="M92" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N92" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>10259</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B93" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43952</v>
       </c>
       <c r="C93" s="72">
         <v>43931</v>
       </c>
       <c r="D93" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-21</v>
       </c>
       <c r="E93" s="73">
@@ -10333,46 +10423,46 @@
         <v>791</v>
       </c>
       <c r="G93" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H93" s="74">
         <v>184</v>
       </c>
       <c r="I93" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>116</v>
       </c>
       <c r="J93" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>55</v>
       </c>
       <c r="K93" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>17</v>
       </c>
       <c r="L93" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43948</v>
       </c>
       <c r="M93" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N93" s="75">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>11050</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B94" s="72">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>43955</v>
       </c>
       <c r="C94" s="72">
         <v>43932</v>
       </c>
       <c r="D94" s="73">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>-23</v>
       </c>
       <c r="E94" s="73">
@@ -10382,82 +10472,83 @@
         <v>717</v>
       </c>
       <c r="G94" s="74">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H94" s="74">
         <v>161</v>
       </c>
       <c r="I94" s="74">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>139</v>
       </c>
       <c r="J94" s="73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>58</v>
       </c>
       <c r="K94" s="73">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>14</v>
       </c>
       <c r="L94" s="72">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>43946</v>
       </c>
       <c r="M94" s="75" t="s">
         <v>46</v>
       </c>
       <c r="N94" s="75">
+        <f t="shared" si="46"/>
+        <v>11767</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B95" s="72">
+        <f t="shared" si="37"/>
+        <v>43958</v>
+      </c>
+      <c r="C95" s="72">
+        <v>43933</v>
+      </c>
+      <c r="D95" s="73">
+        <f t="shared" si="41"/>
+        <v>-25</v>
+      </c>
+      <c r="E95" s="73">
+        <v>18</v>
+      </c>
+      <c r="F95" s="73">
+        <v>827</v>
+      </c>
+      <c r="G95" s="74">
+        <f t="shared" si="32"/>
+        <v>300</v>
+      </c>
+      <c r="H95" s="74">
+        <v>220</v>
+      </c>
+      <c r="I95" s="74">
+        <f t="shared" si="42"/>
+        <v>80</v>
+      </c>
+      <c r="J95" s="73">
+        <f t="shared" si="43"/>
+        <v>61</v>
+      </c>
+      <c r="K95" s="73">
         <f t="shared" si="44"/>
-        <v>11767</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="57">
-        <f t="shared" si="35"/>
-        <v>43958</v>
-      </c>
-      <c r="C95" s="57"/>
-      <c r="D95" s="61">
-        <f t="shared" si="39"/>
-        <v>-23</v>
-      </c>
-      <c r="E95" s="4">
-        <v>18</v>
-      </c>
-      <c r="F95" s="4">
-        <v>827</v>
-      </c>
-      <c r="G95" s="60">
-        <f t="shared" si="30"/>
-        <v>300</v>
-      </c>
-      <c r="H95" s="60">
-        <f t="shared" ref="H94:H95" si="45">G95</f>
-        <v>300</v>
-      </c>
-      <c r="I95" s="60">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="J95" s="61">
-        <f t="shared" si="41"/>
-        <v>61</v>
-      </c>
-      <c r="K95" s="61">
-        <f t="shared" si="42"/>
         <v>11</v>
       </c>
-      <c r="L95" s="57">
-        <f t="shared" si="43"/>
-        <v>43946</v>
-      </c>
-      <c r="M95" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N95" s="63">
-        <f t="shared" si="44"/>
-        <v>11767</v>
+      <c r="L95" s="72">
+        <f t="shared" si="45"/>
+        <v>43944</v>
+      </c>
+      <c r="M95" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N95" s="75">
+        <f t="shared" si="46"/>
+        <v>12594</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -10467,8 +10558,8 @@
       </c>
       <c r="C96" s="65"/>
       <c r="D96" s="61">
-        <f t="shared" si="38"/>
-        <v>-23</v>
+        <f t="shared" si="40"/>
+        <v>-25</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>59</v>
@@ -10477,35 +10568,35 @@
         <v>337</v>
       </c>
       <c r="G96" s="60">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>300</v>
       </c>
       <c r="H96" s="60">
-        <f t="shared" ref="H96" si="46">G96</f>
+        <f t="shared" ref="H96" si="47">G96</f>
         <v>300</v>
       </c>
       <c r="I96" s="60">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="J96" s="61">
-        <f t="shared" si="32"/>
-        <v>72</v>
-      </c>
-      <c r="K96" s="61">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
+      <c r="J96" s="61">
+        <f t="shared" si="34"/>
+        <v>72</v>
+      </c>
+      <c r="K96" s="61">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
       <c r="L96" s="57">
-        <f t="shared" si="34"/>
-        <v>43946</v>
+        <f t="shared" si="36"/>
+        <v>43944</v>
       </c>
       <c r="M96" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N96" s="63">
-        <f t="shared" si="37"/>
-        <v>11767</v>
+        <f t="shared" si="39"/>
+        <v>12594</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -10527,11 +10618,11 @@
       </c>
       <c r="H97" s="67">
         <f>SUM(H75:H96)</f>
-        <v>3291</v>
+        <v>3211</v>
       </c>
       <c r="I97" s="67">
         <f>SUM(I75:I96)</f>
-        <v>3309</v>
+        <v>3389</v>
       </c>
       <c r="J97" s="68">
         <f>SUM(J75:J96)</f>

</xml_diff>

<commit_message>
Implementados os últimos arquivos do Capítulo 8 de web scraping
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE77CCA-E049-497E-A5A6-96ABD24C16F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C985CBF8-864B-4D88-8185-4486633E11F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6320,7 +6320,7 @@
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67"/>
+      <selection activeCell="G62" sqref="G62:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7520,11 +7520,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43944</v>
+        <v>43945</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -7554,7 +7554,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -7574,11 +7574,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43948</v>
+        <v>43949</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -7608,7 +7608,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -7628,11 +7628,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -7682,11 +7682,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -7716,7 +7716,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -7736,11 +7736,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43960</v>
+        <v>43961</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -7790,11 +7790,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -7824,7 +7824,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -7841,11 +7841,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -7892,11 +7892,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43972</v>
+        <v>43973</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -7943,11 +7943,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43976</v>
+        <v>43977</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -7994,11 +7994,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43980</v>
+        <v>43981</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -8028,7 +8028,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -8045,11 +8045,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -8096,11 +8096,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -8130,7 +8130,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -8147,11 +8147,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -8198,11 +8198,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43996</v>
+        <v>43997</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -8232,7 +8232,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -8249,11 +8249,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -8283,7 +8283,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -8300,11 +8300,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -8821,54 +8821,52 @@
       <c r="A60" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="57">
+      <c r="B60" s="72">
         <f t="shared" si="26"/>
         <v>43926</v>
       </c>
-      <c r="C60" s="57">
-        <f t="shared" ref="C59:C70" ca="1" si="30">IF(M59="S",TODAY()+A$55,C59+4)</f>
-        <v>43945</v>
-      </c>
-      <c r="D60" s="58">
-        <f t="shared" ca="1" si="29"/>
-        <v>19</v>
-      </c>
-      <c r="E60" s="4">
+      <c r="C60" s="72">
+        <v>43942</v>
+      </c>
+      <c r="D60" s="73">
+        <f t="shared" si="29"/>
+        <v>16</v>
+      </c>
+      <c r="E60" s="73">
         <v>8</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60" s="73">
         <v>12</v>
       </c>
-      <c r="G60" s="60">
+      <c r="G60" s="74">
         <f t="shared" si="21"/>
         <v>400</v>
       </c>
-      <c r="H60" s="69">
-        <f t="shared" ref="H59:H70" si="31">G60</f>
-        <v>400</v>
-      </c>
-      <c r="I60" s="69">
+      <c r="H60" s="74">
+        <v>181</v>
+      </c>
+      <c r="I60" s="74">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="61">
+        <v>219</v>
+      </c>
+      <c r="J60" s="73">
         <f t="shared" si="23"/>
         <v>29</v>
       </c>
-      <c r="K60" s="61">
+      <c r="K60" s="73">
         <f t="shared" si="24"/>
         <v>43</v>
       </c>
-      <c r="L60" s="57">
-        <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
-      </c>
-      <c r="M60" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N60" s="63">
+      <c r="L60" s="72">
+        <f t="shared" si="25"/>
+        <v>43985</v>
+      </c>
+      <c r="M60" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N60" s="75">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8880,12 +8878,12 @@
         <v>43930</v>
       </c>
       <c r="C61" s="57">
-        <f t="shared" ca="1" si="30"/>
-        <v>43949</v>
+        <f t="shared" ref="C60:C70" ca="1" si="30">IF(M60="S",TODAY()+A$55,C60+4)</f>
+        <v>43946</v>
       </c>
       <c r="D61" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -8898,7 +8896,7 @@
         <v>400</v>
       </c>
       <c r="H61" s="69">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="H60:H70" si="31">G61</f>
         <v>400</v>
       </c>
       <c r="I61" s="69">
@@ -8915,14 +8913,14 @@
       </c>
       <c r="L61" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N61" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8935,11 +8933,11 @@
       </c>
       <c r="C62" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43953</v>
+        <v>43950</v>
       </c>
       <c r="D62" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -8969,14 +8967,14 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N62" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8989,11 +8987,11 @@
       </c>
       <c r="C63" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43957</v>
+        <v>43954</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -9023,14 +9021,14 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N63" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9040,11 +9038,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43961</v>
+        <v>43958</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -9074,14 +9072,14 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N64" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9091,11 +9089,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43965</v>
+        <v>43962</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -9125,14 +9123,14 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N65" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9142,11 +9140,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43969</v>
+        <v>43966</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -9176,14 +9174,14 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N66" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9193,11 +9191,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43973</v>
+        <v>43970</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -9227,14 +9225,14 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N67" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9244,11 +9242,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43977</v>
+        <v>43974</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -9278,14 +9276,14 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N68" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9295,11 +9293,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9329,14 +9327,14 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43988</v>
+        <v>43985</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9346,11 +9344,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43985</v>
+        <v>43982</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9380,14 +9378,14 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43982</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
         <f t="shared" si="28"/>
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9409,11 +9407,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>5907</v>
+        <v>5688</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>1293</v>
+        <v>1512</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>
@@ -12170,11 +12168,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43944</v>
+        <v>43945</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -12204,7 +12202,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -12224,11 +12222,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43948</v>
+        <v>43949</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -12258,7 +12256,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -12278,11 +12276,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -12312,7 +12310,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -12332,11 +12330,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -12366,7 +12364,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -12386,11 +12384,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43960</v>
+        <v>43961</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -12420,7 +12418,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -12440,11 +12438,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -12474,7 +12472,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -12491,11 +12489,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -12525,7 +12523,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -12542,11 +12540,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43972</v>
+        <v>43973</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -12576,7 +12574,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -12593,11 +12591,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43976</v>
+        <v>43977</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -12627,7 +12625,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -12644,11 +12642,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43980</v>
+        <v>43981</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -12678,7 +12676,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -12695,11 +12693,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -12729,7 +12727,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -12746,11 +12744,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -12780,7 +12778,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -12797,11 +12795,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -12831,7 +12829,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -12848,11 +12846,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43996</v>
+        <v>43997</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -12882,7 +12880,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -12899,11 +12897,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -12933,7 +12931,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -12950,11 +12948,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -12984,7 +12982,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -13425,11 +13423,11 @@
       </c>
       <c r="C59" s="57">
         <f t="shared" ref="C59:C70" ca="1" si="30">IF(M58="S",TODAY()+A$55,C58+4)</f>
-        <v>43945</v>
+        <v>43946</v>
       </c>
       <c r="D59" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E59" s="4">
         <v>7</v>
@@ -13459,7 +13457,7 @@
       </c>
       <c r="L59" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M59" s="63" t="s">
         <v>49</v>
@@ -13479,11 +13477,11 @@
       </c>
       <c r="C60" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43949</v>
+        <v>43950</v>
       </c>
       <c r="D60" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -13513,7 +13511,7 @@
       </c>
       <c r="L60" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M60" s="63" t="s">
         <v>49</v>
@@ -13533,11 +13531,11 @@
       </c>
       <c r="C61" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="D61" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -13567,7 +13565,7 @@
       </c>
       <c r="L61" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
@@ -13587,11 +13585,11 @@
       </c>
       <c r="C62" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D62" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -13621,7 +13619,7 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
@@ -13641,11 +13639,11 @@
       </c>
       <c r="C63" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -13675,7 +13673,7 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
@@ -13692,11 +13690,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -13726,7 +13724,7 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
@@ -13743,11 +13741,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -13777,7 +13775,7 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
@@ -13794,11 +13792,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -13828,7 +13826,7 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
@@ -13845,11 +13843,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -13879,7 +13877,7 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
@@ -13896,11 +13894,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43981</v>
+        <v>43982</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -13930,7 +13928,7 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
@@ -13947,11 +13945,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -13981,7 +13979,7 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
@@ -13998,11 +13996,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43989</v>
+        <v>43990</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -14032,7 +14030,7 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43989</v>
+        <v>43990</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Implementados os arquivos do Capítulo 9 sobre Ler e escrever em idiomas naturais
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C985CBF8-864B-4D88-8185-4486633E11F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897147E2-C4FB-42A6-8CE3-B7EFCA1E3DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6320,7 +6320,7 @@
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62:G63"/>
+      <selection activeCell="B61" sqref="B61:N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8873,54 +8873,52 @@
       <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B61" s="57">
+      <c r="B61" s="72">
         <f t="shared" si="26"/>
         <v>43930</v>
       </c>
-      <c r="C61" s="57">
-        <f t="shared" ref="C60:C70" ca="1" si="30">IF(M60="S",TODAY()+A$55,C60+4)</f>
-        <v>43946</v>
-      </c>
-      <c r="D61" s="58">
-        <f t="shared" ca="1" si="29"/>
-        <v>16</v>
-      </c>
-      <c r="E61" s="4">
+      <c r="C61" s="72">
+        <v>43942</v>
+      </c>
+      <c r="D61" s="73">
+        <f t="shared" si="29"/>
+        <v>12</v>
+      </c>
+      <c r="E61" s="73">
         <v>9</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="73">
         <v>22</v>
       </c>
-      <c r="G61" s="60">
+      <c r="G61" s="74">
         <f t="shared" si="21"/>
         <v>400</v>
       </c>
-      <c r="H61" s="69">
-        <f t="shared" ref="H60:H70" si="31">G61</f>
-        <v>400</v>
-      </c>
-      <c r="I61" s="69">
+      <c r="H61" s="74">
+        <v>238</v>
+      </c>
+      <c r="I61" s="74">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J61" s="61">
+        <v>162</v>
+      </c>
+      <c r="J61" s="73">
         <f t="shared" si="23"/>
         <v>33</v>
       </c>
-      <c r="K61" s="61">
+      <c r="K61" s="73">
         <f t="shared" si="24"/>
         <v>39</v>
       </c>
-      <c r="L61" s="57">
-        <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
-      </c>
-      <c r="M61" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N61" s="63">
+      <c r="L61" s="72">
+        <f t="shared" si="25"/>
+        <v>43981</v>
+      </c>
+      <c r="M61" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N61" s="75">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8932,12 +8930,12 @@
         <v>43934</v>
       </c>
       <c r="C62" s="57">
-        <f t="shared" ca="1" si="30"/>
-        <v>43950</v>
+        <f t="shared" ref="C61:C70" ca="1" si="30">IF(M61="S",TODAY()+A$55,C61+4)</f>
+        <v>43946</v>
       </c>
       <c r="D62" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -8950,7 +8948,7 @@
         <v>400</v>
       </c>
       <c r="H62" s="69">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="H61:H70" si="31">G62</f>
         <v>400</v>
       </c>
       <c r="I62" s="69">
@@ -8967,14 +8965,14 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N62" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8987,11 +8985,11 @@
       </c>
       <c r="C63" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43954</v>
+        <v>43950</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -9021,14 +9019,14 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N63" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9038,11 +9036,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43958</v>
+        <v>43954</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -9072,14 +9070,14 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N64" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9089,11 +9087,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43962</v>
+        <v>43958</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -9123,14 +9121,14 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N65" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9140,11 +9138,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43966</v>
+        <v>43962</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -9174,14 +9172,14 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N66" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9191,11 +9189,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43970</v>
+        <v>43966</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -9225,14 +9223,14 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N67" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9242,11 +9240,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43974</v>
+        <v>43970</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -9276,14 +9274,14 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N68" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9293,11 +9291,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43978</v>
+        <v>43974</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9327,14 +9325,14 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43985</v>
+        <v>43981</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9344,11 +9342,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43982</v>
+        <v>43978</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9378,14 +9376,14 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43982</v>
+        <v>43978</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
         <f t="shared" si="28"/>
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9407,11 +9405,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>5688</v>
+        <v>5526</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>1512</v>
+        <v>1674</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>

</xml_diff>

<commit_message>
Implementados os arquivos do Capitulo 9 do livro de webscraping, referente à rastreamento de logins e formulários
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897147E2-C4FB-42A6-8CE3-B7EFCA1E3DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BD2736-DD32-4643-B7C1-D80BA6704EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24960" yWindow="3840" windowWidth="21600" windowHeight="11775" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -6320,7 +6320,7 @@
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61:N61"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7520,11 +7520,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43945</v>
+        <v>43946</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -7554,7 +7554,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -7574,11 +7574,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43949</v>
+        <v>43950</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -7608,7 +7608,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -7628,11 +7628,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -7682,11 +7682,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -7716,7 +7716,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -7736,11 +7736,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -7790,11 +7790,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -7824,7 +7824,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -7841,11 +7841,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -7892,11 +7892,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -7943,11 +7943,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -7994,11 +7994,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43981</v>
+        <v>43982</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -8028,7 +8028,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -8045,11 +8045,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -8096,11 +8096,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43989</v>
+        <v>43990</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -8130,7 +8130,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -8147,11 +8147,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -8198,11 +8198,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -8232,7 +8232,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -8249,11 +8249,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -8283,7 +8283,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -8300,11 +8300,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -8925,54 +8925,52 @@
       <c r="A62" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B62" s="57">
+      <c r="B62" s="72">
         <f t="shared" si="26"/>
         <v>43934</v>
       </c>
-      <c r="C62" s="57">
-        <f t="shared" ref="C61:C70" ca="1" si="30">IF(M61="S",TODAY()+A$55,C61+4)</f>
-        <v>43946</v>
-      </c>
-      <c r="D62" s="58">
-        <f t="shared" ca="1" si="29"/>
-        <v>12</v>
-      </c>
-      <c r="E62" s="4">
+      <c r="C62" s="72">
+        <v>43943</v>
+      </c>
+      <c r="D62" s="73">
+        <f t="shared" si="29"/>
+        <v>9</v>
+      </c>
+      <c r="E62" s="73">
         <v>10</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62" s="73">
         <v>10</v>
       </c>
-      <c r="G62" s="60">
+      <c r="G62" s="74">
         <f t="shared" si="21"/>
         <v>400</v>
       </c>
-      <c r="H62" s="69">
-        <f t="shared" ref="H61:H70" si="31">G62</f>
-        <v>400</v>
-      </c>
-      <c r="I62" s="69">
+      <c r="H62" s="74">
+        <v>91</v>
+      </c>
+      <c r="I62" s="74">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="61">
+        <v>309</v>
+      </c>
+      <c r="J62" s="73">
         <f t="shared" si="23"/>
         <v>37</v>
       </c>
-      <c r="K62" s="61">
+      <c r="K62" s="73">
         <f t="shared" si="24"/>
         <v>35</v>
       </c>
-      <c r="L62" s="57">
-        <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
-      </c>
-      <c r="M62" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N62" s="63">
+      <c r="L62" s="72">
+        <f t="shared" si="25"/>
+        <v>43978</v>
+      </c>
+      <c r="M62" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N62" s="75">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
@@ -8984,12 +8982,12 @@
         <v>43938</v>
       </c>
       <c r="C63" s="57">
-        <f t="shared" ca="1" si="30"/>
-        <v>43950</v>
+        <f t="shared" ref="C62:C70" ca="1" si="30">IF(M62="S",TODAY()+A$55,C62+4)</f>
+        <v>43947</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -9002,7 +9000,7 @@
         <v>400</v>
       </c>
       <c r="H63" s="69">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="H62:H70" si="31">G63</f>
         <v>400</v>
       </c>
       <c r="I63" s="69">
@@ -9019,14 +9017,14 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N63" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9036,11 +9034,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43954</v>
+        <v>43951</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -9070,14 +9068,14 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N64" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9087,11 +9085,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43958</v>
+        <v>43955</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -9121,14 +9119,14 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N65" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9138,11 +9136,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43962</v>
+        <v>43959</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -9172,14 +9170,14 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N66" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9189,11 +9187,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43966</v>
+        <v>43963</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -9223,14 +9221,14 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N67" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9240,11 +9238,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43970</v>
+        <v>43967</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -9274,14 +9272,14 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N68" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9291,11 +9289,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43974</v>
+        <v>43971</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9325,14 +9323,14 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43981</v>
+        <v>43978</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9342,11 +9340,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9376,14 +9374,14 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
         <f t="shared" si="28"/>
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9405,11 +9403,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>5526</v>
+        <v>5217</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>1674</v>
+        <v>1983</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>
@@ -12166,11 +12164,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43945</v>
+        <v>43946</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -12200,7 +12198,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -12220,11 +12218,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43949</v>
+        <v>43950</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -12254,7 +12252,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -12274,11 +12272,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -12308,7 +12306,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -12328,11 +12326,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -12362,7 +12360,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -12382,11 +12380,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -12416,7 +12414,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -12436,11 +12434,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -12470,7 +12468,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -12487,11 +12485,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -12521,7 +12519,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -12538,11 +12536,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -12572,7 +12570,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -12589,11 +12587,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -12623,7 +12621,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -12640,11 +12638,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43981</v>
+        <v>43982</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -12674,7 +12672,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -12691,11 +12689,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -12725,7 +12723,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -12742,11 +12740,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43989</v>
+        <v>43990</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -12776,7 +12774,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -12793,11 +12791,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -12827,7 +12825,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -12844,11 +12842,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -12878,7 +12876,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -12895,11 +12893,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -12929,7 +12927,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -12946,11 +12944,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -12980,7 +12978,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -13421,11 +13419,11 @@
       </c>
       <c r="C59" s="57">
         <f t="shared" ref="C59:C70" ca="1" si="30">IF(M58="S",TODAY()+A$55,C58+4)</f>
-        <v>43946</v>
+        <v>43947</v>
       </c>
       <c r="D59" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E59" s="4">
         <v>7</v>
@@ -13455,7 +13453,7 @@
       </c>
       <c r="L59" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M59" s="63" t="s">
         <v>49</v>
@@ -13475,11 +13473,11 @@
       </c>
       <c r="C60" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="D60" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -13509,7 +13507,7 @@
       </c>
       <c r="L60" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M60" s="63" t="s">
         <v>49</v>
@@ -13529,11 +13527,11 @@
       </c>
       <c r="C61" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="D61" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -13563,7 +13561,7 @@
       </c>
       <c r="L61" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
@@ -13583,11 +13581,11 @@
       </c>
       <c r="C62" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D62" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -13617,7 +13615,7 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
@@ -13637,11 +13635,11 @@
       </c>
       <c r="C63" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43962</v>
+        <v>43963</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -13671,7 +13669,7 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
@@ -13688,11 +13686,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -13722,7 +13720,7 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
@@ -13739,11 +13737,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -13773,7 +13771,7 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
@@ -13790,11 +13788,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43974</v>
+        <v>43975</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -13824,7 +13822,7 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
@@ -13841,11 +13839,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43978</v>
+        <v>43979</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -13875,7 +13873,7 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
@@ -13892,11 +13890,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -13926,7 +13924,7 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
@@ -13943,11 +13941,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -13977,7 +13975,7 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
@@ -13994,11 +13992,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -14028,7 +14026,7 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Implementado os scripts python referentes ao Capítulo 11 do Livro de Web Scraping sobre Scraping de Javascript
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BD2736-DD32-4643-B7C1-D80BA6704EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD147B32-334C-4BAA-8DFA-BDE3DB2245AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24960" yWindow="3840" windowWidth="21600" windowHeight="11775" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6319,8 +6319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7520,11 +7520,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43946</v>
+        <v>43947</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -7554,7 +7554,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -7574,11 +7574,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -7608,7 +7608,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -7628,11 +7628,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -7682,11 +7682,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -7716,7 +7716,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -7736,11 +7736,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43962</v>
+        <v>43963</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -7790,11 +7790,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -7824,7 +7824,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -7841,11 +7841,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -7892,11 +7892,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43974</v>
+        <v>43975</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -7943,11 +7943,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43978</v>
+        <v>43979</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -7994,11 +7994,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -8028,7 +8028,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -8045,11 +8045,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -8079,7 +8079,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -8096,11 +8096,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -8130,7 +8130,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -8147,11 +8147,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -8198,11 +8198,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -8232,7 +8232,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -8249,11 +8249,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -8283,7 +8283,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -8300,11 +8300,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -8977,54 +8977,52 @@
       <c r="A63" s="1">
         <v>100</v>
       </c>
-      <c r="B63" s="57">
+      <c r="B63" s="72">
         <f t="shared" si="26"/>
         <v>43938</v>
       </c>
-      <c r="C63" s="57">
-        <f t="shared" ref="C62:C70" ca="1" si="30">IF(M62="S",TODAY()+A$55,C62+4)</f>
-        <v>43947</v>
-      </c>
-      <c r="D63" s="58">
-        <f t="shared" ca="1" si="29"/>
-        <v>9</v>
-      </c>
-      <c r="E63" s="4">
+      <c r="C63" s="72">
+        <v>43944</v>
+      </c>
+      <c r="D63" s="73">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="E63" s="73">
         <v>11</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="73">
         <v>16</v>
       </c>
-      <c r="G63" s="60">
+      <c r="G63" s="74">
         <f t="shared" si="21"/>
         <v>400</v>
       </c>
-      <c r="H63" s="69">
-        <f t="shared" ref="H62:H70" si="31">G63</f>
-        <v>400</v>
-      </c>
-      <c r="I63" s="69">
+      <c r="H63" s="74">
+        <v>115</v>
+      </c>
+      <c r="I63" s="74">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J63" s="61">
+        <v>285</v>
+      </c>
+      <c r="J63" s="73">
         <f t="shared" si="23"/>
         <v>41</v>
       </c>
-      <c r="K63" s="61">
+      <c r="K63" s="73">
         <f t="shared" si="24"/>
         <v>31</v>
       </c>
-      <c r="L63" s="57">
-        <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
-      </c>
-      <c r="M63" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N63" s="63">
+      <c r="L63" s="72">
+        <f t="shared" si="25"/>
+        <v>43975</v>
+      </c>
+      <c r="M63" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N63" s="75">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9033,12 +9031,12 @@
         <v>43942</v>
       </c>
       <c r="C64" s="57">
-        <f t="shared" ca="1" si="30"/>
-        <v>43951</v>
+        <f t="shared" ref="C63:C70" ca="1" si="30">IF(M63="S",TODAY()+A$55,C63+4)</f>
+        <v>43948</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -9051,7 +9049,7 @@
         <v>400</v>
       </c>
       <c r="H64" s="69">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="H63:H70" si="31">G64</f>
         <v>400</v>
       </c>
       <c r="I64" s="69">
@@ -9068,14 +9066,14 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N64" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9085,11 +9083,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43955</v>
+        <v>43952</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -9119,14 +9117,14 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N65" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9136,11 +9134,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43959</v>
+        <v>43956</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -9170,14 +9168,14 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N66" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9187,11 +9185,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43963</v>
+        <v>43960</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -9221,14 +9219,14 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N67" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9238,11 +9236,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43967</v>
+        <v>43964</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -9272,14 +9270,14 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N68" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9289,11 +9287,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43971</v>
+        <v>43968</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9323,14 +9321,14 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43978</v>
+        <v>43975</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9340,11 +9338,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43975</v>
+        <v>43972</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9374,14 +9372,14 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43975</v>
+        <v>43972</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
         <f t="shared" si="28"/>
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9403,11 +9401,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>5217</v>
+        <v>4932</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>1983</v>
+        <v>2268</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>
@@ -12164,11 +12162,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43946</v>
+        <v>43947</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -12198,7 +12196,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -12218,11 +12216,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -12252,7 +12250,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -12272,11 +12270,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -12306,7 +12304,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -12326,11 +12324,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -12360,7 +12358,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -12380,11 +12378,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43962</v>
+        <v>43963</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -12414,7 +12412,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -12434,11 +12432,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -12468,7 +12466,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -12485,11 +12483,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -12519,7 +12517,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -12536,11 +12534,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43974</v>
+        <v>43975</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -12570,7 +12568,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -12587,11 +12585,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43978</v>
+        <v>43979</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -12621,7 +12619,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -12638,11 +12636,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -12672,7 +12670,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -12689,11 +12687,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -12723,7 +12721,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -12740,11 +12738,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -12774,7 +12772,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -12791,11 +12789,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -12825,7 +12823,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -12842,11 +12840,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -12876,7 +12874,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -12893,11 +12891,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -12927,7 +12925,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -12944,11 +12942,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -12978,7 +12976,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -13419,11 +13417,11 @@
       </c>
       <c r="C59" s="57">
         <f t="shared" ref="C59:C70" ca="1" si="30">IF(M58="S",TODAY()+A$55,C58+4)</f>
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="D59" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E59" s="4">
         <v>7</v>
@@ -13453,7 +13451,7 @@
       </c>
       <c r="L59" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M59" s="63" t="s">
         <v>49</v>
@@ -13473,11 +13471,11 @@
       </c>
       <c r="C60" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="D60" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -13507,7 +13505,7 @@
       </c>
       <c r="L60" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M60" s="63" t="s">
         <v>49</v>
@@ -13527,11 +13525,11 @@
       </c>
       <c r="C61" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="D61" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -13561,7 +13559,7 @@
       </c>
       <c r="L61" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
@@ -13581,11 +13579,11 @@
       </c>
       <c r="C62" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="D62" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -13615,7 +13613,7 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
@@ -13635,11 +13633,11 @@
       </c>
       <c r="C63" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43963</v>
+        <v>43964</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -13669,7 +13667,7 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
@@ -13686,11 +13684,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43967</v>
+        <v>43968</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -13720,7 +13718,7 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
@@ -13737,11 +13735,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -13771,7 +13769,7 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
@@ -13788,11 +13786,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43975</v>
+        <v>43976</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -13822,7 +13820,7 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
@@ -13839,11 +13837,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43979</v>
+        <v>43980</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -13873,7 +13871,7 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
@@ -13890,11 +13888,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43983</v>
+        <v>43984</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -13924,7 +13922,7 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
@@ -13941,11 +13939,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -13975,7 +13973,7 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
@@ -13992,11 +13990,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -14026,7 +14024,7 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Implementados os arquivos do CApítulo 16 relativo à web crawling em parealelo
</commit_message>
<xml_diff>
--- a/planejamento.xlsx
+++ b/planejamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Estudos\200DaysProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AEB3B7-465F-47B7-8201-2BA6CD89B3E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3B6322-83F9-491A-8D65-4619E5282849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -721,6 +721,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -751,7 +752,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4886,11 +4886,11 @@
       <c r="H4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="100">
+      <c r="I4" s="101">
         <f>J3+1</f>
         <v>43900</v>
       </c>
-      <c r="J4" s="94">
+      <c r="J4" s="95">
         <f>I4+D4+D5+D6-1</f>
         <v>43971</v>
       </c>
@@ -4918,8 +4918,8 @@
       <c r="H5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="100"/>
-      <c r="J5" s="95"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="96"/>
       <c r="L5" s="86"/>
     </row>
     <row r="6" spans="1:12 1025:1025" s="77" customFormat="1" x14ac:dyDescent="0.25">
@@ -4944,8 +4944,8 @@
       <c r="H6" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="95"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="96"/>
       <c r="L6" s="86"/>
     </row>
     <row r="7" spans="1:12 1025:1025" s="80" customFormat="1" x14ac:dyDescent="0.25">
@@ -4970,11 +4970,11 @@
       <c r="H7" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="100">
+      <c r="I7" s="101">
         <f>J4+1</f>
         <v>43972</v>
       </c>
-      <c r="J7" s="96">
+      <c r="J7" s="97">
         <f>I7+D7+D8-1</f>
         <v>44038</v>
       </c>
@@ -5002,8 +5002,8 @@
       <c r="H8" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="97"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="98"/>
       <c r="L8" s="87"/>
     </row>
     <row r="9" spans="1:12 1025:1025" s="83" customFormat="1" x14ac:dyDescent="0.25">
@@ -5028,11 +5028,11 @@
       <c r="H9" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="100">
+      <c r="I9" s="101">
         <f>J7+1</f>
         <v>44039</v>
       </c>
-      <c r="J9" s="98">
+      <c r="J9" s="99">
         <f>I9+D9+D10-1</f>
         <v>44068</v>
       </c>
@@ -5060,8 +5060,8 @@
       <c r="H10" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="99"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="100"/>
       <c r="L10" s="88"/>
     </row>
     <row r="11" spans="1:12 1025:1025" x14ac:dyDescent="0.25">
@@ -6346,7 +6346,7 @@
   <dimension ref="A1:AMJ148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O67" sqref="O67"/>
+      <selection activeCell="B68" sqref="B68:O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6369,18 +6369,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="H1" s="103" t="s">
+      <c r="B1" s="103"/>
+      <c r="H1" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
     </row>
     <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -7219,10 +7219,10 @@
       <c r="I24" s="47"/>
     </row>
     <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="101"/>
+      <c r="B25" s="102"/>
     </row>
     <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43956</v>
+        <v>43965</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44021</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -7601,11 +7601,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43960</v>
+        <v>43969</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44022</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -7655,11 +7655,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43964</v>
+        <v>43973</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -7689,7 +7689,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44023</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -7709,11 +7709,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43968</v>
+        <v>43977</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -7743,7 +7743,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44015</v>
+        <v>44024</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -7763,11 +7763,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43972</v>
+        <v>43981</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -7797,7 +7797,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44016</v>
+        <v>44025</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -7817,11 +7817,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43976</v>
+        <v>43985</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -7851,7 +7851,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44017</v>
+        <v>44026</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -7868,11 +7868,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43980</v>
+        <v>43989</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -7902,7 +7902,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44018</v>
+        <v>44027</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -7919,11 +7919,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43984</v>
+        <v>43993</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -7953,7 +7953,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44019</v>
+        <v>44028</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -7970,11 +7970,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43988</v>
+        <v>43997</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -8004,7 +8004,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44020</v>
+        <v>44029</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -8021,11 +8021,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43992</v>
+        <v>44001</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -8055,7 +8055,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44021</v>
+        <v>44030</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -8072,11 +8072,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43996</v>
+        <v>44005</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -8106,7 +8106,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44022</v>
+        <v>44031</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -8123,11 +8123,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44000</v>
+        <v>44009</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -8157,7 +8157,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44023</v>
+        <v>44032</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -8174,11 +8174,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -8208,7 +8208,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44024</v>
+        <v>44033</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -8225,11 +8225,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44008</v>
+        <v>44017</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -8259,7 +8259,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44025</v>
+        <v>44034</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -8276,11 +8276,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44012</v>
+        <v>44021</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -8310,7 +8310,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44026</v>
+        <v>44035</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -8327,11 +8327,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44016</v>
+        <v>44025</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -8361,7 +8361,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44016</v>
+        <v>44025</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -8420,11 +8420,11 @@
       <c r="L49" s="47"/>
     </row>
     <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="101"/>
-      <c r="C51" s="101"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="102"/>
     </row>
     <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
@@ -9300,70 +9300,68 @@
         <v>43968</v>
       </c>
       <c r="M67" s="75" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N67" s="75">
         <f t="shared" si="28"/>
-        <v>244</v>
-      </c>
-      <c r="O67" s="104">
+        <v>257</v>
+      </c>
+      <c r="O67" s="94">
         <f t="shared" si="29"/>
         <v>7.4</v>
       </c>
     </row>
     <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="B68" s="57">
+      <c r="B68" s="72">
         <f t="shared" si="26"/>
         <v>43958</v>
       </c>
-      <c r="C68" s="57">
-        <f t="shared" ref="C67:C70" ca="1" si="31">IF(M67="S",TODAY()+A$55,C67+4)</f>
-        <v>43957</v>
-      </c>
-      <c r="D68" s="58">
-        <f t="shared" ca="1" si="30"/>
-        <v>-1</v>
-      </c>
-      <c r="E68" s="4">
+      <c r="C68" s="72">
+        <v>43962</v>
+      </c>
+      <c r="D68" s="73">
+        <f t="shared" si="30"/>
+        <v>4</v>
+      </c>
+      <c r="E68" s="73">
         <v>16</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68" s="73">
         <v>19</v>
       </c>
-      <c r="G68" s="60">
+      <c r="G68" s="74">
         <f t="shared" si="21"/>
         <v>400</v>
       </c>
-      <c r="H68" s="69">
-        <f t="shared" ref="H67:H70" si="32">G68</f>
-        <v>400</v>
-      </c>
-      <c r="I68" s="69">
+      <c r="H68" s="74">
+        <v>153</v>
+      </c>
+      <c r="I68" s="74">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J68" s="61">
+        <v>247</v>
+      </c>
+      <c r="J68" s="73">
         <f t="shared" si="23"/>
         <v>61</v>
       </c>
-      <c r="K68" s="61">
+      <c r="K68" s="73">
         <f t="shared" si="24"/>
         <v>11</v>
       </c>
-      <c r="L68" s="57">
-        <f t="shared" ca="1" si="25"/>
-        <v>43968</v>
-      </c>
-      <c r="M68" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N68" s="63">
+      <c r="L68" s="72">
+        <f t="shared" si="25"/>
+        <v>43973</v>
+      </c>
+      <c r="M68" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N68" s="75">
         <f t="shared" si="28"/>
-        <v>244</v>
-      </c>
-      <c r="O68" s="93">
+        <v>276</v>
+      </c>
+      <c r="O68" s="94">
         <f t="shared" si="29"/>
-        <v>21.1</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="69" spans="1:1024" x14ac:dyDescent="0.25">
@@ -9372,12 +9370,12 @@
         <v>43962</v>
       </c>
       <c r="C69" s="57">
-        <f t="shared" ca="1" si="31"/>
-        <v>43961</v>
+        <f t="shared" ref="C68:C70" ca="1" si="31">IF(M68="S",TODAY()+A$55,C68+4)</f>
+        <v>43966</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="30"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -9390,7 +9388,7 @@
         <v>400</v>
       </c>
       <c r="H69" s="69">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="H68:H70" si="32">G69</f>
         <v>400</v>
       </c>
       <c r="I69" s="69">
@@ -9407,14 +9405,14 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43968</v>
+        <v>43973</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N69" s="63">
         <f t="shared" si="28"/>
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="O69" s="93">
         <f t="shared" si="29"/>
@@ -9428,11 +9426,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="31"/>
-        <v>43965</v>
+        <v>43970</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="30"/>
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -9462,14 +9460,14 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>43965</v>
+        <v>43970</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
       </c>
       <c r="N70" s="63">
         <f t="shared" si="28"/>
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="O70" s="93">
         <f t="shared" si="29"/>
@@ -9495,11 +9493,11 @@
       </c>
       <c r="H71" s="67">
         <f>SUM(H53:H70)</f>
-        <v>3933</v>
+        <v>3686</v>
       </c>
       <c r="I71" s="67">
         <f>SUM(I53:I70)</f>
-        <v>3267</v>
+        <v>3514</v>
       </c>
       <c r="J71" s="68">
         <f>SUM(J53:J70)</f>
@@ -9515,10 +9513,10 @@
       <c r="L72" s="71"/>
     </row>
     <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A73" s="101" t="s">
+      <c r="A73" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="101"/>
+      <c r="B73" s="102"/>
       <c r="K73" s="71"/>
       <c r="L73" s="71"/>
     </row>
@@ -10732,10 +10730,10 @@
       <c r="J98" s="47"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" s="101" t="s">
+      <c r="A100" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="B100" s="101"/>
+      <c r="B100" s="102"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="19" t="s">
@@ -12023,10 +12021,10 @@
       <c r="N125" s="47"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A128" s="101" t="s">
+      <c r="A128" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="B128" s="101"/>
+      <c r="B128" s="102"/>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="19" t="s">
@@ -13625,18 +13623,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="H1" s="103" t="s">
+      <c r="B1" s="103"/>
+      <c r="H1" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
     </row>
     <row r="2" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -14475,10 +14473,10 @@
       <c r="I24" s="47"/>
     </row>
     <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="101"/>
+      <c r="B25" s="102"/>
     </row>
     <row r="26" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
@@ -14803,11 +14801,11 @@
       </c>
       <c r="C32" s="57">
         <f ca="1">IF(M31="S",TODAY()+A$29,C31+4)</f>
-        <v>43956</v>
+        <v>43965</v>
       </c>
       <c r="D32" s="58">
         <f t="shared" ref="D32:D47" ca="1" si="18">IF(C32="",D31,C32-B32)</f>
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E32" s="4">
         <v>6</v>
@@ -14837,7 +14835,7 @@
       </c>
       <c r="L32" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44012</v>
+        <v>44021</v>
       </c>
       <c r="M32" s="63" t="s">
         <v>49</v>
@@ -14857,11 +14855,11 @@
       </c>
       <c r="C33" s="57">
         <f t="shared" ref="C33:C47" ca="1" si="20">IF(M32="S",TODAY()+A$29,C32+4)</f>
-        <v>43960</v>
+        <v>43969</v>
       </c>
       <c r="D33" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E33" s="4">
         <v>7</v>
@@ -14891,7 +14889,7 @@
       </c>
       <c r="L33" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44013</v>
+        <v>44022</v>
       </c>
       <c r="M33" s="63" t="s">
         <v>49</v>
@@ -14911,11 +14909,11 @@
       </c>
       <c r="C34" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43964</v>
+        <v>43973</v>
       </c>
       <c r="D34" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -14945,7 +14943,7 @@
       </c>
       <c r="L34" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44014</v>
+        <v>44023</v>
       </c>
       <c r="M34" s="63" t="s">
         <v>49</v>
@@ -14965,11 +14963,11 @@
       </c>
       <c r="C35" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43968</v>
+        <v>43977</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E35" s="4">
         <v>9</v>
@@ -14999,7 +14997,7 @@
       </c>
       <c r="L35" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44015</v>
+        <v>44024</v>
       </c>
       <c r="M35" s="63" t="s">
         <v>49</v>
@@ -15019,11 +15017,11 @@
       </c>
       <c r="C36" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43972</v>
+        <v>43981</v>
       </c>
       <c r="D36" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E36" s="4">
         <v>10</v>
@@ -15053,7 +15051,7 @@
       </c>
       <c r="L36" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44016</v>
+        <v>44025</v>
       </c>
       <c r="M36" s="63" t="s">
         <v>49</v>
@@ -15073,11 +15071,11 @@
       </c>
       <c r="C37" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43976</v>
+        <v>43985</v>
       </c>
       <c r="D37" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E37" s="4">
         <v>11</v>
@@ -15107,7 +15105,7 @@
       </c>
       <c r="L37" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44017</v>
+        <v>44026</v>
       </c>
       <c r="M37" s="63" t="s">
         <v>49</v>
@@ -15124,11 +15122,11 @@
       </c>
       <c r="C38" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43980</v>
+        <v>43989</v>
       </c>
       <c r="D38" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E38" s="4">
         <v>12</v>
@@ -15158,7 +15156,7 @@
       </c>
       <c r="L38" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44018</v>
+        <v>44027</v>
       </c>
       <c r="M38" s="63" t="s">
         <v>49</v>
@@ -15175,11 +15173,11 @@
       </c>
       <c r="C39" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43984</v>
+        <v>43993</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E39" s="4">
         <v>13</v>
@@ -15209,7 +15207,7 @@
       </c>
       <c r="L39" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44019</v>
+        <v>44028</v>
       </c>
       <c r="M39" s="63" t="s">
         <v>49</v>
@@ -15226,11 +15224,11 @@
       </c>
       <c r="C40" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43988</v>
+        <v>43997</v>
       </c>
       <c r="D40" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E40" s="4">
         <v>14</v>
@@ -15260,7 +15258,7 @@
       </c>
       <c r="L40" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44020</v>
+        <v>44029</v>
       </c>
       <c r="M40" s="63" t="s">
         <v>49</v>
@@ -15277,11 +15275,11 @@
       </c>
       <c r="C41" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43992</v>
+        <v>44001</v>
       </c>
       <c r="D41" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E41" s="4">
         <v>15</v>
@@ -15311,7 +15309,7 @@
       </c>
       <c r="L41" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44021</v>
+        <v>44030</v>
       </c>
       <c r="M41" s="63" t="s">
         <v>49</v>
@@ -15328,11 +15326,11 @@
       </c>
       <c r="C42" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>43996</v>
+        <v>44005</v>
       </c>
       <c r="D42" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E42" s="4">
         <v>16</v>
@@ -15362,7 +15360,7 @@
       </c>
       <c r="L42" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44022</v>
+        <v>44031</v>
       </c>
       <c r="M42" s="63" t="s">
         <v>49</v>
@@ -15379,11 +15377,11 @@
       </c>
       <c r="C43" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44000</v>
+        <v>44009</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E43" s="4">
         <v>17</v>
@@ -15413,7 +15411,7 @@
       </c>
       <c r="L43" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44023</v>
+        <v>44032</v>
       </c>
       <c r="M43" s="63" t="s">
         <v>49</v>
@@ -15430,11 +15428,11 @@
       </c>
       <c r="C44" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="D44" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E44" s="4">
         <v>18</v>
@@ -15464,7 +15462,7 @@
       </c>
       <c r="L44" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44024</v>
+        <v>44033</v>
       </c>
       <c r="M44" s="63" t="s">
         <v>49</v>
@@ -15481,11 +15479,11 @@
       </c>
       <c r="C45" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44008</v>
+        <v>44017</v>
       </c>
       <c r="D45" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E45" s="4">
         <v>19</v>
@@ -15515,7 +15513,7 @@
       </c>
       <c r="L45" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44025</v>
+        <v>44034</v>
       </c>
       <c r="M45" s="63" t="s">
         <v>49</v>
@@ -15532,11 +15530,11 @@
       </c>
       <c r="C46" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44012</v>
+        <v>44021</v>
       </c>
       <c r="D46" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>53</v>
@@ -15566,7 +15564,7 @@
       </c>
       <c r="L46" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44026</v>
+        <v>44035</v>
       </c>
       <c r="M46" s="63" t="s">
         <v>49</v>
@@ -15583,11 +15581,11 @@
       </c>
       <c r="C47" s="57">
         <f t="shared" ca="1" si="20"/>
-        <v>44016</v>
+        <v>44025</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" ca="1" si="18"/>
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>54</v>
@@ -15617,7 +15615,7 @@
       </c>
       <c r="L47" s="62">
         <f t="shared" ca="1" si="15"/>
-        <v>44016</v>
+        <v>44025</v>
       </c>
       <c r="M47" s="63" t="s">
         <v>49</v>
@@ -15676,11 +15674,11 @@
       <c r="L49" s="47"/>
     </row>
     <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="101"/>
-      <c r="C51" s="101"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="102"/>
     </row>
     <row r="52" spans="1:1024" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
@@ -16058,11 +16056,11 @@
       </c>
       <c r="C59" s="57">
         <f t="shared" ref="C59:C70" ca="1" si="30">IF(M58="S",TODAY()+A$55,C58+4)</f>
-        <v>43957</v>
+        <v>43966</v>
       </c>
       <c r="D59" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E59" s="4">
         <v>7</v>
@@ -16092,7 +16090,7 @@
       </c>
       <c r="L59" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M59" s="63" t="s">
         <v>49</v>
@@ -16112,11 +16110,11 @@
       </c>
       <c r="C60" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43961</v>
+        <v>43970</v>
       </c>
       <c r="D60" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -16146,7 +16144,7 @@
       </c>
       <c r="L60" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M60" s="63" t="s">
         <v>49</v>
@@ -16166,11 +16164,11 @@
       </c>
       <c r="C61" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43965</v>
+        <v>43974</v>
       </c>
       <c r="D61" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E61" s="4">
         <v>9</v>
@@ -16200,7 +16198,7 @@
       </c>
       <c r="L61" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M61" s="63" t="s">
         <v>49</v>
@@ -16220,11 +16218,11 @@
       </c>
       <c r="C62" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43969</v>
+        <v>43978</v>
       </c>
       <c r="D62" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E62" s="4">
         <v>10</v>
@@ -16254,7 +16252,7 @@
       </c>
       <c r="L62" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M62" s="63" t="s">
         <v>49</v>
@@ -16274,11 +16272,11 @@
       </c>
       <c r="C63" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43973</v>
+        <v>43982</v>
       </c>
       <c r="D63" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E63" s="4">
         <v>11</v>
@@ -16308,7 +16306,7 @@
       </c>
       <c r="L63" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M63" s="63" t="s">
         <v>49</v>
@@ -16325,11 +16323,11 @@
       </c>
       <c r="C64" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43977</v>
+        <v>43986</v>
       </c>
       <c r="D64" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E64" s="4">
         <v>12</v>
@@ -16359,7 +16357,7 @@
       </c>
       <c r="L64" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M64" s="63" t="s">
         <v>49</v>
@@ -16376,11 +16374,11 @@
       </c>
       <c r="C65" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43981</v>
+        <v>43990</v>
       </c>
       <c r="D65" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E65" s="4">
         <v>13</v>
@@ -16410,7 +16408,7 @@
       </c>
       <c r="L65" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M65" s="63" t="s">
         <v>49</v>
@@ -16427,11 +16425,11 @@
       </c>
       <c r="C66" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43985</v>
+        <v>43994</v>
       </c>
       <c r="D66" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E66" s="4">
         <v>14</v>
@@ -16461,7 +16459,7 @@
       </c>
       <c r="L66" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M66" s="63" t="s">
         <v>49</v>
@@ -16478,11 +16476,11 @@
       </c>
       <c r="C67" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43989</v>
+        <v>43998</v>
       </c>
       <c r="D67" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E67" s="4">
         <v>15</v>
@@ -16512,7 +16510,7 @@
       </c>
       <c r="L67" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M67" s="63" t="s">
         <v>49</v>
@@ -16529,11 +16527,11 @@
       </c>
       <c r="C68" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43993</v>
+        <v>44002</v>
       </c>
       <c r="D68" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E68" s="4">
         <v>16</v>
@@ -16563,7 +16561,7 @@
       </c>
       <c r="L68" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M68" s="63" t="s">
         <v>49</v>
@@ -16580,11 +16578,11 @@
       </c>
       <c r="C69" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>43997</v>
+        <v>44006</v>
       </c>
       <c r="D69" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E69" s="4">
         <v>17</v>
@@ -16614,7 +16612,7 @@
       </c>
       <c r="L69" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44004</v>
+        <v>44013</v>
       </c>
       <c r="M69" s="63" t="s">
         <v>49</v>
@@ -16631,11 +16629,11 @@
       </c>
       <c r="C70" s="57">
         <f t="shared" ca="1" si="30"/>
-        <v>44001</v>
+        <v>44010</v>
       </c>
       <c r="D70" s="58">
         <f t="shared" ca="1" si="29"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E70" s="4">
         <v>18</v>
@@ -16665,7 +16663,7 @@
       </c>
       <c r="L70" s="57">
         <f t="shared" ca="1" si="25"/>
-        <v>44001</v>
+        <v>44010</v>
       </c>
       <c r="M70" s="63" t="s">
         <v>49</v>
@@ -16714,10 +16712,10 @@
       <c r="L72" s="71"/>
     </row>
     <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A73" s="101" t="s">
+      <c r="A73" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="101"/>
+      <c r="B73" s="102"/>
       <c r="K73" s="71"/>
       <c r="L73" s="71"/>
     </row>

</xml_diff>